<commit_message>
Correction du fichier d'audit SEO
</commit_message>
<xml_diff>
--- a/Analyses/Modèle-audit-SEO.xlsx
+++ b/Analyses/Modèle-audit-SEO.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="49">
   <si>
     <t>Catégorie</t>
   </si>
@@ -178,9 +178,6 @@
     <t xml:space="preserve"> Contraste faible entre le texte ou logo et couleur de fond des  transparents dans page d'accueil.</t>
   </si>
   <si>
-    <t xml:space="preserve"> Les pages du site doivent être cohérente et l'utilisateur doit savoir où il se trouve.</t>
-  </si>
-  <si>
     <t>Présenter la même barre de 
 navigation sur les 2 pages avec un lien "Accueil" et un lien "Contact".
 Mettre le lien de la page différencié</t>
@@ -229,19 +226,22 @@
     <t>PERFORMANCE</t>
   </si>
   <si>
-    <t>?</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> ARIA</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> </t>
+    <t>X</t>
+  </si>
+  <si>
+    <t>Fait</t>
+  </si>
+  <si>
+    <t>Oui</t>
+  </si>
+  <si>
+    <t>Non</t>
   </si>
   <si>
     <r>
-      <t xml:space="preserve"> Barres de navigation dans les 2
- pages doivent être cohérente entre
- elles (Version </t>
+      <t xml:space="preserve">Barres de navigation dans les 2
+pages doivent être cohérente entre
+elles (Version </t>
     </r>
     <r>
       <rPr>
@@ -278,11 +278,11 @@
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
-      <t>) et préciser sur quelle page l'utilisateur se trouve.</t>
+      <t>)   et préciser sur quelle page l'utilisateur se trouve.</t>
     </r>
   </si>
   <si>
-    <t>X</t>
+    <t>Les pages du site doivent être cohérente et l'utilisateur doit savoir où il se trouve.</t>
   </si>
 </sst>
 </file>
@@ -356,7 +356,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -386,25 +386,24 @@
         <fgColor rgb="FFF2F2F2"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="12">
+  <borders count="14">
     <border>
       <left/>
       <right/>
       <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
       <bottom/>
       <diagonal/>
     </border>
@@ -445,7 +444,7 @@
       <right style="thin">
         <color indexed="64"/>
       </right>
-      <top style="medium">
+      <top style="thin">
         <color indexed="64"/>
       </top>
       <bottom style="thin">
@@ -457,13 +456,28 @@
       <left style="thin">
         <color indexed="64"/>
       </left>
-      <right style="thin">
+      <right style="medium">
         <color indexed="64"/>
       </right>
-      <top style="medium">
+      <top style="thin">
         <color indexed="64"/>
       </top>
       <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
@@ -472,12 +486,40 @@
       <left style="thin">
         <color indexed="64"/>
       </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
       <right style="medium">
         <color indexed="64"/>
       </right>
-      <top style="medium">
+      <top style="thin">
         <color indexed="64"/>
       </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
       <bottom style="thin">
         <color indexed="64"/>
       </bottom>
@@ -490,9 +532,7 @@
       <right style="thin">
         <color indexed="64"/>
       </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
+      <top/>
       <bottom style="thin">
         <color indexed="64"/>
       </bottom>
@@ -505,9 +545,7 @@
       <right style="medium">
         <color indexed="64"/>
       </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
+      <top/>
       <bottom style="thin">
         <color indexed="64"/>
       </bottom>
@@ -520,7 +558,7 @@
       <right style="thin">
         <color indexed="64"/>
       </right>
-      <top style="thin">
+      <top style="medium">
         <color indexed="64"/>
       </top>
       <bottom style="medium">
@@ -535,7 +573,7 @@
       <right style="thin">
         <color indexed="64"/>
       </right>
-      <top style="thin">
+      <top style="medium">
         <color indexed="64"/>
       </top>
       <bottom style="medium">
@@ -550,7 +588,7 @@
       <right style="medium">
         <color indexed="64"/>
       </right>
-      <top style="thin">
+      <top style="medium">
         <color indexed="64"/>
       </top>
       <bottom style="medium">
@@ -561,9 +599,9 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -583,89 +621,107 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -880,10 +936,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B2:AB993"/>
+  <dimension ref="B1:AB992"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="I18" sqref="I18:I20"/>
+      <selection activeCell="E38" sqref="E38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.33203125" defaultRowHeight="15" customHeight="1"/>
@@ -894,38 +950,41 @@
     <col min="4" max="4" width="27" style="2" customWidth="1"/>
     <col min="5" max="8" width="24.77734375" style="2" customWidth="1"/>
     <col min="9" max="9" width="7.77734375" style="4" customWidth="1"/>
-    <col min="10" max="10" width="10.5546875" style="5" customWidth="1"/>
+    <col min="10" max="10" width="10.5546875" style="3" customWidth="1"/>
     <col min="11" max="12" width="10.5546875" style="4" customWidth="1"/>
     <col min="13" max="28" width="10.5546875" style="2" customWidth="1"/>
     <col min="29" max="16384" width="11.33203125" style="2"/>
   </cols>
   <sheetData>
+    <row r="1" spans="2:28" ht="15" customHeight="1" thickBot="1"/>
     <row r="2" spans="2:28" ht="15.75" customHeight="1" thickBot="1">
-      <c r="B2" s="7" t="s">
+      <c r="B2" s="32" t="s">
         <v>14</v>
       </c>
-      <c r="C2" s="8" t="s">
+      <c r="C2" s="33" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="8" t="s">
+      <c r="D2" s="33" t="s">
         <v>1</v>
       </c>
-      <c r="E2" s="8" t="s">
+      <c r="E2" s="33" t="s">
         <v>2</v>
       </c>
-      <c r="F2" s="8" t="s">
+      <c r="F2" s="33" t="s">
         <v>3</v>
       </c>
-      <c r="G2" s="8" t="s">
+      <c r="G2" s="33" t="s">
         <v>4</v>
       </c>
-      <c r="H2" s="8" t="s">
+      <c r="H2" s="33" t="s">
         <v>5</v>
       </c>
-      <c r="I2" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="J2" s="32"/>
+      <c r="I2" s="34" t="s">
+        <v>38</v>
+      </c>
+      <c r="J2" s="35" t="s">
+        <v>44</v>
+      </c>
       <c r="K2" s="6"/>
       <c r="L2" s="6"/>
       <c r="M2" s="1"/>
@@ -946,193 +1005,153 @@
       <c r="AB2" s="1"/>
     </row>
     <row r="3" spans="2:28" ht="15.75" customHeight="1">
-      <c r="B3" s="24">
+      <c r="B3" s="28">
         <v>1</v>
       </c>
-      <c r="C3" s="21" t="s">
-        <v>43</v>
-      </c>
-      <c r="D3" s="21" t="s">
+      <c r="C3" s="19" t="s">
+        <v>42</v>
+      </c>
+      <c r="D3" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="E3" s="27" t="s">
+      <c r="E3" s="29" t="s">
         <v>16</v>
       </c>
-      <c r="F3" s="27" t="s">
+      <c r="F3" s="29" t="s">
+        <v>41</v>
+      </c>
+      <c r="G3" s="29" t="s">
+        <v>17</v>
+      </c>
+      <c r="H3" s="30"/>
+      <c r="I3" s="31">
+        <v>1</v>
+      </c>
+      <c r="J3" s="37" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="4" spans="2:28" ht="15.75" customHeight="1">
+      <c r="B4" s="8"/>
+      <c r="C4" s="7"/>
+      <c r="D4" s="7"/>
+      <c r="E4" s="9"/>
+      <c r="F4" s="9"/>
+      <c r="G4" s="9"/>
+      <c r="H4" s="9"/>
+      <c r="I4" s="20"/>
+      <c r="J4" s="38"/>
+    </row>
+    <row r="5" spans="2:28" ht="15.75" customHeight="1">
+      <c r="B5" s="10">
+        <v>2</v>
+      </c>
+      <c r="C5" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="G3" s="27" t="s">
-        <v>17</v>
-      </c>
-      <c r="H3" s="29"/>
-      <c r="I3" s="15">
-        <v>1</v>
-      </c>
-      <c r="K3" s="4">
-        <v>1</v>
-      </c>
-      <c r="L3" s="4">
-        <f>COUNTIF($I$3:$I$32,K3)</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="2:28" ht="15.75" customHeight="1">
-      <c r="B4" s="25"/>
-      <c r="C4" s="22"/>
-      <c r="D4" s="22"/>
-      <c r="E4" s="28"/>
-      <c r="F4" s="28"/>
-      <c r="G4" s="28"/>
-      <c r="H4" s="28"/>
-      <c r="I4" s="14"/>
-      <c r="K4" s="4">
+      <c r="D5" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="E5" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="F5" s="16"/>
+      <c r="G5" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="H5" s="13"/>
+      <c r="I5" s="21">
         <v>2</v>
       </c>
-      <c r="L4" s="4">
-        <f>COUNTIF($I$3:$I$32,K4)</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="2:28" ht="15.75" customHeight="1">
-      <c r="B5" s="26">
-        <v>2</v>
-      </c>
-      <c r="C5" s="16" t="s">
-        <v>43</v>
-      </c>
-      <c r="D5" s="19" t="s">
-        <v>8</v>
-      </c>
-      <c r="E5" s="20" t="s">
-        <v>16</v>
-      </c>
-      <c r="F5" s="31"/>
-      <c r="G5" s="20" t="s">
-        <v>18</v>
-      </c>
-      <c r="H5" s="19"/>
-      <c r="I5" s="13">
-        <v>2</v>
-      </c>
-      <c r="K5" s="4">
-        <v>3</v>
-      </c>
-      <c r="L5" s="4">
-        <f>COUNTIF($I$3:$I$32,K5)</f>
-        <v>1</v>
+      <c r="J5" s="38" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="6" spans="2:28" ht="15.75" customHeight="1">
-      <c r="B6" s="26"/>
-      <c r="C6" s="16"/>
-      <c r="D6" s="19"/>
-      <c r="E6" s="19"/>
-      <c r="F6" s="31"/>
-      <c r="G6" s="19"/>
-      <c r="H6" s="19"/>
-      <c r="I6" s="13"/>
-      <c r="K6" s="4">
-        <v>4</v>
-      </c>
-      <c r="L6" s="4">
-        <f>COUNTIF($I$3:$I$32,K6)</f>
-        <v>1</v>
-      </c>
+      <c r="B6" s="10"/>
+      <c r="C6" s="11"/>
+      <c r="D6" s="13"/>
+      <c r="E6" s="13"/>
+      <c r="F6" s="16"/>
+      <c r="G6" s="13"/>
+      <c r="H6" s="13"/>
+      <c r="I6" s="21"/>
+      <c r="J6" s="38"/>
     </row>
     <row r="7" spans="2:28" ht="15.75" customHeight="1">
-      <c r="B7" s="25">
+      <c r="B7" s="8">
         <v>3</v>
       </c>
       <c r="C7" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="D7" s="23" t="s">
+      <c r="D7" s="15" t="s">
         <v>27</v>
       </c>
-      <c r="E7" s="23" t="s">
+      <c r="E7" s="15" t="s">
         <v>24</v>
       </c>
       <c r="F7" s="17"/>
-      <c r="G7" s="23" t="s">
+      <c r="G7" s="15" t="s">
         <v>19</v>
       </c>
       <c r="H7" s="17"/>
-      <c r="I7" s="14">
+      <c r="I7" s="20">
         <v>6</v>
       </c>
-      <c r="K7" s="4">
-        <v>5</v>
-      </c>
-      <c r="L7" s="4">
-        <f>COUNTIF($I$3:$I$32,K7)</f>
-        <v>1</v>
+      <c r="J7" s="36" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="8" spans="2:28" ht="15.75" customHeight="1">
-      <c r="B8" s="25"/>
+      <c r="B8" s="8"/>
       <c r="C8" s="18"/>
       <c r="D8" s="17"/>
       <c r="E8" s="17"/>
       <c r="F8" s="17"/>
       <c r="G8" s="17"/>
       <c r="H8" s="17"/>
-      <c r="I8" s="14"/>
-      <c r="K8" s="4">
+      <c r="I8" s="20"/>
+      <c r="J8" s="36"/>
+    </row>
+    <row r="9" spans="2:28" ht="15.75" customHeight="1">
+      <c r="B9" s="10">
+        <v>4</v>
+      </c>
+      <c r="C9" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="L8" s="4">
-        <f>COUNTIF($I$3:$I$32,K8)</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="2:28" ht="15.75" customHeight="1">
-      <c r="B9" s="26">
-        <v>4</v>
-      </c>
-      <c r="C9" s="16" t="s">
-        <v>6</v>
-      </c>
-      <c r="D9" s="20" t="s">
+      <c r="D9" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="E9" s="20" t="s">
+      <c r="E9" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="F9" s="19"/>
-      <c r="G9" s="20" t="s">
+      <c r="F9" s="13"/>
+      <c r="G9" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="H9" s="19"/>
-      <c r="I9" s="13">
+      <c r="H9" s="13"/>
+      <c r="I9" s="21">
         <v>7</v>
       </c>
-      <c r="K9" s="4">
-        <v>7</v>
-      </c>
-      <c r="L9" s="4">
-        <f>COUNTIF($I$3:$I$32,K9)</f>
-        <v>1</v>
+      <c r="J9" s="36" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="10" spans="2:28" ht="15.75" customHeight="1">
-      <c r="B10" s="26"/>
-      <c r="C10" s="16"/>
-      <c r="D10" s="19"/>
-      <c r="E10" s="19"/>
-      <c r="F10" s="19"/>
-      <c r="G10" s="19"/>
-      <c r="H10" s="19"/>
-      <c r="I10" s="13"/>
-      <c r="K10" s="4">
-        <v>8</v>
-      </c>
-      <c r="L10" s="4">
-        <f>COUNTIF($I$3:$I$32,K10)</f>
-        <v>1</v>
-      </c>
+      <c r="B10" s="10"/>
+      <c r="C10" s="11"/>
+      <c r="D10" s="13"/>
+      <c r="E10" s="13"/>
+      <c r="F10" s="13"/>
+      <c r="G10" s="13"/>
+      <c r="H10" s="13"/>
+      <c r="I10" s="21"/>
+      <c r="J10" s="36"/>
     </row>
     <row r="11" spans="2:28" ht="15.75" customHeight="1">
-      <c r="B11" s="25">
+      <c r="B11" s="8">
         <v>5</v>
       </c>
       <c r="C11" s="18" t="s">
@@ -1141,357 +1160,354 @@
       <c r="D11" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="E11" s="23" t="s">
-        <v>40</v>
+      <c r="E11" s="15" t="s">
+        <v>39</v>
       </c>
       <c r="F11" s="17"/>
-      <c r="G11" s="23" t="s">
+      <c r="G11" s="15" t="s">
         <v>21</v>
       </c>
       <c r="H11" s="17"/>
-      <c r="I11" s="14">
+      <c r="I11" s="20">
         <v>5</v>
       </c>
-      <c r="K11" s="4">
-        <v>9</v>
-      </c>
-      <c r="L11" s="4">
-        <f>COUNTIF($I$3:$I$32,K11)</f>
-        <v>1</v>
+      <c r="J11" s="36" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="12" spans="2:28" ht="15.75" customHeight="1">
-      <c r="B12" s="25"/>
+      <c r="B12" s="8"/>
       <c r="C12" s="18"/>
       <c r="D12" s="17"/>
       <c r="E12" s="17"/>
       <c r="F12" s="17"/>
       <c r="G12" s="17"/>
       <c r="H12" s="17"/>
-      <c r="I12" s="14"/>
-      <c r="K12" s="4">
-        <v>10</v>
-      </c>
-      <c r="L12" s="4">
-        <f>COUNTIF($I$3:$I$32,K12)</f>
-        <v>1</v>
-      </c>
+      <c r="I12" s="20"/>
+      <c r="J12" s="36"/>
     </row>
     <row r="13" spans="2:28" ht="15.75" customHeight="1">
-      <c r="B13" s="26">
+      <c r="B13" s="10">
         <v>6</v>
       </c>
-      <c r="C13" s="16" t="s">
+      <c r="C13" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="D13" s="19" t="s">
+      <c r="D13" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="E13" s="20" t="s">
-        <v>38</v>
-      </c>
-      <c r="F13" s="19"/>
-      <c r="G13" s="20" t="s">
+      <c r="E13" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="F13" s="13"/>
+      <c r="G13" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="H13" s="19"/>
-      <c r="I13" s="13">
+      <c r="H13" s="13"/>
+      <c r="I13" s="21">
         <v>8</v>
       </c>
+      <c r="J13" s="36" t="s">
+        <v>46</v>
+      </c>
     </row>
     <row r="14" spans="2:28" ht="15.75" customHeight="1">
-      <c r="B14" s="26"/>
-      <c r="C14" s="16"/>
-      <c r="D14" s="19"/>
-      <c r="E14" s="19"/>
-      <c r="F14" s="19"/>
-      <c r="G14" s="19"/>
-      <c r="H14" s="19"/>
-      <c r="I14" s="13"/>
+      <c r="B14" s="10"/>
+      <c r="C14" s="11"/>
+      <c r="D14" s="13"/>
+      <c r="E14" s="13"/>
+      <c r="F14" s="13"/>
+      <c r="G14" s="13"/>
+      <c r="H14" s="13"/>
+      <c r="I14" s="21"/>
+      <c r="J14" s="36"/>
     </row>
     <row r="15" spans="2:28" ht="15.75" customHeight="1">
-      <c r="B15" s="25">
+      <c r="B15" s="8">
         <v>7</v>
       </c>
       <c r="C15" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="D15" s="23" t="s">
+      <c r="D15" s="15" t="s">
         <v>29</v>
       </c>
-      <c r="E15" s="23" t="s">
+      <c r="E15" s="15" t="s">
         <v>26</v>
       </c>
       <c r="F15" s="17"/>
-      <c r="G15" s="23" t="s">
+      <c r="G15" s="15" t="s">
         <v>23</v>
       </c>
       <c r="H15" s="17"/>
-      <c r="I15" s="14">
+      <c r="I15" s="20">
         <v>9</v>
       </c>
+      <c r="J15" s="36" t="s">
+        <v>46</v>
+      </c>
     </row>
     <row r="16" spans="2:28" ht="15.75" customHeight="1">
-      <c r="B16" s="25"/>
+      <c r="B16" s="8"/>
       <c r="C16" s="18"/>
       <c r="D16" s="17"/>
       <c r="E16" s="17"/>
       <c r="F16" s="17"/>
       <c r="G16" s="17"/>
       <c r="H16" s="17"/>
-      <c r="I16" s="14"/>
+      <c r="I16" s="20"/>
+      <c r="J16" s="36"/>
     </row>
     <row r="17" spans="2:10" ht="15.75" customHeight="1">
-      <c r="B17" s="25"/>
+      <c r="B17" s="8"/>
       <c r="C17" s="18"/>
       <c r="D17" s="17"/>
       <c r="E17" s="17"/>
       <c r="F17" s="17"/>
       <c r="G17" s="17"/>
       <c r="H17" s="17"/>
-      <c r="I17" s="14"/>
+      <c r="I17" s="20"/>
+      <c r="J17" s="36"/>
     </row>
     <row r="18" spans="2:10" ht="15.75" customHeight="1">
-      <c r="B18" s="26">
+      <c r="B18" s="10">
         <v>8</v>
       </c>
-      <c r="C18" s="16" t="s">
+      <c r="C18" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="D18" s="20" t="s">
+      <c r="D18" s="12" t="s">
         <v>35</v>
       </c>
-      <c r="E18" s="19" t="s">
+      <c r="E18" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="F18" s="19"/>
-      <c r="G18" s="20" t="s">
+      <c r="F18" s="13"/>
+      <c r="G18" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="H18" s="19"/>
-      <c r="I18" s="13" t="s">
+      <c r="H18" s="13"/>
+      <c r="I18" s="21" t="s">
+        <v>43</v>
+      </c>
+      <c r="J18" s="36" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="19" spans="2:10" ht="15.75" customHeight="1">
+      <c r="B19" s="10"/>
+      <c r="C19" s="11"/>
+      <c r="D19" s="13"/>
+      <c r="E19" s="13"/>
+      <c r="F19" s="13"/>
+      <c r="G19" s="13"/>
+      <c r="H19" s="13"/>
+      <c r="I19" s="21"/>
+      <c r="J19" s="36"/>
+    </row>
+    <row r="20" spans="2:10" ht="15.75" customHeight="1">
+      <c r="B20" s="10"/>
+      <c r="C20" s="11"/>
+      <c r="D20" s="13"/>
+      <c r="E20" s="13"/>
+      <c r="F20" s="13"/>
+      <c r="G20" s="13"/>
+      <c r="H20" s="13"/>
+      <c r="I20" s="21"/>
+      <c r="J20" s="36"/>
+    </row>
+    <row r="21" spans="2:10" ht="15.75" customHeight="1">
+      <c r="B21" s="8">
+        <v>9</v>
+      </c>
+      <c r="C21" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="D21" s="14" t="s">
+        <v>40</v>
+      </c>
+      <c r="E21" s="14" t="s">
+        <v>31</v>
+      </c>
+      <c r="F21" s="9"/>
+      <c r="G21" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="H21" s="9"/>
+      <c r="I21" s="20">
+        <v>3</v>
+      </c>
+      <c r="J21" s="36" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="22" spans="2:10" ht="15.75" customHeight="1">
+      <c r="B22" s="8"/>
+      <c r="C22" s="7"/>
+      <c r="D22" s="14"/>
+      <c r="E22" s="9"/>
+      <c r="F22" s="9"/>
+      <c r="G22" s="9"/>
+      <c r="H22" s="9"/>
+      <c r="I22" s="20"/>
+      <c r="J22" s="36"/>
+    </row>
+    <row r="23" spans="2:10" ht="15.75" customHeight="1">
+      <c r="B23" s="8"/>
+      <c r="C23" s="7"/>
+      <c r="D23" s="14"/>
+      <c r="E23" s="9"/>
+      <c r="F23" s="9"/>
+      <c r="G23" s="9"/>
+      <c r="H23" s="9"/>
+      <c r="I23" s="20"/>
+      <c r="J23" s="36"/>
+    </row>
+    <row r="24" spans="2:10" ht="15.75" customHeight="1">
+      <c r="B24" s="10">
+        <v>10</v>
+      </c>
+      <c r="C24" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="D24" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="E24" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="F24" s="13"/>
+      <c r="G24" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="H24" s="13"/>
+      <c r="I24" s="21">
+        <v>10</v>
+      </c>
+      <c r="J24" s="36" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="25" spans="2:10" ht="15.75" customHeight="1">
+      <c r="B25" s="10"/>
+      <c r="C25" s="11"/>
+      <c r="D25" s="13"/>
+      <c r="E25" s="13"/>
+      <c r="F25" s="13"/>
+      <c r="G25" s="12"/>
+      <c r="H25" s="13"/>
+      <c r="I25" s="21"/>
+      <c r="J25" s="36"/>
+    </row>
+    <row r="26" spans="2:10" ht="15.75" customHeight="1">
+      <c r="B26" s="10"/>
+      <c r="C26" s="11"/>
+      <c r="D26" s="13"/>
+      <c r="E26" s="13"/>
+      <c r="F26" s="13"/>
+      <c r="G26" s="12"/>
+      <c r="H26" s="13"/>
+      <c r="I26" s="21"/>
+      <c r="J26" s="36"/>
+    </row>
+    <row r="27" spans="2:10" ht="15.75" customHeight="1">
+      <c r="B27" s="8">
+        <v>11</v>
+      </c>
+      <c r="C27" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="D27" s="14" t="s">
+        <v>47</v>
+      </c>
+      <c r="E27" s="15" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="19" spans="2:10" ht="15.75" customHeight="1">
-      <c r="B19" s="26"/>
-      <c r="C19" s="16"/>
-      <c r="D19" s="19"/>
-      <c r="E19" s="19"/>
-      <c r="F19" s="19"/>
-      <c r="G19" s="19"/>
-      <c r="H19" s="19"/>
-      <c r="I19" s="13"/>
-    </row>
-    <row r="20" spans="2:10" ht="15.75" customHeight="1">
-      <c r="B20" s="26"/>
-      <c r="C20" s="16"/>
-      <c r="D20" s="19"/>
-      <c r="E20" s="19"/>
-      <c r="F20" s="19"/>
-      <c r="G20" s="19"/>
-      <c r="H20" s="19"/>
-      <c r="I20" s="13"/>
-    </row>
-    <row r="21" spans="2:10" ht="15.75" customHeight="1">
-      <c r="B21" s="25">
-        <v>9</v>
-      </c>
-      <c r="C21" s="22" t="s">
-        <v>9</v>
-      </c>
-      <c r="D21" s="30" t="s">
-        <v>41</v>
-      </c>
-      <c r="E21" s="30" t="s">
-        <v>31</v>
-      </c>
-      <c r="F21" s="28"/>
-      <c r="G21" s="28" t="s">
-        <v>30</v>
-      </c>
-      <c r="H21" s="28"/>
-      <c r="I21" s="14">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="22" spans="2:10" ht="15.75" customHeight="1">
-      <c r="B22" s="25"/>
-      <c r="C22" s="22"/>
-      <c r="D22" s="30"/>
-      <c r="E22" s="28"/>
-      <c r="F22" s="28"/>
-      <c r="G22" s="28"/>
-      <c r="H22" s="28"/>
-      <c r="I22" s="14"/>
-    </row>
-    <row r="23" spans="2:10" ht="15.75" customHeight="1">
-      <c r="B23" s="25"/>
-      <c r="C23" s="22"/>
-      <c r="D23" s="30"/>
-      <c r="E23" s="28"/>
-      <c r="F23" s="28"/>
-      <c r="G23" s="28"/>
-      <c r="H23" s="28"/>
-      <c r="I23" s="14"/>
-    </row>
-    <row r="24" spans="2:10" ht="15.75" customHeight="1">
-      <c r="B24" s="26">
-        <v>10</v>
-      </c>
-      <c r="C24" s="16" t="s">
-        <v>9</v>
-      </c>
-      <c r="D24" s="20" t="s">
-        <v>34</v>
-      </c>
-      <c r="E24" s="19" t="s">
-        <v>32</v>
-      </c>
-      <c r="F24" s="19"/>
-      <c r="G24" s="20" t="s">
-        <v>33</v>
-      </c>
-      <c r="H24" s="19"/>
-      <c r="I24" s="13">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="25" spans="2:10" ht="15.75" customHeight="1">
-      <c r="B25" s="26"/>
-      <c r="C25" s="16"/>
-      <c r="D25" s="19"/>
-      <c r="E25" s="19"/>
-      <c r="F25" s="19"/>
-      <c r="G25" s="20"/>
-      <c r="H25" s="19"/>
-      <c r="I25" s="13"/>
-    </row>
-    <row r="26" spans="2:10" ht="15.75" customHeight="1">
-      <c r="B26" s="26"/>
-      <c r="C26" s="16"/>
-      <c r="D26" s="19"/>
-      <c r="E26" s="19"/>
-      <c r="F26" s="19"/>
-      <c r="G26" s="20"/>
-      <c r="H26" s="19"/>
-      <c r="I26" s="13"/>
-    </row>
-    <row r="27" spans="2:10" ht="15.75" customHeight="1">
-      <c r="B27" s="25">
-        <v>11</v>
-      </c>
-      <c r="C27" s="22" t="s">
-        <v>10</v>
-      </c>
-      <c r="D27" s="30" t="s">
-        <v>47</v>
-      </c>
-      <c r="E27" s="23" t="s">
+      <c r="F27" s="9"/>
+      <c r="G27" s="14" t="s">
         <v>36</v>
       </c>
-      <c r="F27" s="28"/>
-      <c r="G27" s="30" t="s">
-        <v>37</v>
-      </c>
-      <c r="H27" s="28"/>
-      <c r="I27" s="14">
+      <c r="H27" s="9"/>
+      <c r="I27" s="20">
         <v>4</v>
       </c>
-      <c r="J27" s="33"/>
+      <c r="J27" s="39" t="s">
+        <v>46</v>
+      </c>
     </row>
     <row r="28" spans="2:10" ht="15.75" customHeight="1">
-      <c r="B28" s="25"/>
-      <c r="C28" s="22"/>
-      <c r="D28" s="30"/>
-      <c r="E28" s="23"/>
-      <c r="F28" s="28"/>
-      <c r="G28" s="30"/>
-      <c r="H28" s="28"/>
-      <c r="I28" s="14"/>
-      <c r="J28" s="34"/>
+      <c r="B28" s="8"/>
+      <c r="C28" s="7"/>
+      <c r="D28" s="14"/>
+      <c r="E28" s="15"/>
+      <c r="F28" s="9"/>
+      <c r="G28" s="14"/>
+      <c r="H28" s="9"/>
+      <c r="I28" s="20"/>
+      <c r="J28" s="36"/>
     </row>
     <row r="29" spans="2:10" ht="15.75" customHeight="1">
-      <c r="B29" s="25"/>
-      <c r="C29" s="22"/>
-      <c r="D29" s="30"/>
-      <c r="E29" s="23"/>
-      <c r="F29" s="28"/>
-      <c r="G29" s="30"/>
-      <c r="H29" s="28"/>
-      <c r="I29" s="14"/>
-      <c r="J29" s="34"/>
+      <c r="B29" s="8"/>
+      <c r="C29" s="7"/>
+      <c r="D29" s="14"/>
+      <c r="E29" s="15"/>
+      <c r="F29" s="9"/>
+      <c r="G29" s="14"/>
+      <c r="H29" s="9"/>
+      <c r="I29" s="20"/>
+      <c r="J29" s="36"/>
     </row>
     <row r="30" spans="2:10" ht="15.75" customHeight="1">
-      <c r="B30" s="25"/>
-      <c r="C30" s="22"/>
-      <c r="D30" s="30"/>
-      <c r="E30" s="23"/>
-      <c r="F30" s="28"/>
-      <c r="G30" s="30"/>
-      <c r="H30" s="28"/>
-      <c r="I30" s="14"/>
-      <c r="J30" s="34"/>
+      <c r="B30" s="8"/>
+      <c r="C30" s="7"/>
+      <c r="D30" s="14"/>
+      <c r="E30" s="15"/>
+      <c r="F30" s="9"/>
+      <c r="G30" s="14"/>
+      <c r="H30" s="9"/>
+      <c r="I30" s="20"/>
+      <c r="J30" s="36"/>
     </row>
     <row r="31" spans="2:10" ht="15.75" customHeight="1">
-      <c r="B31" s="25"/>
-      <c r="C31" s="22"/>
-      <c r="D31" s="30"/>
-      <c r="E31" s="23"/>
-      <c r="F31" s="28"/>
-      <c r="G31" s="30"/>
-      <c r="H31" s="28"/>
-      <c r="I31" s="14"/>
-      <c r="J31" s="34"/>
-    </row>
-    <row r="32" spans="2:10" ht="15.75" customHeight="1">
-      <c r="B32" s="25"/>
-      <c r="C32" s="22"/>
-      <c r="D32" s="30"/>
-      <c r="E32" s="23"/>
-      <c r="F32" s="28"/>
-      <c r="G32" s="30"/>
-      <c r="H32" s="28"/>
-      <c r="I32" s="14"/>
-      <c r="J32" s="34"/>
-    </row>
-    <row r="33" spans="2:9" ht="15.75" customHeight="1" thickBot="1">
-      <c r="B33" s="9">
-        <v>12</v>
-      </c>
-      <c r="C33" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="D33" s="11" t="s">
-        <v>45</v>
-      </c>
-      <c r="E33" s="11" t="s">
-        <v>46</v>
-      </c>
-      <c r="F33" s="11"/>
-      <c r="G33" s="11"/>
-      <c r="H33" s="11"/>
-      <c r="I33" s="12" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="34" spans="2:9" ht="15.75" customHeight="1">
-      <c r="D34" s="5"/>
-    </row>
-    <row r="35" spans="2:9" ht="15.75" customHeight="1"/>
-    <row r="36" spans="2:9" ht="15.75" customHeight="1"/>
-    <row r="37" spans="2:9" ht="15.75" customHeight="1"/>
-    <row r="38" spans="2:9" ht="15.75" customHeight="1"/>
-    <row r="39" spans="2:9" ht="15.75" customHeight="1"/>
-    <row r="40" spans="2:9" ht="15.75" customHeight="1"/>
-    <row r="41" spans="2:9" ht="15.75" customHeight="1"/>
-    <row r="42" spans="2:9" ht="15.75" customHeight="1"/>
-    <row r="43" spans="2:9" ht="15.75" customHeight="1"/>
-    <row r="44" spans="2:9" ht="15.75" customHeight="1"/>
-    <row r="45" spans="2:9" ht="15.75" customHeight="1"/>
-    <row r="46" spans="2:9" ht="15.75" customHeight="1"/>
-    <row r="47" spans="2:9" ht="15.75" customHeight="1"/>
-    <row r="48" spans="2:9" ht="15.75" customHeight="1"/>
+      <c r="B31" s="8"/>
+      <c r="C31" s="7"/>
+      <c r="D31" s="14"/>
+      <c r="E31" s="15"/>
+      <c r="F31" s="9"/>
+      <c r="G31" s="14"/>
+      <c r="H31" s="9"/>
+      <c r="I31" s="20"/>
+      <c r="J31" s="36"/>
+    </row>
+    <row r="32" spans="2:10" ht="15.75" customHeight="1" thickBot="1">
+      <c r="B32" s="22"/>
+      <c r="C32" s="23"/>
+      <c r="D32" s="24"/>
+      <c r="E32" s="25"/>
+      <c r="F32" s="26"/>
+      <c r="G32" s="24"/>
+      <c r="H32" s="26"/>
+      <c r="I32" s="27"/>
+      <c r="J32" s="40"/>
+    </row>
+    <row r="33" spans="4:4" ht="15.75" customHeight="1">
+      <c r="D33" s="5"/>
+    </row>
+    <row r="34" spans="4:4" ht="15.75" customHeight="1"/>
+    <row r="35" spans="4:4" ht="15.75" customHeight="1"/>
+    <row r="36" spans="4:4" ht="15.75" customHeight="1"/>
+    <row r="37" spans="4:4" ht="15.75" customHeight="1"/>
+    <row r="38" spans="4:4" ht="15.75" customHeight="1"/>
+    <row r="39" spans="4:4" ht="15.75" customHeight="1"/>
+    <row r="40" spans="4:4" ht="15.75" customHeight="1"/>
+    <row r="41" spans="4:4" ht="15.75" customHeight="1"/>
+    <row r="42" spans="4:4" ht="15.75" customHeight="1"/>
+    <row r="43" spans="4:4" ht="15.75" customHeight="1"/>
+    <row r="44" spans="4:4" ht="15.75" customHeight="1"/>
+    <row r="45" spans="4:4" ht="15.75" customHeight="1"/>
+    <row r="46" spans="4:4" ht="15.75" customHeight="1"/>
+    <row r="47" spans="4:4" ht="15.75" customHeight="1"/>
+    <row r="48" spans="4:4" ht="15.75" customHeight="1"/>
     <row r="49" ht="15.75" customHeight="1"/>
     <row r="50" ht="15.75" customHeight="1"/>
     <row r="51" ht="15.75" customHeight="1"/>
@@ -2436,42 +2452,58 @@
     <row r="990" ht="15.75" customHeight="1"/>
     <row r="991" ht="15.75" customHeight="1"/>
     <row r="992" ht="15.75" customHeight="1"/>
-    <row r="993" ht="15.75" customHeight="1"/>
   </sheetData>
-  <mergeCells count="89">
-    <mergeCell ref="J27:J32"/>
-    <mergeCell ref="C27:C32"/>
-    <mergeCell ref="B27:B32"/>
-    <mergeCell ref="H27:H32"/>
-    <mergeCell ref="I27:I32"/>
-    <mergeCell ref="B24:B26"/>
-    <mergeCell ref="C24:C26"/>
-    <mergeCell ref="D24:D26"/>
-    <mergeCell ref="E24:E26"/>
-    <mergeCell ref="F24:F26"/>
-    <mergeCell ref="H24:H26"/>
-    <mergeCell ref="G27:G32"/>
-    <mergeCell ref="F27:F32"/>
-    <mergeCell ref="E27:E32"/>
-    <mergeCell ref="D27:D32"/>
-    <mergeCell ref="G24:G26"/>
-    <mergeCell ref="F3:F4"/>
-    <mergeCell ref="F5:F6"/>
-    <mergeCell ref="F7:F8"/>
-    <mergeCell ref="F9:F10"/>
-    <mergeCell ref="F11:F12"/>
-    <mergeCell ref="F21:F23"/>
-    <mergeCell ref="B21:B23"/>
-    <mergeCell ref="C21:C23"/>
-    <mergeCell ref="G21:G23"/>
-    <mergeCell ref="H21:H23"/>
-    <mergeCell ref="D21:D23"/>
-    <mergeCell ref="E21:E23"/>
-    <mergeCell ref="E5:E6"/>
-    <mergeCell ref="E7:E8"/>
-    <mergeCell ref="E9:E10"/>
-    <mergeCell ref="E11:E12"/>
-    <mergeCell ref="E13:E14"/>
+  <mergeCells count="99">
+    <mergeCell ref="J13:J14"/>
+    <mergeCell ref="J15:J17"/>
+    <mergeCell ref="J18:J20"/>
+    <mergeCell ref="J21:J23"/>
+    <mergeCell ref="J24:J26"/>
+    <mergeCell ref="J3:J4"/>
+    <mergeCell ref="J5:J6"/>
+    <mergeCell ref="J7:J8"/>
+    <mergeCell ref="J9:J10"/>
+    <mergeCell ref="J11:J12"/>
+    <mergeCell ref="I13:I14"/>
+    <mergeCell ref="I15:I17"/>
+    <mergeCell ref="I18:I20"/>
+    <mergeCell ref="I21:I23"/>
+    <mergeCell ref="I24:I26"/>
+    <mergeCell ref="I3:I4"/>
+    <mergeCell ref="I5:I6"/>
+    <mergeCell ref="I7:I8"/>
+    <mergeCell ref="I9:I10"/>
+    <mergeCell ref="I11:I12"/>
+    <mergeCell ref="C9:C10"/>
+    <mergeCell ref="D11:D12"/>
+    <mergeCell ref="C11:C12"/>
+    <mergeCell ref="D13:D14"/>
+    <mergeCell ref="C13:C14"/>
+    <mergeCell ref="D9:D10"/>
+    <mergeCell ref="C3:C4"/>
+    <mergeCell ref="D3:D4"/>
+    <mergeCell ref="C5:C6"/>
+    <mergeCell ref="D5:D6"/>
+    <mergeCell ref="C7:C8"/>
+    <mergeCell ref="D7:D8"/>
+    <mergeCell ref="B3:B4"/>
+    <mergeCell ref="B5:B6"/>
+    <mergeCell ref="B7:B8"/>
+    <mergeCell ref="B9:B10"/>
+    <mergeCell ref="B11:B12"/>
+    <mergeCell ref="B13:B14"/>
+    <mergeCell ref="B15:B17"/>
+    <mergeCell ref="G18:G20"/>
+    <mergeCell ref="E18:E20"/>
+    <mergeCell ref="C18:C20"/>
+    <mergeCell ref="B18:B20"/>
+    <mergeCell ref="F18:F20"/>
+    <mergeCell ref="E15:E17"/>
+    <mergeCell ref="D15:D17"/>
+    <mergeCell ref="D18:D20"/>
+    <mergeCell ref="F13:F14"/>
+    <mergeCell ref="C15:C17"/>
+    <mergeCell ref="F15:F17"/>
     <mergeCell ref="H18:H20"/>
     <mergeCell ref="E3:E4"/>
     <mergeCell ref="G3:G4"/>
@@ -2488,46 +2520,39 @@
     <mergeCell ref="G11:G12"/>
     <mergeCell ref="G13:G14"/>
     <mergeCell ref="G15:G17"/>
-    <mergeCell ref="B13:B14"/>
-    <mergeCell ref="B15:B17"/>
-    <mergeCell ref="G18:G20"/>
-    <mergeCell ref="E18:E20"/>
-    <mergeCell ref="C18:C20"/>
-    <mergeCell ref="B18:B20"/>
-    <mergeCell ref="F18:F20"/>
-    <mergeCell ref="E15:E17"/>
-    <mergeCell ref="D15:D17"/>
-    <mergeCell ref="D18:D20"/>
-    <mergeCell ref="F13:F14"/>
-    <mergeCell ref="C15:C17"/>
-    <mergeCell ref="F15:F17"/>
-    <mergeCell ref="B3:B4"/>
-    <mergeCell ref="B5:B6"/>
-    <mergeCell ref="B7:B8"/>
-    <mergeCell ref="B9:B10"/>
-    <mergeCell ref="B11:B12"/>
-    <mergeCell ref="C3:C4"/>
-    <mergeCell ref="D3:D4"/>
-    <mergeCell ref="C5:C6"/>
-    <mergeCell ref="D5:D6"/>
-    <mergeCell ref="C7:C8"/>
-    <mergeCell ref="D7:D8"/>
-    <mergeCell ref="C9:C10"/>
-    <mergeCell ref="D11:D12"/>
-    <mergeCell ref="C11:C12"/>
-    <mergeCell ref="D13:D14"/>
-    <mergeCell ref="C13:C14"/>
-    <mergeCell ref="D9:D10"/>
-    <mergeCell ref="I3:I4"/>
-    <mergeCell ref="I5:I6"/>
-    <mergeCell ref="I7:I8"/>
-    <mergeCell ref="I9:I10"/>
-    <mergeCell ref="I11:I12"/>
-    <mergeCell ref="I13:I14"/>
-    <mergeCell ref="I15:I17"/>
-    <mergeCell ref="I18:I20"/>
-    <mergeCell ref="I21:I23"/>
-    <mergeCell ref="I24:I26"/>
+    <mergeCell ref="E5:E6"/>
+    <mergeCell ref="E7:E8"/>
+    <mergeCell ref="E9:E10"/>
+    <mergeCell ref="E11:E12"/>
+    <mergeCell ref="E13:E14"/>
+    <mergeCell ref="F21:F23"/>
+    <mergeCell ref="B21:B23"/>
+    <mergeCell ref="C21:C23"/>
+    <mergeCell ref="G21:G23"/>
+    <mergeCell ref="H21:H23"/>
+    <mergeCell ref="D21:D23"/>
+    <mergeCell ref="E21:E23"/>
+    <mergeCell ref="F3:F4"/>
+    <mergeCell ref="F5:F6"/>
+    <mergeCell ref="F7:F8"/>
+    <mergeCell ref="F9:F10"/>
+    <mergeCell ref="F11:F12"/>
+    <mergeCell ref="H24:H26"/>
+    <mergeCell ref="G27:G32"/>
+    <mergeCell ref="F27:F32"/>
+    <mergeCell ref="E27:E32"/>
+    <mergeCell ref="D27:D32"/>
+    <mergeCell ref="G24:G26"/>
+    <mergeCell ref="B24:B26"/>
+    <mergeCell ref="C24:C26"/>
+    <mergeCell ref="D24:D26"/>
+    <mergeCell ref="E24:E26"/>
+    <mergeCell ref="F24:F26"/>
+    <mergeCell ref="J27:J32"/>
+    <mergeCell ref="C27:C32"/>
+    <mergeCell ref="B27:B32"/>
+    <mergeCell ref="H27:H32"/>
+    <mergeCell ref="I27:I32"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape" r:id="rId1"/>

</xml_diff>

<commit_message>
Analyses des performances après 3eme correction
</commit_message>
<xml_diff>
--- a/Analyses/Modèle-audit-SEO.xlsx
+++ b/Analyses/Modèle-audit-SEO.xlsx
@@ -703,101 +703,101 @@
     <xf numFmtId="0" fontId="7" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="7" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1015,7 +1015,7 @@
   <dimension ref="B1:AB992"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3:J33"/>
+      <selection activeCell="J21" sqref="J21:J23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.33203125" defaultRowHeight="15" customHeight="1"/>
@@ -1081,490 +1081,490 @@
       <c r="AB2" s="1"/>
     </row>
     <row r="3" spans="2:28" ht="15.75" customHeight="1">
-      <c r="B3" s="39">
+      <c r="B3" s="41">
         <v>1</v>
       </c>
-      <c r="C3" s="40" t="s">
+      <c r="C3" s="42" t="s">
         <v>42</v>
       </c>
-      <c r="D3" s="40" t="s">
+      <c r="D3" s="42" t="s">
         <v>7</v>
       </c>
-      <c r="E3" s="41" t="s">
+      <c r="E3" s="36" t="s">
         <v>16</v>
       </c>
-      <c r="F3" s="41" t="s">
+      <c r="F3" s="36" t="s">
         <v>41</v>
       </c>
-      <c r="G3" s="41" t="s">
+      <c r="G3" s="36" t="s">
         <v>17</v>
       </c>
-      <c r="H3" s="42"/>
+      <c r="H3" s="39"/>
       <c r="I3" s="43">
         <v>1</v>
       </c>
-      <c r="J3" s="44" t="s">
+      <c r="J3" s="45" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="4" spans="2:28" ht="15.75" customHeight="1">
-      <c r="B4" s="26"/>
-      <c r="C4" s="24"/>
-      <c r="D4" s="24"/>
-      <c r="E4" s="28"/>
-      <c r="F4" s="28"/>
-      <c r="G4" s="28"/>
-      <c r="H4" s="28"/>
-      <c r="I4" s="18"/>
-      <c r="J4" s="16"/>
+      <c r="B4" s="22"/>
+      <c r="C4" s="20"/>
+      <c r="D4" s="20"/>
+      <c r="E4" s="24"/>
+      <c r="F4" s="24"/>
+      <c r="G4" s="24"/>
+      <c r="H4" s="24"/>
+      <c r="I4" s="26"/>
+      <c r="J4" s="46"/>
     </row>
     <row r="5" spans="2:28" ht="15.75" customHeight="1">
-      <c r="B5" s="27">
+      <c r="B5" s="28">
         <v>2</v>
       </c>
-      <c r="C5" s="19" t="s">
+      <c r="C5" s="29" t="s">
         <v>42</v>
       </c>
-      <c r="D5" s="22" t="s">
+      <c r="D5" s="31" t="s">
         <v>8</v>
       </c>
-      <c r="E5" s="23" t="s">
+      <c r="E5" s="30" t="s">
         <v>16</v>
       </c>
-      <c r="F5" s="30"/>
-      <c r="G5" s="23" t="s">
+      <c r="F5" s="37"/>
+      <c r="G5" s="30" t="s">
         <v>18</v>
       </c>
-      <c r="H5" s="22"/>
-      <c r="I5" s="17">
+      <c r="H5" s="31"/>
+      <c r="I5" s="44">
         <v>2</v>
       </c>
-      <c r="J5" s="16" t="s">
+      <c r="J5" s="46" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="6" spans="2:28" ht="15.75" customHeight="1">
-      <c r="B6" s="27"/>
-      <c r="C6" s="19"/>
-      <c r="D6" s="22"/>
-      <c r="E6" s="22"/>
-      <c r="F6" s="30"/>
-      <c r="G6" s="22"/>
-      <c r="H6" s="22"/>
-      <c r="I6" s="17"/>
-      <c r="J6" s="16"/>
+      <c r="B6" s="28"/>
+      <c r="C6" s="29"/>
+      <c r="D6" s="31"/>
+      <c r="E6" s="31"/>
+      <c r="F6" s="37"/>
+      <c r="G6" s="31"/>
+      <c r="H6" s="31"/>
+      <c r="I6" s="44"/>
+      <c r="J6" s="46"/>
     </row>
     <row r="7" spans="2:28" ht="15.75" customHeight="1">
-      <c r="B7" s="26">
+      <c r="B7" s="22">
         <v>3</v>
       </c>
-      <c r="C7" s="21" t="s">
+      <c r="C7" s="40" t="s">
         <v>6</v>
       </c>
-      <c r="D7" s="25" t="s">
+      <c r="D7" s="34" t="s">
         <v>27</v>
       </c>
-      <c r="E7" s="25" t="s">
+      <c r="E7" s="34" t="s">
         <v>24</v>
       </c>
-      <c r="F7" s="20"/>
-      <c r="G7" s="25" t="s">
+      <c r="F7" s="38"/>
+      <c r="G7" s="34" t="s">
         <v>19</v>
       </c>
-      <c r="H7" s="20"/>
-      <c r="I7" s="18">
+      <c r="H7" s="38"/>
+      <c r="I7" s="26">
         <v>6</v>
       </c>
-      <c r="J7" s="15" t="s">
+      <c r="J7" s="18" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="8" spans="2:28" ht="15.75" customHeight="1">
-      <c r="B8" s="26"/>
-      <c r="C8" s="21"/>
-      <c r="D8" s="20"/>
-      <c r="E8" s="20"/>
-      <c r="F8" s="20"/>
-      <c r="G8" s="20"/>
-      <c r="H8" s="20"/>
-      <c r="I8" s="18"/>
-      <c r="J8" s="15"/>
+      <c r="B8" s="22"/>
+      <c r="C8" s="40"/>
+      <c r="D8" s="38"/>
+      <c r="E8" s="38"/>
+      <c r="F8" s="38"/>
+      <c r="G8" s="38"/>
+      <c r="H8" s="38"/>
+      <c r="I8" s="26"/>
+      <c r="J8" s="18"/>
     </row>
     <row r="9" spans="2:28" ht="15.75" customHeight="1">
-      <c r="B9" s="27">
+      <c r="B9" s="28">
         <v>4</v>
       </c>
-      <c r="C9" s="19" t="s">
+      <c r="C9" s="29" t="s">
         <v>6</v>
       </c>
-      <c r="D9" s="23" t="s">
+      <c r="D9" s="30" t="s">
         <v>28</v>
       </c>
-      <c r="E9" s="23" t="s">
+      <c r="E9" s="30" t="s">
         <v>25</v>
       </c>
-      <c r="F9" s="22"/>
-      <c r="G9" s="23" t="s">
+      <c r="F9" s="31"/>
+      <c r="G9" s="30" t="s">
         <v>20</v>
       </c>
-      <c r="H9" s="22"/>
-      <c r="I9" s="17">
+      <c r="H9" s="31"/>
+      <c r="I9" s="44">
         <v>7</v>
       </c>
-      <c r="J9" s="15" t="s">
+      <c r="J9" s="18" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="10" spans="2:28" ht="15.75" customHeight="1">
-      <c r="B10" s="27"/>
-      <c r="C10" s="19"/>
-      <c r="D10" s="22"/>
-      <c r="E10" s="22"/>
-      <c r="F10" s="22"/>
-      <c r="G10" s="22"/>
-      <c r="H10" s="22"/>
-      <c r="I10" s="17"/>
-      <c r="J10" s="15"/>
+      <c r="B10" s="28"/>
+      <c r="C10" s="29"/>
+      <c r="D10" s="31"/>
+      <c r="E10" s="31"/>
+      <c r="F10" s="31"/>
+      <c r="G10" s="31"/>
+      <c r="H10" s="31"/>
+      <c r="I10" s="44"/>
+      <c r="J10" s="18"/>
     </row>
     <row r="11" spans="2:28" ht="15.75" customHeight="1">
-      <c r="B11" s="26">
+      <c r="B11" s="22">
         <v>5</v>
       </c>
-      <c r="C11" s="21" t="s">
+      <c r="C11" s="40" t="s">
         <v>10</v>
       </c>
-      <c r="D11" s="20" t="s">
+      <c r="D11" s="38" t="s">
         <v>11</v>
       </c>
-      <c r="E11" s="25" t="s">
+      <c r="E11" s="34" t="s">
         <v>39</v>
       </c>
-      <c r="F11" s="20"/>
-      <c r="G11" s="25" t="s">
+      <c r="F11" s="38"/>
+      <c r="G11" s="34" t="s">
         <v>21</v>
       </c>
-      <c r="H11" s="20"/>
-      <c r="I11" s="18">
+      <c r="H11" s="38"/>
+      <c r="I11" s="26">
         <v>5</v>
       </c>
-      <c r="J11" s="15" t="s">
+      <c r="J11" s="18" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="12" spans="2:28" ht="15.75" customHeight="1">
-      <c r="B12" s="26"/>
-      <c r="C12" s="21"/>
-      <c r="D12" s="20"/>
-      <c r="E12" s="20"/>
-      <c r="F12" s="20"/>
-      <c r="G12" s="20"/>
-      <c r="H12" s="20"/>
-      <c r="I12" s="18"/>
-      <c r="J12" s="15"/>
+      <c r="B12" s="22"/>
+      <c r="C12" s="40"/>
+      <c r="D12" s="38"/>
+      <c r="E12" s="38"/>
+      <c r="F12" s="38"/>
+      <c r="G12" s="38"/>
+      <c r="H12" s="38"/>
+      <c r="I12" s="26"/>
+      <c r="J12" s="18"/>
     </row>
     <row r="13" spans="2:28" ht="15.75" customHeight="1">
-      <c r="B13" s="27">
+      <c r="B13" s="28">
         <v>6</v>
       </c>
-      <c r="C13" s="19" t="s">
+      <c r="C13" s="29" t="s">
         <v>6</v>
       </c>
-      <c r="D13" s="22" t="s">
+      <c r="D13" s="31" t="s">
         <v>12</v>
       </c>
-      <c r="E13" s="23" t="s">
+      <c r="E13" s="30" t="s">
         <v>37</v>
       </c>
-      <c r="F13" s="22"/>
-      <c r="G13" s="23" t="s">
+      <c r="F13" s="31"/>
+      <c r="G13" s="30" t="s">
         <v>22</v>
       </c>
-      <c r="H13" s="22"/>
-      <c r="I13" s="17">
+      <c r="H13" s="31"/>
+      <c r="I13" s="44">
         <v>8</v>
       </c>
-      <c r="J13" s="15" t="s">
+      <c r="J13" s="18" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="14" spans="2:28" ht="15.75" customHeight="1">
-      <c r="B14" s="27"/>
-      <c r="C14" s="19"/>
-      <c r="D14" s="22"/>
-      <c r="E14" s="22"/>
-      <c r="F14" s="22"/>
-      <c r="G14" s="22"/>
-      <c r="H14" s="22"/>
-      <c r="I14" s="17"/>
-      <c r="J14" s="15"/>
+      <c r="B14" s="28"/>
+      <c r="C14" s="29"/>
+      <c r="D14" s="31"/>
+      <c r="E14" s="31"/>
+      <c r="F14" s="31"/>
+      <c r="G14" s="31"/>
+      <c r="H14" s="31"/>
+      <c r="I14" s="44"/>
+      <c r="J14" s="18"/>
     </row>
     <row r="15" spans="2:28" ht="15.75" customHeight="1">
-      <c r="B15" s="26">
+      <c r="B15" s="22">
         <v>7</v>
       </c>
-      <c r="C15" s="21" t="s">
+      <c r="C15" s="40" t="s">
         <v>6</v>
       </c>
-      <c r="D15" s="25" t="s">
+      <c r="D15" s="34" t="s">
         <v>29</v>
       </c>
-      <c r="E15" s="25" t="s">
+      <c r="E15" s="34" t="s">
         <v>26</v>
       </c>
-      <c r="F15" s="20"/>
-      <c r="G15" s="25" t="s">
+      <c r="F15" s="38"/>
+      <c r="G15" s="34" t="s">
         <v>23</v>
       </c>
-      <c r="H15" s="20"/>
-      <c r="I15" s="18">
+      <c r="H15" s="38"/>
+      <c r="I15" s="26">
         <v>9</v>
       </c>
-      <c r="J15" s="15" t="s">
+      <c r="J15" s="18" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="16" spans="2:28" ht="15.75" customHeight="1">
-      <c r="B16" s="26"/>
-      <c r="C16" s="21"/>
-      <c r="D16" s="20"/>
-      <c r="E16" s="20"/>
-      <c r="F16" s="20"/>
-      <c r="G16" s="20"/>
-      <c r="H16" s="20"/>
-      <c r="I16" s="18"/>
-      <c r="J16" s="15"/>
+      <c r="B16" s="22"/>
+      <c r="C16" s="40"/>
+      <c r="D16" s="38"/>
+      <c r="E16" s="38"/>
+      <c r="F16" s="38"/>
+      <c r="G16" s="38"/>
+      <c r="H16" s="38"/>
+      <c r="I16" s="26"/>
+      <c r="J16" s="18"/>
     </row>
     <row r="17" spans="2:10" ht="15.75" customHeight="1">
-      <c r="B17" s="26"/>
-      <c r="C17" s="21"/>
-      <c r="D17" s="20"/>
-      <c r="E17" s="20"/>
-      <c r="F17" s="20"/>
-      <c r="G17" s="20"/>
-      <c r="H17" s="20"/>
-      <c r="I17" s="18"/>
-      <c r="J17" s="15"/>
+      <c r="B17" s="22"/>
+      <c r="C17" s="40"/>
+      <c r="D17" s="38"/>
+      <c r="E17" s="38"/>
+      <c r="F17" s="38"/>
+      <c r="G17" s="38"/>
+      <c r="H17" s="38"/>
+      <c r="I17" s="26"/>
+      <c r="J17" s="18"/>
     </row>
     <row r="18" spans="2:10" ht="15.75" customHeight="1">
-      <c r="B18" s="27">
+      <c r="B18" s="28">
         <v>8</v>
       </c>
-      <c r="C18" s="19" t="s">
+      <c r="C18" s="29" t="s">
         <v>9</v>
       </c>
-      <c r="D18" s="23" t="s">
+      <c r="D18" s="30" t="s">
         <v>35</v>
       </c>
-      <c r="E18" s="22" t="s">
+      <c r="E18" s="31" t="s">
         <v>13</v>
       </c>
-      <c r="F18" s="22"/>
-      <c r="G18" s="23" t="s">
+      <c r="F18" s="31"/>
+      <c r="G18" s="30" t="s">
         <v>15</v>
       </c>
-      <c r="H18" s="22"/>
-      <c r="I18" s="17" t="s">
+      <c r="H18" s="31"/>
+      <c r="I18" s="44" t="s">
         <v>43</v>
       </c>
-      <c r="J18" s="15" t="s">
+      <c r="J18" s="18" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="19" spans="2:10" ht="15.75" customHeight="1">
-      <c r="B19" s="27"/>
-      <c r="C19" s="19"/>
-      <c r="D19" s="22"/>
-      <c r="E19" s="22"/>
-      <c r="F19" s="22"/>
-      <c r="G19" s="22"/>
-      <c r="H19" s="22"/>
-      <c r="I19" s="17"/>
-      <c r="J19" s="15"/>
+      <c r="B19" s="28"/>
+      <c r="C19" s="29"/>
+      <c r="D19" s="31"/>
+      <c r="E19" s="31"/>
+      <c r="F19" s="31"/>
+      <c r="G19" s="31"/>
+      <c r="H19" s="31"/>
+      <c r="I19" s="44"/>
+      <c r="J19" s="18"/>
     </row>
     <row r="20" spans="2:10" ht="15.75" customHeight="1">
-      <c r="B20" s="27"/>
-      <c r="C20" s="19"/>
-      <c r="D20" s="22"/>
-      <c r="E20" s="22"/>
-      <c r="F20" s="22"/>
-      <c r="G20" s="22"/>
-      <c r="H20" s="22"/>
-      <c r="I20" s="17"/>
-      <c r="J20" s="15"/>
+      <c r="B20" s="28"/>
+      <c r="C20" s="29"/>
+      <c r="D20" s="31"/>
+      <c r="E20" s="31"/>
+      <c r="F20" s="31"/>
+      <c r="G20" s="31"/>
+      <c r="H20" s="31"/>
+      <c r="I20" s="44"/>
+      <c r="J20" s="18"/>
     </row>
     <row r="21" spans="2:10" ht="15.75" customHeight="1">
-      <c r="B21" s="26">
+      <c r="B21" s="22">
         <v>9</v>
       </c>
-      <c r="C21" s="24" t="s">
+      <c r="C21" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="D21" s="29" t="s">
+      <c r="D21" s="32" t="s">
         <v>40</v>
       </c>
-      <c r="E21" s="29" t="s">
+      <c r="E21" s="32" t="s">
         <v>31</v>
       </c>
-      <c r="F21" s="28"/>
-      <c r="G21" s="28" t="s">
+      <c r="F21" s="24"/>
+      <c r="G21" s="24" t="s">
         <v>30</v>
       </c>
-      <c r="H21" s="28"/>
-      <c r="I21" s="18">
+      <c r="H21" s="24"/>
+      <c r="I21" s="26">
         <v>3</v>
       </c>
-      <c r="J21" s="15" t="s">
+      <c r="J21" s="46" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="22" spans="2:10" ht="15.75" customHeight="1">
+      <c r="B22" s="22"/>
+      <c r="C22" s="20"/>
+      <c r="D22" s="32"/>
+      <c r="E22" s="24"/>
+      <c r="F22" s="24"/>
+      <c r="G22" s="24"/>
+      <c r="H22" s="24"/>
+      <c r="I22" s="26"/>
+      <c r="J22" s="46"/>
+    </row>
+    <row r="23" spans="2:10" ht="15.75" customHeight="1">
+      <c r="B23" s="22"/>
+      <c r="C23" s="20"/>
+      <c r="D23" s="32"/>
+      <c r="E23" s="24"/>
+      <c r="F23" s="24"/>
+      <c r="G23" s="24"/>
+      <c r="H23" s="24"/>
+      <c r="I23" s="26"/>
+      <c r="J23" s="46"/>
+    </row>
+    <row r="24" spans="2:10" ht="15.75" customHeight="1">
+      <c r="B24" s="28">
+        <v>10</v>
+      </c>
+      <c r="C24" s="29" t="s">
+        <v>9</v>
+      </c>
+      <c r="D24" s="30" t="s">
+        <v>34</v>
+      </c>
+      <c r="E24" s="31" t="s">
+        <v>32</v>
+      </c>
+      <c r="F24" s="31"/>
+      <c r="G24" s="30" t="s">
+        <v>33</v>
+      </c>
+      <c r="H24" s="31"/>
+      <c r="I24" s="44">
+        <v>10</v>
+      </c>
+      <c r="J24" s="18" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="22" spans="2:10" ht="15.75" customHeight="1">
-      <c r="B22" s="26"/>
-      <c r="C22" s="24"/>
-      <c r="D22" s="29"/>
-      <c r="E22" s="28"/>
-      <c r="F22" s="28"/>
-      <c r="G22" s="28"/>
-      <c r="H22" s="28"/>
-      <c r="I22" s="18"/>
-      <c r="J22" s="15"/>
-    </row>
-    <row r="23" spans="2:10" ht="15.75" customHeight="1">
-      <c r="B23" s="26"/>
-      <c r="C23" s="24"/>
-      <c r="D23" s="29"/>
-      <c r="E23" s="28"/>
-      <c r="F23" s="28"/>
-      <c r="G23" s="28"/>
-      <c r="H23" s="28"/>
-      <c r="I23" s="18"/>
-      <c r="J23" s="15"/>
-    </row>
-    <row r="24" spans="2:10" ht="15.75" customHeight="1">
-      <c r="B24" s="27">
+    <row r="25" spans="2:10" ht="15.75" customHeight="1">
+      <c r="B25" s="28"/>
+      <c r="C25" s="29"/>
+      <c r="D25" s="31"/>
+      <c r="E25" s="31"/>
+      <c r="F25" s="31"/>
+      <c r="G25" s="30"/>
+      <c r="H25" s="31"/>
+      <c r="I25" s="44"/>
+      <c r="J25" s="18"/>
+    </row>
+    <row r="26" spans="2:10" ht="15.75" customHeight="1">
+      <c r="B26" s="28"/>
+      <c r="C26" s="29"/>
+      <c r="D26" s="31"/>
+      <c r="E26" s="31"/>
+      <c r="F26" s="31"/>
+      <c r="G26" s="30"/>
+      <c r="H26" s="31"/>
+      <c r="I26" s="44"/>
+      <c r="J26" s="18"/>
+    </row>
+    <row r="27" spans="2:10" ht="15.75" customHeight="1">
+      <c r="B27" s="22">
+        <v>11</v>
+      </c>
+      <c r="C27" s="20" t="s">
         <v>10</v>
       </c>
-      <c r="C24" s="19" t="s">
-        <v>9</v>
-      </c>
-      <c r="D24" s="23" t="s">
-        <v>34</v>
-      </c>
-      <c r="E24" s="22" t="s">
-        <v>32</v>
-      </c>
-      <c r="F24" s="22"/>
-      <c r="G24" s="23" t="s">
-        <v>33</v>
-      </c>
-      <c r="H24" s="22"/>
-      <c r="I24" s="17">
-        <v>10</v>
-      </c>
-      <c r="J24" s="15" t="s">
+      <c r="D27" s="32" t="s">
+        <v>47</v>
+      </c>
+      <c r="E27" s="34" t="s">
+        <v>48</v>
+      </c>
+      <c r="F27" s="24"/>
+      <c r="G27" s="32" t="s">
+        <v>36</v>
+      </c>
+      <c r="H27" s="24"/>
+      <c r="I27" s="26">
+        <v>4</v>
+      </c>
+      <c r="J27" s="17" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="25" spans="2:10" ht="15.75" customHeight="1">
-      <c r="B25" s="27"/>
-      <c r="C25" s="19"/>
-      <c r="D25" s="22"/>
-      <c r="E25" s="22"/>
-      <c r="F25" s="22"/>
-      <c r="G25" s="23"/>
-      <c r="H25" s="22"/>
-      <c r="I25" s="17"/>
-      <c r="J25" s="15"/>
-    </row>
-    <row r="26" spans="2:10" ht="15.75" customHeight="1">
-      <c r="B26" s="27"/>
-      <c r="C26" s="19"/>
-      <c r="D26" s="22"/>
-      <c r="E26" s="22"/>
-      <c r="F26" s="22"/>
-      <c r="G26" s="23"/>
-      <c r="H26" s="22"/>
-      <c r="I26" s="17"/>
-      <c r="J26" s="15"/>
-    </row>
-    <row r="27" spans="2:10" ht="15.75" customHeight="1">
-      <c r="B27" s="26">
-        <v>11</v>
-      </c>
-      <c r="C27" s="24" t="s">
-        <v>10</v>
-      </c>
-      <c r="D27" s="29" t="s">
-        <v>47</v>
-      </c>
-      <c r="E27" s="25" t="s">
-        <v>48</v>
-      </c>
-      <c r="F27" s="28"/>
-      <c r="G27" s="29" t="s">
-        <v>36</v>
-      </c>
-      <c r="H27" s="28"/>
-      <c r="I27" s="18">
-        <v>4</v>
-      </c>
-      <c r="J27" s="31" t="s">
-        <v>46</v>
-      </c>
-    </row>
     <row r="28" spans="2:10" ht="15.75" customHeight="1">
-      <c r="B28" s="26"/>
-      <c r="C28" s="24"/>
-      <c r="D28" s="29"/>
-      <c r="E28" s="25"/>
-      <c r="F28" s="28"/>
-      <c r="G28" s="29"/>
-      <c r="H28" s="28"/>
-      <c r="I28" s="18"/>
-      <c r="J28" s="15"/>
+      <c r="B28" s="22"/>
+      <c r="C28" s="20"/>
+      <c r="D28" s="32"/>
+      <c r="E28" s="34"/>
+      <c r="F28" s="24"/>
+      <c r="G28" s="32"/>
+      <c r="H28" s="24"/>
+      <c r="I28" s="26"/>
+      <c r="J28" s="18"/>
     </row>
     <row r="29" spans="2:10" ht="15.75" customHeight="1">
-      <c r="B29" s="26"/>
-      <c r="C29" s="24"/>
-      <c r="D29" s="29"/>
-      <c r="E29" s="25"/>
-      <c r="F29" s="28"/>
-      <c r="G29" s="29"/>
-      <c r="H29" s="28"/>
-      <c r="I29" s="18"/>
-      <c r="J29" s="15"/>
+      <c r="B29" s="22"/>
+      <c r="C29" s="20"/>
+      <c r="D29" s="32"/>
+      <c r="E29" s="34"/>
+      <c r="F29" s="24"/>
+      <c r="G29" s="32"/>
+      <c r="H29" s="24"/>
+      <c r="I29" s="26"/>
+      <c r="J29" s="18"/>
     </row>
     <row r="30" spans="2:10" ht="15.75" customHeight="1">
-      <c r="B30" s="26"/>
-      <c r="C30" s="24"/>
-      <c r="D30" s="29"/>
-      <c r="E30" s="25"/>
-      <c r="F30" s="28"/>
-      <c r="G30" s="29"/>
-      <c r="H30" s="28"/>
-      <c r="I30" s="18"/>
-      <c r="J30" s="15"/>
+      <c r="B30" s="22"/>
+      <c r="C30" s="20"/>
+      <c r="D30" s="32"/>
+      <c r="E30" s="34"/>
+      <c r="F30" s="24"/>
+      <c r="G30" s="32"/>
+      <c r="H30" s="24"/>
+      <c r="I30" s="26"/>
+      <c r="J30" s="18"/>
     </row>
     <row r="31" spans="2:10" ht="15.75" customHeight="1">
-      <c r="B31" s="26"/>
-      <c r="C31" s="24"/>
-      <c r="D31" s="29"/>
-      <c r="E31" s="25"/>
-      <c r="F31" s="28"/>
-      <c r="G31" s="29"/>
-      <c r="H31" s="28"/>
-      <c r="I31" s="18"/>
-      <c r="J31" s="15"/>
+      <c r="B31" s="22"/>
+      <c r="C31" s="20"/>
+      <c r="D31" s="32"/>
+      <c r="E31" s="34"/>
+      <c r="F31" s="24"/>
+      <c r="G31" s="32"/>
+      <c r="H31" s="24"/>
+      <c r="I31" s="26"/>
+      <c r="J31" s="18"/>
     </row>
     <row r="32" spans="2:10" ht="15.75" customHeight="1">
-      <c r="B32" s="32"/>
-      <c r="C32" s="33"/>
-      <c r="D32" s="34"/>
+      <c r="B32" s="23"/>
+      <c r="C32" s="21"/>
+      <c r="D32" s="33"/>
       <c r="E32" s="35"/>
-      <c r="F32" s="36"/>
-      <c r="G32" s="34"/>
-      <c r="H32" s="36"/>
-      <c r="I32" s="37"/>
-      <c r="J32" s="38"/>
+      <c r="F32" s="25"/>
+      <c r="G32" s="33"/>
+      <c r="H32" s="25"/>
+      <c r="I32" s="27"/>
+      <c r="J32" s="19"/>
     </row>
     <row r="33" spans="2:10" ht="63" customHeight="1" thickBot="1">
       <c r="B33" s="6">
@@ -1576,14 +1576,14 @@
       <c r="D33" s="8" t="s">
         <v>49</v>
       </c>
-      <c r="E33" s="45" t="s">
+      <c r="E33" s="15" t="s">
         <v>50</v>
       </c>
-      <c r="F33" s="45"/>
-      <c r="G33" s="46" t="s">
+      <c r="F33" s="15"/>
+      <c r="G33" s="16" t="s">
         <v>51</v>
       </c>
-      <c r="H33" s="45"/>
+      <c r="H33" s="15"/>
       <c r="I33" s="9" t="s">
         <v>43</v>
       </c>
@@ -2552,39 +2552,56 @@
     <row r="992" ht="15.75" customHeight="1"/>
   </sheetData>
   <mergeCells count="99">
-    <mergeCell ref="J27:J32"/>
-    <mergeCell ref="C27:C32"/>
-    <mergeCell ref="B27:B32"/>
-    <mergeCell ref="H27:H32"/>
-    <mergeCell ref="I27:I32"/>
-    <mergeCell ref="B24:B26"/>
-    <mergeCell ref="C24:C26"/>
-    <mergeCell ref="D24:D26"/>
-    <mergeCell ref="E24:E26"/>
-    <mergeCell ref="F24:F26"/>
-    <mergeCell ref="H24:H26"/>
-    <mergeCell ref="G27:G32"/>
-    <mergeCell ref="F27:F32"/>
-    <mergeCell ref="E27:E32"/>
-    <mergeCell ref="D27:D32"/>
-    <mergeCell ref="G24:G26"/>
-    <mergeCell ref="F3:F4"/>
-    <mergeCell ref="F5:F6"/>
-    <mergeCell ref="F7:F8"/>
-    <mergeCell ref="F9:F10"/>
-    <mergeCell ref="F11:F12"/>
-    <mergeCell ref="F21:F23"/>
-    <mergeCell ref="B21:B23"/>
-    <mergeCell ref="C21:C23"/>
-    <mergeCell ref="G21:G23"/>
-    <mergeCell ref="H21:H23"/>
-    <mergeCell ref="D21:D23"/>
-    <mergeCell ref="E21:E23"/>
-    <mergeCell ref="E5:E6"/>
-    <mergeCell ref="E7:E8"/>
-    <mergeCell ref="E9:E10"/>
-    <mergeCell ref="E11:E12"/>
-    <mergeCell ref="E13:E14"/>
+    <mergeCell ref="J13:J14"/>
+    <mergeCell ref="J15:J17"/>
+    <mergeCell ref="J18:J20"/>
+    <mergeCell ref="J21:J23"/>
+    <mergeCell ref="J24:J26"/>
+    <mergeCell ref="J3:J4"/>
+    <mergeCell ref="J5:J6"/>
+    <mergeCell ref="J7:J8"/>
+    <mergeCell ref="J9:J10"/>
+    <mergeCell ref="J11:J12"/>
+    <mergeCell ref="I13:I14"/>
+    <mergeCell ref="I15:I17"/>
+    <mergeCell ref="I18:I20"/>
+    <mergeCell ref="I21:I23"/>
+    <mergeCell ref="I24:I26"/>
+    <mergeCell ref="I3:I4"/>
+    <mergeCell ref="I5:I6"/>
+    <mergeCell ref="I7:I8"/>
+    <mergeCell ref="I9:I10"/>
+    <mergeCell ref="I11:I12"/>
+    <mergeCell ref="C9:C10"/>
+    <mergeCell ref="D11:D12"/>
+    <mergeCell ref="C11:C12"/>
+    <mergeCell ref="D13:D14"/>
+    <mergeCell ref="C13:C14"/>
+    <mergeCell ref="D9:D10"/>
+    <mergeCell ref="C3:C4"/>
+    <mergeCell ref="D3:D4"/>
+    <mergeCell ref="C5:C6"/>
+    <mergeCell ref="D5:D6"/>
+    <mergeCell ref="C7:C8"/>
+    <mergeCell ref="D7:D8"/>
+    <mergeCell ref="B3:B4"/>
+    <mergeCell ref="B5:B6"/>
+    <mergeCell ref="B7:B8"/>
+    <mergeCell ref="B9:B10"/>
+    <mergeCell ref="B11:B12"/>
+    <mergeCell ref="B13:B14"/>
+    <mergeCell ref="B15:B17"/>
+    <mergeCell ref="G18:G20"/>
+    <mergeCell ref="E18:E20"/>
+    <mergeCell ref="C18:C20"/>
+    <mergeCell ref="B18:B20"/>
+    <mergeCell ref="F18:F20"/>
+    <mergeCell ref="E15:E17"/>
+    <mergeCell ref="D15:D17"/>
+    <mergeCell ref="D18:D20"/>
+    <mergeCell ref="F13:F14"/>
+    <mergeCell ref="C15:C17"/>
+    <mergeCell ref="F15:F17"/>
     <mergeCell ref="H18:H20"/>
     <mergeCell ref="E3:E4"/>
     <mergeCell ref="G3:G4"/>
@@ -2601,56 +2618,39 @@
     <mergeCell ref="G11:G12"/>
     <mergeCell ref="G13:G14"/>
     <mergeCell ref="G15:G17"/>
-    <mergeCell ref="B13:B14"/>
-    <mergeCell ref="B15:B17"/>
-    <mergeCell ref="G18:G20"/>
-    <mergeCell ref="E18:E20"/>
-    <mergeCell ref="C18:C20"/>
-    <mergeCell ref="B18:B20"/>
-    <mergeCell ref="F18:F20"/>
-    <mergeCell ref="E15:E17"/>
-    <mergeCell ref="D15:D17"/>
-    <mergeCell ref="D18:D20"/>
-    <mergeCell ref="F13:F14"/>
-    <mergeCell ref="C15:C17"/>
-    <mergeCell ref="F15:F17"/>
-    <mergeCell ref="B3:B4"/>
-    <mergeCell ref="B5:B6"/>
-    <mergeCell ref="B7:B8"/>
-    <mergeCell ref="B9:B10"/>
-    <mergeCell ref="B11:B12"/>
-    <mergeCell ref="C3:C4"/>
-    <mergeCell ref="D3:D4"/>
-    <mergeCell ref="C5:C6"/>
-    <mergeCell ref="D5:D6"/>
-    <mergeCell ref="C7:C8"/>
-    <mergeCell ref="D7:D8"/>
-    <mergeCell ref="C9:C10"/>
-    <mergeCell ref="D11:D12"/>
-    <mergeCell ref="C11:C12"/>
-    <mergeCell ref="D13:D14"/>
-    <mergeCell ref="C13:C14"/>
-    <mergeCell ref="D9:D10"/>
-    <mergeCell ref="I3:I4"/>
-    <mergeCell ref="I5:I6"/>
-    <mergeCell ref="I7:I8"/>
-    <mergeCell ref="I9:I10"/>
-    <mergeCell ref="I11:I12"/>
-    <mergeCell ref="I13:I14"/>
-    <mergeCell ref="I15:I17"/>
-    <mergeCell ref="I18:I20"/>
-    <mergeCell ref="I21:I23"/>
-    <mergeCell ref="I24:I26"/>
-    <mergeCell ref="J3:J4"/>
-    <mergeCell ref="J5:J6"/>
-    <mergeCell ref="J7:J8"/>
-    <mergeCell ref="J9:J10"/>
-    <mergeCell ref="J11:J12"/>
-    <mergeCell ref="J13:J14"/>
-    <mergeCell ref="J15:J17"/>
-    <mergeCell ref="J18:J20"/>
-    <mergeCell ref="J21:J23"/>
-    <mergeCell ref="J24:J26"/>
+    <mergeCell ref="E5:E6"/>
+    <mergeCell ref="E7:E8"/>
+    <mergeCell ref="E9:E10"/>
+    <mergeCell ref="E11:E12"/>
+    <mergeCell ref="E13:E14"/>
+    <mergeCell ref="F21:F23"/>
+    <mergeCell ref="B21:B23"/>
+    <mergeCell ref="C21:C23"/>
+    <mergeCell ref="G21:G23"/>
+    <mergeCell ref="H21:H23"/>
+    <mergeCell ref="D21:D23"/>
+    <mergeCell ref="E21:E23"/>
+    <mergeCell ref="F3:F4"/>
+    <mergeCell ref="F5:F6"/>
+    <mergeCell ref="F7:F8"/>
+    <mergeCell ref="F9:F10"/>
+    <mergeCell ref="F11:F12"/>
+    <mergeCell ref="H24:H26"/>
+    <mergeCell ref="G27:G32"/>
+    <mergeCell ref="F27:F32"/>
+    <mergeCell ref="E27:E32"/>
+    <mergeCell ref="D27:D32"/>
+    <mergeCell ref="G24:G26"/>
+    <mergeCell ref="B24:B26"/>
+    <mergeCell ref="C24:C26"/>
+    <mergeCell ref="D24:D26"/>
+    <mergeCell ref="E24:E26"/>
+    <mergeCell ref="F24:F26"/>
+    <mergeCell ref="J27:J32"/>
+    <mergeCell ref="C27:C32"/>
+    <mergeCell ref="B27:B32"/>
+    <mergeCell ref="H27:H32"/>
+    <mergeCell ref="I27:I32"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape" r:id="rId1"/>

</xml_diff>

<commit_message>
4. Analyses des performances apres la 4eme correction
</commit_message>
<xml_diff>
--- a/Analyses/Modèle-audit-SEO.xlsx
+++ b/Analyses/Modèle-audit-SEO.xlsx
@@ -1015,7 +1015,7 @@
   <dimension ref="B1:AB992"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="J21" sqref="J21:J23"/>
+      <selection activeCell="J9" sqref="J9:J10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.33203125" defaultRowHeight="15" customHeight="1"/>
@@ -1173,7 +1173,7 @@
       </c>
       <c r="H7" s="38"/>
       <c r="I7" s="26">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="J7" s="18" t="s">
         <v>46</v>
@@ -1209,10 +1209,10 @@
       </c>
       <c r="H9" s="31"/>
       <c r="I9" s="44">
-        <v>7</v>
-      </c>
-      <c r="J9" s="18" t="s">
-        <v>46</v>
+        <v>4</v>
+      </c>
+      <c r="J9" s="46" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="10" spans="2:28" ht="15.75" customHeight="1">
@@ -1224,7 +1224,7 @@
       <c r="G10" s="31"/>
       <c r="H10" s="31"/>
       <c r="I10" s="44"/>
-      <c r="J10" s="18"/>
+      <c r="J10" s="46"/>
     </row>
     <row r="11" spans="2:28" ht="15.75" customHeight="1">
       <c r="B11" s="22">
@@ -1245,7 +1245,7 @@
       </c>
       <c r="H11" s="38"/>
       <c r="I11" s="26">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="J11" s="18" t="s">
         <v>46</v>
@@ -1505,7 +1505,7 @@
       </c>
       <c r="H27" s="24"/>
       <c r="I27" s="26">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="J27" s="17" t="s">
         <v>46</v>

</xml_diff>

<commit_message>
Analyse des performances apres 5eme correction
</commit_message>
<xml_diff>
--- a/Analyses/Modèle-audit-SEO.xlsx
+++ b/Analyses/Modèle-audit-SEO.xlsx
@@ -710,93 +710,93 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1015,7 +1015,7 @@
   <dimension ref="B1:AB992"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="I33" sqref="I33"/>
+      <selection activeCell="H24" sqref="H24:H32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.33203125" defaultRowHeight="15" customHeight="1"/>
@@ -1081,490 +1081,490 @@
       <c r="AB2" s="1"/>
     </row>
     <row r="3" spans="2:28" ht="15.75" customHeight="1">
-      <c r="B3" s="31">
+      <c r="B3" s="41">
         <v>1</v>
       </c>
-      <c r="C3" s="28" t="s">
+      <c r="C3" s="42" t="s">
         <v>42</v>
       </c>
-      <c r="D3" s="28" t="s">
+      <c r="D3" s="42" t="s">
         <v>7</v>
       </c>
-      <c r="E3" s="34" t="s">
+      <c r="E3" s="36" t="s">
         <v>16</v>
       </c>
-      <c r="F3" s="34" t="s">
+      <c r="F3" s="36" t="s">
         <v>41</v>
       </c>
-      <c r="G3" s="34" t="s">
+      <c r="G3" s="36" t="s">
         <v>17</v>
       </c>
-      <c r="H3" s="36"/>
-      <c r="I3" s="22">
+      <c r="H3" s="39"/>
+      <c r="I3" s="43">
         <v>1</v>
       </c>
-      <c r="J3" s="19" t="s">
+      <c r="J3" s="45" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="4" spans="2:28" ht="15.75" customHeight="1">
-      <c r="B4" s="32"/>
-      <c r="C4" s="29"/>
-      <c r="D4" s="29"/>
-      <c r="E4" s="35"/>
-      <c r="F4" s="35"/>
-      <c r="G4" s="35"/>
-      <c r="H4" s="35"/>
-      <c r="I4" s="21"/>
-      <c r="J4" s="18"/>
+      <c r="B4" s="22"/>
+      <c r="C4" s="20"/>
+      <c r="D4" s="20"/>
+      <c r="E4" s="24"/>
+      <c r="F4" s="24"/>
+      <c r="G4" s="24"/>
+      <c r="H4" s="24"/>
+      <c r="I4" s="26"/>
+      <c r="J4" s="46"/>
     </row>
     <row r="5" spans="2:28" ht="15.75" customHeight="1">
-      <c r="B5" s="33">
+      <c r="B5" s="28">
         <v>2</v>
       </c>
-      <c r="C5" s="23" t="s">
+      <c r="C5" s="29" t="s">
         <v>42</v>
       </c>
-      <c r="D5" s="26" t="s">
+      <c r="D5" s="31" t="s">
         <v>8</v>
       </c>
-      <c r="E5" s="27" t="s">
+      <c r="E5" s="30" t="s">
         <v>16</v>
       </c>
-      <c r="F5" s="38"/>
-      <c r="G5" s="27" t="s">
+      <c r="F5" s="37"/>
+      <c r="G5" s="30" t="s">
         <v>18</v>
       </c>
-      <c r="H5" s="26"/>
-      <c r="I5" s="20">
+      <c r="H5" s="31"/>
+      <c r="I5" s="44">
         <v>2</v>
       </c>
-      <c r="J5" s="18" t="s">
+      <c r="J5" s="46" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="6" spans="2:28" ht="15.75" customHeight="1">
-      <c r="B6" s="33"/>
-      <c r="C6" s="23"/>
-      <c r="D6" s="26"/>
-      <c r="E6" s="26"/>
-      <c r="F6" s="38"/>
-      <c r="G6" s="26"/>
-      <c r="H6" s="26"/>
-      <c r="I6" s="20"/>
-      <c r="J6" s="18"/>
+      <c r="B6" s="28"/>
+      <c r="C6" s="29"/>
+      <c r="D6" s="31"/>
+      <c r="E6" s="31"/>
+      <c r="F6" s="37"/>
+      <c r="G6" s="31"/>
+      <c r="H6" s="31"/>
+      <c r="I6" s="44"/>
+      <c r="J6" s="46"/>
     </row>
     <row r="7" spans="2:28" ht="15.75" customHeight="1">
-      <c r="B7" s="32">
+      <c r="B7" s="22">
         <v>3</v>
       </c>
-      <c r="C7" s="25" t="s">
+      <c r="C7" s="40" t="s">
         <v>6</v>
       </c>
-      <c r="D7" s="30" t="s">
+      <c r="D7" s="34" t="s">
         <v>27</v>
       </c>
-      <c r="E7" s="30" t="s">
+      <c r="E7" s="34" t="s">
         <v>24</v>
       </c>
-      <c r="F7" s="24"/>
-      <c r="G7" s="30" t="s">
+      <c r="F7" s="38"/>
+      <c r="G7" s="34" t="s">
         <v>19</v>
       </c>
-      <c r="H7" s="24"/>
-      <c r="I7" s="21">
+      <c r="H7" s="38"/>
+      <c r="I7" s="26">
         <v>6</v>
       </c>
-      <c r="J7" s="17" t="s">
+      <c r="J7" s="18" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="8" spans="2:28" ht="15.75" customHeight="1">
-      <c r="B8" s="32"/>
-      <c r="C8" s="25"/>
-      <c r="D8" s="24"/>
-      <c r="E8" s="24"/>
-      <c r="F8" s="24"/>
-      <c r="G8" s="24"/>
-      <c r="H8" s="24"/>
-      <c r="I8" s="21"/>
-      <c r="J8" s="17"/>
+      <c r="B8" s="22"/>
+      <c r="C8" s="40"/>
+      <c r="D8" s="38"/>
+      <c r="E8" s="38"/>
+      <c r="F8" s="38"/>
+      <c r="G8" s="38"/>
+      <c r="H8" s="38"/>
+      <c r="I8" s="26"/>
+      <c r="J8" s="18"/>
     </row>
     <row r="9" spans="2:28" ht="15.75" customHeight="1">
-      <c r="B9" s="33">
+      <c r="B9" s="28">
         <v>4</v>
       </c>
-      <c r="C9" s="23" t="s">
+      <c r="C9" s="29" t="s">
         <v>6</v>
       </c>
-      <c r="D9" s="27" t="s">
+      <c r="D9" s="30" t="s">
         <v>28</v>
       </c>
-      <c r="E9" s="27" t="s">
+      <c r="E9" s="30" t="s">
         <v>25</v>
       </c>
-      <c r="F9" s="26"/>
-      <c r="G9" s="27" t="s">
+      <c r="F9" s="31"/>
+      <c r="G9" s="30" t="s">
         <v>20</v>
       </c>
-      <c r="H9" s="26"/>
-      <c r="I9" s="20">
+      <c r="H9" s="31"/>
+      <c r="I9" s="44">
         <v>4</v>
       </c>
-      <c r="J9" s="18" t="s">
+      <c r="J9" s="46" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="10" spans="2:28" ht="15.75" customHeight="1">
-      <c r="B10" s="33"/>
-      <c r="C10" s="23"/>
-      <c r="D10" s="26"/>
-      <c r="E10" s="26"/>
-      <c r="F10" s="26"/>
-      <c r="G10" s="26"/>
-      <c r="H10" s="26"/>
-      <c r="I10" s="20"/>
-      <c r="J10" s="18"/>
+      <c r="B10" s="28"/>
+      <c r="C10" s="29"/>
+      <c r="D10" s="31"/>
+      <c r="E10" s="31"/>
+      <c r="F10" s="31"/>
+      <c r="G10" s="31"/>
+      <c r="H10" s="31"/>
+      <c r="I10" s="44"/>
+      <c r="J10" s="46"/>
     </row>
     <row r="11" spans="2:28" ht="15.75" customHeight="1">
-      <c r="B11" s="32">
+      <c r="B11" s="22">
         <v>5</v>
       </c>
-      <c r="C11" s="25" t="s">
+      <c r="C11" s="40" t="s">
         <v>10</v>
       </c>
-      <c r="D11" s="24" t="s">
+      <c r="D11" s="38" t="s">
         <v>11</v>
       </c>
-      <c r="E11" s="30" t="s">
+      <c r="E11" s="34" t="s">
         <v>39</v>
       </c>
-      <c r="F11" s="24"/>
-      <c r="G11" s="30" t="s">
+      <c r="F11" s="38"/>
+      <c r="G11" s="34" t="s">
         <v>21</v>
       </c>
-      <c r="H11" s="24"/>
-      <c r="I11" s="21">
+      <c r="H11" s="38"/>
+      <c r="I11" s="26">
         <v>5</v>
       </c>
-      <c r="J11" s="17" t="s">
+      <c r="J11" s="46" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="12" spans="2:28" ht="15.75" customHeight="1">
+      <c r="B12" s="22"/>
+      <c r="C12" s="40"/>
+      <c r="D12" s="38"/>
+      <c r="E12" s="38"/>
+      <c r="F12" s="38"/>
+      <c r="G12" s="38"/>
+      <c r="H12" s="38"/>
+      <c r="I12" s="26"/>
+      <c r="J12" s="46"/>
+    </row>
+    <row r="13" spans="2:28" ht="15.75" customHeight="1">
+      <c r="B13" s="28">
+        <v>6</v>
+      </c>
+      <c r="C13" s="29" t="s">
+        <v>6</v>
+      </c>
+      <c r="D13" s="31" t="s">
+        <v>12</v>
+      </c>
+      <c r="E13" s="30" t="s">
+        <v>37</v>
+      </c>
+      <c r="F13" s="31"/>
+      <c r="G13" s="30" t="s">
+        <v>22</v>
+      </c>
+      <c r="H13" s="31"/>
+      <c r="I13" s="44">
+        <v>8</v>
+      </c>
+      <c r="J13" s="18" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="12" spans="2:28" ht="15.75" customHeight="1">
-      <c r="B12" s="32"/>
-      <c r="C12" s="25"/>
-      <c r="D12" s="24"/>
-      <c r="E12" s="24"/>
-      <c r="F12" s="24"/>
-      <c r="G12" s="24"/>
-      <c r="H12" s="24"/>
-      <c r="I12" s="21"/>
-      <c r="J12" s="17"/>
-    </row>
-    <row r="13" spans="2:28" ht="15.75" customHeight="1">
-      <c r="B13" s="33">
+    <row r="14" spans="2:28" ht="15.75" customHeight="1">
+      <c r="B14" s="28"/>
+      <c r="C14" s="29"/>
+      <c r="D14" s="31"/>
+      <c r="E14" s="31"/>
+      <c r="F14" s="31"/>
+      <c r="G14" s="31"/>
+      <c r="H14" s="31"/>
+      <c r="I14" s="44"/>
+      <c r="J14" s="18"/>
+    </row>
+    <row r="15" spans="2:28" ht="15.75" customHeight="1">
+      <c r="B15" s="22">
+        <v>7</v>
+      </c>
+      <c r="C15" s="40" t="s">
         <v>6</v>
       </c>
-      <c r="C13" s="23" t="s">
-        <v>6</v>
-      </c>
-      <c r="D13" s="26" t="s">
-        <v>12</v>
-      </c>
-      <c r="E13" s="27" t="s">
-        <v>37</v>
-      </c>
-      <c r="F13" s="26"/>
-      <c r="G13" s="27" t="s">
-        <v>22</v>
-      </c>
-      <c r="H13" s="26"/>
-      <c r="I13" s="20">
+      <c r="D15" s="34" t="s">
+        <v>29</v>
+      </c>
+      <c r="E15" s="34" t="s">
+        <v>26</v>
+      </c>
+      <c r="F15" s="38"/>
+      <c r="G15" s="34" t="s">
+        <v>23</v>
+      </c>
+      <c r="H15" s="38"/>
+      <c r="I15" s="26">
+        <v>9</v>
+      </c>
+      <c r="J15" s="18" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="16" spans="2:28" ht="15.75" customHeight="1">
+      <c r="B16" s="22"/>
+      <c r="C16" s="40"/>
+      <c r="D16" s="38"/>
+      <c r="E16" s="38"/>
+      <c r="F16" s="38"/>
+      <c r="G16" s="38"/>
+      <c r="H16" s="38"/>
+      <c r="I16" s="26"/>
+      <c r="J16" s="18"/>
+    </row>
+    <row r="17" spans="2:10" ht="15.75" customHeight="1">
+      <c r="B17" s="22"/>
+      <c r="C17" s="40"/>
+      <c r="D17" s="38"/>
+      <c r="E17" s="38"/>
+      <c r="F17" s="38"/>
+      <c r="G17" s="38"/>
+      <c r="H17" s="38"/>
+      <c r="I17" s="26"/>
+      <c r="J17" s="18"/>
+    </row>
+    <row r="18" spans="2:10" ht="15.75" customHeight="1">
+      <c r="B18" s="28">
         <v>8</v>
       </c>
-      <c r="J13" s="17" t="s">
+      <c r="C18" s="29" t="s">
+        <v>9</v>
+      </c>
+      <c r="D18" s="30" t="s">
+        <v>35</v>
+      </c>
+      <c r="E18" s="31" t="s">
+        <v>13</v>
+      </c>
+      <c r="F18" s="31"/>
+      <c r="G18" s="30" t="s">
+        <v>15</v>
+      </c>
+      <c r="H18" s="31"/>
+      <c r="I18" s="44" t="s">
+        <v>43</v>
+      </c>
+      <c r="J18" s="18" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="14" spans="2:28" ht="15.75" customHeight="1">
-      <c r="B14" s="33"/>
-      <c r="C14" s="23"/>
-      <c r="D14" s="26"/>
-      <c r="E14" s="26"/>
-      <c r="F14" s="26"/>
-      <c r="G14" s="26"/>
-      <c r="H14" s="26"/>
-      <c r="I14" s="20"/>
-      <c r="J14" s="17"/>
-    </row>
-    <row r="15" spans="2:28" ht="15.75" customHeight="1">
-      <c r="B15" s="32">
+    <row r="19" spans="2:10" ht="15.75" customHeight="1">
+      <c r="B19" s="28"/>
+      <c r="C19" s="29"/>
+      <c r="D19" s="31"/>
+      <c r="E19" s="31"/>
+      <c r="F19" s="31"/>
+      <c r="G19" s="31"/>
+      <c r="H19" s="31"/>
+      <c r="I19" s="44"/>
+      <c r="J19" s="18"/>
+    </row>
+    <row r="20" spans="2:10" ht="15.75" customHeight="1">
+      <c r="B20" s="28"/>
+      <c r="C20" s="29"/>
+      <c r="D20" s="31"/>
+      <c r="E20" s="31"/>
+      <c r="F20" s="31"/>
+      <c r="G20" s="31"/>
+      <c r="H20" s="31"/>
+      <c r="I20" s="44"/>
+      <c r="J20" s="18"/>
+    </row>
+    <row r="21" spans="2:10" ht="15.75" customHeight="1">
+      <c r="B21" s="22">
+        <v>9</v>
+      </c>
+      <c r="C21" s="20" t="s">
+        <v>9</v>
+      </c>
+      <c r="D21" s="32" t="s">
+        <v>40</v>
+      </c>
+      <c r="E21" s="32" t="s">
+        <v>31</v>
+      </c>
+      <c r="F21" s="24"/>
+      <c r="G21" s="24" t="s">
+        <v>30</v>
+      </c>
+      <c r="H21" s="24"/>
+      <c r="I21" s="26">
+        <v>3</v>
+      </c>
+      <c r="J21" s="46" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="22" spans="2:10" ht="15.75" customHeight="1">
+      <c r="B22" s="22"/>
+      <c r="C22" s="20"/>
+      <c r="D22" s="32"/>
+      <c r="E22" s="24"/>
+      <c r="F22" s="24"/>
+      <c r="G22" s="24"/>
+      <c r="H22" s="24"/>
+      <c r="I22" s="26"/>
+      <c r="J22" s="46"/>
+    </row>
+    <row r="23" spans="2:10" ht="15.75" customHeight="1">
+      <c r="B23" s="22"/>
+      <c r="C23" s="20"/>
+      <c r="D23" s="32"/>
+      <c r="E23" s="24"/>
+      <c r="F23" s="24"/>
+      <c r="G23" s="24"/>
+      <c r="H23" s="24"/>
+      <c r="I23" s="26"/>
+      <c r="J23" s="46"/>
+    </row>
+    <row r="24" spans="2:10" ht="15.75" customHeight="1">
+      <c r="B24" s="28">
+        <v>10</v>
+      </c>
+      <c r="C24" s="29" t="s">
+        <v>9</v>
+      </c>
+      <c r="D24" s="30" t="s">
+        <v>34</v>
+      </c>
+      <c r="E24" s="31" t="s">
+        <v>32</v>
+      </c>
+      <c r="F24" s="31"/>
+      <c r="G24" s="30" t="s">
+        <v>33</v>
+      </c>
+      <c r="H24" s="31"/>
+      <c r="I24" s="44">
+        <v>10</v>
+      </c>
+      <c r="J24" s="18" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="25" spans="2:10" ht="15.75" customHeight="1">
+      <c r="B25" s="28"/>
+      <c r="C25" s="29"/>
+      <c r="D25" s="31"/>
+      <c r="E25" s="31"/>
+      <c r="F25" s="31"/>
+      <c r="G25" s="30"/>
+      <c r="H25" s="31"/>
+      <c r="I25" s="44"/>
+      <c r="J25" s="18"/>
+    </row>
+    <row r="26" spans="2:10" ht="15.75" customHeight="1">
+      <c r="B26" s="28"/>
+      <c r="C26" s="29"/>
+      <c r="D26" s="31"/>
+      <c r="E26" s="31"/>
+      <c r="F26" s="31"/>
+      <c r="G26" s="30"/>
+      <c r="H26" s="31"/>
+      <c r="I26" s="44"/>
+      <c r="J26" s="18"/>
+    </row>
+    <row r="27" spans="2:10" ht="15.75" customHeight="1">
+      <c r="B27" s="22">
+        <v>11</v>
+      </c>
+      <c r="C27" s="20" t="s">
+        <v>10</v>
+      </c>
+      <c r="D27" s="32" t="s">
+        <v>47</v>
+      </c>
+      <c r="E27" s="34" t="s">
+        <v>48</v>
+      </c>
+      <c r="F27" s="24"/>
+      <c r="G27" s="32" t="s">
+        <v>36</v>
+      </c>
+      <c r="H27" s="24"/>
+      <c r="I27" s="26">
         <v>7</v>
       </c>
-      <c r="C15" s="25" t="s">
-        <v>6</v>
-      </c>
-      <c r="D15" s="30" t="s">
-        <v>29</v>
-      </c>
-      <c r="E15" s="30" t="s">
-        <v>26</v>
-      </c>
-      <c r="F15" s="24"/>
-      <c r="G15" s="30" t="s">
-        <v>23</v>
-      </c>
-      <c r="H15" s="24"/>
-      <c r="I15" s="21">
-        <v>9</v>
-      </c>
-      <c r="J15" s="17" t="s">
+      <c r="J27" s="17" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="16" spans="2:28" ht="15.75" customHeight="1">
-      <c r="B16" s="32"/>
-      <c r="C16" s="25"/>
-      <c r="D16" s="24"/>
-      <c r="E16" s="24"/>
-      <c r="F16" s="24"/>
-      <c r="G16" s="24"/>
-      <c r="H16" s="24"/>
-      <c r="I16" s="21"/>
-      <c r="J16" s="17"/>
-    </row>
-    <row r="17" spans="2:10" ht="15.75" customHeight="1">
-      <c r="B17" s="32"/>
-      <c r="C17" s="25"/>
-      <c r="D17" s="24"/>
-      <c r="E17" s="24"/>
-      <c r="F17" s="24"/>
-      <c r="G17" s="24"/>
-      <c r="H17" s="24"/>
-      <c r="I17" s="21"/>
-      <c r="J17" s="17"/>
-    </row>
-    <row r="18" spans="2:10" ht="15.75" customHeight="1">
-      <c r="B18" s="33">
-        <v>8</v>
-      </c>
-      <c r="C18" s="23" t="s">
-        <v>9</v>
-      </c>
-      <c r="D18" s="27" t="s">
-        <v>35</v>
-      </c>
-      <c r="E18" s="26" t="s">
-        <v>13</v>
-      </c>
-      <c r="F18" s="26"/>
-      <c r="G18" s="27" t="s">
-        <v>15</v>
-      </c>
-      <c r="H18" s="26"/>
-      <c r="I18" s="20" t="s">
-        <v>43</v>
-      </c>
-      <c r="J18" s="17" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="19" spans="2:10" ht="15.75" customHeight="1">
-      <c r="B19" s="33"/>
-      <c r="C19" s="23"/>
-      <c r="D19" s="26"/>
-      <c r="E19" s="26"/>
-      <c r="F19" s="26"/>
-      <c r="G19" s="26"/>
-      <c r="H19" s="26"/>
-      <c r="I19" s="20"/>
-      <c r="J19" s="17"/>
-    </row>
-    <row r="20" spans="2:10" ht="15.75" customHeight="1">
-      <c r="B20" s="33"/>
-      <c r="C20" s="23"/>
-      <c r="D20" s="26"/>
-      <c r="E20" s="26"/>
-      <c r="F20" s="26"/>
-      <c r="G20" s="26"/>
-      <c r="H20" s="26"/>
-      <c r="I20" s="20"/>
-      <c r="J20" s="17"/>
-    </row>
-    <row r="21" spans="2:10" ht="15.75" customHeight="1">
-      <c r="B21" s="32">
-        <v>9</v>
-      </c>
-      <c r="C21" s="29" t="s">
-        <v>9</v>
-      </c>
-      <c r="D21" s="37" t="s">
-        <v>40</v>
-      </c>
-      <c r="E21" s="37" t="s">
-        <v>31</v>
-      </c>
-      <c r="F21" s="35"/>
-      <c r="G21" s="35" t="s">
-        <v>30</v>
-      </c>
-      <c r="H21" s="35"/>
-      <c r="I21" s="21">
-        <v>3</v>
-      </c>
-      <c r="J21" s="18" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="22" spans="2:10" ht="15.75" customHeight="1">
-      <c r="B22" s="32"/>
-      <c r="C22" s="29"/>
-      <c r="D22" s="37"/>
-      <c r="E22" s="35"/>
-      <c r="F22" s="35"/>
-      <c r="G22" s="35"/>
-      <c r="H22" s="35"/>
-      <c r="I22" s="21"/>
-      <c r="J22" s="18"/>
-    </row>
-    <row r="23" spans="2:10" ht="15.75" customHeight="1">
-      <c r="B23" s="32"/>
-      <c r="C23" s="29"/>
-      <c r="D23" s="37"/>
-      <c r="E23" s="35"/>
-      <c r="F23" s="35"/>
-      <c r="G23" s="35"/>
-      <c r="H23" s="35"/>
-      <c r="I23" s="21"/>
-      <c r="J23" s="18"/>
-    </row>
-    <row r="24" spans="2:10" ht="15.75" customHeight="1">
-      <c r="B24" s="33">
-        <v>10</v>
-      </c>
-      <c r="C24" s="23" t="s">
-        <v>9</v>
-      </c>
-      <c r="D24" s="27" t="s">
-        <v>34</v>
-      </c>
-      <c r="E24" s="26" t="s">
-        <v>32</v>
-      </c>
-      <c r="F24" s="26"/>
-      <c r="G24" s="27" t="s">
-        <v>33</v>
-      </c>
-      <c r="H24" s="26"/>
-      <c r="I24" s="20">
-        <v>10</v>
-      </c>
-      <c r="J24" s="17" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="25" spans="2:10" ht="15.75" customHeight="1">
-      <c r="B25" s="33"/>
-      <c r="C25" s="23"/>
-      <c r="D25" s="26"/>
-      <c r="E25" s="26"/>
-      <c r="F25" s="26"/>
-      <c r="G25" s="27"/>
-      <c r="H25" s="26"/>
-      <c r="I25" s="20"/>
-      <c r="J25" s="17"/>
-    </row>
-    <row r="26" spans="2:10" ht="15.75" customHeight="1">
-      <c r="B26" s="33"/>
-      <c r="C26" s="23"/>
-      <c r="D26" s="26"/>
-      <c r="E26" s="26"/>
-      <c r="F26" s="26"/>
-      <c r="G26" s="27"/>
-      <c r="H26" s="26"/>
-      <c r="I26" s="20"/>
-      <c r="J26" s="17"/>
-    </row>
-    <row r="27" spans="2:10" ht="15.75" customHeight="1">
-      <c r="B27" s="32">
-        <v>11</v>
-      </c>
-      <c r="C27" s="29" t="s">
-        <v>10</v>
-      </c>
-      <c r="D27" s="37" t="s">
-        <v>47</v>
-      </c>
-      <c r="E27" s="30" t="s">
-        <v>48</v>
-      </c>
-      <c r="F27" s="35"/>
-      <c r="G27" s="37" t="s">
-        <v>36</v>
-      </c>
-      <c r="H27" s="35"/>
-      <c r="I27" s="21">
-        <v>7</v>
-      </c>
-      <c r="J27" s="42" t="s">
-        <v>46</v>
-      </c>
-    </row>
     <row r="28" spans="2:10" ht="15.75" customHeight="1">
-      <c r="B28" s="32"/>
-      <c r="C28" s="29"/>
-      <c r="D28" s="37"/>
-      <c r="E28" s="30"/>
-      <c r="F28" s="35"/>
-      <c r="G28" s="37"/>
-      <c r="H28" s="35"/>
-      <c r="I28" s="21"/>
-      <c r="J28" s="17"/>
+      <c r="B28" s="22"/>
+      <c r="C28" s="20"/>
+      <c r="D28" s="32"/>
+      <c r="E28" s="34"/>
+      <c r="F28" s="24"/>
+      <c r="G28" s="32"/>
+      <c r="H28" s="24"/>
+      <c r="I28" s="26"/>
+      <c r="J28" s="18"/>
     </row>
     <row r="29" spans="2:10" ht="15.75" customHeight="1">
-      <c r="B29" s="32"/>
-      <c r="C29" s="29"/>
-      <c r="D29" s="37"/>
-      <c r="E29" s="30"/>
-      <c r="F29" s="35"/>
-      <c r="G29" s="37"/>
-      <c r="H29" s="35"/>
-      <c r="I29" s="21"/>
-      <c r="J29" s="17"/>
+      <c r="B29" s="22"/>
+      <c r="C29" s="20"/>
+      <c r="D29" s="32"/>
+      <c r="E29" s="34"/>
+      <c r="F29" s="24"/>
+      <c r="G29" s="32"/>
+      <c r="H29" s="24"/>
+      <c r="I29" s="26"/>
+      <c r="J29" s="18"/>
     </row>
     <row r="30" spans="2:10" ht="15.75" customHeight="1">
-      <c r="B30" s="32"/>
-      <c r="C30" s="29"/>
-      <c r="D30" s="37"/>
-      <c r="E30" s="30"/>
-      <c r="F30" s="35"/>
-      <c r="G30" s="37"/>
-      <c r="H30" s="35"/>
-      <c r="I30" s="21"/>
-      <c r="J30" s="17"/>
+      <c r="B30" s="22"/>
+      <c r="C30" s="20"/>
+      <c r="D30" s="32"/>
+      <c r="E30" s="34"/>
+      <c r="F30" s="24"/>
+      <c r="G30" s="32"/>
+      <c r="H30" s="24"/>
+      <c r="I30" s="26"/>
+      <c r="J30" s="18"/>
     </row>
     <row r="31" spans="2:10" ht="15.75" customHeight="1">
-      <c r="B31" s="32"/>
-      <c r="C31" s="29"/>
-      <c r="D31" s="37"/>
-      <c r="E31" s="30"/>
-      <c r="F31" s="35"/>
-      <c r="G31" s="37"/>
-      <c r="H31" s="35"/>
-      <c r="I31" s="21"/>
-      <c r="J31" s="17"/>
+      <c r="B31" s="22"/>
+      <c r="C31" s="20"/>
+      <c r="D31" s="32"/>
+      <c r="E31" s="34"/>
+      <c r="F31" s="24"/>
+      <c r="G31" s="32"/>
+      <c r="H31" s="24"/>
+      <c r="I31" s="26"/>
+      <c r="J31" s="18"/>
     </row>
     <row r="32" spans="2:10" ht="15.75" customHeight="1">
-      <c r="B32" s="45"/>
-      <c r="C32" s="44"/>
-      <c r="D32" s="39"/>
-      <c r="E32" s="41"/>
-      <c r="F32" s="40"/>
-      <c r="G32" s="39"/>
-      <c r="H32" s="40"/>
-      <c r="I32" s="46"/>
-      <c r="J32" s="43"/>
+      <c r="B32" s="23"/>
+      <c r="C32" s="21"/>
+      <c r="D32" s="33"/>
+      <c r="E32" s="35"/>
+      <c r="F32" s="25"/>
+      <c r="G32" s="33"/>
+      <c r="H32" s="25"/>
+      <c r="I32" s="27"/>
+      <c r="J32" s="19"/>
     </row>
     <row r="33" spans="2:10" ht="63" customHeight="1" thickBot="1">
       <c r="B33" s="6">
@@ -2552,39 +2552,56 @@
     <row r="992" ht="15.75" customHeight="1"/>
   </sheetData>
   <mergeCells count="99">
-    <mergeCell ref="J27:J32"/>
-    <mergeCell ref="C27:C32"/>
-    <mergeCell ref="B27:B32"/>
-    <mergeCell ref="H27:H32"/>
-    <mergeCell ref="I27:I32"/>
-    <mergeCell ref="B24:B26"/>
-    <mergeCell ref="C24:C26"/>
-    <mergeCell ref="D24:D26"/>
-    <mergeCell ref="E24:E26"/>
-    <mergeCell ref="F24:F26"/>
-    <mergeCell ref="H24:H26"/>
-    <mergeCell ref="G27:G32"/>
-    <mergeCell ref="F27:F32"/>
-    <mergeCell ref="E27:E32"/>
-    <mergeCell ref="D27:D32"/>
-    <mergeCell ref="G24:G26"/>
-    <mergeCell ref="F3:F4"/>
-    <mergeCell ref="F5:F6"/>
-    <mergeCell ref="F7:F8"/>
-    <mergeCell ref="F9:F10"/>
-    <mergeCell ref="F11:F12"/>
-    <mergeCell ref="F21:F23"/>
-    <mergeCell ref="B21:B23"/>
-    <mergeCell ref="C21:C23"/>
-    <mergeCell ref="G21:G23"/>
-    <mergeCell ref="H21:H23"/>
-    <mergeCell ref="D21:D23"/>
-    <mergeCell ref="E21:E23"/>
-    <mergeCell ref="E5:E6"/>
-    <mergeCell ref="E7:E8"/>
-    <mergeCell ref="E9:E10"/>
-    <mergeCell ref="E11:E12"/>
-    <mergeCell ref="E13:E14"/>
+    <mergeCell ref="J13:J14"/>
+    <mergeCell ref="J15:J17"/>
+    <mergeCell ref="J18:J20"/>
+    <mergeCell ref="J21:J23"/>
+    <mergeCell ref="J24:J26"/>
+    <mergeCell ref="J3:J4"/>
+    <mergeCell ref="J5:J6"/>
+    <mergeCell ref="J7:J8"/>
+    <mergeCell ref="J9:J10"/>
+    <mergeCell ref="J11:J12"/>
+    <mergeCell ref="I13:I14"/>
+    <mergeCell ref="I15:I17"/>
+    <mergeCell ref="I18:I20"/>
+    <mergeCell ref="I21:I23"/>
+    <mergeCell ref="I24:I26"/>
+    <mergeCell ref="I3:I4"/>
+    <mergeCell ref="I5:I6"/>
+    <mergeCell ref="I7:I8"/>
+    <mergeCell ref="I9:I10"/>
+    <mergeCell ref="I11:I12"/>
+    <mergeCell ref="C9:C10"/>
+    <mergeCell ref="D11:D12"/>
+    <mergeCell ref="C11:C12"/>
+    <mergeCell ref="D13:D14"/>
+    <mergeCell ref="C13:C14"/>
+    <mergeCell ref="D9:D10"/>
+    <mergeCell ref="C3:C4"/>
+    <mergeCell ref="D3:D4"/>
+    <mergeCell ref="C5:C6"/>
+    <mergeCell ref="D5:D6"/>
+    <mergeCell ref="C7:C8"/>
+    <mergeCell ref="D7:D8"/>
+    <mergeCell ref="B3:B4"/>
+    <mergeCell ref="B5:B6"/>
+    <mergeCell ref="B7:B8"/>
+    <mergeCell ref="B9:B10"/>
+    <mergeCell ref="B11:B12"/>
+    <mergeCell ref="B13:B14"/>
+    <mergeCell ref="B15:B17"/>
+    <mergeCell ref="G18:G20"/>
+    <mergeCell ref="E18:E20"/>
+    <mergeCell ref="C18:C20"/>
+    <mergeCell ref="B18:B20"/>
+    <mergeCell ref="F18:F20"/>
+    <mergeCell ref="E15:E17"/>
+    <mergeCell ref="D15:D17"/>
+    <mergeCell ref="D18:D20"/>
+    <mergeCell ref="F13:F14"/>
+    <mergeCell ref="C15:C17"/>
+    <mergeCell ref="F15:F17"/>
     <mergeCell ref="H18:H20"/>
     <mergeCell ref="E3:E4"/>
     <mergeCell ref="G3:G4"/>
@@ -2601,56 +2618,39 @@
     <mergeCell ref="G11:G12"/>
     <mergeCell ref="G13:G14"/>
     <mergeCell ref="G15:G17"/>
-    <mergeCell ref="B13:B14"/>
-    <mergeCell ref="B15:B17"/>
-    <mergeCell ref="G18:G20"/>
-    <mergeCell ref="E18:E20"/>
-    <mergeCell ref="C18:C20"/>
-    <mergeCell ref="B18:B20"/>
-    <mergeCell ref="F18:F20"/>
-    <mergeCell ref="E15:E17"/>
-    <mergeCell ref="D15:D17"/>
-    <mergeCell ref="D18:D20"/>
-    <mergeCell ref="F13:F14"/>
-    <mergeCell ref="C15:C17"/>
-    <mergeCell ref="F15:F17"/>
-    <mergeCell ref="B3:B4"/>
-    <mergeCell ref="B5:B6"/>
-    <mergeCell ref="B7:B8"/>
-    <mergeCell ref="B9:B10"/>
-    <mergeCell ref="B11:B12"/>
-    <mergeCell ref="C3:C4"/>
-    <mergeCell ref="D3:D4"/>
-    <mergeCell ref="C5:C6"/>
-    <mergeCell ref="D5:D6"/>
-    <mergeCell ref="C7:C8"/>
-    <mergeCell ref="D7:D8"/>
-    <mergeCell ref="C9:C10"/>
-    <mergeCell ref="D11:D12"/>
-    <mergeCell ref="C11:C12"/>
-    <mergeCell ref="D13:D14"/>
-    <mergeCell ref="C13:C14"/>
-    <mergeCell ref="D9:D10"/>
-    <mergeCell ref="I3:I4"/>
-    <mergeCell ref="I5:I6"/>
-    <mergeCell ref="I7:I8"/>
-    <mergeCell ref="I9:I10"/>
-    <mergeCell ref="I11:I12"/>
-    <mergeCell ref="I13:I14"/>
-    <mergeCell ref="I15:I17"/>
-    <mergeCell ref="I18:I20"/>
-    <mergeCell ref="I21:I23"/>
-    <mergeCell ref="I24:I26"/>
-    <mergeCell ref="J3:J4"/>
-    <mergeCell ref="J5:J6"/>
-    <mergeCell ref="J7:J8"/>
-    <mergeCell ref="J9:J10"/>
-    <mergeCell ref="J11:J12"/>
-    <mergeCell ref="J13:J14"/>
-    <mergeCell ref="J15:J17"/>
-    <mergeCell ref="J18:J20"/>
-    <mergeCell ref="J21:J23"/>
-    <mergeCell ref="J24:J26"/>
+    <mergeCell ref="E5:E6"/>
+    <mergeCell ref="E7:E8"/>
+    <mergeCell ref="E9:E10"/>
+    <mergeCell ref="E11:E12"/>
+    <mergeCell ref="E13:E14"/>
+    <mergeCell ref="F21:F23"/>
+    <mergeCell ref="B21:B23"/>
+    <mergeCell ref="C21:C23"/>
+    <mergeCell ref="G21:G23"/>
+    <mergeCell ref="H21:H23"/>
+    <mergeCell ref="D21:D23"/>
+    <mergeCell ref="E21:E23"/>
+    <mergeCell ref="F3:F4"/>
+    <mergeCell ref="F5:F6"/>
+    <mergeCell ref="F7:F8"/>
+    <mergeCell ref="F9:F10"/>
+    <mergeCell ref="F11:F12"/>
+    <mergeCell ref="H24:H26"/>
+    <mergeCell ref="G27:G32"/>
+    <mergeCell ref="F27:F32"/>
+    <mergeCell ref="E27:E32"/>
+    <mergeCell ref="D27:D32"/>
+    <mergeCell ref="G24:G26"/>
+    <mergeCell ref="B24:B26"/>
+    <mergeCell ref="C24:C26"/>
+    <mergeCell ref="D24:D26"/>
+    <mergeCell ref="E24:E26"/>
+    <mergeCell ref="F24:F26"/>
+    <mergeCell ref="J27:J32"/>
+    <mergeCell ref="C27:C32"/>
+    <mergeCell ref="B27:B32"/>
+    <mergeCell ref="H27:H32"/>
+    <mergeCell ref="I27:I32"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape" r:id="rId1"/>

</xml_diff>

<commit_message>
Correction du fichier 'Audit du SEO'
</commit_message>
<xml_diff>
--- a/Analyses/Modèle-audit-SEO.xlsx
+++ b/Analyses/Modèle-audit-SEO.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="55">
   <si>
     <t>Catégorie</t>
   </si>
@@ -296,6 +296,20 @@
   <si>
     <t xml:space="preserve"> Ne mettre qu'un titre &lt;h1&gt; et
  mettre titres intermédiaires</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Corriger les différences dans les 
+&lt;head&gt; des fichiers html,
+ notamment les &lt;link stylesheet&gt;
+ et les script.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Corriger les erreurs de relations
+ fichiers</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Mettre en concordance les
+ pages</t>
   </si>
 </sst>
 </file>
@@ -659,7 +673,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="9" fillId="5" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="47">
+  <cellXfs count="53">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -682,9 +696,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -709,95 +720,116 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="6" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1015,7 +1047,7 @@
   <dimension ref="B1:AB992"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="H24" sqref="H24:H32"/>
+      <selection activeCell="B3" sqref="B3:J34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.33203125" defaultRowHeight="15" customHeight="1"/>
@@ -1034,31 +1066,31 @@
   <sheetData>
     <row r="1" spans="2:28" ht="15" customHeight="1" thickBot="1"/>
     <row r="2" spans="2:28" ht="15.75" customHeight="1" thickBot="1">
-      <c r="B2" s="10" t="s">
+      <c r="B2" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="C2" s="11" t="s">
+      <c r="C2" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="11" t="s">
+      <c r="D2" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="E2" s="11" t="s">
+      <c r="E2" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="F2" s="11" t="s">
+      <c r="F2" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="G2" s="11" t="s">
+      <c r="G2" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="H2" s="11" t="s">
+      <c r="H2" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="I2" s="12" t="s">
+      <c r="I2" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="J2" s="13" t="s">
+      <c r="J2" s="12" t="s">
         <v>44</v>
       </c>
       <c r="K2" s="5"/>
@@ -1081,84 +1113,84 @@
       <c r="AB2" s="1"/>
     </row>
     <row r="3" spans="2:28" ht="15.75" customHeight="1">
-      <c r="B3" s="41">
+      <c r="B3" s="35">
         <v>1</v>
       </c>
-      <c r="C3" s="42" t="s">
+      <c r="C3" s="32" t="s">
         <v>42</v>
       </c>
-      <c r="D3" s="42" t="s">
+      <c r="D3" s="32" t="s">
         <v>7</v>
       </c>
-      <c r="E3" s="36" t="s">
+      <c r="E3" s="38" t="s">
         <v>16</v>
       </c>
-      <c r="F3" s="36" t="s">
+      <c r="F3" s="38" t="s">
         <v>41</v>
       </c>
-      <c r="G3" s="36" t="s">
+      <c r="G3" s="38" t="s">
         <v>17</v>
       </c>
-      <c r="H3" s="39"/>
-      <c r="I3" s="43">
+      <c r="H3" s="40"/>
+      <c r="I3" s="26">
         <v>1</v>
       </c>
-      <c r="J3" s="45" t="s">
+      <c r="J3" s="23" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="4" spans="2:28" ht="15.75" customHeight="1">
-      <c r="B4" s="22"/>
-      <c r="C4" s="20"/>
-      <c r="D4" s="20"/>
-      <c r="E4" s="24"/>
-      <c r="F4" s="24"/>
-      <c r="G4" s="24"/>
-      <c r="H4" s="24"/>
-      <c r="I4" s="26"/>
-      <c r="J4" s="46"/>
+      <c r="B4" s="36"/>
+      <c r="C4" s="33"/>
+      <c r="D4" s="33"/>
+      <c r="E4" s="39"/>
+      <c r="F4" s="39"/>
+      <c r="G4" s="39"/>
+      <c r="H4" s="39"/>
+      <c r="I4" s="25"/>
+      <c r="J4" s="22"/>
     </row>
     <row r="5" spans="2:28" ht="15.75" customHeight="1">
-      <c r="B5" s="28">
+      <c r="B5" s="37">
         <v>2</v>
       </c>
-      <c r="C5" s="29" t="s">
+      <c r="C5" s="27" t="s">
         <v>42</v>
       </c>
-      <c r="D5" s="31" t="s">
+      <c r="D5" s="30" t="s">
         <v>8</v>
       </c>
-      <c r="E5" s="30" t="s">
+      <c r="E5" s="31" t="s">
         <v>16</v>
       </c>
-      <c r="F5" s="37"/>
-      <c r="G5" s="30" t="s">
+      <c r="F5" s="42"/>
+      <c r="G5" s="31" t="s">
         <v>18</v>
       </c>
-      <c r="H5" s="31"/>
-      <c r="I5" s="44">
+      <c r="H5" s="30"/>
+      <c r="I5" s="24">
         <v>2</v>
       </c>
-      <c r="J5" s="46" t="s">
+      <c r="J5" s="22" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="6" spans="2:28" ht="15.75" customHeight="1">
-      <c r="B6" s="28"/>
-      <c r="C6" s="29"/>
-      <c r="D6" s="31"/>
-      <c r="E6" s="31"/>
-      <c r="F6" s="37"/>
-      <c r="G6" s="31"/>
-      <c r="H6" s="31"/>
-      <c r="I6" s="44"/>
-      <c r="J6" s="46"/>
+      <c r="B6" s="37"/>
+      <c r="C6" s="27"/>
+      <c r="D6" s="30"/>
+      <c r="E6" s="30"/>
+      <c r="F6" s="42"/>
+      <c r="G6" s="30"/>
+      <c r="H6" s="30"/>
+      <c r="I6" s="24"/>
+      <c r="J6" s="22"/>
     </row>
     <row r="7" spans="2:28" ht="15.75" customHeight="1">
-      <c r="B7" s="22">
+      <c r="B7" s="36">
         <v>3</v>
       </c>
-      <c r="C7" s="40" t="s">
+      <c r="C7" s="29" t="s">
         <v>6</v>
       </c>
       <c r="D7" s="34" t="s">
@@ -1167,142 +1199,142 @@
       <c r="E7" s="34" t="s">
         <v>24</v>
       </c>
-      <c r="F7" s="38"/>
+      <c r="F7" s="28"/>
       <c r="G7" s="34" t="s">
         <v>19</v>
       </c>
-      <c r="H7" s="38"/>
-      <c r="I7" s="26">
+      <c r="H7" s="28"/>
+      <c r="I7" s="25">
         <v>6</v>
       </c>
-      <c r="J7" s="18" t="s">
+      <c r="J7" s="21" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="8" spans="2:28" ht="15.75" customHeight="1">
-      <c r="B8" s="22"/>
-      <c r="C8" s="40"/>
-      <c r="D8" s="38"/>
-      <c r="E8" s="38"/>
-      <c r="F8" s="38"/>
-      <c r="G8" s="38"/>
-      <c r="H8" s="38"/>
-      <c r="I8" s="26"/>
-      <c r="J8" s="18"/>
+      <c r="B8" s="36"/>
+      <c r="C8" s="29"/>
+      <c r="D8" s="28"/>
+      <c r="E8" s="28"/>
+      <c r="F8" s="28"/>
+      <c r="G8" s="28"/>
+      <c r="H8" s="28"/>
+      <c r="I8" s="25"/>
+      <c r="J8" s="21"/>
     </row>
     <row r="9" spans="2:28" ht="15.75" customHeight="1">
-      <c r="B9" s="28">
+      <c r="B9" s="37">
         <v>4</v>
       </c>
-      <c r="C9" s="29" t="s">
+      <c r="C9" s="27" t="s">
         <v>6</v>
       </c>
-      <c r="D9" s="30" t="s">
+      <c r="D9" s="31" t="s">
         <v>28</v>
       </c>
-      <c r="E9" s="30" t="s">
+      <c r="E9" s="31" t="s">
         <v>25</v>
       </c>
-      <c r="F9" s="31"/>
-      <c r="G9" s="30" t="s">
+      <c r="F9" s="30"/>
+      <c r="G9" s="31" t="s">
         <v>20</v>
       </c>
-      <c r="H9" s="31"/>
-      <c r="I9" s="44">
+      <c r="H9" s="30"/>
+      <c r="I9" s="24">
         <v>4</v>
       </c>
-      <c r="J9" s="46" t="s">
+      <c r="J9" s="22" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="10" spans="2:28" ht="15.75" customHeight="1">
-      <c r="B10" s="28"/>
-      <c r="C10" s="29"/>
-      <c r="D10" s="31"/>
-      <c r="E10" s="31"/>
-      <c r="F10" s="31"/>
-      <c r="G10" s="31"/>
-      <c r="H10" s="31"/>
-      <c r="I10" s="44"/>
-      <c r="J10" s="46"/>
+      <c r="B10" s="37"/>
+      <c r="C10" s="27"/>
+      <c r="D10" s="30"/>
+      <c r="E10" s="30"/>
+      <c r="F10" s="30"/>
+      <c r="G10" s="30"/>
+      <c r="H10" s="30"/>
+      <c r="I10" s="24"/>
+      <c r="J10" s="22"/>
     </row>
     <row r="11" spans="2:28" ht="15.75" customHeight="1">
-      <c r="B11" s="22">
+      <c r="B11" s="36">
         <v>5</v>
       </c>
-      <c r="C11" s="40" t="s">
+      <c r="C11" s="29" t="s">
         <v>10</v>
       </c>
-      <c r="D11" s="38" t="s">
+      <c r="D11" s="28" t="s">
         <v>11</v>
       </c>
       <c r="E11" s="34" t="s">
         <v>39</v>
       </c>
-      <c r="F11" s="38"/>
+      <c r="F11" s="28"/>
       <c r="G11" s="34" t="s">
         <v>21</v>
       </c>
-      <c r="H11" s="38"/>
-      <c r="I11" s="26">
+      <c r="H11" s="28"/>
+      <c r="I11" s="25">
         <v>5</v>
       </c>
-      <c r="J11" s="46" t="s">
+      <c r="J11" s="22" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="12" spans="2:28" ht="15.75" customHeight="1">
-      <c r="B12" s="22"/>
-      <c r="C12" s="40"/>
-      <c r="D12" s="38"/>
-      <c r="E12" s="38"/>
-      <c r="F12" s="38"/>
-      <c r="G12" s="38"/>
-      <c r="H12" s="38"/>
-      <c r="I12" s="26"/>
-      <c r="J12" s="46"/>
+      <c r="B12" s="36"/>
+      <c r="C12" s="29"/>
+      <c r="D12" s="28"/>
+      <c r="E12" s="28"/>
+      <c r="F12" s="28"/>
+      <c r="G12" s="28"/>
+      <c r="H12" s="28"/>
+      <c r="I12" s="25"/>
+      <c r="J12" s="22"/>
     </row>
     <row r="13" spans="2:28" ht="15.75" customHeight="1">
-      <c r="B13" s="28">
+      <c r="B13" s="37">
         <v>6</v>
       </c>
-      <c r="C13" s="29" t="s">
+      <c r="C13" s="27" t="s">
         <v>6</v>
       </c>
-      <c r="D13" s="31" t="s">
+      <c r="D13" s="30" t="s">
         <v>12</v>
       </c>
-      <c r="E13" s="30" t="s">
+      <c r="E13" s="31" t="s">
         <v>37</v>
       </c>
-      <c r="F13" s="31"/>
-      <c r="G13" s="30" t="s">
+      <c r="F13" s="30"/>
+      <c r="G13" s="31" t="s">
         <v>22</v>
       </c>
-      <c r="H13" s="31"/>
-      <c r="I13" s="44">
+      <c r="H13" s="30"/>
+      <c r="I13" s="24">
         <v>8</v>
       </c>
-      <c r="J13" s="18" t="s">
+      <c r="J13" s="21" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="14" spans="2:28" ht="15.75" customHeight="1">
-      <c r="B14" s="28"/>
-      <c r="C14" s="29"/>
-      <c r="D14" s="31"/>
-      <c r="E14" s="31"/>
-      <c r="F14" s="31"/>
-      <c r="G14" s="31"/>
-      <c r="H14" s="31"/>
-      <c r="I14" s="44"/>
-      <c r="J14" s="18"/>
+      <c r="B14" s="37"/>
+      <c r="C14" s="27"/>
+      <c r="D14" s="30"/>
+      <c r="E14" s="30"/>
+      <c r="F14" s="30"/>
+      <c r="G14" s="30"/>
+      <c r="H14" s="30"/>
+      <c r="I14" s="24"/>
+      <c r="J14" s="21"/>
     </row>
     <row r="15" spans="2:28" ht="15.75" customHeight="1">
-      <c r="B15" s="22">
+      <c r="B15" s="36">
         <v>7</v>
       </c>
-      <c r="C15" s="40" t="s">
+      <c r="C15" s="29" t="s">
         <v>6</v>
       </c>
       <c r="D15" s="34" t="s">
@@ -1311,287 +1343,311 @@
       <c r="E15" s="34" t="s">
         <v>26</v>
       </c>
-      <c r="F15" s="38"/>
+      <c r="F15" s="28"/>
       <c r="G15" s="34" t="s">
         <v>23</v>
       </c>
-      <c r="H15" s="38"/>
-      <c r="I15" s="26">
+      <c r="H15" s="28"/>
+      <c r="I15" s="25">
         <v>9</v>
       </c>
-      <c r="J15" s="18" t="s">
+      <c r="J15" s="21" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="16" spans="2:28" ht="15.75" customHeight="1">
-      <c r="B16" s="22"/>
-      <c r="C16" s="40"/>
-      <c r="D16" s="38"/>
-      <c r="E16" s="38"/>
-      <c r="F16" s="38"/>
-      <c r="G16" s="38"/>
-      <c r="H16" s="38"/>
-      <c r="I16" s="26"/>
-      <c r="J16" s="18"/>
+      <c r="B16" s="36"/>
+      <c r="C16" s="29"/>
+      <c r="D16" s="28"/>
+      <c r="E16" s="28"/>
+      <c r="F16" s="28"/>
+      <c r="G16" s="28"/>
+      <c r="H16" s="28"/>
+      <c r="I16" s="25"/>
+      <c r="J16" s="21"/>
     </row>
     <row r="17" spans="2:10" ht="15.75" customHeight="1">
-      <c r="B17" s="22"/>
-      <c r="C17" s="40"/>
-      <c r="D17" s="38"/>
-      <c r="E17" s="38"/>
-      <c r="F17" s="38"/>
-      <c r="G17" s="38"/>
-      <c r="H17" s="38"/>
-      <c r="I17" s="26"/>
-      <c r="J17" s="18"/>
+      <c r="B17" s="36"/>
+      <c r="C17" s="29"/>
+      <c r="D17" s="28"/>
+      <c r="E17" s="28"/>
+      <c r="F17" s="28"/>
+      <c r="G17" s="28"/>
+      <c r="H17" s="28"/>
+      <c r="I17" s="25"/>
+      <c r="J17" s="21"/>
     </row>
     <row r="18" spans="2:10" ht="15.75" customHeight="1">
-      <c r="B18" s="28">
+      <c r="B18" s="37">
         <v>8</v>
       </c>
-      <c r="C18" s="29" t="s">
+      <c r="C18" s="27" t="s">
         <v>9</v>
       </c>
-      <c r="D18" s="30" t="s">
+      <c r="D18" s="31" t="s">
         <v>35</v>
       </c>
-      <c r="E18" s="31" t="s">
+      <c r="E18" s="30" t="s">
         <v>13</v>
       </c>
-      <c r="F18" s="31"/>
-      <c r="G18" s="30" t="s">
+      <c r="F18" s="30"/>
+      <c r="G18" s="31" t="s">
         <v>15</v>
       </c>
-      <c r="H18" s="31"/>
-      <c r="I18" s="44" t="s">
+      <c r="H18" s="30"/>
+      <c r="I18" s="24" t="s">
         <v>43</v>
       </c>
-      <c r="J18" s="18" t="s">
+      <c r="J18" s="21" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="19" spans="2:10" ht="15.75" customHeight="1">
-      <c r="B19" s="28"/>
-      <c r="C19" s="29"/>
-      <c r="D19" s="31"/>
-      <c r="E19" s="31"/>
-      <c r="F19" s="31"/>
-      <c r="G19" s="31"/>
-      <c r="H19" s="31"/>
-      <c r="I19" s="44"/>
-      <c r="J19" s="18"/>
+      <c r="B19" s="37"/>
+      <c r="C19" s="27"/>
+      <c r="D19" s="30"/>
+      <c r="E19" s="30"/>
+      <c r="F19" s="30"/>
+      <c r="G19" s="30"/>
+      <c r="H19" s="30"/>
+      <c r="I19" s="24"/>
+      <c r="J19" s="21"/>
     </row>
     <row r="20" spans="2:10" ht="15.75" customHeight="1">
-      <c r="B20" s="28"/>
-      <c r="C20" s="29"/>
-      <c r="D20" s="31"/>
-      <c r="E20" s="31"/>
-      <c r="F20" s="31"/>
-      <c r="G20" s="31"/>
-      <c r="H20" s="31"/>
-      <c r="I20" s="44"/>
-      <c r="J20" s="18"/>
+      <c r="B20" s="37"/>
+      <c r="C20" s="27"/>
+      <c r="D20" s="30"/>
+      <c r="E20" s="30"/>
+      <c r="F20" s="30"/>
+      <c r="G20" s="30"/>
+      <c r="H20" s="30"/>
+      <c r="I20" s="24"/>
+      <c r="J20" s="21"/>
     </row>
     <row r="21" spans="2:10" ht="15.75" customHeight="1">
-      <c r="B21" s="22">
+      <c r="B21" s="36">
         <v>9</v>
       </c>
-      <c r="C21" s="20" t="s">
+      <c r="C21" s="33" t="s">
         <v>9</v>
       </c>
-      <c r="D21" s="32" t="s">
+      <c r="D21" s="41" t="s">
         <v>40</v>
       </c>
-      <c r="E21" s="32" t="s">
+      <c r="E21" s="41" t="s">
         <v>31</v>
       </c>
-      <c r="F21" s="24"/>
-      <c r="G21" s="24" t="s">
+      <c r="F21" s="39"/>
+      <c r="G21" s="39" t="s">
         <v>30</v>
       </c>
-      <c r="H21" s="24"/>
-      <c r="I21" s="26">
+      <c r="H21" s="39"/>
+      <c r="I21" s="25">
         <v>3</v>
       </c>
-      <c r="J21" s="46" t="s">
+      <c r="J21" s="22" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="22" spans="2:10" ht="15.75" customHeight="1">
-      <c r="B22" s="22"/>
-      <c r="C22" s="20"/>
-      <c r="D22" s="32"/>
-      <c r="E22" s="24"/>
-      <c r="F22" s="24"/>
-      <c r="G22" s="24"/>
-      <c r="H22" s="24"/>
-      <c r="I22" s="26"/>
-      <c r="J22" s="46"/>
+      <c r="B22" s="36"/>
+      <c r="C22" s="33"/>
+      <c r="D22" s="41"/>
+      <c r="E22" s="39"/>
+      <c r="F22" s="39"/>
+      <c r="G22" s="39"/>
+      <c r="H22" s="39"/>
+      <c r="I22" s="25"/>
+      <c r="J22" s="22"/>
     </row>
     <row r="23" spans="2:10" ht="15.75" customHeight="1">
-      <c r="B23" s="22"/>
-      <c r="C23" s="20"/>
-      <c r="D23" s="32"/>
-      <c r="E23" s="24"/>
-      <c r="F23" s="24"/>
-      <c r="G23" s="24"/>
-      <c r="H23" s="24"/>
-      <c r="I23" s="26"/>
-      <c r="J23" s="46"/>
+      <c r="B23" s="36"/>
+      <c r="C23" s="33"/>
+      <c r="D23" s="41"/>
+      <c r="E23" s="39"/>
+      <c r="F23" s="39"/>
+      <c r="G23" s="39"/>
+      <c r="H23" s="39"/>
+      <c r="I23" s="25"/>
+      <c r="J23" s="22"/>
     </row>
     <row r="24" spans="2:10" ht="15.75" customHeight="1">
-      <c r="B24" s="28">
+      <c r="B24" s="37">
         <v>10</v>
       </c>
-      <c r="C24" s="29" t="s">
+      <c r="C24" s="27" t="s">
         <v>9</v>
       </c>
-      <c r="D24" s="30" t="s">
+      <c r="D24" s="31" t="s">
         <v>34</v>
       </c>
-      <c r="E24" s="31" t="s">
+      <c r="E24" s="30" t="s">
         <v>32</v>
       </c>
-      <c r="F24" s="31"/>
-      <c r="G24" s="30" t="s">
+      <c r="F24" s="30"/>
+      <c r="G24" s="31" t="s">
         <v>33</v>
       </c>
-      <c r="H24" s="31"/>
-      <c r="I24" s="44">
+      <c r="H24" s="30"/>
+      <c r="I24" s="24">
         <v>10</v>
       </c>
-      <c r="J24" s="18" t="s">
+      <c r="J24" s="21" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="25" spans="2:10" ht="15.75" customHeight="1">
-      <c r="B25" s="28"/>
-      <c r="C25" s="29"/>
-      <c r="D25" s="31"/>
-      <c r="E25" s="31"/>
-      <c r="F25" s="31"/>
-      <c r="G25" s="30"/>
-      <c r="H25" s="31"/>
-      <c r="I25" s="44"/>
-      <c r="J25" s="18"/>
+      <c r="B25" s="37"/>
+      <c r="C25" s="27"/>
+      <c r="D25" s="30"/>
+      <c r="E25" s="30"/>
+      <c r="F25" s="30"/>
+      <c r="G25" s="31"/>
+      <c r="H25" s="30"/>
+      <c r="I25" s="24"/>
+      <c r="J25" s="21"/>
     </row>
     <row r="26" spans="2:10" ht="15.75" customHeight="1">
-      <c r="B26" s="28"/>
-      <c r="C26" s="29"/>
-      <c r="D26" s="31"/>
-      <c r="E26" s="31"/>
-      <c r="F26" s="31"/>
-      <c r="G26" s="30"/>
-      <c r="H26" s="31"/>
-      <c r="I26" s="44"/>
-      <c r="J26" s="18"/>
+      <c r="B26" s="37"/>
+      <c r="C26" s="27"/>
+      <c r="D26" s="30"/>
+      <c r="E26" s="30"/>
+      <c r="F26" s="30"/>
+      <c r="G26" s="31"/>
+      <c r="H26" s="30"/>
+      <c r="I26" s="24"/>
+      <c r="J26" s="21"/>
     </row>
     <row r="27" spans="2:10" ht="15.75" customHeight="1">
-      <c r="B27" s="22">
+      <c r="B27" s="36">
         <v>11</v>
       </c>
-      <c r="C27" s="20" t="s">
+      <c r="C27" s="33" t="s">
         <v>10</v>
       </c>
-      <c r="D27" s="32" t="s">
+      <c r="D27" s="41" t="s">
         <v>47</v>
       </c>
       <c r="E27" s="34" t="s">
         <v>48</v>
       </c>
-      <c r="F27" s="24"/>
-      <c r="G27" s="32" t="s">
+      <c r="F27" s="39"/>
+      <c r="G27" s="41" t="s">
         <v>36</v>
       </c>
-      <c r="H27" s="24"/>
-      <c r="I27" s="26">
+      <c r="H27" s="39"/>
+      <c r="I27" s="25">
         <v>7</v>
       </c>
-      <c r="J27" s="17" t="s">
+      <c r="J27" s="46" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="28" spans="2:10" ht="15.75" customHeight="1">
-      <c r="B28" s="22"/>
-      <c r="C28" s="20"/>
-      <c r="D28" s="32"/>
+      <c r="B28" s="36"/>
+      <c r="C28" s="33"/>
+      <c r="D28" s="41"/>
       <c r="E28" s="34"/>
-      <c r="F28" s="24"/>
-      <c r="G28" s="32"/>
-      <c r="H28" s="24"/>
-      <c r="I28" s="26"/>
-      <c r="J28" s="18"/>
+      <c r="F28" s="39"/>
+      <c r="G28" s="41"/>
+      <c r="H28" s="39"/>
+      <c r="I28" s="25"/>
+      <c r="J28" s="21"/>
     </row>
     <row r="29" spans="2:10" ht="15.75" customHeight="1">
-      <c r="B29" s="22"/>
-      <c r="C29" s="20"/>
-      <c r="D29" s="32"/>
+      <c r="B29" s="36"/>
+      <c r="C29" s="33"/>
+      <c r="D29" s="41"/>
       <c r="E29" s="34"/>
-      <c r="F29" s="24"/>
-      <c r="G29" s="32"/>
-      <c r="H29" s="24"/>
-      <c r="I29" s="26"/>
-      <c r="J29" s="18"/>
+      <c r="F29" s="39"/>
+      <c r="G29" s="41"/>
+      <c r="H29" s="39"/>
+      <c r="I29" s="25"/>
+      <c r="J29" s="21"/>
     </row>
     <row r="30" spans="2:10" ht="15.75" customHeight="1">
-      <c r="B30" s="22"/>
-      <c r="C30" s="20"/>
-      <c r="D30" s="32"/>
+      <c r="B30" s="36"/>
+      <c r="C30" s="33"/>
+      <c r="D30" s="41"/>
       <c r="E30" s="34"/>
-      <c r="F30" s="24"/>
-      <c r="G30" s="32"/>
-      <c r="H30" s="24"/>
-      <c r="I30" s="26"/>
-      <c r="J30" s="18"/>
+      <c r="F30" s="39"/>
+      <c r="G30" s="41"/>
+      <c r="H30" s="39"/>
+      <c r="I30" s="25"/>
+      <c r="J30" s="21"/>
     </row>
     <row r="31" spans="2:10" ht="15.75" customHeight="1">
-      <c r="B31" s="22"/>
-      <c r="C31" s="20"/>
-      <c r="D31" s="32"/>
+      <c r="B31" s="36"/>
+      <c r="C31" s="33"/>
+      <c r="D31" s="41"/>
       <c r="E31" s="34"/>
-      <c r="F31" s="24"/>
-      <c r="G31" s="32"/>
-      <c r="H31" s="24"/>
-      <c r="I31" s="26"/>
-      <c r="J31" s="18"/>
+      <c r="F31" s="39"/>
+      <c r="G31" s="41"/>
+      <c r="H31" s="39"/>
+      <c r="I31" s="25"/>
+      <c r="J31" s="21"/>
     </row>
     <row r="32" spans="2:10" ht="15.75" customHeight="1">
-      <c r="B32" s="23"/>
-      <c r="C32" s="21"/>
-      <c r="D32" s="33"/>
-      <c r="E32" s="35"/>
-      <c r="F32" s="25"/>
-      <c r="G32" s="33"/>
-      <c r="H32" s="25"/>
-      <c r="I32" s="27"/>
-      <c r="J32" s="19"/>
-    </row>
-    <row r="33" spans="2:10" ht="63" customHeight="1" thickBot="1">
-      <c r="B33" s="6">
+      <c r="B32" s="49"/>
+      <c r="C32" s="48"/>
+      <c r="D32" s="43"/>
+      <c r="E32" s="45"/>
+      <c r="F32" s="44"/>
+      <c r="G32" s="43"/>
+      <c r="H32" s="44"/>
+      <c r="I32" s="50"/>
+      <c r="J32" s="47"/>
+    </row>
+    <row r="33" spans="2:10" ht="63" customHeight="1">
+      <c r="B33" s="18">
         <v>12</v>
       </c>
-      <c r="C33" s="7" t="s">
+      <c r="C33" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="D33" s="8" t="s">
+      <c r="D33" s="20" t="s">
         <v>49</v>
       </c>
-      <c r="E33" s="15" t="s">
+      <c r="E33" s="51" t="s">
         <v>50</v>
       </c>
-      <c r="F33" s="15"/>
-      <c r="G33" s="16" t="s">
+      <c r="F33" s="51"/>
+      <c r="G33" s="52" t="s">
         <v>51</v>
       </c>
-      <c r="H33" s="15"/>
-      <c r="I33" s="9" t="s">
+      <c r="H33" s="51"/>
+      <c r="I33" s="19" t="s">
         <v>43</v>
       </c>
-      <c r="J33" s="14" t="s">
+      <c r="J33" s="16" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="34" spans="2:10" ht="15.75" customHeight="1"/>
+    <row r="34" spans="2:10" ht="63" customHeight="1" thickBot="1">
+      <c r="B34" s="6">
+        <v>13</v>
+      </c>
+      <c r="C34" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="D34" s="15" t="s">
+        <v>52</v>
+      </c>
+      <c r="E34" s="15" t="s">
+        <v>54</v>
+      </c>
+      <c r="F34" s="14"/>
+      <c r="G34" s="15" t="s">
+        <v>53</v>
+      </c>
+      <c r="H34" s="14"/>
+      <c r="I34" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="J34" s="13" t="s">
+        <v>46</v>
+      </c>
+    </row>
     <row r="35" spans="2:10" ht="15.75" customHeight="1"/>
     <row r="36" spans="2:10" ht="15.75" customHeight="1"/>
     <row r="37" spans="2:10" ht="15.75" customHeight="1"/>
@@ -2552,56 +2608,39 @@
     <row r="992" ht="15.75" customHeight="1"/>
   </sheetData>
   <mergeCells count="99">
-    <mergeCell ref="J13:J14"/>
-    <mergeCell ref="J15:J17"/>
-    <mergeCell ref="J18:J20"/>
-    <mergeCell ref="J21:J23"/>
-    <mergeCell ref="J24:J26"/>
-    <mergeCell ref="J3:J4"/>
-    <mergeCell ref="J5:J6"/>
-    <mergeCell ref="J7:J8"/>
-    <mergeCell ref="J9:J10"/>
-    <mergeCell ref="J11:J12"/>
-    <mergeCell ref="I13:I14"/>
-    <mergeCell ref="I15:I17"/>
-    <mergeCell ref="I18:I20"/>
-    <mergeCell ref="I21:I23"/>
-    <mergeCell ref="I24:I26"/>
-    <mergeCell ref="I3:I4"/>
-    <mergeCell ref="I5:I6"/>
-    <mergeCell ref="I7:I8"/>
-    <mergeCell ref="I9:I10"/>
-    <mergeCell ref="I11:I12"/>
-    <mergeCell ref="C9:C10"/>
-    <mergeCell ref="D11:D12"/>
-    <mergeCell ref="C11:C12"/>
-    <mergeCell ref="D13:D14"/>
-    <mergeCell ref="C13:C14"/>
-    <mergeCell ref="D9:D10"/>
-    <mergeCell ref="C3:C4"/>
-    <mergeCell ref="D3:D4"/>
-    <mergeCell ref="C5:C6"/>
-    <mergeCell ref="D5:D6"/>
-    <mergeCell ref="C7:C8"/>
-    <mergeCell ref="D7:D8"/>
-    <mergeCell ref="B3:B4"/>
-    <mergeCell ref="B5:B6"/>
-    <mergeCell ref="B7:B8"/>
-    <mergeCell ref="B9:B10"/>
-    <mergeCell ref="B11:B12"/>
-    <mergeCell ref="B13:B14"/>
-    <mergeCell ref="B15:B17"/>
-    <mergeCell ref="G18:G20"/>
-    <mergeCell ref="E18:E20"/>
-    <mergeCell ref="C18:C20"/>
-    <mergeCell ref="B18:B20"/>
-    <mergeCell ref="F18:F20"/>
-    <mergeCell ref="E15:E17"/>
-    <mergeCell ref="D15:D17"/>
-    <mergeCell ref="D18:D20"/>
-    <mergeCell ref="F13:F14"/>
-    <mergeCell ref="C15:C17"/>
-    <mergeCell ref="F15:F17"/>
+    <mergeCell ref="J27:J32"/>
+    <mergeCell ref="C27:C32"/>
+    <mergeCell ref="B27:B32"/>
+    <mergeCell ref="H27:H32"/>
+    <mergeCell ref="I27:I32"/>
+    <mergeCell ref="B24:B26"/>
+    <mergeCell ref="C24:C26"/>
+    <mergeCell ref="D24:D26"/>
+    <mergeCell ref="E24:E26"/>
+    <mergeCell ref="F24:F26"/>
+    <mergeCell ref="H24:H26"/>
+    <mergeCell ref="G27:G32"/>
+    <mergeCell ref="F27:F32"/>
+    <mergeCell ref="E27:E32"/>
+    <mergeCell ref="D27:D32"/>
+    <mergeCell ref="G24:G26"/>
+    <mergeCell ref="F3:F4"/>
+    <mergeCell ref="F5:F6"/>
+    <mergeCell ref="F7:F8"/>
+    <mergeCell ref="F9:F10"/>
+    <mergeCell ref="F11:F12"/>
+    <mergeCell ref="F21:F23"/>
+    <mergeCell ref="B21:B23"/>
+    <mergeCell ref="C21:C23"/>
+    <mergeCell ref="G21:G23"/>
+    <mergeCell ref="H21:H23"/>
+    <mergeCell ref="D21:D23"/>
+    <mergeCell ref="E21:E23"/>
+    <mergeCell ref="E5:E6"/>
+    <mergeCell ref="E7:E8"/>
+    <mergeCell ref="E9:E10"/>
+    <mergeCell ref="E11:E12"/>
+    <mergeCell ref="E13:E14"/>
     <mergeCell ref="H18:H20"/>
     <mergeCell ref="E3:E4"/>
     <mergeCell ref="G3:G4"/>
@@ -2618,39 +2657,56 @@
     <mergeCell ref="G11:G12"/>
     <mergeCell ref="G13:G14"/>
     <mergeCell ref="G15:G17"/>
-    <mergeCell ref="E5:E6"/>
-    <mergeCell ref="E7:E8"/>
-    <mergeCell ref="E9:E10"/>
-    <mergeCell ref="E11:E12"/>
-    <mergeCell ref="E13:E14"/>
-    <mergeCell ref="F21:F23"/>
-    <mergeCell ref="B21:B23"/>
-    <mergeCell ref="C21:C23"/>
-    <mergeCell ref="G21:G23"/>
-    <mergeCell ref="H21:H23"/>
-    <mergeCell ref="D21:D23"/>
-    <mergeCell ref="E21:E23"/>
-    <mergeCell ref="F3:F4"/>
-    <mergeCell ref="F5:F6"/>
-    <mergeCell ref="F7:F8"/>
-    <mergeCell ref="F9:F10"/>
-    <mergeCell ref="F11:F12"/>
-    <mergeCell ref="H24:H26"/>
-    <mergeCell ref="G27:G32"/>
-    <mergeCell ref="F27:F32"/>
-    <mergeCell ref="E27:E32"/>
-    <mergeCell ref="D27:D32"/>
-    <mergeCell ref="G24:G26"/>
-    <mergeCell ref="B24:B26"/>
-    <mergeCell ref="C24:C26"/>
-    <mergeCell ref="D24:D26"/>
-    <mergeCell ref="E24:E26"/>
-    <mergeCell ref="F24:F26"/>
-    <mergeCell ref="J27:J32"/>
-    <mergeCell ref="C27:C32"/>
-    <mergeCell ref="B27:B32"/>
-    <mergeCell ref="H27:H32"/>
-    <mergeCell ref="I27:I32"/>
+    <mergeCell ref="B13:B14"/>
+    <mergeCell ref="B15:B17"/>
+    <mergeCell ref="G18:G20"/>
+    <mergeCell ref="E18:E20"/>
+    <mergeCell ref="C18:C20"/>
+    <mergeCell ref="B18:B20"/>
+    <mergeCell ref="F18:F20"/>
+    <mergeCell ref="E15:E17"/>
+    <mergeCell ref="D15:D17"/>
+    <mergeCell ref="D18:D20"/>
+    <mergeCell ref="F13:F14"/>
+    <mergeCell ref="C15:C17"/>
+    <mergeCell ref="F15:F17"/>
+    <mergeCell ref="B3:B4"/>
+    <mergeCell ref="B5:B6"/>
+    <mergeCell ref="B7:B8"/>
+    <mergeCell ref="B9:B10"/>
+    <mergeCell ref="B11:B12"/>
+    <mergeCell ref="C3:C4"/>
+    <mergeCell ref="D3:D4"/>
+    <mergeCell ref="C5:C6"/>
+    <mergeCell ref="D5:D6"/>
+    <mergeCell ref="C7:C8"/>
+    <mergeCell ref="D7:D8"/>
+    <mergeCell ref="C9:C10"/>
+    <mergeCell ref="D11:D12"/>
+    <mergeCell ref="C11:C12"/>
+    <mergeCell ref="D13:D14"/>
+    <mergeCell ref="C13:C14"/>
+    <mergeCell ref="D9:D10"/>
+    <mergeCell ref="I3:I4"/>
+    <mergeCell ref="I5:I6"/>
+    <mergeCell ref="I7:I8"/>
+    <mergeCell ref="I9:I10"/>
+    <mergeCell ref="I11:I12"/>
+    <mergeCell ref="I13:I14"/>
+    <mergeCell ref="I15:I17"/>
+    <mergeCell ref="I18:I20"/>
+    <mergeCell ref="I21:I23"/>
+    <mergeCell ref="I24:I26"/>
+    <mergeCell ref="J3:J4"/>
+    <mergeCell ref="J5:J6"/>
+    <mergeCell ref="J7:J8"/>
+    <mergeCell ref="J9:J10"/>
+    <mergeCell ref="J11:J12"/>
+    <mergeCell ref="J13:J14"/>
+    <mergeCell ref="J15:J17"/>
+    <mergeCell ref="J18:J20"/>
+    <mergeCell ref="J21:J23"/>
+    <mergeCell ref="J24:J26"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape" r:id="rId1"/>

</xml_diff>

<commit_message>
Analyse des performances apres la 6eme correction
</commit_message>
<xml_diff>
--- a/Analyses/Modèle-audit-SEO.xlsx
+++ b/Analyses/Modèle-audit-SEO.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="56">
   <si>
     <t>Catégorie</t>
   </si>
@@ -310,6 +310,9 @@
   <si>
     <t xml:space="preserve"> Mettre en concordance les
  pages</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> La correction du point 13 (ordre 6) a entrainé la correction des points 10 et 11. Par conséquent , ses points ont été remplacé par les points 6 et 8</t>
   </si>
 </sst>
 </file>
@@ -383,7 +386,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -425,8 +428,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="17">
+  <borders count="20">
     <border>
       <left/>
       <right/>
@@ -668,12 +677,49 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="9" fillId="5" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="53">
+  <cellXfs count="56">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -711,9 +757,6 @@
     <xf numFmtId="0" fontId="5" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -742,94 +785,106 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1047,7 +1102,7 @@
   <dimension ref="B1:AB992"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="A33" sqref="A33:XFD33"/>
+      <selection activeCell="B36" sqref="B36:J36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.33203125" defaultRowHeight="15" customHeight="1"/>
@@ -1113,513 +1168,513 @@
       <c r="AB2" s="1"/>
     </row>
     <row r="3" spans="2:28" ht="15.75" customHeight="1">
-      <c r="B3" s="47">
+      <c r="B3" s="36">
         <v>1</v>
       </c>
-      <c r="C3" s="48" t="s">
+      <c r="C3" s="33" t="s">
         <v>42</v>
       </c>
-      <c r="D3" s="48" t="s">
+      <c r="D3" s="33" t="s">
         <v>7</v>
       </c>
-      <c r="E3" s="42" t="s">
+      <c r="E3" s="39" t="s">
         <v>16</v>
       </c>
-      <c r="F3" s="42" t="s">
+      <c r="F3" s="39" t="s">
         <v>41</v>
       </c>
-      <c r="G3" s="42" t="s">
+      <c r="G3" s="39" t="s">
         <v>17</v>
       </c>
-      <c r="H3" s="45"/>
-      <c r="I3" s="49">
+      <c r="H3" s="41"/>
+      <c r="I3" s="27">
         <v>1</v>
       </c>
-      <c r="J3" s="51" t="s">
+      <c r="J3" s="24" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="4" spans="2:28" ht="15.75" customHeight="1">
-      <c r="B4" s="28"/>
-      <c r="C4" s="26"/>
-      <c r="D4" s="26"/>
-      <c r="E4" s="30"/>
-      <c r="F4" s="30"/>
-      <c r="G4" s="30"/>
-      <c r="H4" s="30"/>
-      <c r="I4" s="32"/>
-      <c r="J4" s="52"/>
+      <c r="B4" s="37"/>
+      <c r="C4" s="34"/>
+      <c r="D4" s="34"/>
+      <c r="E4" s="40"/>
+      <c r="F4" s="40"/>
+      <c r="G4" s="40"/>
+      <c r="H4" s="40"/>
+      <c r="I4" s="26"/>
+      <c r="J4" s="23"/>
     </row>
     <row r="5" spans="2:28" ht="15.75" customHeight="1">
-      <c r="B5" s="34">
+      <c r="B5" s="38">
         <v>2</v>
       </c>
-      <c r="C5" s="35" t="s">
+      <c r="C5" s="28" t="s">
         <v>42</v>
       </c>
-      <c r="D5" s="37" t="s">
+      <c r="D5" s="31" t="s">
         <v>8</v>
       </c>
-      <c r="E5" s="36" t="s">
+      <c r="E5" s="32" t="s">
         <v>16</v>
       </c>
       <c r="F5" s="43"/>
-      <c r="G5" s="36" t="s">
+      <c r="G5" s="32" t="s">
         <v>18</v>
       </c>
-      <c r="H5" s="37"/>
-      <c r="I5" s="50">
+      <c r="H5" s="31"/>
+      <c r="I5" s="25">
         <v>2</v>
       </c>
-      <c r="J5" s="52" t="s">
+      <c r="J5" s="23" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="6" spans="2:28" ht="15.75" customHeight="1">
-      <c r="B6" s="34"/>
-      <c r="C6" s="35"/>
-      <c r="D6" s="37"/>
-      <c r="E6" s="37"/>
+      <c r="B6" s="38"/>
+      <c r="C6" s="28"/>
+      <c r="D6" s="31"/>
+      <c r="E6" s="31"/>
       <c r="F6" s="43"/>
-      <c r="G6" s="37"/>
-      <c r="H6" s="37"/>
-      <c r="I6" s="50"/>
-      <c r="J6" s="52"/>
+      <c r="G6" s="31"/>
+      <c r="H6" s="31"/>
+      <c r="I6" s="25"/>
+      <c r="J6" s="23"/>
     </row>
     <row r="7" spans="2:28" ht="15.75" customHeight="1">
-      <c r="B7" s="28">
+      <c r="B7" s="37">
         <v>3</v>
       </c>
-      <c r="C7" s="46" t="s">
+      <c r="C7" s="30" t="s">
         <v>6</v>
       </c>
-      <c r="D7" s="40" t="s">
+      <c r="D7" s="35" t="s">
         <v>27</v>
       </c>
-      <c r="E7" s="40" t="s">
+      <c r="E7" s="35" t="s">
         <v>24</v>
       </c>
-      <c r="F7" s="44"/>
-      <c r="G7" s="40" t="s">
+      <c r="F7" s="29"/>
+      <c r="G7" s="35" t="s">
         <v>19</v>
       </c>
-      <c r="H7" s="44"/>
-      <c r="I7" s="32">
+      <c r="H7" s="29"/>
+      <c r="I7" s="26">
+        <v>10</v>
+      </c>
+      <c r="J7" s="22" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="8" spans="2:28" ht="15.75" customHeight="1">
+      <c r="B8" s="37"/>
+      <c r="C8" s="30"/>
+      <c r="D8" s="29"/>
+      <c r="E8" s="29"/>
+      <c r="F8" s="29"/>
+      <c r="G8" s="29"/>
+      <c r="H8" s="29"/>
+      <c r="I8" s="26"/>
+      <c r="J8" s="22"/>
+    </row>
+    <row r="9" spans="2:28" ht="15.75" customHeight="1">
+      <c r="B9" s="38">
+        <v>4</v>
+      </c>
+      <c r="C9" s="28" t="s">
+        <v>6</v>
+      </c>
+      <c r="D9" s="32" t="s">
+        <v>28</v>
+      </c>
+      <c r="E9" s="32" t="s">
+        <v>25</v>
+      </c>
+      <c r="F9" s="31"/>
+      <c r="G9" s="32" t="s">
+        <v>20</v>
+      </c>
+      <c r="H9" s="31"/>
+      <c r="I9" s="25">
+        <v>4</v>
+      </c>
+      <c r="J9" s="23" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="10" spans="2:28" ht="15.75" customHeight="1">
+      <c r="B10" s="38"/>
+      <c r="C10" s="28"/>
+      <c r="D10" s="31"/>
+      <c r="E10" s="31"/>
+      <c r="F10" s="31"/>
+      <c r="G10" s="31"/>
+      <c r="H10" s="31"/>
+      <c r="I10" s="25"/>
+      <c r="J10" s="23"/>
+    </row>
+    <row r="11" spans="2:28" ht="15.75" customHeight="1">
+      <c r="B11" s="37">
+        <v>5</v>
+      </c>
+      <c r="C11" s="30" t="s">
+        <v>10</v>
+      </c>
+      <c r="D11" s="29" t="s">
+        <v>11</v>
+      </c>
+      <c r="E11" s="35" t="s">
+        <v>39</v>
+      </c>
+      <c r="F11" s="29"/>
+      <c r="G11" s="35" t="s">
+        <v>21</v>
+      </c>
+      <c r="H11" s="29"/>
+      <c r="I11" s="26">
+        <v>5</v>
+      </c>
+      <c r="J11" s="23" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="12" spans="2:28" ht="15.75" customHeight="1">
+      <c r="B12" s="37"/>
+      <c r="C12" s="30"/>
+      <c r="D12" s="29"/>
+      <c r="E12" s="29"/>
+      <c r="F12" s="29"/>
+      <c r="G12" s="29"/>
+      <c r="H12" s="29"/>
+      <c r="I12" s="26"/>
+      <c r="J12" s="23"/>
+    </row>
+    <row r="13" spans="2:28" ht="15.75" customHeight="1">
+      <c r="B13" s="38">
+        <v>6</v>
+      </c>
+      <c r="C13" s="28" t="s">
+        <v>6</v>
+      </c>
+      <c r="D13" s="31" t="s">
+        <v>12</v>
+      </c>
+      <c r="E13" s="32" t="s">
+        <v>37</v>
+      </c>
+      <c r="F13" s="31"/>
+      <c r="G13" s="32" t="s">
+        <v>22</v>
+      </c>
+      <c r="H13" s="31"/>
+      <c r="I13" s="25">
+        <v>8</v>
+      </c>
+      <c r="J13" s="22" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="14" spans="2:28" ht="15.75" customHeight="1">
+      <c r="B14" s="38"/>
+      <c r="C14" s="28"/>
+      <c r="D14" s="31"/>
+      <c r="E14" s="31"/>
+      <c r="F14" s="31"/>
+      <c r="G14" s="31"/>
+      <c r="H14" s="31"/>
+      <c r="I14" s="25"/>
+      <c r="J14" s="22"/>
+    </row>
+    <row r="15" spans="2:28" ht="15.75" customHeight="1">
+      <c r="B15" s="37">
         <v>7</v>
       </c>
-      <c r="J7" s="24" t="s">
+      <c r="C15" s="30" t="s">
+        <v>6</v>
+      </c>
+      <c r="D15" s="35" t="s">
+        <v>29</v>
+      </c>
+      <c r="E15" s="35" t="s">
+        <v>26</v>
+      </c>
+      <c r="F15" s="29"/>
+      <c r="G15" s="35" t="s">
+        <v>23</v>
+      </c>
+      <c r="H15" s="29"/>
+      <c r="I15" s="26">
+        <v>9</v>
+      </c>
+      <c r="J15" s="22" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="8" spans="2:28" ht="15.75" customHeight="1">
-      <c r="B8" s="28"/>
-      <c r="C8" s="46"/>
-      <c r="D8" s="44"/>
-      <c r="E8" s="44"/>
-      <c r="F8" s="44"/>
-      <c r="G8" s="44"/>
-      <c r="H8" s="44"/>
-      <c r="I8" s="32"/>
-      <c r="J8" s="24"/>
-    </row>
-    <row r="9" spans="2:28" ht="15.75" customHeight="1">
-      <c r="B9" s="34">
-        <v>4</v>
-      </c>
-      <c r="C9" s="35" t="s">
-        <v>6</v>
-      </c>
-      <c r="D9" s="36" t="s">
-        <v>28</v>
-      </c>
-      <c r="E9" s="36" t="s">
-        <v>25</v>
-      </c>
-      <c r="F9" s="37"/>
-      <c r="G9" s="36" t="s">
-        <v>20</v>
-      </c>
-      <c r="H9" s="37"/>
-      <c r="I9" s="50">
-        <v>4</v>
-      </c>
-      <c r="J9" s="52" t="s">
+    <row r="16" spans="2:28" ht="15.75" customHeight="1">
+      <c r="B16" s="37"/>
+      <c r="C16" s="30"/>
+      <c r="D16" s="29"/>
+      <c r="E16" s="29"/>
+      <c r="F16" s="29"/>
+      <c r="G16" s="29"/>
+      <c r="H16" s="29"/>
+      <c r="I16" s="26"/>
+      <c r="J16" s="22"/>
+    </row>
+    <row r="17" spans="2:10" ht="15.75" customHeight="1">
+      <c r="B17" s="37"/>
+      <c r="C17" s="30"/>
+      <c r="D17" s="29"/>
+      <c r="E17" s="29"/>
+      <c r="F17" s="29"/>
+      <c r="G17" s="29"/>
+      <c r="H17" s="29"/>
+      <c r="I17" s="26"/>
+      <c r="J17" s="22"/>
+    </row>
+    <row r="18" spans="2:10" ht="15.75" customHeight="1">
+      <c r="B18" s="38">
+        <v>8</v>
+      </c>
+      <c r="C18" s="28" t="s">
+        <v>9</v>
+      </c>
+      <c r="D18" s="32" t="s">
+        <v>35</v>
+      </c>
+      <c r="E18" s="31" t="s">
+        <v>13</v>
+      </c>
+      <c r="F18" s="31"/>
+      <c r="G18" s="32" t="s">
+        <v>15</v>
+      </c>
+      <c r="H18" s="31"/>
+      <c r="I18" s="25">
+        <v>7</v>
+      </c>
+      <c r="J18" s="22" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="19" spans="2:10" ht="15.75" customHeight="1">
+      <c r="B19" s="38"/>
+      <c r="C19" s="28"/>
+      <c r="D19" s="31"/>
+      <c r="E19" s="31"/>
+      <c r="F19" s="31"/>
+      <c r="G19" s="31"/>
+      <c r="H19" s="31"/>
+      <c r="I19" s="25"/>
+      <c r="J19" s="22"/>
+    </row>
+    <row r="20" spans="2:10" ht="15.75" customHeight="1">
+      <c r="B20" s="38"/>
+      <c r="C20" s="28"/>
+      <c r="D20" s="31"/>
+      <c r="E20" s="31"/>
+      <c r="F20" s="31"/>
+      <c r="G20" s="31"/>
+      <c r="H20" s="31"/>
+      <c r="I20" s="25"/>
+      <c r="J20" s="22"/>
+    </row>
+    <row r="21" spans="2:10" ht="15.75" customHeight="1">
+      <c r="B21" s="37">
+        <v>9</v>
+      </c>
+      <c r="C21" s="34" t="s">
+        <v>9</v>
+      </c>
+      <c r="D21" s="42" t="s">
+        <v>40</v>
+      </c>
+      <c r="E21" s="42" t="s">
+        <v>31</v>
+      </c>
+      <c r="F21" s="40"/>
+      <c r="G21" s="40" t="s">
+        <v>30</v>
+      </c>
+      <c r="H21" s="40"/>
+      <c r="I21" s="26">
+        <v>3</v>
+      </c>
+      <c r="J21" s="23" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="10" spans="2:28" ht="15.75" customHeight="1">
-      <c r="B10" s="34"/>
-      <c r="C10" s="35"/>
-      <c r="D10" s="37"/>
-      <c r="E10" s="37"/>
-      <c r="F10" s="37"/>
-      <c r="G10" s="37"/>
-      <c r="H10" s="37"/>
-      <c r="I10" s="50"/>
-      <c r="J10" s="52"/>
-    </row>
-    <row r="11" spans="2:28" ht="15.75" customHeight="1">
-      <c r="B11" s="28">
-        <v>5</v>
-      </c>
-      <c r="C11" s="46" t="s">
+    <row r="22" spans="2:10" ht="15.75" customHeight="1">
+      <c r="B22" s="37"/>
+      <c r="C22" s="34"/>
+      <c r="D22" s="42"/>
+      <c r="E22" s="40"/>
+      <c r="F22" s="40"/>
+      <c r="G22" s="40"/>
+      <c r="H22" s="40"/>
+      <c r="I22" s="26"/>
+      <c r="J22" s="23"/>
+    </row>
+    <row r="23" spans="2:10" ht="15.75" customHeight="1">
+      <c r="B23" s="37"/>
+      <c r="C23" s="34"/>
+      <c r="D23" s="42"/>
+      <c r="E23" s="40"/>
+      <c r="F23" s="40"/>
+      <c r="G23" s="40"/>
+      <c r="H23" s="40"/>
+      <c r="I23" s="26"/>
+      <c r="J23" s="23"/>
+    </row>
+    <row r="24" spans="2:10" ht="15.75" customHeight="1">
+      <c r="B24" s="38">
         <v>10</v>
       </c>
-      <c r="D11" s="44" t="s">
+      <c r="C24" s="28" t="s">
+        <v>9</v>
+      </c>
+      <c r="D24" s="32" t="s">
+        <v>34</v>
+      </c>
+      <c r="E24" s="31" t="s">
+        <v>32</v>
+      </c>
+      <c r="F24" s="31"/>
+      <c r="G24" s="32" t="s">
+        <v>33</v>
+      </c>
+      <c r="H24" s="31"/>
+      <c r="I24" s="25" t="s">
+        <v>43</v>
+      </c>
+      <c r="J24" s="22" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="25" spans="2:10" ht="15.75" customHeight="1">
+      <c r="B25" s="38"/>
+      <c r="C25" s="28"/>
+      <c r="D25" s="31"/>
+      <c r="E25" s="31"/>
+      <c r="F25" s="31"/>
+      <c r="G25" s="32"/>
+      <c r="H25" s="31"/>
+      <c r="I25" s="25"/>
+      <c r="J25" s="22"/>
+    </row>
+    <row r="26" spans="2:10" ht="15.75" customHeight="1">
+      <c r="B26" s="38"/>
+      <c r="C26" s="28"/>
+      <c r="D26" s="31"/>
+      <c r="E26" s="31"/>
+      <c r="F26" s="31"/>
+      <c r="G26" s="32"/>
+      <c r="H26" s="31"/>
+      <c r="I26" s="25"/>
+      <c r="J26" s="22"/>
+    </row>
+    <row r="27" spans="2:10" ht="15.75" customHeight="1">
+      <c r="B27" s="37">
         <v>11</v>
       </c>
-      <c r="E11" s="40" t="s">
-        <v>39</v>
-      </c>
-      <c r="F11" s="44"/>
-      <c r="G11" s="40" t="s">
-        <v>21</v>
-      </c>
-      <c r="H11" s="44"/>
-      <c r="I11" s="32">
-        <v>5</v>
-      </c>
-      <c r="J11" s="52" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="12" spans="2:28" ht="15.75" customHeight="1">
-      <c r="B12" s="28"/>
-      <c r="C12" s="46"/>
-      <c r="D12" s="44"/>
-      <c r="E12" s="44"/>
-      <c r="F12" s="44"/>
-      <c r="G12" s="44"/>
-      <c r="H12" s="44"/>
-      <c r="I12" s="32"/>
-      <c r="J12" s="52"/>
-    </row>
-    <row r="13" spans="2:28" ht="15.75" customHeight="1">
-      <c r="B13" s="34">
-        <v>6</v>
-      </c>
-      <c r="C13" s="35" t="s">
-        <v>6</v>
-      </c>
-      <c r="D13" s="37" t="s">
+      <c r="C27" s="34" t="s">
+        <v>10</v>
+      </c>
+      <c r="D27" s="42" t="s">
+        <v>47</v>
+      </c>
+      <c r="E27" s="35" t="s">
+        <v>48</v>
+      </c>
+      <c r="F27" s="40"/>
+      <c r="G27" s="42" t="s">
+        <v>36</v>
+      </c>
+      <c r="H27" s="40"/>
+      <c r="I27" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="J27" s="47" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="28" spans="2:10" ht="15.75" customHeight="1">
+      <c r="B28" s="37"/>
+      <c r="C28" s="34"/>
+      <c r="D28" s="42"/>
+      <c r="E28" s="35"/>
+      <c r="F28" s="40"/>
+      <c r="G28" s="42"/>
+      <c r="H28" s="40"/>
+      <c r="I28" s="26"/>
+      <c r="J28" s="22"/>
+    </row>
+    <row r="29" spans="2:10" ht="15.75" customHeight="1">
+      <c r="B29" s="37"/>
+      <c r="C29" s="34"/>
+      <c r="D29" s="42"/>
+      <c r="E29" s="35"/>
+      <c r="F29" s="40"/>
+      <c r="G29" s="42"/>
+      <c r="H29" s="40"/>
+      <c r="I29" s="26"/>
+      <c r="J29" s="22"/>
+    </row>
+    <row r="30" spans="2:10" ht="15.75" customHeight="1">
+      <c r="B30" s="37"/>
+      <c r="C30" s="34"/>
+      <c r="D30" s="42"/>
+      <c r="E30" s="35"/>
+      <c r="F30" s="40"/>
+      <c r="G30" s="42"/>
+      <c r="H30" s="40"/>
+      <c r="I30" s="26"/>
+      <c r="J30" s="22"/>
+    </row>
+    <row r="31" spans="2:10" ht="15.75" customHeight="1">
+      <c r="B31" s="37"/>
+      <c r="C31" s="34"/>
+      <c r="D31" s="42"/>
+      <c r="E31" s="35"/>
+      <c r="F31" s="40"/>
+      <c r="G31" s="42"/>
+      <c r="H31" s="40"/>
+      <c r="I31" s="26"/>
+      <c r="J31" s="22"/>
+    </row>
+    <row r="32" spans="2:10" ht="15.75" customHeight="1">
+      <c r="B32" s="50"/>
+      <c r="C32" s="49"/>
+      <c r="D32" s="44"/>
+      <c r="E32" s="46"/>
+      <c r="F32" s="45"/>
+      <c r="G32" s="44"/>
+      <c r="H32" s="45"/>
+      <c r="I32" s="51"/>
+      <c r="J32" s="48"/>
+    </row>
+    <row r="33" spans="2:10" ht="63" customHeight="1">
+      <c r="B33" s="17">
         <v>12</v>
       </c>
-      <c r="E13" s="36" t="s">
-        <v>37</v>
-      </c>
-      <c r="F13" s="37"/>
-      <c r="G13" s="36" t="s">
-        <v>22</v>
-      </c>
-      <c r="H13" s="37"/>
-      <c r="I13" s="50" t="s">
+      <c r="C33" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="D33" s="19" t="s">
+        <v>49</v>
+      </c>
+      <c r="E33" s="20" t="s">
+        <v>50</v>
+      </c>
+      <c r="F33" s="20"/>
+      <c r="G33" s="21" t="s">
+        <v>51</v>
+      </c>
+      <c r="H33" s="20"/>
+      <c r="I33" s="18" t="s">
         <v>43</v>
       </c>
-      <c r="J13" s="24" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="14" spans="2:28" ht="15.75" customHeight="1">
-      <c r="B14" s="34"/>
-      <c r="C14" s="35"/>
-      <c r="D14" s="37"/>
-      <c r="E14" s="37"/>
-      <c r="F14" s="37"/>
-      <c r="G14" s="37"/>
-      <c r="H14" s="37"/>
-      <c r="I14" s="50"/>
-      <c r="J14" s="24"/>
-    </row>
-    <row r="15" spans="2:28" ht="15.75" customHeight="1">
-      <c r="B15" s="28">
-        <v>7</v>
-      </c>
-      <c r="C15" s="46" t="s">
-        <v>6</v>
-      </c>
-      <c r="D15" s="40" t="s">
-        <v>29</v>
-      </c>
-      <c r="E15" s="40" t="s">
-        <v>26</v>
-      </c>
-      <c r="F15" s="44"/>
-      <c r="G15" s="40" t="s">
-        <v>23</v>
-      </c>
-      <c r="H15" s="44"/>
-      <c r="I15" s="32">
-        <v>9</v>
-      </c>
-      <c r="J15" s="24" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="16" spans="2:28" ht="15.75" customHeight="1">
-      <c r="B16" s="28"/>
-      <c r="C16" s="46"/>
-      <c r="D16" s="44"/>
-      <c r="E16" s="44"/>
-      <c r="F16" s="44"/>
-      <c r="G16" s="44"/>
-      <c r="H16" s="44"/>
-      <c r="I16" s="32"/>
-      <c r="J16" s="24"/>
-    </row>
-    <row r="17" spans="2:10" ht="15.75" customHeight="1">
-      <c r="B17" s="28"/>
-      <c r="C17" s="46"/>
-      <c r="D17" s="44"/>
-      <c r="E17" s="44"/>
-      <c r="F17" s="44"/>
-      <c r="G17" s="44"/>
-      <c r="H17" s="44"/>
-      <c r="I17" s="32"/>
-      <c r="J17" s="24"/>
-    </row>
-    <row r="18" spans="2:10" ht="15.75" customHeight="1">
-      <c r="B18" s="34">
-        <v>8</v>
-      </c>
-      <c r="C18" s="35" t="s">
-        <v>9</v>
-      </c>
-      <c r="D18" s="36" t="s">
-        <v>35</v>
-      </c>
-      <c r="E18" s="37" t="s">
-        <v>13</v>
-      </c>
-      <c r="F18" s="37"/>
-      <c r="G18" s="36" t="s">
-        <v>15</v>
-      </c>
-      <c r="H18" s="37"/>
-      <c r="I18" s="50" t="s">
-        <v>43</v>
-      </c>
-      <c r="J18" s="24" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="19" spans="2:10" ht="15.75" customHeight="1">
-      <c r="B19" s="34"/>
-      <c r="C19" s="35"/>
-      <c r="D19" s="37"/>
-      <c r="E19" s="37"/>
-      <c r="F19" s="37"/>
-      <c r="G19" s="37"/>
-      <c r="H19" s="37"/>
-      <c r="I19" s="50"/>
-      <c r="J19" s="24"/>
-    </row>
-    <row r="20" spans="2:10" ht="15.75" customHeight="1">
-      <c r="B20" s="34"/>
-      <c r="C20" s="35"/>
-      <c r="D20" s="37"/>
-      <c r="E20" s="37"/>
-      <c r="F20" s="37"/>
-      <c r="G20" s="37"/>
-      <c r="H20" s="37"/>
-      <c r="I20" s="50"/>
-      <c r="J20" s="24"/>
-    </row>
-    <row r="21" spans="2:10" ht="15.75" customHeight="1">
-      <c r="B21" s="28">
-        <v>9</v>
-      </c>
-      <c r="C21" s="26" t="s">
-        <v>9</v>
-      </c>
-      <c r="D21" s="38" t="s">
-        <v>40</v>
-      </c>
-      <c r="E21" s="38" t="s">
-        <v>31</v>
-      </c>
-      <c r="F21" s="30"/>
-      <c r="G21" s="30" t="s">
-        <v>30</v>
-      </c>
-      <c r="H21" s="30"/>
-      <c r="I21" s="32">
-        <v>3</v>
-      </c>
-      <c r="J21" s="52" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="22" spans="2:10" ht="15.75" customHeight="1">
-      <c r="B22" s="28"/>
-      <c r="C22" s="26"/>
-      <c r="D22" s="38"/>
-      <c r="E22" s="30"/>
-      <c r="F22" s="30"/>
-      <c r="G22" s="30"/>
-      <c r="H22" s="30"/>
-      <c r="I22" s="32"/>
-      <c r="J22" s="52"/>
-    </row>
-    <row r="23" spans="2:10" ht="15.75" customHeight="1">
-      <c r="B23" s="28"/>
-      <c r="C23" s="26"/>
-      <c r="D23" s="38"/>
-      <c r="E23" s="30"/>
-      <c r="F23" s="30"/>
-      <c r="G23" s="30"/>
-      <c r="H23" s="30"/>
-      <c r="I23" s="32"/>
-      <c r="J23" s="52"/>
-    </row>
-    <row r="24" spans="2:10" ht="15.75" customHeight="1">
-      <c r="B24" s="34">
-        <v>10</v>
-      </c>
-      <c r="C24" s="35" t="s">
-        <v>9</v>
-      </c>
-      <c r="D24" s="36" t="s">
-        <v>34</v>
-      </c>
-      <c r="E24" s="37" t="s">
-        <v>32</v>
-      </c>
-      <c r="F24" s="37"/>
-      <c r="G24" s="36" t="s">
-        <v>33</v>
-      </c>
-      <c r="H24" s="37"/>
-      <c r="I24" s="50">
-        <v>10</v>
-      </c>
-      <c r="J24" s="24" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="25" spans="2:10" ht="15.75" customHeight="1">
-      <c r="B25" s="34"/>
-      <c r="C25" s="35"/>
-      <c r="D25" s="37"/>
-      <c r="E25" s="37"/>
-      <c r="F25" s="37"/>
-      <c r="G25" s="36"/>
-      <c r="H25" s="37"/>
-      <c r="I25" s="50"/>
-      <c r="J25" s="24"/>
-    </row>
-    <row r="26" spans="2:10" ht="15.75" customHeight="1">
-      <c r="B26" s="34"/>
-      <c r="C26" s="35"/>
-      <c r="D26" s="37"/>
-      <c r="E26" s="37"/>
-      <c r="F26" s="37"/>
-      <c r="G26" s="36"/>
-      <c r="H26" s="37"/>
-      <c r="I26" s="50"/>
-      <c r="J26" s="24"/>
-    </row>
-    <row r="27" spans="2:10" ht="15.75" customHeight="1">
-      <c r="B27" s="28">
-        <v>11</v>
-      </c>
-      <c r="C27" s="26" t="s">
-        <v>10</v>
-      </c>
-      <c r="D27" s="38" t="s">
-        <v>47</v>
-      </c>
-      <c r="E27" s="40" t="s">
-        <v>48</v>
-      </c>
-      <c r="F27" s="30"/>
-      <c r="G27" s="38" t="s">
-        <v>36</v>
-      </c>
-      <c r="H27" s="30"/>
-      <c r="I27" s="32">
-        <v>8</v>
-      </c>
-      <c r="J27" s="23" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="28" spans="2:10" ht="15.75" customHeight="1">
-      <c r="B28" s="28"/>
-      <c r="C28" s="26"/>
-      <c r="D28" s="38"/>
-      <c r="E28" s="40"/>
-      <c r="F28" s="30"/>
-      <c r="G28" s="38"/>
-      <c r="H28" s="30"/>
-      <c r="I28" s="32"/>
-      <c r="J28" s="24"/>
-    </row>
-    <row r="29" spans="2:10" ht="15.75" customHeight="1">
-      <c r="B29" s="28"/>
-      <c r="C29" s="26"/>
-      <c r="D29" s="38"/>
-      <c r="E29" s="40"/>
-      <c r="F29" s="30"/>
-      <c r="G29" s="38"/>
-      <c r="H29" s="30"/>
-      <c r="I29" s="32"/>
-      <c r="J29" s="24"/>
-    </row>
-    <row r="30" spans="2:10" ht="15.75" customHeight="1">
-      <c r="B30" s="28"/>
-      <c r="C30" s="26"/>
-      <c r="D30" s="38"/>
-      <c r="E30" s="40"/>
-      <c r="F30" s="30"/>
-      <c r="G30" s="38"/>
-      <c r="H30" s="30"/>
-      <c r="I30" s="32"/>
-      <c r="J30" s="24"/>
-    </row>
-    <row r="31" spans="2:10" ht="15.75" customHeight="1">
-      <c r="B31" s="28"/>
-      <c r="C31" s="26"/>
-      <c r="D31" s="38"/>
-      <c r="E31" s="40"/>
-      <c r="F31" s="30"/>
-      <c r="G31" s="38"/>
-      <c r="H31" s="30"/>
-      <c r="I31" s="32"/>
-      <c r="J31" s="24"/>
-    </row>
-    <row r="32" spans="2:10" ht="15.75" customHeight="1">
-      <c r="B32" s="29"/>
-      <c r="C32" s="27"/>
-      <c r="D32" s="39"/>
-      <c r="E32" s="41"/>
-      <c r="F32" s="31"/>
-      <c r="G32" s="39"/>
-      <c r="H32" s="31"/>
-      <c r="I32" s="33"/>
-      <c r="J32" s="25"/>
-    </row>
-    <row r="33" spans="2:10" ht="63" customHeight="1">
-      <c r="B33" s="18">
-        <v>12</v>
-      </c>
-      <c r="C33" s="17" t="s">
-        <v>10</v>
-      </c>
-      <c r="D33" s="20" t="s">
-        <v>49</v>
-      </c>
-      <c r="E33" s="21" t="s">
-        <v>50</v>
-      </c>
-      <c r="F33" s="21"/>
-      <c r="G33" s="22" t="s">
-        <v>51</v>
-      </c>
-      <c r="H33" s="21"/>
-      <c r="I33" s="19" t="s">
-        <v>43</v>
-      </c>
-      <c r="J33" s="16" t="s">
+      <c r="J33" s="15" t="s">
         <v>46</v>
       </c>
     </row>
@@ -1630,26 +1685,38 @@
       <c r="C34" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="D34" s="15" t="s">
+      <c r="D34" s="14" t="s">
         <v>52</v>
       </c>
-      <c r="E34" s="15" t="s">
+      <c r="E34" s="14" t="s">
         <v>54</v>
       </c>
-      <c r="F34" s="14"/>
-      <c r="G34" s="15" t="s">
+      <c r="F34" s="13"/>
+      <c r="G34" s="14" t="s">
         <v>53</v>
       </c>
-      <c r="H34" s="14"/>
+      <c r="H34" s="13"/>
       <c r="I34" s="8">
         <v>6</v>
       </c>
-      <c r="J34" s="13" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="35" spans="2:10" ht="15.75" customHeight="1"/>
-    <row r="36" spans="2:10" ht="15.75" customHeight="1"/>
+      <c r="J34" s="52" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="35" spans="2:10" ht="15.75" customHeight="1" thickBot="1"/>
+    <row r="36" spans="2:10" ht="15.75" customHeight="1" thickBot="1">
+      <c r="B36" s="53" t="s">
+        <v>55</v>
+      </c>
+      <c r="C36" s="54"/>
+      <c r="D36" s="54"/>
+      <c r="E36" s="54"/>
+      <c r="F36" s="54"/>
+      <c r="G36" s="54"/>
+      <c r="H36" s="54"/>
+      <c r="I36" s="54"/>
+      <c r="J36" s="55"/>
+    </row>
     <row r="37" spans="2:10" ht="15.75" customHeight="1"/>
     <row r="38" spans="2:10" ht="15.75" customHeight="1"/>
     <row r="39" spans="2:10" ht="15.75" customHeight="1"/>
@@ -2607,57 +2674,41 @@
     <row r="991" ht="15.75" customHeight="1"/>
     <row r="992" ht="15.75" customHeight="1"/>
   </sheetData>
-  <mergeCells count="99">
-    <mergeCell ref="J13:J14"/>
-    <mergeCell ref="J15:J17"/>
-    <mergeCell ref="J18:J20"/>
-    <mergeCell ref="J21:J23"/>
-    <mergeCell ref="J24:J26"/>
-    <mergeCell ref="J3:J4"/>
-    <mergeCell ref="J5:J6"/>
-    <mergeCell ref="J7:J8"/>
-    <mergeCell ref="J9:J10"/>
-    <mergeCell ref="J11:J12"/>
-    <mergeCell ref="I13:I14"/>
-    <mergeCell ref="I15:I17"/>
-    <mergeCell ref="I18:I20"/>
-    <mergeCell ref="I21:I23"/>
-    <mergeCell ref="I24:I26"/>
-    <mergeCell ref="I3:I4"/>
-    <mergeCell ref="I5:I6"/>
-    <mergeCell ref="I7:I8"/>
-    <mergeCell ref="I9:I10"/>
-    <mergeCell ref="I11:I12"/>
-    <mergeCell ref="C9:C10"/>
-    <mergeCell ref="D11:D12"/>
-    <mergeCell ref="C11:C12"/>
-    <mergeCell ref="D13:D14"/>
-    <mergeCell ref="C13:C14"/>
-    <mergeCell ref="D9:D10"/>
-    <mergeCell ref="C3:C4"/>
-    <mergeCell ref="D3:D4"/>
-    <mergeCell ref="C5:C6"/>
-    <mergeCell ref="D5:D6"/>
-    <mergeCell ref="C7:C8"/>
-    <mergeCell ref="D7:D8"/>
-    <mergeCell ref="B3:B4"/>
-    <mergeCell ref="B5:B6"/>
-    <mergeCell ref="B7:B8"/>
-    <mergeCell ref="B9:B10"/>
-    <mergeCell ref="B11:B12"/>
-    <mergeCell ref="B13:B14"/>
-    <mergeCell ref="B15:B17"/>
-    <mergeCell ref="G18:G20"/>
-    <mergeCell ref="E18:E20"/>
-    <mergeCell ref="C18:C20"/>
-    <mergeCell ref="B18:B20"/>
-    <mergeCell ref="F18:F20"/>
-    <mergeCell ref="E15:E17"/>
-    <mergeCell ref="D15:D17"/>
-    <mergeCell ref="D18:D20"/>
-    <mergeCell ref="F13:F14"/>
-    <mergeCell ref="C15:C17"/>
-    <mergeCell ref="F15:F17"/>
+  <mergeCells count="100">
+    <mergeCell ref="B36:J36"/>
+    <mergeCell ref="J27:J32"/>
+    <mergeCell ref="C27:C32"/>
+    <mergeCell ref="B27:B32"/>
+    <mergeCell ref="H27:H32"/>
+    <mergeCell ref="I27:I32"/>
+    <mergeCell ref="B24:B26"/>
+    <mergeCell ref="C24:C26"/>
+    <mergeCell ref="D24:D26"/>
+    <mergeCell ref="E24:E26"/>
+    <mergeCell ref="F24:F26"/>
+    <mergeCell ref="H24:H26"/>
+    <mergeCell ref="G27:G32"/>
+    <mergeCell ref="F27:F32"/>
+    <mergeCell ref="E27:E32"/>
+    <mergeCell ref="D27:D32"/>
+    <mergeCell ref="G24:G26"/>
+    <mergeCell ref="F3:F4"/>
+    <mergeCell ref="F5:F6"/>
+    <mergeCell ref="F7:F8"/>
+    <mergeCell ref="F9:F10"/>
+    <mergeCell ref="F11:F12"/>
+    <mergeCell ref="F21:F23"/>
+    <mergeCell ref="B21:B23"/>
+    <mergeCell ref="C21:C23"/>
+    <mergeCell ref="G21:G23"/>
+    <mergeCell ref="H21:H23"/>
+    <mergeCell ref="D21:D23"/>
+    <mergeCell ref="E21:E23"/>
+    <mergeCell ref="E5:E6"/>
+    <mergeCell ref="E7:E8"/>
+    <mergeCell ref="E9:E10"/>
+    <mergeCell ref="E11:E12"/>
+    <mergeCell ref="E13:E14"/>
     <mergeCell ref="H18:H20"/>
     <mergeCell ref="E3:E4"/>
     <mergeCell ref="G3:G4"/>
@@ -2674,39 +2725,56 @@
     <mergeCell ref="G11:G12"/>
     <mergeCell ref="G13:G14"/>
     <mergeCell ref="G15:G17"/>
-    <mergeCell ref="E5:E6"/>
-    <mergeCell ref="E7:E8"/>
-    <mergeCell ref="E9:E10"/>
-    <mergeCell ref="E11:E12"/>
-    <mergeCell ref="E13:E14"/>
-    <mergeCell ref="F21:F23"/>
-    <mergeCell ref="B21:B23"/>
-    <mergeCell ref="C21:C23"/>
-    <mergeCell ref="G21:G23"/>
-    <mergeCell ref="H21:H23"/>
-    <mergeCell ref="D21:D23"/>
-    <mergeCell ref="E21:E23"/>
-    <mergeCell ref="F3:F4"/>
-    <mergeCell ref="F5:F6"/>
-    <mergeCell ref="F7:F8"/>
-    <mergeCell ref="F9:F10"/>
-    <mergeCell ref="F11:F12"/>
-    <mergeCell ref="H24:H26"/>
-    <mergeCell ref="G27:G32"/>
-    <mergeCell ref="F27:F32"/>
-    <mergeCell ref="E27:E32"/>
-    <mergeCell ref="D27:D32"/>
-    <mergeCell ref="G24:G26"/>
-    <mergeCell ref="B24:B26"/>
-    <mergeCell ref="C24:C26"/>
-    <mergeCell ref="D24:D26"/>
-    <mergeCell ref="E24:E26"/>
-    <mergeCell ref="F24:F26"/>
-    <mergeCell ref="J27:J32"/>
-    <mergeCell ref="C27:C32"/>
-    <mergeCell ref="B27:B32"/>
-    <mergeCell ref="H27:H32"/>
-    <mergeCell ref="I27:I32"/>
+    <mergeCell ref="B13:B14"/>
+    <mergeCell ref="B15:B17"/>
+    <mergeCell ref="G18:G20"/>
+    <mergeCell ref="E18:E20"/>
+    <mergeCell ref="C18:C20"/>
+    <mergeCell ref="B18:B20"/>
+    <mergeCell ref="F18:F20"/>
+    <mergeCell ref="E15:E17"/>
+    <mergeCell ref="D15:D17"/>
+    <mergeCell ref="D18:D20"/>
+    <mergeCell ref="F13:F14"/>
+    <mergeCell ref="C15:C17"/>
+    <mergeCell ref="F15:F17"/>
+    <mergeCell ref="B3:B4"/>
+    <mergeCell ref="B5:B6"/>
+    <mergeCell ref="B7:B8"/>
+    <mergeCell ref="B9:B10"/>
+    <mergeCell ref="B11:B12"/>
+    <mergeCell ref="C3:C4"/>
+    <mergeCell ref="D3:D4"/>
+    <mergeCell ref="C5:C6"/>
+    <mergeCell ref="D5:D6"/>
+    <mergeCell ref="C7:C8"/>
+    <mergeCell ref="D7:D8"/>
+    <mergeCell ref="C9:C10"/>
+    <mergeCell ref="D11:D12"/>
+    <mergeCell ref="C11:C12"/>
+    <mergeCell ref="D13:D14"/>
+    <mergeCell ref="C13:C14"/>
+    <mergeCell ref="D9:D10"/>
+    <mergeCell ref="I3:I4"/>
+    <mergeCell ref="I5:I6"/>
+    <mergeCell ref="I7:I8"/>
+    <mergeCell ref="I9:I10"/>
+    <mergeCell ref="I11:I12"/>
+    <mergeCell ref="I13:I14"/>
+    <mergeCell ref="I15:I17"/>
+    <mergeCell ref="I18:I20"/>
+    <mergeCell ref="I21:I23"/>
+    <mergeCell ref="I24:I26"/>
+    <mergeCell ref="J3:J4"/>
+    <mergeCell ref="J5:J6"/>
+    <mergeCell ref="J7:J8"/>
+    <mergeCell ref="J9:J10"/>
+    <mergeCell ref="J11:J12"/>
+    <mergeCell ref="J13:J14"/>
+    <mergeCell ref="J15:J17"/>
+    <mergeCell ref="J18:J20"/>
+    <mergeCell ref="J21:J23"/>
+    <mergeCell ref="J24:J26"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape" r:id="rId1"/>

</xml_diff>

<commit_message>
Analyse des performances apres 7eme correction
</commit_message>
<xml_diff>
--- a/Analyses/Modèle-audit-SEO.xlsx
+++ b/Analyses/Modèle-audit-SEO.xlsx
@@ -9,6 +9,9 @@
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Feuil1!$B$2:$J$34</definedName>
+  </definedNames>
   <calcPr calcId="125725"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
@@ -70,10 +73,6 @@
   </si>
   <si>
     <t>N°</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Corriger la couleur du
- transparent</t>
   </si>
   <si>
     <t xml:space="preserve"> Images trop lourde donc
@@ -173,9 +172,6 @@
     <t xml:space="preserve"> Formulaire de contact trop compact
  (éléments se chevauchent) dans
  page de contact.</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Contraste faible entre le texte ou logo et couleur de fond des  transparents dans page d'accueil.</t>
   </si>
   <si>
     <t>Présenter la même barre de 
@@ -313,6 +309,15 @@
   </si>
   <si>
     <t xml:space="preserve"> La correction du point 13 (ordre 6) a entrainé la correction des points 10 et 11. Par conséquent , ses points ont été remplacé par les points 6 et 8</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Contraste faible entre le texte ou
+ logo et couleur de fond dans pages
+ html.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Corriger la couleur du
+ texte et/ou du fond.</t>
   </si>
 </sst>
 </file>
@@ -784,6 +789,9 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -859,6 +867,15 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -873,18 +890,6 @@
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1102,7 +1107,7 @@
   <dimension ref="B1:AB992"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="B36" sqref="B36:J36"/>
+      <selection activeCell="G18" sqref="G18:G20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.33203125" defaultRowHeight="15" customHeight="1"/>
@@ -1143,10 +1148,10 @@
         <v>5</v>
       </c>
       <c r="I2" s="11" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="J2" s="12" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="K2" s="5"/>
       <c r="L2" s="5"/>
@@ -1168,490 +1173,490 @@
       <c r="AB2" s="1"/>
     </row>
     <row r="3" spans="2:28" ht="15.75" customHeight="1">
-      <c r="B3" s="36">
+      <c r="B3" s="37">
         <v>1</v>
       </c>
-      <c r="C3" s="33" t="s">
-        <v>42</v>
-      </c>
-      <c r="D3" s="33" t="s">
+      <c r="C3" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="D3" s="34" t="s">
         <v>7</v>
       </c>
-      <c r="E3" s="39" t="s">
+      <c r="E3" s="40" t="s">
+        <v>15</v>
+      </c>
+      <c r="F3" s="40" t="s">
+        <v>39</v>
+      </c>
+      <c r="G3" s="40" t="s">
         <v>16</v>
       </c>
-      <c r="F3" s="39" t="s">
+      <c r="H3" s="42"/>
+      <c r="I3" s="28">
+        <v>1</v>
+      </c>
+      <c r="J3" s="25" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="4" spans="2:28" ht="15.75" customHeight="1">
+      <c r="B4" s="38"/>
+      <c r="C4" s="35"/>
+      <c r="D4" s="35"/>
+      <c r="E4" s="41"/>
+      <c r="F4" s="41"/>
+      <c r="G4" s="41"/>
+      <c r="H4" s="41"/>
+      <c r="I4" s="27"/>
+      <c r="J4" s="24"/>
+    </row>
+    <row r="5" spans="2:28" ht="15.75" customHeight="1">
+      <c r="B5" s="39">
+        <v>2</v>
+      </c>
+      <c r="C5" s="29" t="s">
+        <v>40</v>
+      </c>
+      <c r="D5" s="32" t="s">
+        <v>8</v>
+      </c>
+      <c r="E5" s="33" t="s">
+        <v>15</v>
+      </c>
+      <c r="F5" s="44"/>
+      <c r="G5" s="33" t="s">
+        <v>17</v>
+      </c>
+      <c r="H5" s="32"/>
+      <c r="I5" s="26">
+        <v>2</v>
+      </c>
+      <c r="J5" s="24" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="6" spans="2:28" ht="15.75" customHeight="1">
+      <c r="B6" s="39"/>
+      <c r="C6" s="29"/>
+      <c r="D6" s="32"/>
+      <c r="E6" s="32"/>
+      <c r="F6" s="44"/>
+      <c r="G6" s="32"/>
+      <c r="H6" s="32"/>
+      <c r="I6" s="26"/>
+      <c r="J6" s="24"/>
+    </row>
+    <row r="7" spans="2:28" ht="15.75" customHeight="1">
+      <c r="B7" s="38">
+        <v>3</v>
+      </c>
+      <c r="C7" s="31" t="s">
+        <v>6</v>
+      </c>
+      <c r="D7" s="36" t="s">
+        <v>26</v>
+      </c>
+      <c r="E7" s="36" t="s">
+        <v>23</v>
+      </c>
+      <c r="F7" s="30"/>
+      <c r="G7" s="36" t="s">
+        <v>18</v>
+      </c>
+      <c r="H7" s="30"/>
+      <c r="I7" s="27">
+        <v>10</v>
+      </c>
+      <c r="J7" s="23" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="8" spans="2:28" ht="15.75" customHeight="1">
+      <c r="B8" s="38"/>
+      <c r="C8" s="31"/>
+      <c r="D8" s="30"/>
+      <c r="E8" s="30"/>
+      <c r="F8" s="30"/>
+      <c r="G8" s="30"/>
+      <c r="H8" s="30"/>
+      <c r="I8" s="27"/>
+      <c r="J8" s="23"/>
+    </row>
+    <row r="9" spans="2:28" ht="15.75" customHeight="1">
+      <c r="B9" s="39">
+        <v>4</v>
+      </c>
+      <c r="C9" s="29" t="s">
+        <v>6</v>
+      </c>
+      <c r="D9" s="33" t="s">
+        <v>27</v>
+      </c>
+      <c r="E9" s="33" t="s">
+        <v>24</v>
+      </c>
+      <c r="F9" s="32"/>
+      <c r="G9" s="33" t="s">
+        <v>19</v>
+      </c>
+      <c r="H9" s="32"/>
+      <c r="I9" s="26">
+        <v>4</v>
+      </c>
+      <c r="J9" s="24" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="10" spans="2:28" ht="15.75" customHeight="1">
+      <c r="B10" s="39"/>
+      <c r="C10" s="29"/>
+      <c r="D10" s="32"/>
+      <c r="E10" s="32"/>
+      <c r="F10" s="32"/>
+      <c r="G10" s="32"/>
+      <c r="H10" s="32"/>
+      <c r="I10" s="26"/>
+      <c r="J10" s="24"/>
+    </row>
+    <row r="11" spans="2:28" ht="15.75" customHeight="1">
+      <c r="B11" s="38">
+        <v>5</v>
+      </c>
+      <c r="C11" s="31" t="s">
+        <v>10</v>
+      </c>
+      <c r="D11" s="30" t="s">
+        <v>11</v>
+      </c>
+      <c r="E11" s="36" t="s">
+        <v>37</v>
+      </c>
+      <c r="F11" s="30"/>
+      <c r="G11" s="36" t="s">
+        <v>20</v>
+      </c>
+      <c r="H11" s="30"/>
+      <c r="I11" s="27">
+        <v>5</v>
+      </c>
+      <c r="J11" s="24" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="12" spans="2:28" ht="15.75" customHeight="1">
+      <c r="B12" s="38"/>
+      <c r="C12" s="31"/>
+      <c r="D12" s="30"/>
+      <c r="E12" s="30"/>
+      <c r="F12" s="30"/>
+      <c r="G12" s="30"/>
+      <c r="H12" s="30"/>
+      <c r="I12" s="27"/>
+      <c r="J12" s="24"/>
+    </row>
+    <row r="13" spans="2:28" ht="15.75" customHeight="1">
+      <c r="B13" s="39">
+        <v>6</v>
+      </c>
+      <c r="C13" s="29" t="s">
+        <v>6</v>
+      </c>
+      <c r="D13" s="32" t="s">
+        <v>12</v>
+      </c>
+      <c r="E13" s="33" t="s">
+        <v>35</v>
+      </c>
+      <c r="F13" s="32"/>
+      <c r="G13" s="33" t="s">
+        <v>21</v>
+      </c>
+      <c r="H13" s="32"/>
+      <c r="I13" s="26">
+        <v>8</v>
+      </c>
+      <c r="J13" s="23" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="14" spans="2:28" ht="15.75" customHeight="1">
+      <c r="B14" s="39"/>
+      <c r="C14" s="29"/>
+      <c r="D14" s="32"/>
+      <c r="E14" s="32"/>
+      <c r="F14" s="32"/>
+      <c r="G14" s="32"/>
+      <c r="H14" s="32"/>
+      <c r="I14" s="26"/>
+      <c r="J14" s="23"/>
+    </row>
+    <row r="15" spans="2:28" ht="15.75" customHeight="1">
+      <c r="B15" s="38">
+        <v>7</v>
+      </c>
+      <c r="C15" s="31" t="s">
+        <v>6</v>
+      </c>
+      <c r="D15" s="36" t="s">
+        <v>28</v>
+      </c>
+      <c r="E15" s="36" t="s">
+        <v>25</v>
+      </c>
+      <c r="F15" s="30"/>
+      <c r="G15" s="36" t="s">
+        <v>22</v>
+      </c>
+      <c r="H15" s="30"/>
+      <c r="I15" s="27">
+        <v>9</v>
+      </c>
+      <c r="J15" s="23" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="16" spans="2:28" ht="15.75" customHeight="1">
+      <c r="B16" s="38"/>
+      <c r="C16" s="31"/>
+      <c r="D16" s="30"/>
+      <c r="E16" s="30"/>
+      <c r="F16" s="30"/>
+      <c r="G16" s="30"/>
+      <c r="H16" s="30"/>
+      <c r="I16" s="27"/>
+      <c r="J16" s="23"/>
+    </row>
+    <row r="17" spans="2:10" ht="15.75" customHeight="1">
+      <c r="B17" s="38"/>
+      <c r="C17" s="31"/>
+      <c r="D17" s="30"/>
+      <c r="E17" s="30"/>
+      <c r="F17" s="30"/>
+      <c r="G17" s="30"/>
+      <c r="H17" s="30"/>
+      <c r="I17" s="27"/>
+      <c r="J17" s="23"/>
+    </row>
+    <row r="18" spans="2:10" ht="15.75" customHeight="1">
+      <c r="B18" s="39">
+        <v>8</v>
+      </c>
+      <c r="C18" s="29" t="s">
+        <v>9</v>
+      </c>
+      <c r="D18" s="33" t="s">
+        <v>54</v>
+      </c>
+      <c r="E18" s="32" t="s">
+        <v>13</v>
+      </c>
+      <c r="F18" s="32"/>
+      <c r="G18" s="33" t="s">
+        <v>55</v>
+      </c>
+      <c r="H18" s="32"/>
+      <c r="I18" s="26">
+        <v>7</v>
+      </c>
+      <c r="J18" s="23" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="19" spans="2:10" ht="15.75" customHeight="1">
+      <c r="B19" s="39"/>
+      <c r="C19" s="29"/>
+      <c r="D19" s="32"/>
+      <c r="E19" s="32"/>
+      <c r="F19" s="32"/>
+      <c r="G19" s="32"/>
+      <c r="H19" s="32"/>
+      <c r="I19" s="26"/>
+      <c r="J19" s="23"/>
+    </row>
+    <row r="20" spans="2:10" ht="15.75" customHeight="1">
+      <c r="B20" s="39"/>
+      <c r="C20" s="29"/>
+      <c r="D20" s="32"/>
+      <c r="E20" s="32"/>
+      <c r="F20" s="32"/>
+      <c r="G20" s="32"/>
+      <c r="H20" s="32"/>
+      <c r="I20" s="26"/>
+      <c r="J20" s="23"/>
+    </row>
+    <row r="21" spans="2:10" ht="15.75" customHeight="1">
+      <c r="B21" s="38">
+        <v>9</v>
+      </c>
+      <c r="C21" s="35" t="s">
+        <v>9</v>
+      </c>
+      <c r="D21" s="43" t="s">
+        <v>38</v>
+      </c>
+      <c r="E21" s="43" t="s">
+        <v>30</v>
+      </c>
+      <c r="F21" s="41"/>
+      <c r="G21" s="41" t="s">
+        <v>29</v>
+      </c>
+      <c r="H21" s="41"/>
+      <c r="I21" s="27">
+        <v>3</v>
+      </c>
+      <c r="J21" s="24" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="22" spans="2:10" ht="15.75" customHeight="1">
+      <c r="B22" s="38"/>
+      <c r="C22" s="35"/>
+      <c r="D22" s="43"/>
+      <c r="E22" s="41"/>
+      <c r="F22" s="41"/>
+      <c r="G22" s="41"/>
+      <c r="H22" s="41"/>
+      <c r="I22" s="27"/>
+      <c r="J22" s="24"/>
+    </row>
+    <row r="23" spans="2:10" ht="15.75" customHeight="1">
+      <c r="B23" s="38"/>
+      <c r="C23" s="35"/>
+      <c r="D23" s="43"/>
+      <c r="E23" s="41"/>
+      <c r="F23" s="41"/>
+      <c r="G23" s="41"/>
+      <c r="H23" s="41"/>
+      <c r="I23" s="27"/>
+      <c r="J23" s="24"/>
+    </row>
+    <row r="24" spans="2:10" ht="15.75" customHeight="1">
+      <c r="B24" s="39">
+        <v>10</v>
+      </c>
+      <c r="C24" s="29" t="s">
+        <v>9</v>
+      </c>
+      <c r="D24" s="33" t="s">
+        <v>33</v>
+      </c>
+      <c r="E24" s="32" t="s">
+        <v>31</v>
+      </c>
+      <c r="F24" s="32"/>
+      <c r="G24" s="33" t="s">
+        <v>32</v>
+      </c>
+      <c r="H24" s="32"/>
+      <c r="I24" s="26" t="s">
         <v>41</v>
       </c>
-      <c r="G3" s="39" t="s">
-        <v>17</v>
-      </c>
-      <c r="H3" s="41"/>
-      <c r="I3" s="27">
-        <v>1</v>
-      </c>
-      <c r="J3" s="24" t="s">
+      <c r="J24" s="23" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="25" spans="2:10" ht="15.75" customHeight="1">
+      <c r="B25" s="39"/>
+      <c r="C25" s="29"/>
+      <c r="D25" s="32"/>
+      <c r="E25" s="32"/>
+      <c r="F25" s="32"/>
+      <c r="G25" s="33"/>
+      <c r="H25" s="32"/>
+      <c r="I25" s="26"/>
+      <c r="J25" s="23"/>
+    </row>
+    <row r="26" spans="2:10" ht="15.75" customHeight="1">
+      <c r="B26" s="39"/>
+      <c r="C26" s="29"/>
+      <c r="D26" s="32"/>
+      <c r="E26" s="32"/>
+      <c r="F26" s="32"/>
+      <c r="G26" s="33"/>
+      <c r="H26" s="32"/>
+      <c r="I26" s="26"/>
+      <c r="J26" s="23"/>
+    </row>
+    <row r="27" spans="2:10" ht="15.75" customHeight="1">
+      <c r="B27" s="38">
+        <v>11</v>
+      </c>
+      <c r="C27" s="35" t="s">
+        <v>10</v>
+      </c>
+      <c r="D27" s="43" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="4" spans="2:28" ht="15.75" customHeight="1">
-      <c r="B4" s="37"/>
-      <c r="C4" s="34"/>
-      <c r="D4" s="34"/>
-      <c r="E4" s="40"/>
-      <c r="F4" s="40"/>
-      <c r="G4" s="40"/>
-      <c r="H4" s="40"/>
-      <c r="I4" s="26"/>
-      <c r="J4" s="23"/>
-    </row>
-    <row r="5" spans="2:28" ht="15.75" customHeight="1">
-      <c r="B5" s="38">
-        <v>2</v>
-      </c>
-      <c r="C5" s="28" t="s">
-        <v>42</v>
-      </c>
-      <c r="D5" s="31" t="s">
-        <v>8</v>
-      </c>
-      <c r="E5" s="32" t="s">
-        <v>16</v>
-      </c>
-      <c r="F5" s="43"/>
-      <c r="G5" s="32" t="s">
-        <v>18</v>
-      </c>
-      <c r="H5" s="31"/>
-      <c r="I5" s="25">
-        <v>2</v>
-      </c>
-      <c r="J5" s="23" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="6" spans="2:28" ht="15.75" customHeight="1">
-      <c r="B6" s="38"/>
-      <c r="C6" s="28"/>
-      <c r="D6" s="31"/>
-      <c r="E6" s="31"/>
-      <c r="F6" s="43"/>
-      <c r="G6" s="31"/>
-      <c r="H6" s="31"/>
-      <c r="I6" s="25"/>
-      <c r="J6" s="23"/>
-    </row>
-    <row r="7" spans="2:28" ht="15.75" customHeight="1">
-      <c r="B7" s="37">
-        <v>3</v>
-      </c>
-      <c r="C7" s="30" t="s">
-        <v>6</v>
-      </c>
-      <c r="D7" s="35" t="s">
-        <v>27</v>
-      </c>
-      <c r="E7" s="35" t="s">
-        <v>24</v>
-      </c>
-      <c r="F7" s="29"/>
-      <c r="G7" s="35" t="s">
-        <v>19</v>
-      </c>
-      <c r="H7" s="29"/>
-      <c r="I7" s="26">
-        <v>10</v>
-      </c>
-      <c r="J7" s="22" t="s">
+      <c r="E27" s="36" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="8" spans="2:28" ht="15.75" customHeight="1">
-      <c r="B8" s="37"/>
-      <c r="C8" s="30"/>
-      <c r="D8" s="29"/>
-      <c r="E8" s="29"/>
-      <c r="F8" s="29"/>
-      <c r="G8" s="29"/>
-      <c r="H8" s="29"/>
-      <c r="I8" s="26"/>
-      <c r="J8" s="22"/>
-    </row>
-    <row r="9" spans="2:28" ht="15.75" customHeight="1">
-      <c r="B9" s="38">
-        <v>4</v>
-      </c>
-      <c r="C9" s="28" t="s">
-        <v>6</v>
-      </c>
-      <c r="D9" s="32" t="s">
-        <v>28</v>
-      </c>
-      <c r="E9" s="32" t="s">
-        <v>25</v>
-      </c>
-      <c r="F9" s="31"/>
-      <c r="G9" s="32" t="s">
-        <v>20</v>
-      </c>
-      <c r="H9" s="31"/>
-      <c r="I9" s="25">
-        <v>4</v>
-      </c>
-      <c r="J9" s="23" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="10" spans="2:28" ht="15.75" customHeight="1">
-      <c r="B10" s="38"/>
-      <c r="C10" s="28"/>
-      <c r="D10" s="31"/>
-      <c r="E10" s="31"/>
-      <c r="F10" s="31"/>
-      <c r="G10" s="31"/>
-      <c r="H10" s="31"/>
-      <c r="I10" s="25"/>
-      <c r="J10" s="23"/>
-    </row>
-    <row r="11" spans="2:28" ht="15.75" customHeight="1">
-      <c r="B11" s="37">
-        <v>5</v>
-      </c>
-      <c r="C11" s="30" t="s">
-        <v>10</v>
-      </c>
-      <c r="D11" s="29" t="s">
-        <v>11</v>
-      </c>
-      <c r="E11" s="35" t="s">
-        <v>39</v>
-      </c>
-      <c r="F11" s="29"/>
-      <c r="G11" s="35" t="s">
-        <v>21</v>
-      </c>
-      <c r="H11" s="29"/>
-      <c r="I11" s="26">
-        <v>5</v>
-      </c>
-      <c r="J11" s="23" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="12" spans="2:28" ht="15.75" customHeight="1">
-      <c r="B12" s="37"/>
-      <c r="C12" s="30"/>
-      <c r="D12" s="29"/>
-      <c r="E12" s="29"/>
-      <c r="F12" s="29"/>
-      <c r="G12" s="29"/>
-      <c r="H12" s="29"/>
-      <c r="I12" s="26"/>
-      <c r="J12" s="23"/>
-    </row>
-    <row r="13" spans="2:28" ht="15.75" customHeight="1">
-      <c r="B13" s="38">
-        <v>6</v>
-      </c>
-      <c r="C13" s="28" t="s">
-        <v>6</v>
-      </c>
-      <c r="D13" s="31" t="s">
-        <v>12</v>
-      </c>
-      <c r="E13" s="32" t="s">
-        <v>37</v>
-      </c>
-      <c r="F13" s="31"/>
-      <c r="G13" s="32" t="s">
-        <v>22</v>
-      </c>
-      <c r="H13" s="31"/>
-      <c r="I13" s="25">
-        <v>8</v>
-      </c>
-      <c r="J13" s="22" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="14" spans="2:28" ht="15.75" customHeight="1">
-      <c r="B14" s="38"/>
-      <c r="C14" s="28"/>
-      <c r="D14" s="31"/>
-      <c r="E14" s="31"/>
-      <c r="F14" s="31"/>
-      <c r="G14" s="31"/>
-      <c r="H14" s="31"/>
-      <c r="I14" s="25"/>
-      <c r="J14" s="22"/>
-    </row>
-    <row r="15" spans="2:28" ht="15.75" customHeight="1">
-      <c r="B15" s="37">
-        <v>7</v>
-      </c>
-      <c r="C15" s="30" t="s">
-        <v>6</v>
-      </c>
-      <c r="D15" s="35" t="s">
-        <v>29</v>
-      </c>
-      <c r="E15" s="35" t="s">
-        <v>26</v>
-      </c>
-      <c r="F15" s="29"/>
-      <c r="G15" s="35" t="s">
-        <v>23</v>
-      </c>
-      <c r="H15" s="29"/>
-      <c r="I15" s="26">
-        <v>9</v>
-      </c>
-      <c r="J15" s="22" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="16" spans="2:28" ht="15.75" customHeight="1">
-      <c r="B16" s="37"/>
-      <c r="C16" s="30"/>
-      <c r="D16" s="29"/>
-      <c r="E16" s="29"/>
-      <c r="F16" s="29"/>
-      <c r="G16" s="29"/>
-      <c r="H16" s="29"/>
-      <c r="I16" s="26"/>
-      <c r="J16" s="22"/>
-    </row>
-    <row r="17" spans="2:10" ht="15.75" customHeight="1">
-      <c r="B17" s="37"/>
-      <c r="C17" s="30"/>
-      <c r="D17" s="29"/>
-      <c r="E17" s="29"/>
-      <c r="F17" s="29"/>
-      <c r="G17" s="29"/>
-      <c r="H17" s="29"/>
-      <c r="I17" s="26"/>
-      <c r="J17" s="22"/>
-    </row>
-    <row r="18" spans="2:10" ht="15.75" customHeight="1">
-      <c r="B18" s="38">
-        <v>8</v>
-      </c>
-      <c r="C18" s="28" t="s">
-        <v>9</v>
-      </c>
-      <c r="D18" s="32" t="s">
-        <v>35</v>
-      </c>
-      <c r="E18" s="31" t="s">
-        <v>13</v>
-      </c>
-      <c r="F18" s="31"/>
-      <c r="G18" s="32" t="s">
-        <v>15</v>
-      </c>
-      <c r="H18" s="31"/>
-      <c r="I18" s="25">
-        <v>7</v>
-      </c>
-      <c r="J18" s="22" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="19" spans="2:10" ht="15.75" customHeight="1">
-      <c r="B19" s="38"/>
-      <c r="C19" s="28"/>
-      <c r="D19" s="31"/>
-      <c r="E19" s="31"/>
-      <c r="F19" s="31"/>
-      <c r="G19" s="31"/>
-      <c r="H19" s="31"/>
-      <c r="I19" s="25"/>
-      <c r="J19" s="22"/>
-    </row>
-    <row r="20" spans="2:10" ht="15.75" customHeight="1">
-      <c r="B20" s="38"/>
-      <c r="C20" s="28"/>
-      <c r="D20" s="31"/>
-      <c r="E20" s="31"/>
-      <c r="F20" s="31"/>
-      <c r="G20" s="31"/>
-      <c r="H20" s="31"/>
-      <c r="I20" s="25"/>
-      <c r="J20" s="22"/>
-    </row>
-    <row r="21" spans="2:10" ht="15.75" customHeight="1">
-      <c r="B21" s="37">
-        <v>9</v>
-      </c>
-      <c r="C21" s="34" t="s">
-        <v>9</v>
-      </c>
-      <c r="D21" s="42" t="s">
-        <v>40</v>
-      </c>
-      <c r="E21" s="42" t="s">
-        <v>31</v>
-      </c>
-      <c r="F21" s="40"/>
-      <c r="G21" s="40" t="s">
-        <v>30</v>
-      </c>
-      <c r="H21" s="40"/>
-      <c r="I21" s="26">
-        <v>3</v>
-      </c>
-      <c r="J21" s="23" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="22" spans="2:10" ht="15.75" customHeight="1">
-      <c r="B22" s="37"/>
-      <c r="C22" s="34"/>
-      <c r="D22" s="42"/>
-      <c r="E22" s="40"/>
-      <c r="F22" s="40"/>
-      <c r="G22" s="40"/>
-      <c r="H22" s="40"/>
-      <c r="I22" s="26"/>
-      <c r="J22" s="23"/>
-    </row>
-    <row r="23" spans="2:10" ht="15.75" customHeight="1">
-      <c r="B23" s="37"/>
-      <c r="C23" s="34"/>
-      <c r="D23" s="42"/>
-      <c r="E23" s="40"/>
-      <c r="F23" s="40"/>
-      <c r="G23" s="40"/>
-      <c r="H23" s="40"/>
-      <c r="I23" s="26"/>
-      <c r="J23" s="23"/>
-    </row>
-    <row r="24" spans="2:10" ht="15.75" customHeight="1">
-      <c r="B24" s="38">
-        <v>10</v>
-      </c>
-      <c r="C24" s="28" t="s">
-        <v>9</v>
-      </c>
-      <c r="D24" s="32" t="s">
+      <c r="F27" s="41"/>
+      <c r="G27" s="43" t="s">
         <v>34</v>
       </c>
-      <c r="E24" s="31" t="s">
-        <v>32</v>
-      </c>
-      <c r="F24" s="31"/>
-      <c r="G24" s="32" t="s">
-        <v>33</v>
-      </c>
-      <c r="H24" s="31"/>
-      <c r="I24" s="25" t="s">
-        <v>43</v>
-      </c>
-      <c r="J24" s="22" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="25" spans="2:10" ht="15.75" customHeight="1">
-      <c r="B25" s="38"/>
-      <c r="C25" s="28"/>
-      <c r="D25" s="31"/>
-      <c r="E25" s="31"/>
-      <c r="F25" s="31"/>
-      <c r="G25" s="32"/>
-      <c r="H25" s="31"/>
-      <c r="I25" s="25"/>
-      <c r="J25" s="22"/>
-    </row>
-    <row r="26" spans="2:10" ht="15.75" customHeight="1">
-      <c r="B26" s="38"/>
-      <c r="C26" s="28"/>
-      <c r="D26" s="31"/>
-      <c r="E26" s="31"/>
-      <c r="F26" s="31"/>
-      <c r="G26" s="32"/>
-      <c r="H26" s="31"/>
-      <c r="I26" s="25"/>
-      <c r="J26" s="22"/>
-    </row>
-    <row r="27" spans="2:10" ht="15.75" customHeight="1">
-      <c r="B27" s="37">
-        <v>11</v>
-      </c>
-      <c r="C27" s="34" t="s">
-        <v>10</v>
-      </c>
-      <c r="D27" s="42" t="s">
-        <v>47</v>
-      </c>
-      <c r="E27" s="35" t="s">
-        <v>48</v>
-      </c>
-      <c r="F27" s="40"/>
-      <c r="G27" s="42" t="s">
-        <v>36</v>
-      </c>
-      <c r="H27" s="40"/>
-      <c r="I27" s="26" t="s">
-        <v>43</v>
-      </c>
-      <c r="J27" s="47" t="s">
-        <v>46</v>
+      <c r="H27" s="41"/>
+      <c r="I27" s="27" t="s">
+        <v>41</v>
+      </c>
+      <c r="J27" s="51" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="28" spans="2:10" ht="15.75" customHeight="1">
-      <c r="B28" s="37"/>
-      <c r="C28" s="34"/>
-      <c r="D28" s="42"/>
-      <c r="E28" s="35"/>
-      <c r="F28" s="40"/>
-      <c r="G28" s="42"/>
-      <c r="H28" s="40"/>
-      <c r="I28" s="26"/>
-      <c r="J28" s="22"/>
+      <c r="B28" s="38"/>
+      <c r="C28" s="35"/>
+      <c r="D28" s="43"/>
+      <c r="E28" s="36"/>
+      <c r="F28" s="41"/>
+      <c r="G28" s="43"/>
+      <c r="H28" s="41"/>
+      <c r="I28" s="27"/>
+      <c r="J28" s="23"/>
     </row>
     <row r="29" spans="2:10" ht="15.75" customHeight="1">
-      <c r="B29" s="37"/>
-      <c r="C29" s="34"/>
-      <c r="D29" s="42"/>
-      <c r="E29" s="35"/>
-      <c r="F29" s="40"/>
-      <c r="G29" s="42"/>
-      <c r="H29" s="40"/>
-      <c r="I29" s="26"/>
-      <c r="J29" s="22"/>
+      <c r="B29" s="38"/>
+      <c r="C29" s="35"/>
+      <c r="D29" s="43"/>
+      <c r="E29" s="36"/>
+      <c r="F29" s="41"/>
+      <c r="G29" s="43"/>
+      <c r="H29" s="41"/>
+      <c r="I29" s="27"/>
+      <c r="J29" s="23"/>
     </row>
     <row r="30" spans="2:10" ht="15.75" customHeight="1">
-      <c r="B30" s="37"/>
-      <c r="C30" s="34"/>
-      <c r="D30" s="42"/>
-      <c r="E30" s="35"/>
-      <c r="F30" s="40"/>
-      <c r="G30" s="42"/>
-      <c r="H30" s="40"/>
-      <c r="I30" s="26"/>
-      <c r="J30" s="22"/>
+      <c r="B30" s="38"/>
+      <c r="C30" s="35"/>
+      <c r="D30" s="43"/>
+      <c r="E30" s="36"/>
+      <c r="F30" s="41"/>
+      <c r="G30" s="43"/>
+      <c r="H30" s="41"/>
+      <c r="I30" s="27"/>
+      <c r="J30" s="23"/>
     </row>
     <row r="31" spans="2:10" ht="15.75" customHeight="1">
-      <c r="B31" s="37"/>
-      <c r="C31" s="34"/>
-      <c r="D31" s="42"/>
-      <c r="E31" s="35"/>
-      <c r="F31" s="40"/>
-      <c r="G31" s="42"/>
-      <c r="H31" s="40"/>
-      <c r="I31" s="26"/>
-      <c r="J31" s="22"/>
+      <c r="B31" s="38"/>
+      <c r="C31" s="35"/>
+      <c r="D31" s="43"/>
+      <c r="E31" s="36"/>
+      <c r="F31" s="41"/>
+      <c r="G31" s="43"/>
+      <c r="H31" s="41"/>
+      <c r="I31" s="27"/>
+      <c r="J31" s="23"/>
     </row>
     <row r="32" spans="2:10" ht="15.75" customHeight="1">
-      <c r="B32" s="50"/>
-      <c r="C32" s="49"/>
-      <c r="D32" s="44"/>
-      <c r="E32" s="46"/>
-      <c r="F32" s="45"/>
-      <c r="G32" s="44"/>
-      <c r="H32" s="45"/>
-      <c r="I32" s="51"/>
-      <c r="J32" s="48"/>
+      <c r="B32" s="54"/>
+      <c r="C32" s="53"/>
+      <c r="D32" s="45"/>
+      <c r="E32" s="47"/>
+      <c r="F32" s="46"/>
+      <c r="G32" s="45"/>
+      <c r="H32" s="46"/>
+      <c r="I32" s="55"/>
+      <c r="J32" s="52"/>
     </row>
     <row r="33" spans="2:10" ht="63" customHeight="1">
       <c r="B33" s="17">
@@ -1661,21 +1666,21 @@
         <v>10</v>
       </c>
       <c r="D33" s="19" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="E33" s="20" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="F33" s="20"/>
       <c r="G33" s="21" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="H33" s="20"/>
       <c r="I33" s="18" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="J33" s="15" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="34" spans="2:10" ht="63" customHeight="1" thickBot="1">
@@ -1683,39 +1688,39 @@
         <v>13</v>
       </c>
       <c r="C34" s="7" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D34" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="E34" s="14" t="s">
         <v>52</v>
-      </c>
-      <c r="E34" s="14" t="s">
-        <v>54</v>
       </c>
       <c r="F34" s="13"/>
       <c r="G34" s="14" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="H34" s="13"/>
       <c r="I34" s="8">
         <v>6</v>
       </c>
-      <c r="J34" s="52" t="s">
-        <v>45</v>
+      <c r="J34" s="22" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="35" spans="2:10" ht="15.75" customHeight="1" thickBot="1"/>
     <row r="36" spans="2:10" ht="15.75" customHeight="1" thickBot="1">
-      <c r="B36" s="53" t="s">
-        <v>55</v>
-      </c>
-      <c r="C36" s="54"/>
-      <c r="D36" s="54"/>
-      <c r="E36" s="54"/>
-      <c r="F36" s="54"/>
-      <c r="G36" s="54"/>
-      <c r="H36" s="54"/>
-      <c r="I36" s="54"/>
-      <c r="J36" s="55"/>
+      <c r="B36" s="48" t="s">
+        <v>53</v>
+      </c>
+      <c r="C36" s="49"/>
+      <c r="D36" s="49"/>
+      <c r="E36" s="49"/>
+      <c r="F36" s="49"/>
+      <c r="G36" s="49"/>
+      <c r="H36" s="49"/>
+      <c r="I36" s="49"/>
+      <c r="J36" s="50"/>
     </row>
     <row r="37" spans="2:10" ht="15.75" customHeight="1"/>
     <row r="38" spans="2:10" ht="15.75" customHeight="1"/>
@@ -2674,6 +2679,7 @@
     <row r="991" ht="15.75" customHeight="1"/>
     <row r="992" ht="15.75" customHeight="1"/>
   </sheetData>
+  <autoFilter ref="B2:J34"/>
   <mergeCells count="100">
     <mergeCell ref="B36:J36"/>
     <mergeCell ref="J27:J32"/>

</xml_diff>

<commit_message>
7. Analyses des performances apres 7eme correction
</commit_message>
<xml_diff>
--- a/Analyses/Modèle-audit-SEO.xlsx
+++ b/Analyses/Modèle-audit-SEO.xlsx
@@ -792,103 +792,103 @@
     <xf numFmtId="0" fontId="7" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1107,7 +1107,7 @@
   <dimension ref="B1:AB992"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="G18" sqref="G18:G20"/>
+      <selection activeCell="I15" sqref="I15:I17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.33203125" defaultRowHeight="15" customHeight="1"/>
@@ -1173,490 +1173,490 @@
       <c r="AB2" s="1"/>
     </row>
     <row r="3" spans="2:28" ht="15.75" customHeight="1">
-      <c r="B3" s="37">
+      <c r="B3" s="50">
         <v>1</v>
       </c>
-      <c r="C3" s="34" t="s">
+      <c r="C3" s="51" t="s">
         <v>40</v>
       </c>
-      <c r="D3" s="34" t="s">
+      <c r="D3" s="51" t="s">
         <v>7</v>
       </c>
-      <c r="E3" s="40" t="s">
+      <c r="E3" s="45" t="s">
         <v>15</v>
       </c>
-      <c r="F3" s="40" t="s">
+      <c r="F3" s="45" t="s">
         <v>39</v>
       </c>
-      <c r="G3" s="40" t="s">
+      <c r="G3" s="45" t="s">
         <v>16</v>
       </c>
-      <c r="H3" s="42"/>
-      <c r="I3" s="28">
+      <c r="H3" s="48"/>
+      <c r="I3" s="52">
         <v>1</v>
       </c>
-      <c r="J3" s="25" t="s">
+      <c r="J3" s="54" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="4" spans="2:28" ht="15.75" customHeight="1">
-      <c r="B4" s="38"/>
-      <c r="C4" s="35"/>
-      <c r="D4" s="35"/>
-      <c r="E4" s="41"/>
-      <c r="F4" s="41"/>
-      <c r="G4" s="41"/>
-      <c r="H4" s="41"/>
-      <c r="I4" s="27"/>
-      <c r="J4" s="24"/>
+      <c r="B4" s="31"/>
+      <c r="C4" s="29"/>
+      <c r="D4" s="29"/>
+      <c r="E4" s="33"/>
+      <c r="F4" s="33"/>
+      <c r="G4" s="33"/>
+      <c r="H4" s="33"/>
+      <c r="I4" s="35"/>
+      <c r="J4" s="55"/>
     </row>
     <row r="5" spans="2:28" ht="15.75" customHeight="1">
-      <c r="B5" s="39">
+      <c r="B5" s="37">
         <v>2</v>
       </c>
-      <c r="C5" s="29" t="s">
+      <c r="C5" s="38" t="s">
         <v>40</v>
       </c>
-      <c r="D5" s="32" t="s">
+      <c r="D5" s="40" t="s">
         <v>8</v>
       </c>
-      <c r="E5" s="33" t="s">
+      <c r="E5" s="39" t="s">
         <v>15</v>
       </c>
-      <c r="F5" s="44"/>
-      <c r="G5" s="33" t="s">
+      <c r="F5" s="46"/>
+      <c r="G5" s="39" t="s">
         <v>17</v>
       </c>
-      <c r="H5" s="32"/>
-      <c r="I5" s="26">
+      <c r="H5" s="40"/>
+      <c r="I5" s="53">
         <v>2</v>
       </c>
-      <c r="J5" s="24" t="s">
+      <c r="J5" s="55" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="6" spans="2:28" ht="15.75" customHeight="1">
-      <c r="B6" s="39"/>
-      <c r="C6" s="29"/>
-      <c r="D6" s="32"/>
-      <c r="E6" s="32"/>
-      <c r="F6" s="44"/>
-      <c r="G6" s="32"/>
-      <c r="H6" s="32"/>
-      <c r="I6" s="26"/>
-      <c r="J6" s="24"/>
+      <c r="B6" s="37"/>
+      <c r="C6" s="38"/>
+      <c r="D6" s="40"/>
+      <c r="E6" s="40"/>
+      <c r="F6" s="46"/>
+      <c r="G6" s="40"/>
+      <c r="H6" s="40"/>
+      <c r="I6" s="53"/>
+      <c r="J6" s="55"/>
     </row>
     <row r="7" spans="2:28" ht="15.75" customHeight="1">
-      <c r="B7" s="38">
+      <c r="B7" s="31">
         <v>3</v>
       </c>
-      <c r="C7" s="31" t="s">
+      <c r="C7" s="49" t="s">
         <v>6</v>
       </c>
-      <c r="D7" s="36" t="s">
+      <c r="D7" s="43" t="s">
         <v>26</v>
       </c>
-      <c r="E7" s="36" t="s">
+      <c r="E7" s="43" t="s">
         <v>23</v>
       </c>
-      <c r="F7" s="30"/>
-      <c r="G7" s="36" t="s">
+      <c r="F7" s="47"/>
+      <c r="G7" s="43" t="s">
         <v>18</v>
       </c>
-      <c r="H7" s="30"/>
-      <c r="I7" s="27">
+      <c r="H7" s="47"/>
+      <c r="I7" s="35">
         <v>10</v>
       </c>
-      <c r="J7" s="23" t="s">
+      <c r="J7" s="27" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="8" spans="2:28" ht="15.75" customHeight="1">
-      <c r="B8" s="38"/>
-      <c r="C8" s="31"/>
-      <c r="D8" s="30"/>
-      <c r="E8" s="30"/>
-      <c r="F8" s="30"/>
-      <c r="G8" s="30"/>
-      <c r="H8" s="30"/>
-      <c r="I8" s="27"/>
-      <c r="J8" s="23"/>
+      <c r="B8" s="31"/>
+      <c r="C8" s="49"/>
+      <c r="D8" s="47"/>
+      <c r="E8" s="47"/>
+      <c r="F8" s="47"/>
+      <c r="G8" s="47"/>
+      <c r="H8" s="47"/>
+      <c r="I8" s="35"/>
+      <c r="J8" s="27"/>
     </row>
     <row r="9" spans="2:28" ht="15.75" customHeight="1">
-      <c r="B9" s="39">
+      <c r="B9" s="37">
         <v>4</v>
       </c>
-      <c r="C9" s="29" t="s">
+      <c r="C9" s="38" t="s">
         <v>6</v>
       </c>
-      <c r="D9" s="33" t="s">
+      <c r="D9" s="39" t="s">
         <v>27</v>
       </c>
-      <c r="E9" s="33" t="s">
+      <c r="E9" s="39" t="s">
         <v>24</v>
       </c>
-      <c r="F9" s="32"/>
-      <c r="G9" s="33" t="s">
+      <c r="F9" s="40"/>
+      <c r="G9" s="39" t="s">
         <v>19</v>
       </c>
-      <c r="H9" s="32"/>
-      <c r="I9" s="26">
+      <c r="H9" s="40"/>
+      <c r="I9" s="53">
         <v>4</v>
       </c>
-      <c r="J9" s="24" t="s">
+      <c r="J9" s="55" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="10" spans="2:28" ht="15.75" customHeight="1">
-      <c r="B10" s="39"/>
-      <c r="C10" s="29"/>
-      <c r="D10" s="32"/>
-      <c r="E10" s="32"/>
-      <c r="F10" s="32"/>
-      <c r="G10" s="32"/>
-      <c r="H10" s="32"/>
-      <c r="I10" s="26"/>
-      <c r="J10" s="24"/>
+      <c r="B10" s="37"/>
+      <c r="C10" s="38"/>
+      <c r="D10" s="40"/>
+      <c r="E10" s="40"/>
+      <c r="F10" s="40"/>
+      <c r="G10" s="40"/>
+      <c r="H10" s="40"/>
+      <c r="I10" s="53"/>
+      <c r="J10" s="55"/>
     </row>
     <row r="11" spans="2:28" ht="15.75" customHeight="1">
-      <c r="B11" s="38">
+      <c r="B11" s="31">
         <v>5</v>
       </c>
-      <c r="C11" s="31" t="s">
+      <c r="C11" s="49" t="s">
         <v>10</v>
       </c>
-      <c r="D11" s="30" t="s">
+      <c r="D11" s="47" t="s">
         <v>11</v>
       </c>
-      <c r="E11" s="36" t="s">
+      <c r="E11" s="43" t="s">
         <v>37</v>
       </c>
-      <c r="F11" s="30"/>
-      <c r="G11" s="36" t="s">
+      <c r="F11" s="47"/>
+      <c r="G11" s="43" t="s">
         <v>20</v>
       </c>
-      <c r="H11" s="30"/>
-      <c r="I11" s="27">
+      <c r="H11" s="47"/>
+      <c r="I11" s="35">
         <v>5</v>
       </c>
-      <c r="J11" s="24" t="s">
+      <c r="J11" s="55" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="12" spans="2:28" ht="15.75" customHeight="1">
-      <c r="B12" s="38"/>
-      <c r="C12" s="31"/>
-      <c r="D12" s="30"/>
-      <c r="E12" s="30"/>
-      <c r="F12" s="30"/>
-      <c r="G12" s="30"/>
-      <c r="H12" s="30"/>
-      <c r="I12" s="27"/>
-      <c r="J12" s="24"/>
+      <c r="B12" s="31"/>
+      <c r="C12" s="49"/>
+      <c r="D12" s="47"/>
+      <c r="E12" s="47"/>
+      <c r="F12" s="47"/>
+      <c r="G12" s="47"/>
+      <c r="H12" s="47"/>
+      <c r="I12" s="35"/>
+      <c r="J12" s="55"/>
     </row>
     <row r="13" spans="2:28" ht="15.75" customHeight="1">
-      <c r="B13" s="39">
+      <c r="B13" s="37">
         <v>6</v>
       </c>
-      <c r="C13" s="29" t="s">
+      <c r="C13" s="38" t="s">
         <v>6</v>
       </c>
-      <c r="D13" s="32" t="s">
+      <c r="D13" s="40" t="s">
         <v>12</v>
       </c>
-      <c r="E13" s="33" t="s">
+      <c r="E13" s="39" t="s">
         <v>35</v>
       </c>
-      <c r="F13" s="32"/>
-      <c r="G13" s="33" t="s">
+      <c r="F13" s="40"/>
+      <c r="G13" s="39" t="s">
         <v>21</v>
       </c>
-      <c r="H13" s="32"/>
-      <c r="I13" s="26">
+      <c r="H13" s="40"/>
+      <c r="I13" s="53">
+        <v>9</v>
+      </c>
+      <c r="J13" s="27" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="14" spans="2:28" ht="15.75" customHeight="1">
+      <c r="B14" s="37"/>
+      <c r="C14" s="38"/>
+      <c r="D14" s="40"/>
+      <c r="E14" s="40"/>
+      <c r="F14" s="40"/>
+      <c r="G14" s="40"/>
+      <c r="H14" s="40"/>
+      <c r="I14" s="53"/>
+      <c r="J14" s="27"/>
+    </row>
+    <row r="15" spans="2:28" ht="15.75" customHeight="1">
+      <c r="B15" s="31">
+        <v>7</v>
+      </c>
+      <c r="C15" s="49" t="s">
+        <v>6</v>
+      </c>
+      <c r="D15" s="43" t="s">
+        <v>28</v>
+      </c>
+      <c r="E15" s="43" t="s">
+        <v>25</v>
+      </c>
+      <c r="F15" s="47"/>
+      <c r="G15" s="43" t="s">
+        <v>22</v>
+      </c>
+      <c r="H15" s="47"/>
+      <c r="I15" s="35">
         <v>8</v>
       </c>
-      <c r="J13" s="23" t="s">
+      <c r="J15" s="27" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="14" spans="2:28" ht="15.75" customHeight="1">
-      <c r="B14" s="39"/>
-      <c r="C14" s="29"/>
-      <c r="D14" s="32"/>
-      <c r="E14" s="32"/>
-      <c r="F14" s="32"/>
-      <c r="G14" s="32"/>
-      <c r="H14" s="32"/>
-      <c r="I14" s="26"/>
-      <c r="J14" s="23"/>
-    </row>
-    <row r="15" spans="2:28" ht="15.75" customHeight="1">
-      <c r="B15" s="38">
+    <row r="16" spans="2:28" ht="15.75" customHeight="1">
+      <c r="B16" s="31"/>
+      <c r="C16" s="49"/>
+      <c r="D16" s="47"/>
+      <c r="E16" s="47"/>
+      <c r="F16" s="47"/>
+      <c r="G16" s="47"/>
+      <c r="H16" s="47"/>
+      <c r="I16" s="35"/>
+      <c r="J16" s="27"/>
+    </row>
+    <row r="17" spans="2:10" ht="15.75" customHeight="1">
+      <c r="B17" s="31"/>
+      <c r="C17" s="49"/>
+      <c r="D17" s="47"/>
+      <c r="E17" s="47"/>
+      <c r="F17" s="47"/>
+      <c r="G17" s="47"/>
+      <c r="H17" s="47"/>
+      <c r="I17" s="35"/>
+      <c r="J17" s="27"/>
+    </row>
+    <row r="18" spans="2:10" ht="15.75" customHeight="1">
+      <c r="B18" s="37">
+        <v>8</v>
+      </c>
+      <c r="C18" s="38" t="s">
+        <v>9</v>
+      </c>
+      <c r="D18" s="39" t="s">
+        <v>54</v>
+      </c>
+      <c r="E18" s="40" t="s">
+        <v>13</v>
+      </c>
+      <c r="F18" s="40"/>
+      <c r="G18" s="39" t="s">
+        <v>55</v>
+      </c>
+      <c r="H18" s="40"/>
+      <c r="I18" s="53">
         <v>7</v>
       </c>
-      <c r="C15" s="31" t="s">
-        <v>6</v>
-      </c>
-      <c r="D15" s="36" t="s">
-        <v>28</v>
-      </c>
-      <c r="E15" s="36" t="s">
-        <v>25</v>
-      </c>
-      <c r="F15" s="30"/>
-      <c r="G15" s="36" t="s">
-        <v>22</v>
-      </c>
-      <c r="H15" s="30"/>
-      <c r="I15" s="27">
+      <c r="J18" s="55" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="19" spans="2:10" ht="15.75" customHeight="1">
+      <c r="B19" s="37"/>
+      <c r="C19" s="38"/>
+      <c r="D19" s="40"/>
+      <c r="E19" s="40"/>
+      <c r="F19" s="40"/>
+      <c r="G19" s="40"/>
+      <c r="H19" s="40"/>
+      <c r="I19" s="53"/>
+      <c r="J19" s="55"/>
+    </row>
+    <row r="20" spans="2:10" ht="15.75" customHeight="1">
+      <c r="B20" s="37"/>
+      <c r="C20" s="38"/>
+      <c r="D20" s="40"/>
+      <c r="E20" s="40"/>
+      <c r="F20" s="40"/>
+      <c r="G20" s="40"/>
+      <c r="H20" s="40"/>
+      <c r="I20" s="53"/>
+      <c r="J20" s="55"/>
+    </row>
+    <row r="21" spans="2:10" ht="15.75" customHeight="1">
+      <c r="B21" s="31">
         <v>9</v>
       </c>
-      <c r="J15" s="23" t="s">
+      <c r="C21" s="29" t="s">
+        <v>9</v>
+      </c>
+      <c r="D21" s="41" t="s">
+        <v>38</v>
+      </c>
+      <c r="E21" s="41" t="s">
+        <v>30</v>
+      </c>
+      <c r="F21" s="33"/>
+      <c r="G21" s="33" t="s">
+        <v>29</v>
+      </c>
+      <c r="H21" s="33"/>
+      <c r="I21" s="35">
+        <v>3</v>
+      </c>
+      <c r="J21" s="55" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="22" spans="2:10" ht="15.75" customHeight="1">
+      <c r="B22" s="31"/>
+      <c r="C22" s="29"/>
+      <c r="D22" s="41"/>
+      <c r="E22" s="33"/>
+      <c r="F22" s="33"/>
+      <c r="G22" s="33"/>
+      <c r="H22" s="33"/>
+      <c r="I22" s="35"/>
+      <c r="J22" s="55"/>
+    </row>
+    <row r="23" spans="2:10" ht="15.75" customHeight="1">
+      <c r="B23" s="31"/>
+      <c r="C23" s="29"/>
+      <c r="D23" s="41"/>
+      <c r="E23" s="33"/>
+      <c r="F23" s="33"/>
+      <c r="G23" s="33"/>
+      <c r="H23" s="33"/>
+      <c r="I23" s="35"/>
+      <c r="J23" s="55"/>
+    </row>
+    <row r="24" spans="2:10" ht="15.75" customHeight="1">
+      <c r="B24" s="37">
+        <v>10</v>
+      </c>
+      <c r="C24" s="38" t="s">
+        <v>9</v>
+      </c>
+      <c r="D24" s="39" t="s">
+        <v>33</v>
+      </c>
+      <c r="E24" s="40" t="s">
+        <v>31</v>
+      </c>
+      <c r="F24" s="40"/>
+      <c r="G24" s="39" t="s">
+        <v>32</v>
+      </c>
+      <c r="H24" s="40"/>
+      <c r="I24" s="53" t="s">
+        <v>41</v>
+      </c>
+      <c r="J24" s="27" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="16" spans="2:28" ht="15.75" customHeight="1">
-      <c r="B16" s="38"/>
-      <c r="C16" s="31"/>
-      <c r="D16" s="30"/>
-      <c r="E16" s="30"/>
-      <c r="F16" s="30"/>
-      <c r="G16" s="30"/>
-      <c r="H16" s="30"/>
-      <c r="I16" s="27"/>
-      <c r="J16" s="23"/>
-    </row>
-    <row r="17" spans="2:10" ht="15.75" customHeight="1">
-      <c r="B17" s="38"/>
-      <c r="C17" s="31"/>
-      <c r="D17" s="30"/>
-      <c r="E17" s="30"/>
-      <c r="F17" s="30"/>
-      <c r="G17" s="30"/>
-      <c r="H17" s="30"/>
-      <c r="I17" s="27"/>
-      <c r="J17" s="23"/>
-    </row>
-    <row r="18" spans="2:10" ht="15.75" customHeight="1">
-      <c r="B18" s="39">
-        <v>8</v>
-      </c>
-      <c r="C18" s="29" t="s">
-        <v>9</v>
-      </c>
-      <c r="D18" s="33" t="s">
-        <v>54</v>
-      </c>
-      <c r="E18" s="32" t="s">
-        <v>13</v>
-      </c>
-      <c r="F18" s="32"/>
-      <c r="G18" s="33" t="s">
-        <v>55</v>
-      </c>
-      <c r="H18" s="32"/>
-      <c r="I18" s="26">
-        <v>7</v>
-      </c>
-      <c r="J18" s="23" t="s">
+    <row r="25" spans="2:10" ht="15.75" customHeight="1">
+      <c r="B25" s="37"/>
+      <c r="C25" s="38"/>
+      <c r="D25" s="40"/>
+      <c r="E25" s="40"/>
+      <c r="F25" s="40"/>
+      <c r="G25" s="39"/>
+      <c r="H25" s="40"/>
+      <c r="I25" s="53"/>
+      <c r="J25" s="27"/>
+    </row>
+    <row r="26" spans="2:10" ht="15.75" customHeight="1">
+      <c r="B26" s="37"/>
+      <c r="C26" s="38"/>
+      <c r="D26" s="40"/>
+      <c r="E26" s="40"/>
+      <c r="F26" s="40"/>
+      <c r="G26" s="39"/>
+      <c r="H26" s="40"/>
+      <c r="I26" s="53"/>
+      <c r="J26" s="27"/>
+    </row>
+    <row r="27" spans="2:10" ht="15.75" customHeight="1">
+      <c r="B27" s="31">
+        <v>11</v>
+      </c>
+      <c r="C27" s="29" t="s">
+        <v>10</v>
+      </c>
+      <c r="D27" s="41" t="s">
+        <v>45</v>
+      </c>
+      <c r="E27" s="43" t="s">
+        <v>46</v>
+      </c>
+      <c r="F27" s="33"/>
+      <c r="G27" s="41" t="s">
+        <v>34</v>
+      </c>
+      <c r="H27" s="33"/>
+      <c r="I27" s="35" t="s">
+        <v>41</v>
+      </c>
+      <c r="J27" s="26" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="19" spans="2:10" ht="15.75" customHeight="1">
-      <c r="B19" s="39"/>
-      <c r="C19" s="29"/>
-      <c r="D19" s="32"/>
-      <c r="E19" s="32"/>
-      <c r="F19" s="32"/>
-      <c r="G19" s="32"/>
-      <c r="H19" s="32"/>
-      <c r="I19" s="26"/>
-      <c r="J19" s="23"/>
-    </row>
-    <row r="20" spans="2:10" ht="15.75" customHeight="1">
-      <c r="B20" s="39"/>
-      <c r="C20" s="29"/>
-      <c r="D20" s="32"/>
-      <c r="E20" s="32"/>
-      <c r="F20" s="32"/>
-      <c r="G20" s="32"/>
-      <c r="H20" s="32"/>
-      <c r="I20" s="26"/>
-      <c r="J20" s="23"/>
-    </row>
-    <row r="21" spans="2:10" ht="15.75" customHeight="1">
-      <c r="B21" s="38">
-        <v>9</v>
-      </c>
-      <c r="C21" s="35" t="s">
-        <v>9</v>
-      </c>
-      <c r="D21" s="43" t="s">
-        <v>38</v>
-      </c>
-      <c r="E21" s="43" t="s">
-        <v>30</v>
-      </c>
-      <c r="F21" s="41"/>
-      <c r="G21" s="41" t="s">
-        <v>29</v>
-      </c>
-      <c r="H21" s="41"/>
-      <c r="I21" s="27">
-        <v>3</v>
-      </c>
-      <c r="J21" s="24" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="22" spans="2:10" ht="15.75" customHeight="1">
-      <c r="B22" s="38"/>
-      <c r="C22" s="35"/>
-      <c r="D22" s="43"/>
-      <c r="E22" s="41"/>
-      <c r="F22" s="41"/>
-      <c r="G22" s="41"/>
-      <c r="H22" s="41"/>
-      <c r="I22" s="27"/>
-      <c r="J22" s="24"/>
-    </row>
-    <row r="23" spans="2:10" ht="15.75" customHeight="1">
-      <c r="B23" s="38"/>
-      <c r="C23" s="35"/>
-      <c r="D23" s="43"/>
-      <c r="E23" s="41"/>
-      <c r="F23" s="41"/>
-      <c r="G23" s="41"/>
-      <c r="H23" s="41"/>
-      <c r="I23" s="27"/>
-      <c r="J23" s="24"/>
-    </row>
-    <row r="24" spans="2:10" ht="15.75" customHeight="1">
-      <c r="B24" s="39">
-        <v>10</v>
-      </c>
-      <c r="C24" s="29" t="s">
-        <v>9</v>
-      </c>
-      <c r="D24" s="33" t="s">
-        <v>33</v>
-      </c>
-      <c r="E24" s="32" t="s">
-        <v>31</v>
-      </c>
-      <c r="F24" s="32"/>
-      <c r="G24" s="33" t="s">
-        <v>32</v>
-      </c>
-      <c r="H24" s="32"/>
-      <c r="I24" s="26" t="s">
-        <v>41</v>
-      </c>
-      <c r="J24" s="23" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="25" spans="2:10" ht="15.75" customHeight="1">
-      <c r="B25" s="39"/>
-      <c r="C25" s="29"/>
-      <c r="D25" s="32"/>
-      <c r="E25" s="32"/>
-      <c r="F25" s="32"/>
-      <c r="G25" s="33"/>
-      <c r="H25" s="32"/>
-      <c r="I25" s="26"/>
-      <c r="J25" s="23"/>
-    </row>
-    <row r="26" spans="2:10" ht="15.75" customHeight="1">
-      <c r="B26" s="39"/>
-      <c r="C26" s="29"/>
-      <c r="D26" s="32"/>
-      <c r="E26" s="32"/>
-      <c r="F26" s="32"/>
-      <c r="G26" s="33"/>
-      <c r="H26" s="32"/>
-      <c r="I26" s="26"/>
-      <c r="J26" s="23"/>
-    </row>
-    <row r="27" spans="2:10" ht="15.75" customHeight="1">
-      <c r="B27" s="38">
-        <v>11</v>
-      </c>
-      <c r="C27" s="35" t="s">
-        <v>10</v>
-      </c>
-      <c r="D27" s="43" t="s">
-        <v>45</v>
-      </c>
-      <c r="E27" s="36" t="s">
-        <v>46</v>
-      </c>
-      <c r="F27" s="41"/>
-      <c r="G27" s="43" t="s">
-        <v>34</v>
-      </c>
-      <c r="H27" s="41"/>
-      <c r="I27" s="27" t="s">
-        <v>41</v>
-      </c>
-      <c r="J27" s="51" t="s">
-        <v>44</v>
-      </c>
-    </row>
     <row r="28" spans="2:10" ht="15.75" customHeight="1">
-      <c r="B28" s="38"/>
-      <c r="C28" s="35"/>
-      <c r="D28" s="43"/>
-      <c r="E28" s="36"/>
-      <c r="F28" s="41"/>
-      <c r="G28" s="43"/>
-      <c r="H28" s="41"/>
-      <c r="I28" s="27"/>
-      <c r="J28" s="23"/>
+      <c r="B28" s="31"/>
+      <c r="C28" s="29"/>
+      <c r="D28" s="41"/>
+      <c r="E28" s="43"/>
+      <c r="F28" s="33"/>
+      <c r="G28" s="41"/>
+      <c r="H28" s="33"/>
+      <c r="I28" s="35"/>
+      <c r="J28" s="27"/>
     </row>
     <row r="29" spans="2:10" ht="15.75" customHeight="1">
-      <c r="B29" s="38"/>
-      <c r="C29" s="35"/>
-      <c r="D29" s="43"/>
-      <c r="E29" s="36"/>
-      <c r="F29" s="41"/>
-      <c r="G29" s="43"/>
-      <c r="H29" s="41"/>
-      <c r="I29" s="27"/>
-      <c r="J29" s="23"/>
+      <c r="B29" s="31"/>
+      <c r="C29" s="29"/>
+      <c r="D29" s="41"/>
+      <c r="E29" s="43"/>
+      <c r="F29" s="33"/>
+      <c r="G29" s="41"/>
+      <c r="H29" s="33"/>
+      <c r="I29" s="35"/>
+      <c r="J29" s="27"/>
     </row>
     <row r="30" spans="2:10" ht="15.75" customHeight="1">
-      <c r="B30" s="38"/>
-      <c r="C30" s="35"/>
-      <c r="D30" s="43"/>
-      <c r="E30" s="36"/>
-      <c r="F30" s="41"/>
-      <c r="G30" s="43"/>
-      <c r="H30" s="41"/>
-      <c r="I30" s="27"/>
-      <c r="J30" s="23"/>
+      <c r="B30" s="31"/>
+      <c r="C30" s="29"/>
+      <c r="D30" s="41"/>
+      <c r="E30" s="43"/>
+      <c r="F30" s="33"/>
+      <c r="G30" s="41"/>
+      <c r="H30" s="33"/>
+      <c r="I30" s="35"/>
+      <c r="J30" s="27"/>
     </row>
     <row r="31" spans="2:10" ht="15.75" customHeight="1">
-      <c r="B31" s="38"/>
-      <c r="C31" s="35"/>
-      <c r="D31" s="43"/>
-      <c r="E31" s="36"/>
-      <c r="F31" s="41"/>
-      <c r="G31" s="43"/>
-      <c r="H31" s="41"/>
-      <c r="I31" s="27"/>
-      <c r="J31" s="23"/>
+      <c r="B31" s="31"/>
+      <c r="C31" s="29"/>
+      <c r="D31" s="41"/>
+      <c r="E31" s="43"/>
+      <c r="F31" s="33"/>
+      <c r="G31" s="41"/>
+      <c r="H31" s="33"/>
+      <c r="I31" s="35"/>
+      <c r="J31" s="27"/>
     </row>
     <row r="32" spans="2:10" ht="15.75" customHeight="1">
-      <c r="B32" s="54"/>
-      <c r="C32" s="53"/>
-      <c r="D32" s="45"/>
-      <c r="E32" s="47"/>
-      <c r="F32" s="46"/>
-      <c r="G32" s="45"/>
-      <c r="H32" s="46"/>
-      <c r="I32" s="55"/>
-      <c r="J32" s="52"/>
+      <c r="B32" s="32"/>
+      <c r="C32" s="30"/>
+      <c r="D32" s="42"/>
+      <c r="E32" s="44"/>
+      <c r="F32" s="34"/>
+      <c r="G32" s="42"/>
+      <c r="H32" s="34"/>
+      <c r="I32" s="36"/>
+      <c r="J32" s="28"/>
     </row>
     <row r="33" spans="2:10" ht="63" customHeight="1">
       <c r="B33" s="17">
@@ -1710,17 +1710,17 @@
     </row>
     <row r="35" spans="2:10" ht="15.75" customHeight="1" thickBot="1"/>
     <row r="36" spans="2:10" ht="15.75" customHeight="1" thickBot="1">
-      <c r="B36" s="48" t="s">
+      <c r="B36" s="23" t="s">
         <v>53</v>
       </c>
-      <c r="C36" s="49"/>
-      <c r="D36" s="49"/>
-      <c r="E36" s="49"/>
-      <c r="F36" s="49"/>
-      <c r="G36" s="49"/>
-      <c r="H36" s="49"/>
-      <c r="I36" s="49"/>
-      <c r="J36" s="50"/>
+      <c r="C36" s="24"/>
+      <c r="D36" s="24"/>
+      <c r="E36" s="24"/>
+      <c r="F36" s="24"/>
+      <c r="G36" s="24"/>
+      <c r="H36" s="24"/>
+      <c r="I36" s="24"/>
+      <c r="J36" s="25"/>
     </row>
     <row r="37" spans="2:10" ht="15.75" customHeight="1"/>
     <row r="38" spans="2:10" ht="15.75" customHeight="1"/>
@@ -2681,40 +2681,56 @@
   </sheetData>
   <autoFilter ref="B2:J34"/>
   <mergeCells count="100">
-    <mergeCell ref="B36:J36"/>
-    <mergeCell ref="J27:J32"/>
-    <mergeCell ref="C27:C32"/>
-    <mergeCell ref="B27:B32"/>
-    <mergeCell ref="H27:H32"/>
-    <mergeCell ref="I27:I32"/>
-    <mergeCell ref="B24:B26"/>
-    <mergeCell ref="C24:C26"/>
-    <mergeCell ref="D24:D26"/>
-    <mergeCell ref="E24:E26"/>
-    <mergeCell ref="F24:F26"/>
-    <mergeCell ref="H24:H26"/>
-    <mergeCell ref="G27:G32"/>
-    <mergeCell ref="F27:F32"/>
-    <mergeCell ref="E27:E32"/>
-    <mergeCell ref="D27:D32"/>
-    <mergeCell ref="G24:G26"/>
-    <mergeCell ref="F3:F4"/>
-    <mergeCell ref="F5:F6"/>
-    <mergeCell ref="F7:F8"/>
-    <mergeCell ref="F9:F10"/>
-    <mergeCell ref="F11:F12"/>
-    <mergeCell ref="F21:F23"/>
-    <mergeCell ref="B21:B23"/>
-    <mergeCell ref="C21:C23"/>
-    <mergeCell ref="G21:G23"/>
-    <mergeCell ref="H21:H23"/>
-    <mergeCell ref="D21:D23"/>
-    <mergeCell ref="E21:E23"/>
-    <mergeCell ref="E5:E6"/>
-    <mergeCell ref="E7:E8"/>
-    <mergeCell ref="E9:E10"/>
-    <mergeCell ref="E11:E12"/>
-    <mergeCell ref="E13:E14"/>
+    <mergeCell ref="J13:J14"/>
+    <mergeCell ref="J15:J17"/>
+    <mergeCell ref="J18:J20"/>
+    <mergeCell ref="J21:J23"/>
+    <mergeCell ref="J24:J26"/>
+    <mergeCell ref="J3:J4"/>
+    <mergeCell ref="J5:J6"/>
+    <mergeCell ref="J7:J8"/>
+    <mergeCell ref="J9:J10"/>
+    <mergeCell ref="J11:J12"/>
+    <mergeCell ref="I13:I14"/>
+    <mergeCell ref="I15:I17"/>
+    <mergeCell ref="I18:I20"/>
+    <mergeCell ref="I21:I23"/>
+    <mergeCell ref="I24:I26"/>
+    <mergeCell ref="I3:I4"/>
+    <mergeCell ref="I5:I6"/>
+    <mergeCell ref="I7:I8"/>
+    <mergeCell ref="I9:I10"/>
+    <mergeCell ref="I11:I12"/>
+    <mergeCell ref="C9:C10"/>
+    <mergeCell ref="D11:D12"/>
+    <mergeCell ref="C11:C12"/>
+    <mergeCell ref="D13:D14"/>
+    <mergeCell ref="C13:C14"/>
+    <mergeCell ref="D9:D10"/>
+    <mergeCell ref="C3:C4"/>
+    <mergeCell ref="D3:D4"/>
+    <mergeCell ref="C5:C6"/>
+    <mergeCell ref="D5:D6"/>
+    <mergeCell ref="C7:C8"/>
+    <mergeCell ref="D7:D8"/>
+    <mergeCell ref="B3:B4"/>
+    <mergeCell ref="B5:B6"/>
+    <mergeCell ref="B7:B8"/>
+    <mergeCell ref="B9:B10"/>
+    <mergeCell ref="B11:B12"/>
+    <mergeCell ref="B13:B14"/>
+    <mergeCell ref="B15:B17"/>
+    <mergeCell ref="G18:G20"/>
+    <mergeCell ref="E18:E20"/>
+    <mergeCell ref="C18:C20"/>
+    <mergeCell ref="B18:B20"/>
+    <mergeCell ref="F18:F20"/>
+    <mergeCell ref="E15:E17"/>
+    <mergeCell ref="D15:D17"/>
+    <mergeCell ref="D18:D20"/>
+    <mergeCell ref="F13:F14"/>
+    <mergeCell ref="C15:C17"/>
+    <mergeCell ref="F15:F17"/>
     <mergeCell ref="H18:H20"/>
     <mergeCell ref="E3:E4"/>
     <mergeCell ref="G3:G4"/>
@@ -2731,56 +2747,40 @@
     <mergeCell ref="G11:G12"/>
     <mergeCell ref="G13:G14"/>
     <mergeCell ref="G15:G17"/>
-    <mergeCell ref="B13:B14"/>
-    <mergeCell ref="B15:B17"/>
-    <mergeCell ref="G18:G20"/>
-    <mergeCell ref="E18:E20"/>
-    <mergeCell ref="C18:C20"/>
-    <mergeCell ref="B18:B20"/>
-    <mergeCell ref="F18:F20"/>
-    <mergeCell ref="E15:E17"/>
-    <mergeCell ref="D15:D17"/>
-    <mergeCell ref="D18:D20"/>
-    <mergeCell ref="F13:F14"/>
-    <mergeCell ref="C15:C17"/>
-    <mergeCell ref="F15:F17"/>
-    <mergeCell ref="B3:B4"/>
-    <mergeCell ref="B5:B6"/>
-    <mergeCell ref="B7:B8"/>
-    <mergeCell ref="B9:B10"/>
-    <mergeCell ref="B11:B12"/>
-    <mergeCell ref="C3:C4"/>
-    <mergeCell ref="D3:D4"/>
-    <mergeCell ref="C5:C6"/>
-    <mergeCell ref="D5:D6"/>
-    <mergeCell ref="C7:C8"/>
-    <mergeCell ref="D7:D8"/>
-    <mergeCell ref="C9:C10"/>
-    <mergeCell ref="D11:D12"/>
-    <mergeCell ref="C11:C12"/>
-    <mergeCell ref="D13:D14"/>
-    <mergeCell ref="C13:C14"/>
-    <mergeCell ref="D9:D10"/>
-    <mergeCell ref="I3:I4"/>
-    <mergeCell ref="I5:I6"/>
-    <mergeCell ref="I7:I8"/>
-    <mergeCell ref="I9:I10"/>
-    <mergeCell ref="I11:I12"/>
-    <mergeCell ref="I13:I14"/>
-    <mergeCell ref="I15:I17"/>
-    <mergeCell ref="I18:I20"/>
-    <mergeCell ref="I21:I23"/>
-    <mergeCell ref="I24:I26"/>
-    <mergeCell ref="J3:J4"/>
-    <mergeCell ref="J5:J6"/>
-    <mergeCell ref="J7:J8"/>
-    <mergeCell ref="J9:J10"/>
-    <mergeCell ref="J11:J12"/>
-    <mergeCell ref="J13:J14"/>
-    <mergeCell ref="J15:J17"/>
-    <mergeCell ref="J18:J20"/>
-    <mergeCell ref="J21:J23"/>
-    <mergeCell ref="J24:J26"/>
+    <mergeCell ref="E5:E6"/>
+    <mergeCell ref="E7:E8"/>
+    <mergeCell ref="E9:E10"/>
+    <mergeCell ref="E11:E12"/>
+    <mergeCell ref="E13:E14"/>
+    <mergeCell ref="F21:F23"/>
+    <mergeCell ref="B21:B23"/>
+    <mergeCell ref="C21:C23"/>
+    <mergeCell ref="G21:G23"/>
+    <mergeCell ref="H21:H23"/>
+    <mergeCell ref="D21:D23"/>
+    <mergeCell ref="E21:E23"/>
+    <mergeCell ref="F3:F4"/>
+    <mergeCell ref="F5:F6"/>
+    <mergeCell ref="F7:F8"/>
+    <mergeCell ref="F9:F10"/>
+    <mergeCell ref="F11:F12"/>
+    <mergeCell ref="H24:H26"/>
+    <mergeCell ref="G27:G32"/>
+    <mergeCell ref="F27:F32"/>
+    <mergeCell ref="E27:E32"/>
+    <mergeCell ref="D27:D32"/>
+    <mergeCell ref="G24:G26"/>
+    <mergeCell ref="B24:B26"/>
+    <mergeCell ref="C24:C26"/>
+    <mergeCell ref="D24:D26"/>
+    <mergeCell ref="E24:E26"/>
+    <mergeCell ref="F24:F26"/>
+    <mergeCell ref="B36:J36"/>
+    <mergeCell ref="J27:J32"/>
+    <mergeCell ref="C27:C32"/>
+    <mergeCell ref="B27:B32"/>
+    <mergeCell ref="H27:H32"/>
+    <mergeCell ref="I27:I32"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape" r:id="rId1"/>

</xml_diff>

<commit_message>
Analyses des performances apres 8eme correction
</commit_message>
<xml_diff>
--- a/Analyses/Modèle-audit-SEO.xlsx
+++ b/Analyses/Modèle-audit-SEO.xlsx
@@ -792,6 +792,81 @@
     <xf numFmtId="0" fontId="7" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="8" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -804,91 +879,16 @@
     <xf numFmtId="0" fontId="7" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="6" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1107,7 +1107,7 @@
   <dimension ref="B1:AB992"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="I15" sqref="I15:I17"/>
+      <selection activeCell="J15" sqref="J15:J17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.33203125" defaultRowHeight="15" customHeight="1"/>
@@ -1173,490 +1173,490 @@
       <c r="AB2" s="1"/>
     </row>
     <row r="3" spans="2:28" ht="15.75" customHeight="1">
-      <c r="B3" s="50">
+      <c r="B3" s="37">
         <v>1</v>
       </c>
-      <c r="C3" s="51" t="s">
+      <c r="C3" s="34" t="s">
         <v>40</v>
       </c>
-      <c r="D3" s="51" t="s">
+      <c r="D3" s="34" t="s">
         <v>7</v>
       </c>
-      <c r="E3" s="45" t="s">
+      <c r="E3" s="40" t="s">
         <v>15</v>
       </c>
-      <c r="F3" s="45" t="s">
+      <c r="F3" s="40" t="s">
         <v>39</v>
       </c>
-      <c r="G3" s="45" t="s">
+      <c r="G3" s="40" t="s">
         <v>16</v>
       </c>
-      <c r="H3" s="48"/>
-      <c r="I3" s="52">
+      <c r="H3" s="42"/>
+      <c r="I3" s="28">
         <v>1</v>
       </c>
-      <c r="J3" s="54" t="s">
+      <c r="J3" s="25" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="4" spans="2:28" ht="15.75" customHeight="1">
-      <c r="B4" s="31"/>
-      <c r="C4" s="29"/>
-      <c r="D4" s="29"/>
-      <c r="E4" s="33"/>
-      <c r="F4" s="33"/>
-      <c r="G4" s="33"/>
-      <c r="H4" s="33"/>
-      <c r="I4" s="35"/>
-      <c r="J4" s="55"/>
+      <c r="B4" s="38"/>
+      <c r="C4" s="35"/>
+      <c r="D4" s="35"/>
+      <c r="E4" s="41"/>
+      <c r="F4" s="41"/>
+      <c r="G4" s="41"/>
+      <c r="H4" s="41"/>
+      <c r="I4" s="27"/>
+      <c r="J4" s="24"/>
     </row>
     <row r="5" spans="2:28" ht="15.75" customHeight="1">
-      <c r="B5" s="37">
+      <c r="B5" s="39">
         <v>2</v>
       </c>
-      <c r="C5" s="38" t="s">
+      <c r="C5" s="29" t="s">
         <v>40</v>
       </c>
-      <c r="D5" s="40" t="s">
+      <c r="D5" s="32" t="s">
         <v>8</v>
       </c>
-      <c r="E5" s="39" t="s">
+      <c r="E5" s="33" t="s">
         <v>15</v>
       </c>
-      <c r="F5" s="46"/>
-      <c r="G5" s="39" t="s">
+      <c r="F5" s="44"/>
+      <c r="G5" s="33" t="s">
         <v>17</v>
       </c>
-      <c r="H5" s="40"/>
-      <c r="I5" s="53">
+      <c r="H5" s="32"/>
+      <c r="I5" s="26">
         <v>2</v>
       </c>
-      <c r="J5" s="55" t="s">
+      <c r="J5" s="24" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="6" spans="2:28" ht="15.75" customHeight="1">
-      <c r="B6" s="37"/>
-      <c r="C6" s="38"/>
-      <c r="D6" s="40"/>
-      <c r="E6" s="40"/>
-      <c r="F6" s="46"/>
-      <c r="G6" s="40"/>
-      <c r="H6" s="40"/>
-      <c r="I6" s="53"/>
-      <c r="J6" s="55"/>
+      <c r="B6" s="39"/>
+      <c r="C6" s="29"/>
+      <c r="D6" s="32"/>
+      <c r="E6" s="32"/>
+      <c r="F6" s="44"/>
+      <c r="G6" s="32"/>
+      <c r="H6" s="32"/>
+      <c r="I6" s="26"/>
+      <c r="J6" s="24"/>
     </row>
     <row r="7" spans="2:28" ht="15.75" customHeight="1">
-      <c r="B7" s="31">
+      <c r="B7" s="38">
         <v>3</v>
       </c>
-      <c r="C7" s="49" t="s">
+      <c r="C7" s="31" t="s">
         <v>6</v>
       </c>
-      <c r="D7" s="43" t="s">
+      <c r="D7" s="36" t="s">
         <v>26</v>
       </c>
-      <c r="E7" s="43" t="s">
+      <c r="E7" s="36" t="s">
         <v>23</v>
       </c>
-      <c r="F7" s="47"/>
-      <c r="G7" s="43" t="s">
+      <c r="F7" s="30"/>
+      <c r="G7" s="36" t="s">
         <v>18</v>
       </c>
-      <c r="H7" s="47"/>
-      <c r="I7" s="35">
+      <c r="H7" s="30"/>
+      <c r="I7" s="27">
         <v>10</v>
       </c>
-      <c r="J7" s="27" t="s">
+      <c r="J7" s="23" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="8" spans="2:28" ht="15.75" customHeight="1">
-      <c r="B8" s="31"/>
-      <c r="C8" s="49"/>
-      <c r="D8" s="47"/>
-      <c r="E8" s="47"/>
-      <c r="F8" s="47"/>
-      <c r="G8" s="47"/>
-      <c r="H8" s="47"/>
-      <c r="I8" s="35"/>
-      <c r="J8" s="27"/>
+      <c r="B8" s="38"/>
+      <c r="C8" s="31"/>
+      <c r="D8" s="30"/>
+      <c r="E8" s="30"/>
+      <c r="F8" s="30"/>
+      <c r="G8" s="30"/>
+      <c r="H8" s="30"/>
+      <c r="I8" s="27"/>
+      <c r="J8" s="23"/>
     </row>
     <row r="9" spans="2:28" ht="15.75" customHeight="1">
-      <c r="B9" s="37">
+      <c r="B9" s="39">
         <v>4</v>
       </c>
-      <c r="C9" s="38" t="s">
+      <c r="C9" s="29" t="s">
         <v>6</v>
       </c>
-      <c r="D9" s="39" t="s">
+      <c r="D9" s="33" t="s">
         <v>27</v>
       </c>
-      <c r="E9" s="39" t="s">
+      <c r="E9" s="33" t="s">
         <v>24</v>
       </c>
-      <c r="F9" s="40"/>
-      <c r="G9" s="39" t="s">
+      <c r="F9" s="32"/>
+      <c r="G9" s="33" t="s">
         <v>19</v>
       </c>
-      <c r="H9" s="40"/>
-      <c r="I9" s="53">
+      <c r="H9" s="32"/>
+      <c r="I9" s="26">
         <v>4</v>
       </c>
-      <c r="J9" s="55" t="s">
+      <c r="J9" s="24" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="10" spans="2:28" ht="15.75" customHeight="1">
-      <c r="B10" s="37"/>
-      <c r="C10" s="38"/>
-      <c r="D10" s="40"/>
-      <c r="E10" s="40"/>
-      <c r="F10" s="40"/>
-      <c r="G10" s="40"/>
-      <c r="H10" s="40"/>
-      <c r="I10" s="53"/>
-      <c r="J10" s="55"/>
+      <c r="B10" s="39"/>
+      <c r="C10" s="29"/>
+      <c r="D10" s="32"/>
+      <c r="E10" s="32"/>
+      <c r="F10" s="32"/>
+      <c r="G10" s="32"/>
+      <c r="H10" s="32"/>
+      <c r="I10" s="26"/>
+      <c r="J10" s="24"/>
     </row>
     <row r="11" spans="2:28" ht="15.75" customHeight="1">
-      <c r="B11" s="31">
+      <c r="B11" s="38">
         <v>5</v>
       </c>
-      <c r="C11" s="49" t="s">
+      <c r="C11" s="31" t="s">
         <v>10</v>
       </c>
-      <c r="D11" s="47" t="s">
+      <c r="D11" s="30" t="s">
         <v>11</v>
       </c>
-      <c r="E11" s="43" t="s">
+      <c r="E11" s="36" t="s">
         <v>37</v>
       </c>
-      <c r="F11" s="47"/>
-      <c r="G11" s="43" t="s">
+      <c r="F11" s="30"/>
+      <c r="G11" s="36" t="s">
         <v>20</v>
       </c>
-      <c r="H11" s="47"/>
-      <c r="I11" s="35">
+      <c r="H11" s="30"/>
+      <c r="I11" s="27">
         <v>5</v>
       </c>
-      <c r="J11" s="55" t="s">
+      <c r="J11" s="24" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="12" spans="2:28" ht="15.75" customHeight="1">
-      <c r="B12" s="31"/>
-      <c r="C12" s="49"/>
-      <c r="D12" s="47"/>
-      <c r="E12" s="47"/>
-      <c r="F12" s="47"/>
-      <c r="G12" s="47"/>
-      <c r="H12" s="47"/>
-      <c r="I12" s="35"/>
-      <c r="J12" s="55"/>
+      <c r="B12" s="38"/>
+      <c r="C12" s="31"/>
+      <c r="D12" s="30"/>
+      <c r="E12" s="30"/>
+      <c r="F12" s="30"/>
+      <c r="G12" s="30"/>
+      <c r="H12" s="30"/>
+      <c r="I12" s="27"/>
+      <c r="J12" s="24"/>
     </row>
     <row r="13" spans="2:28" ht="15.75" customHeight="1">
-      <c r="B13" s="37">
+      <c r="B13" s="39">
         <v>6</v>
       </c>
-      <c r="C13" s="38" t="s">
+      <c r="C13" s="29" t="s">
         <v>6</v>
       </c>
-      <c r="D13" s="40" t="s">
+      <c r="D13" s="32" t="s">
         <v>12</v>
       </c>
-      <c r="E13" s="39" t="s">
+      <c r="E13" s="33" t="s">
         <v>35</v>
       </c>
-      <c r="F13" s="40"/>
-      <c r="G13" s="39" t="s">
+      <c r="F13" s="32"/>
+      <c r="G13" s="33" t="s">
         <v>21</v>
       </c>
-      <c r="H13" s="40"/>
-      <c r="I13" s="53">
+      <c r="H13" s="32"/>
+      <c r="I13" s="26">
         <v>9</v>
       </c>
-      <c r="J13" s="27" t="s">
+      <c r="J13" s="23" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="14" spans="2:28" ht="15.75" customHeight="1">
-      <c r="B14" s="37"/>
-      <c r="C14" s="38"/>
-      <c r="D14" s="40"/>
-      <c r="E14" s="40"/>
-      <c r="F14" s="40"/>
-      <c r="G14" s="40"/>
-      <c r="H14" s="40"/>
-      <c r="I14" s="53"/>
-      <c r="J14" s="27"/>
+      <c r="B14" s="39"/>
+      <c r="C14" s="29"/>
+      <c r="D14" s="32"/>
+      <c r="E14" s="32"/>
+      <c r="F14" s="32"/>
+      <c r="G14" s="32"/>
+      <c r="H14" s="32"/>
+      <c r="I14" s="26"/>
+      <c r="J14" s="23"/>
     </row>
     <row r="15" spans="2:28" ht="15.75" customHeight="1">
-      <c r="B15" s="31">
+      <c r="B15" s="38">
         <v>7</v>
       </c>
-      <c r="C15" s="49" t="s">
+      <c r="C15" s="31" t="s">
         <v>6</v>
       </c>
-      <c r="D15" s="43" t="s">
+      <c r="D15" s="36" t="s">
         <v>28</v>
       </c>
-      <c r="E15" s="43" t="s">
+      <c r="E15" s="36" t="s">
         <v>25</v>
       </c>
-      <c r="F15" s="47"/>
-      <c r="G15" s="43" t="s">
+      <c r="F15" s="30"/>
+      <c r="G15" s="36" t="s">
         <v>22</v>
       </c>
-      <c r="H15" s="47"/>
-      <c r="I15" s="35">
+      <c r="H15" s="30"/>
+      <c r="I15" s="27">
         <v>8</v>
       </c>
-      <c r="J15" s="27" t="s">
+      <c r="J15" s="24" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="16" spans="2:28" ht="15.75" customHeight="1">
+      <c r="B16" s="38"/>
+      <c r="C16" s="31"/>
+      <c r="D16" s="30"/>
+      <c r="E16" s="30"/>
+      <c r="F16" s="30"/>
+      <c r="G16" s="30"/>
+      <c r="H16" s="30"/>
+      <c r="I16" s="27"/>
+      <c r="J16" s="24"/>
+    </row>
+    <row r="17" spans="2:10" ht="15.75" customHeight="1">
+      <c r="B17" s="38"/>
+      <c r="C17" s="31"/>
+      <c r="D17" s="30"/>
+      <c r="E17" s="30"/>
+      <c r="F17" s="30"/>
+      <c r="G17" s="30"/>
+      <c r="H17" s="30"/>
+      <c r="I17" s="27"/>
+      <c r="J17" s="24"/>
+    </row>
+    <row r="18" spans="2:10" ht="15.75" customHeight="1">
+      <c r="B18" s="39">
+        <v>8</v>
+      </c>
+      <c r="C18" s="29" t="s">
+        <v>9</v>
+      </c>
+      <c r="D18" s="33" t="s">
+        <v>54</v>
+      </c>
+      <c r="E18" s="32" t="s">
+        <v>13</v>
+      </c>
+      <c r="F18" s="32"/>
+      <c r="G18" s="33" t="s">
+        <v>55</v>
+      </c>
+      <c r="H18" s="32"/>
+      <c r="I18" s="26">
+        <v>7</v>
+      </c>
+      <c r="J18" s="24" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="19" spans="2:10" ht="15.75" customHeight="1">
+      <c r="B19" s="39"/>
+      <c r="C19" s="29"/>
+      <c r="D19" s="32"/>
+      <c r="E19" s="32"/>
+      <c r="F19" s="32"/>
+      <c r="G19" s="32"/>
+      <c r="H19" s="32"/>
+      <c r="I19" s="26"/>
+      <c r="J19" s="24"/>
+    </row>
+    <row r="20" spans="2:10" ht="15.75" customHeight="1">
+      <c r="B20" s="39"/>
+      <c r="C20" s="29"/>
+      <c r="D20" s="32"/>
+      <c r="E20" s="32"/>
+      <c r="F20" s="32"/>
+      <c r="G20" s="32"/>
+      <c r="H20" s="32"/>
+      <c r="I20" s="26"/>
+      <c r="J20" s="24"/>
+    </row>
+    <row r="21" spans="2:10" ht="15.75" customHeight="1">
+      <c r="B21" s="38">
+        <v>9</v>
+      </c>
+      <c r="C21" s="35" t="s">
+        <v>9</v>
+      </c>
+      <c r="D21" s="43" t="s">
+        <v>38</v>
+      </c>
+      <c r="E21" s="43" t="s">
+        <v>30</v>
+      </c>
+      <c r="F21" s="41"/>
+      <c r="G21" s="41" t="s">
+        <v>29</v>
+      </c>
+      <c r="H21" s="41"/>
+      <c r="I21" s="27">
+        <v>3</v>
+      </c>
+      <c r="J21" s="24" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="22" spans="2:10" ht="15.75" customHeight="1">
+      <c r="B22" s="38"/>
+      <c r="C22" s="35"/>
+      <c r="D22" s="43"/>
+      <c r="E22" s="41"/>
+      <c r="F22" s="41"/>
+      <c r="G22" s="41"/>
+      <c r="H22" s="41"/>
+      <c r="I22" s="27"/>
+      <c r="J22" s="24"/>
+    </row>
+    <row r="23" spans="2:10" ht="15.75" customHeight="1">
+      <c r="B23" s="38"/>
+      <c r="C23" s="35"/>
+      <c r="D23" s="43"/>
+      <c r="E23" s="41"/>
+      <c r="F23" s="41"/>
+      <c r="G23" s="41"/>
+      <c r="H23" s="41"/>
+      <c r="I23" s="27"/>
+      <c r="J23" s="24"/>
+    </row>
+    <row r="24" spans="2:10" ht="15.75" customHeight="1">
+      <c r="B24" s="39">
+        <v>10</v>
+      </c>
+      <c r="C24" s="29" t="s">
+        <v>9</v>
+      </c>
+      <c r="D24" s="33" t="s">
+        <v>33</v>
+      </c>
+      <c r="E24" s="32" t="s">
+        <v>31</v>
+      </c>
+      <c r="F24" s="32"/>
+      <c r="G24" s="33" t="s">
+        <v>32</v>
+      </c>
+      <c r="H24" s="32"/>
+      <c r="I24" s="26" t="s">
+        <v>41</v>
+      </c>
+      <c r="J24" s="23" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="16" spans="2:28" ht="15.75" customHeight="1">
-      <c r="B16" s="31"/>
-      <c r="C16" s="49"/>
-      <c r="D16" s="47"/>
-      <c r="E16" s="47"/>
-      <c r="F16" s="47"/>
-      <c r="G16" s="47"/>
-      <c r="H16" s="47"/>
-      <c r="I16" s="35"/>
-      <c r="J16" s="27"/>
-    </row>
-    <row r="17" spans="2:10" ht="15.75" customHeight="1">
-      <c r="B17" s="31"/>
-      <c r="C17" s="49"/>
-      <c r="D17" s="47"/>
-      <c r="E17" s="47"/>
-      <c r="F17" s="47"/>
-      <c r="G17" s="47"/>
-      <c r="H17" s="47"/>
-      <c r="I17" s="35"/>
-      <c r="J17" s="27"/>
-    </row>
-    <row r="18" spans="2:10" ht="15.75" customHeight="1">
-      <c r="B18" s="37">
-        <v>8</v>
-      </c>
-      <c r="C18" s="38" t="s">
-        <v>9</v>
-      </c>
-      <c r="D18" s="39" t="s">
-        <v>54</v>
-      </c>
-      <c r="E18" s="40" t="s">
-        <v>13</v>
-      </c>
-      <c r="F18" s="40"/>
-      <c r="G18" s="39" t="s">
-        <v>55</v>
-      </c>
-      <c r="H18" s="40"/>
-      <c r="I18" s="53">
-        <v>7</v>
-      </c>
-      <c r="J18" s="55" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="19" spans="2:10" ht="15.75" customHeight="1">
-      <c r="B19" s="37"/>
-      <c r="C19" s="38"/>
-      <c r="D19" s="40"/>
-      <c r="E19" s="40"/>
-      <c r="F19" s="40"/>
-      <c r="G19" s="40"/>
-      <c r="H19" s="40"/>
-      <c r="I19" s="53"/>
-      <c r="J19" s="55"/>
-    </row>
-    <row r="20" spans="2:10" ht="15.75" customHeight="1">
-      <c r="B20" s="37"/>
-      <c r="C20" s="38"/>
-      <c r="D20" s="40"/>
-      <c r="E20" s="40"/>
-      <c r="F20" s="40"/>
-      <c r="G20" s="40"/>
-      <c r="H20" s="40"/>
-      <c r="I20" s="53"/>
-      <c r="J20" s="55"/>
-    </row>
-    <row r="21" spans="2:10" ht="15.75" customHeight="1">
-      <c r="B21" s="31">
-        <v>9</v>
-      </c>
-      <c r="C21" s="29" t="s">
-        <v>9</v>
-      </c>
-      <c r="D21" s="41" t="s">
-        <v>38</v>
-      </c>
-      <c r="E21" s="41" t="s">
-        <v>30</v>
-      </c>
-      <c r="F21" s="33"/>
-      <c r="G21" s="33" t="s">
-        <v>29</v>
-      </c>
-      <c r="H21" s="33"/>
-      <c r="I21" s="35">
-        <v>3</v>
-      </c>
-      <c r="J21" s="55" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="22" spans="2:10" ht="15.75" customHeight="1">
-      <c r="B22" s="31"/>
-      <c r="C22" s="29"/>
-      <c r="D22" s="41"/>
-      <c r="E22" s="33"/>
-      <c r="F22" s="33"/>
-      <c r="G22" s="33"/>
-      <c r="H22" s="33"/>
-      <c r="I22" s="35"/>
-      <c r="J22" s="55"/>
-    </row>
-    <row r="23" spans="2:10" ht="15.75" customHeight="1">
-      <c r="B23" s="31"/>
-      <c r="C23" s="29"/>
-      <c r="D23" s="41"/>
-      <c r="E23" s="33"/>
-      <c r="F23" s="33"/>
-      <c r="G23" s="33"/>
-      <c r="H23" s="33"/>
-      <c r="I23" s="35"/>
-      <c r="J23" s="55"/>
-    </row>
-    <row r="24" spans="2:10" ht="15.75" customHeight="1">
-      <c r="B24" s="37">
+    <row r="25" spans="2:10" ht="15.75" customHeight="1">
+      <c r="B25" s="39"/>
+      <c r="C25" s="29"/>
+      <c r="D25" s="32"/>
+      <c r="E25" s="32"/>
+      <c r="F25" s="32"/>
+      <c r="G25" s="33"/>
+      <c r="H25" s="32"/>
+      <c r="I25" s="26"/>
+      <c r="J25" s="23"/>
+    </row>
+    <row r="26" spans="2:10" ht="15.75" customHeight="1">
+      <c r="B26" s="39"/>
+      <c r="C26" s="29"/>
+      <c r="D26" s="32"/>
+      <c r="E26" s="32"/>
+      <c r="F26" s="32"/>
+      <c r="G26" s="33"/>
+      <c r="H26" s="32"/>
+      <c r="I26" s="26"/>
+      <c r="J26" s="23"/>
+    </row>
+    <row r="27" spans="2:10" ht="15.75" customHeight="1">
+      <c r="B27" s="38">
+        <v>11</v>
+      </c>
+      <c r="C27" s="35" t="s">
         <v>10</v>
       </c>
-      <c r="C24" s="38" t="s">
-        <v>9</v>
-      </c>
-      <c r="D24" s="39" t="s">
-        <v>33</v>
-      </c>
-      <c r="E24" s="40" t="s">
-        <v>31</v>
-      </c>
-      <c r="F24" s="40"/>
-      <c r="G24" s="39" t="s">
-        <v>32</v>
-      </c>
-      <c r="H24" s="40"/>
-      <c r="I24" s="53" t="s">
+      <c r="D27" s="43" t="s">
+        <v>45</v>
+      </c>
+      <c r="E27" s="36" t="s">
+        <v>46</v>
+      </c>
+      <c r="F27" s="41"/>
+      <c r="G27" s="43" t="s">
+        <v>34</v>
+      </c>
+      <c r="H27" s="41"/>
+      <c r="I27" s="27" t="s">
         <v>41</v>
       </c>
-      <c r="J24" s="27" t="s">
+      <c r="J27" s="51" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="25" spans="2:10" ht="15.75" customHeight="1">
-      <c r="B25" s="37"/>
-      <c r="C25" s="38"/>
-      <c r="D25" s="40"/>
-      <c r="E25" s="40"/>
-      <c r="F25" s="40"/>
-      <c r="G25" s="39"/>
-      <c r="H25" s="40"/>
-      <c r="I25" s="53"/>
-      <c r="J25" s="27"/>
-    </row>
-    <row r="26" spans="2:10" ht="15.75" customHeight="1">
-      <c r="B26" s="37"/>
-      <c r="C26" s="38"/>
-      <c r="D26" s="40"/>
-      <c r="E26" s="40"/>
-      <c r="F26" s="40"/>
-      <c r="G26" s="39"/>
-      <c r="H26" s="40"/>
-      <c r="I26" s="53"/>
-      <c r="J26" s="27"/>
-    </row>
-    <row r="27" spans="2:10" ht="15.75" customHeight="1">
-      <c r="B27" s="31">
-        <v>11</v>
-      </c>
-      <c r="C27" s="29" t="s">
-        <v>10</v>
-      </c>
-      <c r="D27" s="41" t="s">
-        <v>45</v>
-      </c>
-      <c r="E27" s="43" t="s">
-        <v>46</v>
-      </c>
-      <c r="F27" s="33"/>
-      <c r="G27" s="41" t="s">
-        <v>34</v>
-      </c>
-      <c r="H27" s="33"/>
-      <c r="I27" s="35" t="s">
-        <v>41</v>
-      </c>
-      <c r="J27" s="26" t="s">
-        <v>44</v>
-      </c>
-    </row>
     <row r="28" spans="2:10" ht="15.75" customHeight="1">
-      <c r="B28" s="31"/>
-      <c r="C28" s="29"/>
-      <c r="D28" s="41"/>
-      <c r="E28" s="43"/>
-      <c r="F28" s="33"/>
-      <c r="G28" s="41"/>
-      <c r="H28" s="33"/>
-      <c r="I28" s="35"/>
-      <c r="J28" s="27"/>
+      <c r="B28" s="38"/>
+      <c r="C28" s="35"/>
+      <c r="D28" s="43"/>
+      <c r="E28" s="36"/>
+      <c r="F28" s="41"/>
+      <c r="G28" s="43"/>
+      <c r="H28" s="41"/>
+      <c r="I28" s="27"/>
+      <c r="J28" s="23"/>
     </row>
     <row r="29" spans="2:10" ht="15.75" customHeight="1">
-      <c r="B29" s="31"/>
-      <c r="C29" s="29"/>
-      <c r="D29" s="41"/>
-      <c r="E29" s="43"/>
-      <c r="F29" s="33"/>
-      <c r="G29" s="41"/>
-      <c r="H29" s="33"/>
-      <c r="I29" s="35"/>
-      <c r="J29" s="27"/>
+      <c r="B29" s="38"/>
+      <c r="C29" s="35"/>
+      <c r="D29" s="43"/>
+      <c r="E29" s="36"/>
+      <c r="F29" s="41"/>
+      <c r="G29" s="43"/>
+      <c r="H29" s="41"/>
+      <c r="I29" s="27"/>
+      <c r="J29" s="23"/>
     </row>
     <row r="30" spans="2:10" ht="15.75" customHeight="1">
-      <c r="B30" s="31"/>
-      <c r="C30" s="29"/>
-      <c r="D30" s="41"/>
-      <c r="E30" s="43"/>
-      <c r="F30" s="33"/>
-      <c r="G30" s="41"/>
-      <c r="H30" s="33"/>
-      <c r="I30" s="35"/>
-      <c r="J30" s="27"/>
+      <c r="B30" s="38"/>
+      <c r="C30" s="35"/>
+      <c r="D30" s="43"/>
+      <c r="E30" s="36"/>
+      <c r="F30" s="41"/>
+      <c r="G30" s="43"/>
+      <c r="H30" s="41"/>
+      <c r="I30" s="27"/>
+      <c r="J30" s="23"/>
     </row>
     <row r="31" spans="2:10" ht="15.75" customHeight="1">
-      <c r="B31" s="31"/>
-      <c r="C31" s="29"/>
-      <c r="D31" s="41"/>
-      <c r="E31" s="43"/>
-      <c r="F31" s="33"/>
-      <c r="G31" s="41"/>
-      <c r="H31" s="33"/>
-      <c r="I31" s="35"/>
-      <c r="J31" s="27"/>
+      <c r="B31" s="38"/>
+      <c r="C31" s="35"/>
+      <c r="D31" s="43"/>
+      <c r="E31" s="36"/>
+      <c r="F31" s="41"/>
+      <c r="G31" s="43"/>
+      <c r="H31" s="41"/>
+      <c r="I31" s="27"/>
+      <c r="J31" s="23"/>
     </row>
     <row r="32" spans="2:10" ht="15.75" customHeight="1">
-      <c r="B32" s="32"/>
-      <c r="C32" s="30"/>
-      <c r="D32" s="42"/>
-      <c r="E32" s="44"/>
-      <c r="F32" s="34"/>
-      <c r="G32" s="42"/>
-      <c r="H32" s="34"/>
-      <c r="I32" s="36"/>
-      <c r="J32" s="28"/>
+      <c r="B32" s="54"/>
+      <c r="C32" s="53"/>
+      <c r="D32" s="45"/>
+      <c r="E32" s="47"/>
+      <c r="F32" s="46"/>
+      <c r="G32" s="45"/>
+      <c r="H32" s="46"/>
+      <c r="I32" s="55"/>
+      <c r="J32" s="52"/>
     </row>
     <row r="33" spans="2:10" ht="63" customHeight="1">
       <c r="B33" s="17">
@@ -1710,17 +1710,17 @@
     </row>
     <row r="35" spans="2:10" ht="15.75" customHeight="1" thickBot="1"/>
     <row r="36" spans="2:10" ht="15.75" customHeight="1" thickBot="1">
-      <c r="B36" s="23" t="s">
+      <c r="B36" s="48" t="s">
         <v>53</v>
       </c>
-      <c r="C36" s="24"/>
-      <c r="D36" s="24"/>
-      <c r="E36" s="24"/>
-      <c r="F36" s="24"/>
-      <c r="G36" s="24"/>
-      <c r="H36" s="24"/>
-      <c r="I36" s="24"/>
-      <c r="J36" s="25"/>
+      <c r="C36" s="49"/>
+      <c r="D36" s="49"/>
+      <c r="E36" s="49"/>
+      <c r="F36" s="49"/>
+      <c r="G36" s="49"/>
+      <c r="H36" s="49"/>
+      <c r="I36" s="49"/>
+      <c r="J36" s="50"/>
     </row>
     <row r="37" spans="2:10" ht="15.75" customHeight="1"/>
     <row r="38" spans="2:10" ht="15.75" customHeight="1"/>
@@ -2681,56 +2681,40 @@
   </sheetData>
   <autoFilter ref="B2:J34"/>
   <mergeCells count="100">
-    <mergeCell ref="J13:J14"/>
-    <mergeCell ref="J15:J17"/>
-    <mergeCell ref="J18:J20"/>
-    <mergeCell ref="J21:J23"/>
-    <mergeCell ref="J24:J26"/>
-    <mergeCell ref="J3:J4"/>
-    <mergeCell ref="J5:J6"/>
-    <mergeCell ref="J7:J8"/>
-    <mergeCell ref="J9:J10"/>
-    <mergeCell ref="J11:J12"/>
-    <mergeCell ref="I13:I14"/>
-    <mergeCell ref="I15:I17"/>
-    <mergeCell ref="I18:I20"/>
-    <mergeCell ref="I21:I23"/>
-    <mergeCell ref="I24:I26"/>
-    <mergeCell ref="I3:I4"/>
-    <mergeCell ref="I5:I6"/>
-    <mergeCell ref="I7:I8"/>
-    <mergeCell ref="I9:I10"/>
-    <mergeCell ref="I11:I12"/>
-    <mergeCell ref="C9:C10"/>
-    <mergeCell ref="D11:D12"/>
-    <mergeCell ref="C11:C12"/>
-    <mergeCell ref="D13:D14"/>
-    <mergeCell ref="C13:C14"/>
-    <mergeCell ref="D9:D10"/>
-    <mergeCell ref="C3:C4"/>
-    <mergeCell ref="D3:D4"/>
-    <mergeCell ref="C5:C6"/>
-    <mergeCell ref="D5:D6"/>
-    <mergeCell ref="C7:C8"/>
-    <mergeCell ref="D7:D8"/>
-    <mergeCell ref="B3:B4"/>
-    <mergeCell ref="B5:B6"/>
-    <mergeCell ref="B7:B8"/>
-    <mergeCell ref="B9:B10"/>
-    <mergeCell ref="B11:B12"/>
-    <mergeCell ref="B13:B14"/>
-    <mergeCell ref="B15:B17"/>
-    <mergeCell ref="G18:G20"/>
-    <mergeCell ref="E18:E20"/>
-    <mergeCell ref="C18:C20"/>
-    <mergeCell ref="B18:B20"/>
-    <mergeCell ref="F18:F20"/>
-    <mergeCell ref="E15:E17"/>
-    <mergeCell ref="D15:D17"/>
-    <mergeCell ref="D18:D20"/>
-    <mergeCell ref="F13:F14"/>
-    <mergeCell ref="C15:C17"/>
-    <mergeCell ref="F15:F17"/>
+    <mergeCell ref="B36:J36"/>
+    <mergeCell ref="J27:J32"/>
+    <mergeCell ref="C27:C32"/>
+    <mergeCell ref="B27:B32"/>
+    <mergeCell ref="H27:H32"/>
+    <mergeCell ref="I27:I32"/>
+    <mergeCell ref="B24:B26"/>
+    <mergeCell ref="C24:C26"/>
+    <mergeCell ref="D24:D26"/>
+    <mergeCell ref="E24:E26"/>
+    <mergeCell ref="F24:F26"/>
+    <mergeCell ref="H24:H26"/>
+    <mergeCell ref="G27:G32"/>
+    <mergeCell ref="F27:F32"/>
+    <mergeCell ref="E27:E32"/>
+    <mergeCell ref="D27:D32"/>
+    <mergeCell ref="G24:G26"/>
+    <mergeCell ref="F3:F4"/>
+    <mergeCell ref="F5:F6"/>
+    <mergeCell ref="F7:F8"/>
+    <mergeCell ref="F9:F10"/>
+    <mergeCell ref="F11:F12"/>
+    <mergeCell ref="F21:F23"/>
+    <mergeCell ref="B21:B23"/>
+    <mergeCell ref="C21:C23"/>
+    <mergeCell ref="G21:G23"/>
+    <mergeCell ref="H21:H23"/>
+    <mergeCell ref="D21:D23"/>
+    <mergeCell ref="E21:E23"/>
+    <mergeCell ref="E5:E6"/>
+    <mergeCell ref="E7:E8"/>
+    <mergeCell ref="E9:E10"/>
+    <mergeCell ref="E11:E12"/>
+    <mergeCell ref="E13:E14"/>
     <mergeCell ref="H18:H20"/>
     <mergeCell ref="E3:E4"/>
     <mergeCell ref="G3:G4"/>
@@ -2747,40 +2731,56 @@
     <mergeCell ref="G11:G12"/>
     <mergeCell ref="G13:G14"/>
     <mergeCell ref="G15:G17"/>
-    <mergeCell ref="E5:E6"/>
-    <mergeCell ref="E7:E8"/>
-    <mergeCell ref="E9:E10"/>
-    <mergeCell ref="E11:E12"/>
-    <mergeCell ref="E13:E14"/>
-    <mergeCell ref="F21:F23"/>
-    <mergeCell ref="B21:B23"/>
-    <mergeCell ref="C21:C23"/>
-    <mergeCell ref="G21:G23"/>
-    <mergeCell ref="H21:H23"/>
-    <mergeCell ref="D21:D23"/>
-    <mergeCell ref="E21:E23"/>
-    <mergeCell ref="F3:F4"/>
-    <mergeCell ref="F5:F6"/>
-    <mergeCell ref="F7:F8"/>
-    <mergeCell ref="F9:F10"/>
-    <mergeCell ref="F11:F12"/>
-    <mergeCell ref="H24:H26"/>
-    <mergeCell ref="G27:G32"/>
-    <mergeCell ref="F27:F32"/>
-    <mergeCell ref="E27:E32"/>
-    <mergeCell ref="D27:D32"/>
-    <mergeCell ref="G24:G26"/>
-    <mergeCell ref="B24:B26"/>
-    <mergeCell ref="C24:C26"/>
-    <mergeCell ref="D24:D26"/>
-    <mergeCell ref="E24:E26"/>
-    <mergeCell ref="F24:F26"/>
-    <mergeCell ref="B36:J36"/>
-    <mergeCell ref="J27:J32"/>
-    <mergeCell ref="C27:C32"/>
-    <mergeCell ref="B27:B32"/>
-    <mergeCell ref="H27:H32"/>
-    <mergeCell ref="I27:I32"/>
+    <mergeCell ref="B13:B14"/>
+    <mergeCell ref="B15:B17"/>
+    <mergeCell ref="G18:G20"/>
+    <mergeCell ref="E18:E20"/>
+    <mergeCell ref="C18:C20"/>
+    <mergeCell ref="B18:B20"/>
+    <mergeCell ref="F18:F20"/>
+    <mergeCell ref="E15:E17"/>
+    <mergeCell ref="D15:D17"/>
+    <mergeCell ref="D18:D20"/>
+    <mergeCell ref="F13:F14"/>
+    <mergeCell ref="C15:C17"/>
+    <mergeCell ref="F15:F17"/>
+    <mergeCell ref="B3:B4"/>
+    <mergeCell ref="B5:B6"/>
+    <mergeCell ref="B7:B8"/>
+    <mergeCell ref="B9:B10"/>
+    <mergeCell ref="B11:B12"/>
+    <mergeCell ref="C3:C4"/>
+    <mergeCell ref="D3:D4"/>
+    <mergeCell ref="C5:C6"/>
+    <mergeCell ref="D5:D6"/>
+    <mergeCell ref="C7:C8"/>
+    <mergeCell ref="D7:D8"/>
+    <mergeCell ref="C9:C10"/>
+    <mergeCell ref="D11:D12"/>
+    <mergeCell ref="C11:C12"/>
+    <mergeCell ref="D13:D14"/>
+    <mergeCell ref="C13:C14"/>
+    <mergeCell ref="D9:D10"/>
+    <mergeCell ref="I3:I4"/>
+    <mergeCell ref="I5:I6"/>
+    <mergeCell ref="I7:I8"/>
+    <mergeCell ref="I9:I10"/>
+    <mergeCell ref="I11:I12"/>
+    <mergeCell ref="I13:I14"/>
+    <mergeCell ref="I15:I17"/>
+    <mergeCell ref="I18:I20"/>
+    <mergeCell ref="I21:I23"/>
+    <mergeCell ref="I24:I26"/>
+    <mergeCell ref="J3:J4"/>
+    <mergeCell ref="J5:J6"/>
+    <mergeCell ref="J7:J8"/>
+    <mergeCell ref="J9:J10"/>
+    <mergeCell ref="J11:J12"/>
+    <mergeCell ref="J13:J14"/>
+    <mergeCell ref="J15:J17"/>
+    <mergeCell ref="J18:J20"/>
+    <mergeCell ref="J21:J23"/>
+    <mergeCell ref="J24:J26"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape" r:id="rId1"/>

</xml_diff>

<commit_message>
Analyses des performances apres 9eme correction
</commit_message>
<xml_diff>
--- a/Analyses/Modèle-audit-SEO.xlsx
+++ b/Analyses/Modèle-audit-SEO.xlsx
@@ -66,9 +66,6 @@
     <t xml:space="preserve"> Images servant de citations</t>
   </si>
   <si>
-    <t xml:space="preserve"> Div et meta Keyword</t>
-  </si>
-  <si>
     <t xml:space="preserve"> Mauvaise visibilité du texte</t>
   </si>
   <si>
@@ -97,10 +94,6 @@
   <si>
     <t xml:space="preserve"> Transformer les images en
  texte.</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Noter les mots et clés et les
- redistribuer. Enlever div et méta</t>
   </si>
   <si>
     <t xml:space="preserve"> Ne conserver que les liens vers
@@ -318,6 +311,13 @@
   <si>
     <t xml:space="preserve"> Corriger la couleur du
  texte et/ou du fond.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Div Keyword</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Noter les mots et clés et les
+ redistribuer. Enlever div Keyword</t>
   </si>
 </sst>
 </file>
@@ -792,103 +792,103 @@
     <xf numFmtId="0" fontId="7" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1107,7 +1107,7 @@
   <dimension ref="B1:AB992"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="J15" sqref="J15:J17"/>
+      <selection activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.33203125" defaultRowHeight="15" customHeight="1"/>
@@ -1127,7 +1127,7 @@
     <row r="1" spans="2:28" ht="15" customHeight="1" thickBot="1"/>
     <row r="2" spans="2:28" ht="15.75" customHeight="1" thickBot="1">
       <c r="B2" s="9" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C2" s="10" t="s">
         <v>0</v>
@@ -1148,10 +1148,10 @@
         <v>5</v>
       </c>
       <c r="I2" s="11" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="J2" s="12" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="K2" s="5"/>
       <c r="L2" s="5"/>
@@ -1173,490 +1173,490 @@
       <c r="AB2" s="1"/>
     </row>
     <row r="3" spans="2:28" ht="15.75" customHeight="1">
-      <c r="B3" s="37">
+      <c r="B3" s="50">
         <v>1</v>
       </c>
-      <c r="C3" s="34" t="s">
-        <v>40</v>
-      </c>
-      <c r="D3" s="34" t="s">
+      <c r="C3" s="51" t="s">
+        <v>38</v>
+      </c>
+      <c r="D3" s="51" t="s">
         <v>7</v>
       </c>
-      <c r="E3" s="40" t="s">
+      <c r="E3" s="45" t="s">
+        <v>14</v>
+      </c>
+      <c r="F3" s="45" t="s">
+        <v>37</v>
+      </c>
+      <c r="G3" s="45" t="s">
         <v>15</v>
       </c>
-      <c r="F3" s="40" t="s">
+      <c r="H3" s="48"/>
+      <c r="I3" s="52">
+        <v>1</v>
+      </c>
+      <c r="J3" s="54" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="4" spans="2:28" ht="15.75" customHeight="1">
+      <c r="B4" s="31"/>
+      <c r="C4" s="29"/>
+      <c r="D4" s="29"/>
+      <c r="E4" s="33"/>
+      <c r="F4" s="33"/>
+      <c r="G4" s="33"/>
+      <c r="H4" s="33"/>
+      <c r="I4" s="35"/>
+      <c r="J4" s="55"/>
+    </row>
+    <row r="5" spans="2:28" ht="15.75" customHeight="1">
+      <c r="B5" s="37">
+        <v>2</v>
+      </c>
+      <c r="C5" s="38" t="s">
+        <v>38</v>
+      </c>
+      <c r="D5" s="40" t="s">
+        <v>8</v>
+      </c>
+      <c r="E5" s="39" t="s">
+        <v>14</v>
+      </c>
+      <c r="F5" s="46"/>
+      <c r="G5" s="39" t="s">
+        <v>16</v>
+      </c>
+      <c r="H5" s="40"/>
+      <c r="I5" s="53">
+        <v>2</v>
+      </c>
+      <c r="J5" s="55" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="6" spans="2:28" ht="15.75" customHeight="1">
+      <c r="B6" s="37"/>
+      <c r="C6" s="38"/>
+      <c r="D6" s="40"/>
+      <c r="E6" s="40"/>
+      <c r="F6" s="46"/>
+      <c r="G6" s="40"/>
+      <c r="H6" s="40"/>
+      <c r="I6" s="53"/>
+      <c r="J6" s="55"/>
+    </row>
+    <row r="7" spans="2:28" ht="15.75" customHeight="1">
+      <c r="B7" s="31">
+        <v>3</v>
+      </c>
+      <c r="C7" s="49" t="s">
+        <v>6</v>
+      </c>
+      <c r="D7" s="43" t="s">
+        <v>24</v>
+      </c>
+      <c r="E7" s="43" t="s">
+        <v>21</v>
+      </c>
+      <c r="F7" s="47"/>
+      <c r="G7" s="43" t="s">
+        <v>17</v>
+      </c>
+      <c r="H7" s="47"/>
+      <c r="I7" s="35">
+        <v>10</v>
+      </c>
+      <c r="J7" s="27" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="8" spans="2:28" ht="15.75" customHeight="1">
+      <c r="B8" s="31"/>
+      <c r="C8" s="49"/>
+      <c r="D8" s="47"/>
+      <c r="E8" s="47"/>
+      <c r="F8" s="47"/>
+      <c r="G8" s="47"/>
+      <c r="H8" s="47"/>
+      <c r="I8" s="35"/>
+      <c r="J8" s="27"/>
+    </row>
+    <row r="9" spans="2:28" ht="15.75" customHeight="1">
+      <c r="B9" s="37">
+        <v>4</v>
+      </c>
+      <c r="C9" s="38" t="s">
+        <v>6</v>
+      </c>
+      <c r="D9" s="39" t="s">
+        <v>25</v>
+      </c>
+      <c r="E9" s="39" t="s">
+        <v>22</v>
+      </c>
+      <c r="F9" s="40"/>
+      <c r="G9" s="39" t="s">
+        <v>18</v>
+      </c>
+      <c r="H9" s="40"/>
+      <c r="I9" s="53">
+        <v>4</v>
+      </c>
+      <c r="J9" s="55" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="10" spans="2:28" ht="15.75" customHeight="1">
+      <c r="B10" s="37"/>
+      <c r="C10" s="38"/>
+      <c r="D10" s="40"/>
+      <c r="E10" s="40"/>
+      <c r="F10" s="40"/>
+      <c r="G10" s="40"/>
+      <c r="H10" s="40"/>
+      <c r="I10" s="53"/>
+      <c r="J10" s="55"/>
+    </row>
+    <row r="11" spans="2:28" ht="15.75" customHeight="1">
+      <c r="B11" s="31">
+        <v>5</v>
+      </c>
+      <c r="C11" s="49" t="s">
+        <v>10</v>
+      </c>
+      <c r="D11" s="47" t="s">
+        <v>11</v>
+      </c>
+      <c r="E11" s="43" t="s">
+        <v>35</v>
+      </c>
+      <c r="F11" s="47"/>
+      <c r="G11" s="43" t="s">
+        <v>19</v>
+      </c>
+      <c r="H11" s="47"/>
+      <c r="I11" s="35">
+        <v>5</v>
+      </c>
+      <c r="J11" s="55" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="12" spans="2:28" ht="15.75" customHeight="1">
+      <c r="B12" s="31"/>
+      <c r="C12" s="49"/>
+      <c r="D12" s="47"/>
+      <c r="E12" s="47"/>
+      <c r="F12" s="47"/>
+      <c r="G12" s="47"/>
+      <c r="H12" s="47"/>
+      <c r="I12" s="35"/>
+      <c r="J12" s="55"/>
+    </row>
+    <row r="13" spans="2:28" ht="15.75" customHeight="1">
+      <c r="B13" s="37">
+        <v>6</v>
+      </c>
+      <c r="C13" s="38" t="s">
+        <v>6</v>
+      </c>
+      <c r="D13" s="40" t="s">
+        <v>54</v>
+      </c>
+      <c r="E13" s="39" t="s">
+        <v>33</v>
+      </c>
+      <c r="F13" s="40"/>
+      <c r="G13" s="39" t="s">
+        <v>55</v>
+      </c>
+      <c r="H13" s="40"/>
+      <c r="I13" s="53">
+        <v>9</v>
+      </c>
+      <c r="J13" s="55" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="14" spans="2:28" ht="15.75" customHeight="1">
+      <c r="B14" s="37"/>
+      <c r="C14" s="38"/>
+      <c r="D14" s="40"/>
+      <c r="E14" s="40"/>
+      <c r="F14" s="40"/>
+      <c r="G14" s="40"/>
+      <c r="H14" s="40"/>
+      <c r="I14" s="53"/>
+      <c r="J14" s="55"/>
+    </row>
+    <row r="15" spans="2:28" ht="15.75" customHeight="1">
+      <c r="B15" s="31">
+        <v>7</v>
+      </c>
+      <c r="C15" s="49" t="s">
+        <v>6</v>
+      </c>
+      <c r="D15" s="43" t="s">
+        <v>26</v>
+      </c>
+      <c r="E15" s="43" t="s">
+        <v>23</v>
+      </c>
+      <c r="F15" s="47"/>
+      <c r="G15" s="43" t="s">
+        <v>20</v>
+      </c>
+      <c r="H15" s="47"/>
+      <c r="I15" s="35">
+        <v>8</v>
+      </c>
+      <c r="J15" s="55" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="16" spans="2:28" ht="15.75" customHeight="1">
+      <c r="B16" s="31"/>
+      <c r="C16" s="49"/>
+      <c r="D16" s="47"/>
+      <c r="E16" s="47"/>
+      <c r="F16" s="47"/>
+      <c r="G16" s="47"/>
+      <c r="H16" s="47"/>
+      <c r="I16" s="35"/>
+      <c r="J16" s="55"/>
+    </row>
+    <row r="17" spans="2:10" ht="15.75" customHeight="1">
+      <c r="B17" s="31"/>
+      <c r="C17" s="49"/>
+      <c r="D17" s="47"/>
+      <c r="E17" s="47"/>
+      <c r="F17" s="47"/>
+      <c r="G17" s="47"/>
+      <c r="H17" s="47"/>
+      <c r="I17" s="35"/>
+      <c r="J17" s="55"/>
+    </row>
+    <row r="18" spans="2:10" ht="15.75" customHeight="1">
+      <c r="B18" s="37">
+        <v>8</v>
+      </c>
+      <c r="C18" s="38" t="s">
+        <v>9</v>
+      </c>
+      <c r="D18" s="39" t="s">
+        <v>52</v>
+      </c>
+      <c r="E18" s="40" t="s">
+        <v>12</v>
+      </c>
+      <c r="F18" s="40"/>
+      <c r="G18" s="39" t="s">
+        <v>53</v>
+      </c>
+      <c r="H18" s="40"/>
+      <c r="I18" s="53">
+        <v>7</v>
+      </c>
+      <c r="J18" s="55" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="19" spans="2:10" ht="15.75" customHeight="1">
+      <c r="B19" s="37"/>
+      <c r="C19" s="38"/>
+      <c r="D19" s="40"/>
+      <c r="E19" s="40"/>
+      <c r="F19" s="40"/>
+      <c r="G19" s="40"/>
+      <c r="H19" s="40"/>
+      <c r="I19" s="53"/>
+      <c r="J19" s="55"/>
+    </row>
+    <row r="20" spans="2:10" ht="15.75" customHeight="1">
+      <c r="B20" s="37"/>
+      <c r="C20" s="38"/>
+      <c r="D20" s="40"/>
+      <c r="E20" s="40"/>
+      <c r="F20" s="40"/>
+      <c r="G20" s="40"/>
+      <c r="H20" s="40"/>
+      <c r="I20" s="53"/>
+      <c r="J20" s="55"/>
+    </row>
+    <row r="21" spans="2:10" ht="15.75" customHeight="1">
+      <c r="B21" s="31">
+        <v>9</v>
+      </c>
+      <c r="C21" s="29" t="s">
+        <v>9</v>
+      </c>
+      <c r="D21" s="41" t="s">
+        <v>36</v>
+      </c>
+      <c r="E21" s="41" t="s">
+        <v>28</v>
+      </c>
+      <c r="F21" s="33"/>
+      <c r="G21" s="33" t="s">
+        <v>27</v>
+      </c>
+      <c r="H21" s="33"/>
+      <c r="I21" s="35">
+        <v>3</v>
+      </c>
+      <c r="J21" s="55" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="22" spans="2:10" ht="15.75" customHeight="1">
+      <c r="B22" s="31"/>
+      <c r="C22" s="29"/>
+      <c r="D22" s="41"/>
+      <c r="E22" s="33"/>
+      <c r="F22" s="33"/>
+      <c r="G22" s="33"/>
+      <c r="H22" s="33"/>
+      <c r="I22" s="35"/>
+      <c r="J22" s="55"/>
+    </row>
+    <row r="23" spans="2:10" ht="15.75" customHeight="1">
+      <c r="B23" s="31"/>
+      <c r="C23" s="29"/>
+      <c r="D23" s="41"/>
+      <c r="E23" s="33"/>
+      <c r="F23" s="33"/>
+      <c r="G23" s="33"/>
+      <c r="H23" s="33"/>
+      <c r="I23" s="35"/>
+      <c r="J23" s="55"/>
+    </row>
+    <row r="24" spans="2:10" ht="15.75" customHeight="1">
+      <c r="B24" s="37">
+        <v>10</v>
+      </c>
+      <c r="C24" s="38" t="s">
+        <v>9</v>
+      </c>
+      <c r="D24" s="39" t="s">
+        <v>31</v>
+      </c>
+      <c r="E24" s="40" t="s">
+        <v>29</v>
+      </c>
+      <c r="F24" s="40"/>
+      <c r="G24" s="39" t="s">
+        <v>30</v>
+      </c>
+      <c r="H24" s="40"/>
+      <c r="I24" s="53" t="s">
         <v>39</v>
       </c>
-      <c r="G3" s="40" t="s">
-        <v>16</v>
-      </c>
-      <c r="H3" s="42"/>
-      <c r="I3" s="28">
-        <v>1</v>
-      </c>
-      <c r="J3" s="25" t="s">
+      <c r="J24" s="27" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="25" spans="2:10" ht="15.75" customHeight="1">
+      <c r="B25" s="37"/>
+      <c r="C25" s="38"/>
+      <c r="D25" s="40"/>
+      <c r="E25" s="40"/>
+      <c r="F25" s="40"/>
+      <c r="G25" s="39"/>
+      <c r="H25" s="40"/>
+      <c r="I25" s="53"/>
+      <c r="J25" s="27"/>
+    </row>
+    <row r="26" spans="2:10" ht="15.75" customHeight="1">
+      <c r="B26" s="37"/>
+      <c r="C26" s="38"/>
+      <c r="D26" s="40"/>
+      <c r="E26" s="40"/>
+      <c r="F26" s="40"/>
+      <c r="G26" s="39"/>
+      <c r="H26" s="40"/>
+      <c r="I26" s="53"/>
+      <c r="J26" s="27"/>
+    </row>
+    <row r="27" spans="2:10" ht="15.75" customHeight="1">
+      <c r="B27" s="31">
+        <v>11</v>
+      </c>
+      <c r="C27" s="29" t="s">
+        <v>10</v>
+      </c>
+      <c r="D27" s="41" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="4" spans="2:28" ht="15.75" customHeight="1">
-      <c r="B4" s="38"/>
-      <c r="C4" s="35"/>
-      <c r="D4" s="35"/>
-      <c r="E4" s="41"/>
-      <c r="F4" s="41"/>
-      <c r="G4" s="41"/>
-      <c r="H4" s="41"/>
-      <c r="I4" s="27"/>
-      <c r="J4" s="24"/>
-    </row>
-    <row r="5" spans="2:28" ht="15.75" customHeight="1">
-      <c r="B5" s="39">
-        <v>2</v>
-      </c>
-      <c r="C5" s="29" t="s">
-        <v>40</v>
-      </c>
-      <c r="D5" s="32" t="s">
-        <v>8</v>
-      </c>
-      <c r="E5" s="33" t="s">
-        <v>15</v>
-      </c>
-      <c r="F5" s="44"/>
-      <c r="G5" s="33" t="s">
-        <v>17</v>
-      </c>
-      <c r="H5" s="32"/>
-      <c r="I5" s="26">
-        <v>2</v>
-      </c>
-      <c r="J5" s="24" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="6" spans="2:28" ht="15.75" customHeight="1">
-      <c r="B6" s="39"/>
-      <c r="C6" s="29"/>
-      <c r="D6" s="32"/>
-      <c r="E6" s="32"/>
-      <c r="F6" s="44"/>
-      <c r="G6" s="32"/>
-      <c r="H6" s="32"/>
-      <c r="I6" s="26"/>
-      <c r="J6" s="24"/>
-    </row>
-    <row r="7" spans="2:28" ht="15.75" customHeight="1">
-      <c r="B7" s="38">
-        <v>3</v>
-      </c>
-      <c r="C7" s="31" t="s">
-        <v>6</v>
-      </c>
-      <c r="D7" s="36" t="s">
-        <v>26</v>
-      </c>
-      <c r="E7" s="36" t="s">
-        <v>23</v>
-      </c>
-      <c r="F7" s="30"/>
-      <c r="G7" s="36" t="s">
-        <v>18</v>
-      </c>
-      <c r="H7" s="30"/>
-      <c r="I7" s="27">
-        <v>10</v>
-      </c>
-      <c r="J7" s="23" t="s">
+      <c r="E27" s="43" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="8" spans="2:28" ht="15.75" customHeight="1">
-      <c r="B8" s="38"/>
-      <c r="C8" s="31"/>
-      <c r="D8" s="30"/>
-      <c r="E8" s="30"/>
-      <c r="F8" s="30"/>
-      <c r="G8" s="30"/>
-      <c r="H8" s="30"/>
-      <c r="I8" s="27"/>
-      <c r="J8" s="23"/>
-    </row>
-    <row r="9" spans="2:28" ht="15.75" customHeight="1">
-      <c r="B9" s="39">
-        <v>4</v>
-      </c>
-      <c r="C9" s="29" t="s">
-        <v>6</v>
-      </c>
-      <c r="D9" s="33" t="s">
-        <v>27</v>
-      </c>
-      <c r="E9" s="33" t="s">
-        <v>24</v>
-      </c>
-      <c r="F9" s="32"/>
-      <c r="G9" s="33" t="s">
-        <v>19</v>
-      </c>
-      <c r="H9" s="32"/>
-      <c r="I9" s="26">
-        <v>4</v>
-      </c>
-      <c r="J9" s="24" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="10" spans="2:28" ht="15.75" customHeight="1">
-      <c r="B10" s="39"/>
-      <c r="C10" s="29"/>
-      <c r="D10" s="32"/>
-      <c r="E10" s="32"/>
-      <c r="F10" s="32"/>
-      <c r="G10" s="32"/>
-      <c r="H10" s="32"/>
-      <c r="I10" s="26"/>
-      <c r="J10" s="24"/>
-    </row>
-    <row r="11" spans="2:28" ht="15.75" customHeight="1">
-      <c r="B11" s="38">
-        <v>5</v>
-      </c>
-      <c r="C11" s="31" t="s">
-        <v>10</v>
-      </c>
-      <c r="D11" s="30" t="s">
-        <v>11</v>
-      </c>
-      <c r="E11" s="36" t="s">
-        <v>37</v>
-      </c>
-      <c r="F11" s="30"/>
-      <c r="G11" s="36" t="s">
-        <v>20</v>
-      </c>
-      <c r="H11" s="30"/>
-      <c r="I11" s="27">
-        <v>5</v>
-      </c>
-      <c r="J11" s="24" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="12" spans="2:28" ht="15.75" customHeight="1">
-      <c r="B12" s="38"/>
-      <c r="C12" s="31"/>
-      <c r="D12" s="30"/>
-      <c r="E12" s="30"/>
-      <c r="F12" s="30"/>
-      <c r="G12" s="30"/>
-      <c r="H12" s="30"/>
-      <c r="I12" s="27"/>
-      <c r="J12" s="24"/>
-    </row>
-    <row r="13" spans="2:28" ht="15.75" customHeight="1">
-      <c r="B13" s="39">
-        <v>6</v>
-      </c>
-      <c r="C13" s="29" t="s">
-        <v>6</v>
-      </c>
-      <c r="D13" s="32" t="s">
-        <v>12</v>
-      </c>
-      <c r="E13" s="33" t="s">
-        <v>35</v>
-      </c>
-      <c r="F13" s="32"/>
-      <c r="G13" s="33" t="s">
-        <v>21</v>
-      </c>
-      <c r="H13" s="32"/>
-      <c r="I13" s="26">
-        <v>9</v>
-      </c>
-      <c r="J13" s="23" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="14" spans="2:28" ht="15.75" customHeight="1">
-      <c r="B14" s="39"/>
-      <c r="C14" s="29"/>
-      <c r="D14" s="32"/>
-      <c r="E14" s="32"/>
-      <c r="F14" s="32"/>
-      <c r="G14" s="32"/>
-      <c r="H14" s="32"/>
-      <c r="I14" s="26"/>
-      <c r="J14" s="23"/>
-    </row>
-    <row r="15" spans="2:28" ht="15.75" customHeight="1">
-      <c r="B15" s="38">
-        <v>7</v>
-      </c>
-      <c r="C15" s="31" t="s">
-        <v>6</v>
-      </c>
-      <c r="D15" s="36" t="s">
-        <v>28</v>
-      </c>
-      <c r="E15" s="36" t="s">
-        <v>25</v>
-      </c>
-      <c r="F15" s="30"/>
-      <c r="G15" s="36" t="s">
-        <v>22</v>
-      </c>
-      <c r="H15" s="30"/>
-      <c r="I15" s="27">
-        <v>8</v>
-      </c>
-      <c r="J15" s="24" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="16" spans="2:28" ht="15.75" customHeight="1">
-      <c r="B16" s="38"/>
-      <c r="C16" s="31"/>
-      <c r="D16" s="30"/>
-      <c r="E16" s="30"/>
-      <c r="F16" s="30"/>
-      <c r="G16" s="30"/>
-      <c r="H16" s="30"/>
-      <c r="I16" s="27"/>
-      <c r="J16" s="24"/>
-    </row>
-    <row r="17" spans="2:10" ht="15.75" customHeight="1">
-      <c r="B17" s="38"/>
-      <c r="C17" s="31"/>
-      <c r="D17" s="30"/>
-      <c r="E17" s="30"/>
-      <c r="F17" s="30"/>
-      <c r="G17" s="30"/>
-      <c r="H17" s="30"/>
-      <c r="I17" s="27"/>
-      <c r="J17" s="24"/>
-    </row>
-    <row r="18" spans="2:10" ht="15.75" customHeight="1">
-      <c r="B18" s="39">
-        <v>8</v>
-      </c>
-      <c r="C18" s="29" t="s">
-        <v>9</v>
-      </c>
-      <c r="D18" s="33" t="s">
-        <v>54</v>
-      </c>
-      <c r="E18" s="32" t="s">
-        <v>13</v>
-      </c>
-      <c r="F18" s="32"/>
-      <c r="G18" s="33" t="s">
-        <v>55</v>
-      </c>
-      <c r="H18" s="32"/>
-      <c r="I18" s="26">
-        <v>7</v>
-      </c>
-      <c r="J18" s="24" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="19" spans="2:10" ht="15.75" customHeight="1">
-      <c r="B19" s="39"/>
-      <c r="C19" s="29"/>
-      <c r="D19" s="32"/>
-      <c r="E19" s="32"/>
-      <c r="F19" s="32"/>
-      <c r="G19" s="32"/>
-      <c r="H19" s="32"/>
-      <c r="I19" s="26"/>
-      <c r="J19" s="24"/>
-    </row>
-    <row r="20" spans="2:10" ht="15.75" customHeight="1">
-      <c r="B20" s="39"/>
-      <c r="C20" s="29"/>
-      <c r="D20" s="32"/>
-      <c r="E20" s="32"/>
-      <c r="F20" s="32"/>
-      <c r="G20" s="32"/>
-      <c r="H20" s="32"/>
-      <c r="I20" s="26"/>
-      <c r="J20" s="24"/>
-    </row>
-    <row r="21" spans="2:10" ht="15.75" customHeight="1">
-      <c r="B21" s="38">
-        <v>9</v>
-      </c>
-      <c r="C21" s="35" t="s">
-        <v>9</v>
-      </c>
-      <c r="D21" s="43" t="s">
-        <v>38</v>
-      </c>
-      <c r="E21" s="43" t="s">
-        <v>30</v>
-      </c>
-      <c r="F21" s="41"/>
-      <c r="G21" s="41" t="s">
-        <v>29</v>
-      </c>
-      <c r="H21" s="41"/>
-      <c r="I21" s="27">
-        <v>3</v>
-      </c>
-      <c r="J21" s="24" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="22" spans="2:10" ht="15.75" customHeight="1">
-      <c r="B22" s="38"/>
-      <c r="C22" s="35"/>
-      <c r="D22" s="43"/>
-      <c r="E22" s="41"/>
-      <c r="F22" s="41"/>
-      <c r="G22" s="41"/>
-      <c r="H22" s="41"/>
-      <c r="I22" s="27"/>
-      <c r="J22" s="24"/>
-    </row>
-    <row r="23" spans="2:10" ht="15.75" customHeight="1">
-      <c r="B23" s="38"/>
-      <c r="C23" s="35"/>
-      <c r="D23" s="43"/>
-      <c r="E23" s="41"/>
-      <c r="F23" s="41"/>
-      <c r="G23" s="41"/>
-      <c r="H23" s="41"/>
-      <c r="I23" s="27"/>
-      <c r="J23" s="24"/>
-    </row>
-    <row r="24" spans="2:10" ht="15.75" customHeight="1">
-      <c r="B24" s="39">
-        <v>10</v>
-      </c>
-      <c r="C24" s="29" t="s">
-        <v>9</v>
-      </c>
-      <c r="D24" s="33" t="s">
-        <v>33</v>
-      </c>
-      <c r="E24" s="32" t="s">
-        <v>31</v>
-      </c>
-      <c r="F24" s="32"/>
-      <c r="G24" s="33" t="s">
+      <c r="F27" s="33"/>
+      <c r="G27" s="41" t="s">
         <v>32</v>
       </c>
-      <c r="H24" s="32"/>
-      <c r="I24" s="26" t="s">
-        <v>41</v>
-      </c>
-      <c r="J24" s="23" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="25" spans="2:10" ht="15.75" customHeight="1">
-      <c r="B25" s="39"/>
-      <c r="C25" s="29"/>
-      <c r="D25" s="32"/>
-      <c r="E25" s="32"/>
-      <c r="F25" s="32"/>
-      <c r="G25" s="33"/>
-      <c r="H25" s="32"/>
-      <c r="I25" s="26"/>
-      <c r="J25" s="23"/>
-    </row>
-    <row r="26" spans="2:10" ht="15.75" customHeight="1">
-      <c r="B26" s="39"/>
-      <c r="C26" s="29"/>
-      <c r="D26" s="32"/>
-      <c r="E26" s="32"/>
-      <c r="F26" s="32"/>
-      <c r="G26" s="33"/>
-      <c r="H26" s="32"/>
-      <c r="I26" s="26"/>
-      <c r="J26" s="23"/>
-    </row>
-    <row r="27" spans="2:10" ht="15.75" customHeight="1">
-      <c r="B27" s="38">
-        <v>11</v>
-      </c>
-      <c r="C27" s="35" t="s">
-        <v>10</v>
-      </c>
-      <c r="D27" s="43" t="s">
-        <v>45</v>
-      </c>
-      <c r="E27" s="36" t="s">
-        <v>46</v>
-      </c>
-      <c r="F27" s="41"/>
-      <c r="G27" s="43" t="s">
-        <v>34</v>
-      </c>
-      <c r="H27" s="41"/>
-      <c r="I27" s="27" t="s">
-        <v>41</v>
-      </c>
-      <c r="J27" s="51" t="s">
-        <v>44</v>
+      <c r="H27" s="33"/>
+      <c r="I27" s="35" t="s">
+        <v>39</v>
+      </c>
+      <c r="J27" s="26" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="28" spans="2:10" ht="15.75" customHeight="1">
-      <c r="B28" s="38"/>
-      <c r="C28" s="35"/>
-      <c r="D28" s="43"/>
-      <c r="E28" s="36"/>
-      <c r="F28" s="41"/>
-      <c r="G28" s="43"/>
-      <c r="H28" s="41"/>
-      <c r="I28" s="27"/>
-      <c r="J28" s="23"/>
+      <c r="B28" s="31"/>
+      <c r="C28" s="29"/>
+      <c r="D28" s="41"/>
+      <c r="E28" s="43"/>
+      <c r="F28" s="33"/>
+      <c r="G28" s="41"/>
+      <c r="H28" s="33"/>
+      <c r="I28" s="35"/>
+      <c r="J28" s="27"/>
     </row>
     <row r="29" spans="2:10" ht="15.75" customHeight="1">
-      <c r="B29" s="38"/>
-      <c r="C29" s="35"/>
-      <c r="D29" s="43"/>
-      <c r="E29" s="36"/>
-      <c r="F29" s="41"/>
-      <c r="G29" s="43"/>
-      <c r="H29" s="41"/>
-      <c r="I29" s="27"/>
-      <c r="J29" s="23"/>
+      <c r="B29" s="31"/>
+      <c r="C29" s="29"/>
+      <c r="D29" s="41"/>
+      <c r="E29" s="43"/>
+      <c r="F29" s="33"/>
+      <c r="G29" s="41"/>
+      <c r="H29" s="33"/>
+      <c r="I29" s="35"/>
+      <c r="J29" s="27"/>
     </row>
     <row r="30" spans="2:10" ht="15.75" customHeight="1">
-      <c r="B30" s="38"/>
-      <c r="C30" s="35"/>
-      <c r="D30" s="43"/>
-      <c r="E30" s="36"/>
-      <c r="F30" s="41"/>
-      <c r="G30" s="43"/>
-      <c r="H30" s="41"/>
-      <c r="I30" s="27"/>
-      <c r="J30" s="23"/>
+      <c r="B30" s="31"/>
+      <c r="C30" s="29"/>
+      <c r="D30" s="41"/>
+      <c r="E30" s="43"/>
+      <c r="F30" s="33"/>
+      <c r="G30" s="41"/>
+      <c r="H30" s="33"/>
+      <c r="I30" s="35"/>
+      <c r="J30" s="27"/>
     </row>
     <row r="31" spans="2:10" ht="15.75" customHeight="1">
-      <c r="B31" s="38"/>
-      <c r="C31" s="35"/>
-      <c r="D31" s="43"/>
-      <c r="E31" s="36"/>
-      <c r="F31" s="41"/>
-      <c r="G31" s="43"/>
-      <c r="H31" s="41"/>
-      <c r="I31" s="27"/>
-      <c r="J31" s="23"/>
+      <c r="B31" s="31"/>
+      <c r="C31" s="29"/>
+      <c r="D31" s="41"/>
+      <c r="E31" s="43"/>
+      <c r="F31" s="33"/>
+      <c r="G31" s="41"/>
+      <c r="H31" s="33"/>
+      <c r="I31" s="35"/>
+      <c r="J31" s="27"/>
     </row>
     <row r="32" spans="2:10" ht="15.75" customHeight="1">
-      <c r="B32" s="54"/>
-      <c r="C32" s="53"/>
-      <c r="D32" s="45"/>
-      <c r="E32" s="47"/>
-      <c r="F32" s="46"/>
-      <c r="G32" s="45"/>
-      <c r="H32" s="46"/>
-      <c r="I32" s="55"/>
-      <c r="J32" s="52"/>
+      <c r="B32" s="32"/>
+      <c r="C32" s="30"/>
+      <c r="D32" s="42"/>
+      <c r="E32" s="44"/>
+      <c r="F32" s="34"/>
+      <c r="G32" s="42"/>
+      <c r="H32" s="34"/>
+      <c r="I32" s="36"/>
+      <c r="J32" s="28"/>
     </row>
     <row r="33" spans="2:10" ht="63" customHeight="1">
       <c r="B33" s="17">
@@ -1666,21 +1666,21 @@
         <v>10</v>
       </c>
       <c r="D33" s="19" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="E33" s="20" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="F33" s="20"/>
       <c r="G33" s="21" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="H33" s="20"/>
       <c r="I33" s="18" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="J33" s="15" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="34" spans="2:10" ht="63" customHeight="1" thickBot="1">
@@ -1688,39 +1688,39 @@
         <v>13</v>
       </c>
       <c r="C34" s="7" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D34" s="14" t="s">
+        <v>48</v>
+      </c>
+      <c r="E34" s="14" t="s">
         <v>50</v>
-      </c>
-      <c r="E34" s="14" t="s">
-        <v>52</v>
       </c>
       <c r="F34" s="13"/>
       <c r="G34" s="14" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="H34" s="13"/>
       <c r="I34" s="8">
         <v>6</v>
       </c>
       <c r="J34" s="22" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="35" spans="2:10" ht="15.75" customHeight="1" thickBot="1"/>
     <row r="36" spans="2:10" ht="15.75" customHeight="1" thickBot="1">
-      <c r="B36" s="48" t="s">
-        <v>53</v>
-      </c>
-      <c r="C36" s="49"/>
-      <c r="D36" s="49"/>
-      <c r="E36" s="49"/>
-      <c r="F36" s="49"/>
-      <c r="G36" s="49"/>
-      <c r="H36" s="49"/>
-      <c r="I36" s="49"/>
-      <c r="J36" s="50"/>
+      <c r="B36" s="23" t="s">
+        <v>51</v>
+      </c>
+      <c r="C36" s="24"/>
+      <c r="D36" s="24"/>
+      <c r="E36" s="24"/>
+      <c r="F36" s="24"/>
+      <c r="G36" s="24"/>
+      <c r="H36" s="24"/>
+      <c r="I36" s="24"/>
+      <c r="J36" s="25"/>
     </row>
     <row r="37" spans="2:10" ht="15.75" customHeight="1"/>
     <row r="38" spans="2:10" ht="15.75" customHeight="1"/>
@@ -2681,40 +2681,56 @@
   </sheetData>
   <autoFilter ref="B2:J34"/>
   <mergeCells count="100">
-    <mergeCell ref="B36:J36"/>
-    <mergeCell ref="J27:J32"/>
-    <mergeCell ref="C27:C32"/>
-    <mergeCell ref="B27:B32"/>
-    <mergeCell ref="H27:H32"/>
-    <mergeCell ref="I27:I32"/>
-    <mergeCell ref="B24:B26"/>
-    <mergeCell ref="C24:C26"/>
-    <mergeCell ref="D24:D26"/>
-    <mergeCell ref="E24:E26"/>
-    <mergeCell ref="F24:F26"/>
-    <mergeCell ref="H24:H26"/>
-    <mergeCell ref="G27:G32"/>
-    <mergeCell ref="F27:F32"/>
-    <mergeCell ref="E27:E32"/>
-    <mergeCell ref="D27:D32"/>
-    <mergeCell ref="G24:G26"/>
-    <mergeCell ref="F3:F4"/>
-    <mergeCell ref="F5:F6"/>
-    <mergeCell ref="F7:F8"/>
-    <mergeCell ref="F9:F10"/>
-    <mergeCell ref="F11:F12"/>
-    <mergeCell ref="F21:F23"/>
-    <mergeCell ref="B21:B23"/>
-    <mergeCell ref="C21:C23"/>
-    <mergeCell ref="G21:G23"/>
-    <mergeCell ref="H21:H23"/>
-    <mergeCell ref="D21:D23"/>
-    <mergeCell ref="E21:E23"/>
-    <mergeCell ref="E5:E6"/>
-    <mergeCell ref="E7:E8"/>
-    <mergeCell ref="E9:E10"/>
-    <mergeCell ref="E11:E12"/>
-    <mergeCell ref="E13:E14"/>
+    <mergeCell ref="J13:J14"/>
+    <mergeCell ref="J15:J17"/>
+    <mergeCell ref="J18:J20"/>
+    <mergeCell ref="J21:J23"/>
+    <mergeCell ref="J24:J26"/>
+    <mergeCell ref="J3:J4"/>
+    <mergeCell ref="J5:J6"/>
+    <mergeCell ref="J7:J8"/>
+    <mergeCell ref="J9:J10"/>
+    <mergeCell ref="J11:J12"/>
+    <mergeCell ref="I13:I14"/>
+    <mergeCell ref="I15:I17"/>
+    <mergeCell ref="I18:I20"/>
+    <mergeCell ref="I21:I23"/>
+    <mergeCell ref="I24:I26"/>
+    <mergeCell ref="I3:I4"/>
+    <mergeCell ref="I5:I6"/>
+    <mergeCell ref="I7:I8"/>
+    <mergeCell ref="I9:I10"/>
+    <mergeCell ref="I11:I12"/>
+    <mergeCell ref="C9:C10"/>
+    <mergeCell ref="D11:D12"/>
+    <mergeCell ref="C11:C12"/>
+    <mergeCell ref="D13:D14"/>
+    <mergeCell ref="C13:C14"/>
+    <mergeCell ref="D9:D10"/>
+    <mergeCell ref="C3:C4"/>
+    <mergeCell ref="D3:D4"/>
+    <mergeCell ref="C5:C6"/>
+    <mergeCell ref="D5:D6"/>
+    <mergeCell ref="C7:C8"/>
+    <mergeCell ref="D7:D8"/>
+    <mergeCell ref="B3:B4"/>
+    <mergeCell ref="B5:B6"/>
+    <mergeCell ref="B7:B8"/>
+    <mergeCell ref="B9:B10"/>
+    <mergeCell ref="B11:B12"/>
+    <mergeCell ref="B13:B14"/>
+    <mergeCell ref="B15:B17"/>
+    <mergeCell ref="G18:G20"/>
+    <mergeCell ref="E18:E20"/>
+    <mergeCell ref="C18:C20"/>
+    <mergeCell ref="B18:B20"/>
+    <mergeCell ref="F18:F20"/>
+    <mergeCell ref="E15:E17"/>
+    <mergeCell ref="D15:D17"/>
+    <mergeCell ref="D18:D20"/>
+    <mergeCell ref="F13:F14"/>
+    <mergeCell ref="C15:C17"/>
+    <mergeCell ref="F15:F17"/>
     <mergeCell ref="H18:H20"/>
     <mergeCell ref="E3:E4"/>
     <mergeCell ref="G3:G4"/>
@@ -2731,56 +2747,40 @@
     <mergeCell ref="G11:G12"/>
     <mergeCell ref="G13:G14"/>
     <mergeCell ref="G15:G17"/>
-    <mergeCell ref="B13:B14"/>
-    <mergeCell ref="B15:B17"/>
-    <mergeCell ref="G18:G20"/>
-    <mergeCell ref="E18:E20"/>
-    <mergeCell ref="C18:C20"/>
-    <mergeCell ref="B18:B20"/>
-    <mergeCell ref="F18:F20"/>
-    <mergeCell ref="E15:E17"/>
-    <mergeCell ref="D15:D17"/>
-    <mergeCell ref="D18:D20"/>
-    <mergeCell ref="F13:F14"/>
-    <mergeCell ref="C15:C17"/>
-    <mergeCell ref="F15:F17"/>
-    <mergeCell ref="B3:B4"/>
-    <mergeCell ref="B5:B6"/>
-    <mergeCell ref="B7:B8"/>
-    <mergeCell ref="B9:B10"/>
-    <mergeCell ref="B11:B12"/>
-    <mergeCell ref="C3:C4"/>
-    <mergeCell ref="D3:D4"/>
-    <mergeCell ref="C5:C6"/>
-    <mergeCell ref="D5:D6"/>
-    <mergeCell ref="C7:C8"/>
-    <mergeCell ref="D7:D8"/>
-    <mergeCell ref="C9:C10"/>
-    <mergeCell ref="D11:D12"/>
-    <mergeCell ref="C11:C12"/>
-    <mergeCell ref="D13:D14"/>
-    <mergeCell ref="C13:C14"/>
-    <mergeCell ref="D9:D10"/>
-    <mergeCell ref="I3:I4"/>
-    <mergeCell ref="I5:I6"/>
-    <mergeCell ref="I7:I8"/>
-    <mergeCell ref="I9:I10"/>
-    <mergeCell ref="I11:I12"/>
-    <mergeCell ref="I13:I14"/>
-    <mergeCell ref="I15:I17"/>
-    <mergeCell ref="I18:I20"/>
-    <mergeCell ref="I21:I23"/>
-    <mergeCell ref="I24:I26"/>
-    <mergeCell ref="J3:J4"/>
-    <mergeCell ref="J5:J6"/>
-    <mergeCell ref="J7:J8"/>
-    <mergeCell ref="J9:J10"/>
-    <mergeCell ref="J11:J12"/>
-    <mergeCell ref="J13:J14"/>
-    <mergeCell ref="J15:J17"/>
-    <mergeCell ref="J18:J20"/>
-    <mergeCell ref="J21:J23"/>
-    <mergeCell ref="J24:J26"/>
+    <mergeCell ref="E5:E6"/>
+    <mergeCell ref="E7:E8"/>
+    <mergeCell ref="E9:E10"/>
+    <mergeCell ref="E11:E12"/>
+    <mergeCell ref="E13:E14"/>
+    <mergeCell ref="F21:F23"/>
+    <mergeCell ref="B21:B23"/>
+    <mergeCell ref="C21:C23"/>
+    <mergeCell ref="G21:G23"/>
+    <mergeCell ref="H21:H23"/>
+    <mergeCell ref="D21:D23"/>
+    <mergeCell ref="E21:E23"/>
+    <mergeCell ref="F3:F4"/>
+    <mergeCell ref="F5:F6"/>
+    <mergeCell ref="F7:F8"/>
+    <mergeCell ref="F9:F10"/>
+    <mergeCell ref="F11:F12"/>
+    <mergeCell ref="H24:H26"/>
+    <mergeCell ref="G27:G32"/>
+    <mergeCell ref="F27:F32"/>
+    <mergeCell ref="E27:E32"/>
+    <mergeCell ref="D27:D32"/>
+    <mergeCell ref="G24:G26"/>
+    <mergeCell ref="B24:B26"/>
+    <mergeCell ref="C24:C26"/>
+    <mergeCell ref="D24:D26"/>
+    <mergeCell ref="E24:E26"/>
+    <mergeCell ref="F24:F26"/>
+    <mergeCell ref="B36:J36"/>
+    <mergeCell ref="J27:J32"/>
+    <mergeCell ref="C27:C32"/>
+    <mergeCell ref="B27:B32"/>
+    <mergeCell ref="H27:H32"/>
+    <mergeCell ref="I27:I32"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape" r:id="rId1"/>

</xml_diff>

<commit_message>
Analyses des performances apres la 10eme correction
</commit_message>
<xml_diff>
--- a/Analyses/Modèle-audit-SEO.xlsx
+++ b/Analyses/Modèle-audit-SEO.xlsx
@@ -10,7 +10,7 @@
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Feuil1!$B$2:$J$34</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Feuil1!$B$2:$J$35</definedName>
   </definedNames>
   <calcPr calcId="125725"/>
   <extLst>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="59">
   <si>
     <t>Catégorie</t>
   </si>
@@ -318,6 +318,15 @@
   <si>
     <t xml:space="preserve"> Noter les mots et clés et les
  redistribuer. Enlever div Keyword</t>
+  </si>
+  <si>
+    <t>12 ?</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Police</t>
+  </si>
+  <si>
+    <t>11 ?</t>
   </si>
 </sst>
 </file>
@@ -440,7 +449,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="20">
+  <borders count="17">
     <border>
       <left/>
       <right/>
@@ -563,90 +572,6 @@
       <top style="medium">
         <color indexed="64"/>
       </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
       <bottom style="thin">
         <color indexed="64"/>
       </bottom>
@@ -719,12 +644,51 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="9" fillId="5" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="56">
+  <cellXfs count="55">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -741,155 +705,152 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1104,10 +1065,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B1:AB992"/>
+  <dimension ref="B1:AB993"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="J2" sqref="J2"/>
+      <selection activeCell="J7" sqref="J7:J8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.33203125" defaultRowHeight="15" customHeight="1"/>
@@ -1126,31 +1087,31 @@
   <sheetData>
     <row r="1" spans="2:28" ht="15" customHeight="1" thickBot="1"/>
     <row r="2" spans="2:28" ht="15.75" customHeight="1" thickBot="1">
-      <c r="B2" s="9" t="s">
+      <c r="B2" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="C2" s="10" t="s">
+      <c r="C2" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="10" t="s">
+      <c r="D2" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="E2" s="10" t="s">
+      <c r="E2" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="F2" s="10" t="s">
+      <c r="F2" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="G2" s="10" t="s">
+      <c r="G2" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="H2" s="10" t="s">
+      <c r="H2" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="I2" s="11" t="s">
+      <c r="I2" s="16" t="s">
         <v>34</v>
       </c>
-      <c r="J2" s="12" t="s">
+      <c r="J2" s="17" t="s">
         <v>40</v>
       </c>
       <c r="K2" s="5"/>
@@ -1173,120 +1134,120 @@
       <c r="AB2" s="1"/>
     </row>
     <row r="3" spans="2:28" ht="15.75" customHeight="1">
-      <c r="B3" s="50">
+      <c r="B3" s="43">
         <v>1</v>
       </c>
-      <c r="C3" s="51" t="s">
+      <c r="C3" s="40" t="s">
         <v>38</v>
       </c>
-      <c r="D3" s="51" t="s">
+      <c r="D3" s="40" t="s">
         <v>7</v>
       </c>
-      <c r="E3" s="45" t="s">
+      <c r="E3" s="46" t="s">
         <v>14</v>
       </c>
-      <c r="F3" s="45" t="s">
+      <c r="F3" s="46" t="s">
         <v>37</v>
       </c>
-      <c r="G3" s="45" t="s">
+      <c r="G3" s="46" t="s">
         <v>15</v>
       </c>
       <c r="H3" s="48"/>
-      <c r="I3" s="52">
+      <c r="I3" s="34">
         <v>1</v>
       </c>
-      <c r="J3" s="54" t="s">
+      <c r="J3" s="31" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="4" spans="2:28" ht="15.75" customHeight="1">
-      <c r="B4" s="31"/>
-      <c r="C4" s="29"/>
-      <c r="D4" s="29"/>
-      <c r="E4" s="33"/>
-      <c r="F4" s="33"/>
-      <c r="G4" s="33"/>
-      <c r="H4" s="33"/>
-      <c r="I4" s="35"/>
-      <c r="J4" s="55"/>
+      <c r="B4" s="44"/>
+      <c r="C4" s="41"/>
+      <c r="D4" s="41"/>
+      <c r="E4" s="47"/>
+      <c r="F4" s="47"/>
+      <c r="G4" s="47"/>
+      <c r="H4" s="47"/>
+      <c r="I4" s="33"/>
+      <c r="J4" s="29"/>
     </row>
     <row r="5" spans="2:28" ht="15.75" customHeight="1">
-      <c r="B5" s="37">
+      <c r="B5" s="45">
         <v>2</v>
       </c>
-      <c r="C5" s="38" t="s">
+      <c r="C5" s="35" t="s">
         <v>38</v>
       </c>
-      <c r="D5" s="40" t="s">
+      <c r="D5" s="38" t="s">
         <v>8</v>
       </c>
       <c r="E5" s="39" t="s">
         <v>14</v>
       </c>
-      <c r="F5" s="46"/>
+      <c r="F5" s="50"/>
       <c r="G5" s="39" t="s">
         <v>16</v>
       </c>
-      <c r="H5" s="40"/>
-      <c r="I5" s="53">
+      <c r="H5" s="38"/>
+      <c r="I5" s="32">
         <v>2</v>
       </c>
-      <c r="J5" s="55" t="s">
+      <c r="J5" s="29" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="6" spans="2:28" ht="15.75" customHeight="1">
-      <c r="B6" s="37"/>
-      <c r="C6" s="38"/>
-      <c r="D6" s="40"/>
-      <c r="E6" s="40"/>
-      <c r="F6" s="46"/>
-      <c r="G6" s="40"/>
-      <c r="H6" s="40"/>
-      <c r="I6" s="53"/>
-      <c r="J6" s="55"/>
+      <c r="B6" s="45"/>
+      <c r="C6" s="35"/>
+      <c r="D6" s="38"/>
+      <c r="E6" s="38"/>
+      <c r="F6" s="50"/>
+      <c r="G6" s="38"/>
+      <c r="H6" s="38"/>
+      <c r="I6" s="32"/>
+      <c r="J6" s="29"/>
     </row>
     <row r="7" spans="2:28" ht="15.75" customHeight="1">
-      <c r="B7" s="31">
+      <c r="B7" s="44">
         <v>3</v>
       </c>
-      <c r="C7" s="49" t="s">
+      <c r="C7" s="37" t="s">
         <v>6</v>
       </c>
-      <c r="D7" s="43" t="s">
+      <c r="D7" s="42" t="s">
         <v>24</v>
       </c>
-      <c r="E7" s="43" t="s">
+      <c r="E7" s="42" t="s">
         <v>21</v>
       </c>
-      <c r="F7" s="47"/>
-      <c r="G7" s="43" t="s">
+      <c r="F7" s="36"/>
+      <c r="G7" s="42" t="s">
         <v>17</v>
       </c>
-      <c r="H7" s="47"/>
-      <c r="I7" s="35">
+      <c r="H7" s="36"/>
+      <c r="I7" s="33">
         <v>10</v>
       </c>
-      <c r="J7" s="27" t="s">
-        <v>42</v>
+      <c r="J7" s="29" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="8" spans="2:28" ht="15.75" customHeight="1">
-      <c r="B8" s="31"/>
-      <c r="C8" s="49"/>
-      <c r="D8" s="47"/>
-      <c r="E8" s="47"/>
-      <c r="F8" s="47"/>
-      <c r="G8" s="47"/>
-      <c r="H8" s="47"/>
-      <c r="I8" s="35"/>
-      <c r="J8" s="27"/>
+      <c r="B8" s="44"/>
+      <c r="C8" s="37"/>
+      <c r="D8" s="36"/>
+      <c r="E8" s="36"/>
+      <c r="F8" s="36"/>
+      <c r="G8" s="36"/>
+      <c r="H8" s="36"/>
+      <c r="I8" s="33"/>
+      <c r="J8" s="29"/>
     </row>
     <row r="9" spans="2:28" ht="15.75" customHeight="1">
-      <c r="B9" s="37">
+      <c r="B9" s="45">
         <v>4</v>
       </c>
-      <c r="C9" s="38" t="s">
+      <c r="C9" s="35" t="s">
         <v>6</v>
       </c>
       <c r="D9" s="39" t="s">
@@ -1295,434 +1256,454 @@
       <c r="E9" s="39" t="s">
         <v>22</v>
       </c>
-      <c r="F9" s="40"/>
+      <c r="F9" s="38"/>
       <c r="G9" s="39" t="s">
         <v>18</v>
       </c>
-      <c r="H9" s="40"/>
-      <c r="I9" s="53">
+      <c r="H9" s="38"/>
+      <c r="I9" s="32">
         <v>4</v>
       </c>
-      <c r="J9" s="55" t="s">
+      <c r="J9" s="29" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="10" spans="2:28" ht="15.75" customHeight="1">
-      <c r="B10" s="37"/>
-      <c r="C10" s="38"/>
-      <c r="D10" s="40"/>
-      <c r="E10" s="40"/>
-      <c r="F10" s="40"/>
-      <c r="G10" s="40"/>
-      <c r="H10" s="40"/>
-      <c r="I10" s="53"/>
-      <c r="J10" s="55"/>
+      <c r="B10" s="45"/>
+      <c r="C10" s="35"/>
+      <c r="D10" s="38"/>
+      <c r="E10" s="38"/>
+      <c r="F10" s="38"/>
+      <c r="G10" s="38"/>
+      <c r="H10" s="38"/>
+      <c r="I10" s="32"/>
+      <c r="J10" s="29"/>
     </row>
     <row r="11" spans="2:28" ht="15.75" customHeight="1">
-      <c r="B11" s="31">
+      <c r="B11" s="44">
         <v>5</v>
       </c>
-      <c r="C11" s="49" t="s">
+      <c r="C11" s="37" t="s">
         <v>10</v>
       </c>
-      <c r="D11" s="47" t="s">
+      <c r="D11" s="36" t="s">
         <v>11</v>
       </c>
-      <c r="E11" s="43" t="s">
+      <c r="E11" s="42" t="s">
         <v>35</v>
       </c>
-      <c r="F11" s="47"/>
-      <c r="G11" s="43" t="s">
+      <c r="F11" s="36"/>
+      <c r="G11" s="42" t="s">
         <v>19</v>
       </c>
-      <c r="H11" s="47"/>
-      <c r="I11" s="35">
+      <c r="H11" s="36"/>
+      <c r="I11" s="33">
         <v>5</v>
       </c>
-      <c r="J11" s="55" t="s">
+      <c r="J11" s="29" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="12" spans="2:28" ht="15.75" customHeight="1">
-      <c r="B12" s="31"/>
-      <c r="C12" s="49"/>
-      <c r="D12" s="47"/>
-      <c r="E12" s="47"/>
-      <c r="F12" s="47"/>
-      <c r="G12" s="47"/>
-      <c r="H12" s="47"/>
-      <c r="I12" s="35"/>
-      <c r="J12" s="55"/>
+      <c r="B12" s="44"/>
+      <c r="C12" s="37"/>
+      <c r="D12" s="36"/>
+      <c r="E12" s="36"/>
+      <c r="F12" s="36"/>
+      <c r="G12" s="36"/>
+      <c r="H12" s="36"/>
+      <c r="I12" s="33"/>
+      <c r="J12" s="29"/>
     </row>
     <row r="13" spans="2:28" ht="15.75" customHeight="1">
-      <c r="B13" s="37">
+      <c r="B13" s="45">
         <v>6</v>
       </c>
-      <c r="C13" s="38" t="s">
+      <c r="C13" s="35" t="s">
         <v>6</v>
       </c>
-      <c r="D13" s="40" t="s">
+      <c r="D13" s="38" t="s">
         <v>54</v>
       </c>
       <c r="E13" s="39" t="s">
         <v>33</v>
       </c>
-      <c r="F13" s="40"/>
+      <c r="F13" s="38"/>
       <c r="G13" s="39" t="s">
         <v>55</v>
       </c>
-      <c r="H13" s="40"/>
-      <c r="I13" s="53">
+      <c r="H13" s="38"/>
+      <c r="I13" s="32">
         <v>9</v>
       </c>
-      <c r="J13" s="55" t="s">
+      <c r="J13" s="29" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="14" spans="2:28" ht="15.75" customHeight="1">
-      <c r="B14" s="37"/>
-      <c r="C14" s="38"/>
-      <c r="D14" s="40"/>
-      <c r="E14" s="40"/>
-      <c r="F14" s="40"/>
-      <c r="G14" s="40"/>
-      <c r="H14" s="40"/>
-      <c r="I14" s="53"/>
-      <c r="J14" s="55"/>
+      <c r="B14" s="45"/>
+      <c r="C14" s="35"/>
+      <c r="D14" s="38"/>
+      <c r="E14" s="38"/>
+      <c r="F14" s="38"/>
+      <c r="G14" s="38"/>
+      <c r="H14" s="38"/>
+      <c r="I14" s="32"/>
+      <c r="J14" s="29"/>
     </row>
     <row r="15" spans="2:28" ht="15.75" customHeight="1">
-      <c r="B15" s="31">
+      <c r="B15" s="44">
         <v>7</v>
       </c>
-      <c r="C15" s="49" t="s">
+      <c r="C15" s="37" t="s">
         <v>6</v>
       </c>
-      <c r="D15" s="43" t="s">
+      <c r="D15" s="42" t="s">
         <v>26</v>
       </c>
-      <c r="E15" s="43" t="s">
+      <c r="E15" s="42" t="s">
         <v>23</v>
       </c>
-      <c r="F15" s="47"/>
-      <c r="G15" s="43" t="s">
+      <c r="F15" s="36"/>
+      <c r="G15" s="42" t="s">
         <v>20</v>
       </c>
-      <c r="H15" s="47"/>
-      <c r="I15" s="35">
+      <c r="H15" s="36"/>
+      <c r="I15" s="33">
         <v>8</v>
       </c>
-      <c r="J15" s="55" t="s">
+      <c r="J15" s="29" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="16" spans="2:28" ht="15.75" customHeight="1">
-      <c r="B16" s="31"/>
-      <c r="C16" s="49"/>
-      <c r="D16" s="47"/>
-      <c r="E16" s="47"/>
-      <c r="F16" s="47"/>
-      <c r="G16" s="47"/>
-      <c r="H16" s="47"/>
-      <c r="I16" s="35"/>
-      <c r="J16" s="55"/>
+      <c r="B16" s="44"/>
+      <c r="C16" s="37"/>
+      <c r="D16" s="36"/>
+      <c r="E16" s="36"/>
+      <c r="F16" s="36"/>
+      <c r="G16" s="36"/>
+      <c r="H16" s="36"/>
+      <c r="I16" s="33"/>
+      <c r="J16" s="29"/>
     </row>
     <row r="17" spans="2:10" ht="15.75" customHeight="1">
-      <c r="B17" s="31"/>
-      <c r="C17" s="49"/>
-      <c r="D17" s="47"/>
-      <c r="E17" s="47"/>
-      <c r="F17" s="47"/>
-      <c r="G17" s="47"/>
-      <c r="H17" s="47"/>
-      <c r="I17" s="35"/>
-      <c r="J17" s="55"/>
+      <c r="B17" s="44"/>
+      <c r="C17" s="37"/>
+      <c r="D17" s="36"/>
+      <c r="E17" s="36"/>
+      <c r="F17" s="36"/>
+      <c r="G17" s="36"/>
+      <c r="H17" s="36"/>
+      <c r="I17" s="33"/>
+      <c r="J17" s="29"/>
     </row>
     <row r="18" spans="2:10" ht="15.75" customHeight="1">
-      <c r="B18" s="37">
+      <c r="B18" s="45">
         <v>8</v>
       </c>
-      <c r="C18" s="38" t="s">
+      <c r="C18" s="35" t="s">
         <v>9</v>
       </c>
       <c r="D18" s="39" t="s">
         <v>52</v>
       </c>
-      <c r="E18" s="40" t="s">
+      <c r="E18" s="38" t="s">
         <v>12</v>
       </c>
-      <c r="F18" s="40"/>
+      <c r="F18" s="38"/>
       <c r="G18" s="39" t="s">
         <v>53</v>
       </c>
-      <c r="H18" s="40"/>
-      <c r="I18" s="53">
+      <c r="H18" s="38"/>
+      <c r="I18" s="32">
         <v>7</v>
       </c>
-      <c r="J18" s="55" t="s">
+      <c r="J18" s="29" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="19" spans="2:10" ht="15.75" customHeight="1">
-      <c r="B19" s="37"/>
-      <c r="C19" s="38"/>
-      <c r="D19" s="40"/>
-      <c r="E19" s="40"/>
-      <c r="F19" s="40"/>
-      <c r="G19" s="40"/>
-      <c r="H19" s="40"/>
-      <c r="I19" s="53"/>
-      <c r="J19" s="55"/>
+      <c r="B19" s="45"/>
+      <c r="C19" s="35"/>
+      <c r="D19" s="38"/>
+      <c r="E19" s="38"/>
+      <c r="F19" s="38"/>
+      <c r="G19" s="38"/>
+      <c r="H19" s="38"/>
+      <c r="I19" s="32"/>
+      <c r="J19" s="29"/>
     </row>
     <row r="20" spans="2:10" ht="15.75" customHeight="1">
-      <c r="B20" s="37"/>
-      <c r="C20" s="38"/>
-      <c r="D20" s="40"/>
-      <c r="E20" s="40"/>
-      <c r="F20" s="40"/>
-      <c r="G20" s="40"/>
-      <c r="H20" s="40"/>
-      <c r="I20" s="53"/>
-      <c r="J20" s="55"/>
+      <c r="B20" s="45"/>
+      <c r="C20" s="35"/>
+      <c r="D20" s="38"/>
+      <c r="E20" s="38"/>
+      <c r="F20" s="38"/>
+      <c r="G20" s="38"/>
+      <c r="H20" s="38"/>
+      <c r="I20" s="32"/>
+      <c r="J20" s="29"/>
     </row>
     <row r="21" spans="2:10" ht="15.75" customHeight="1">
-      <c r="B21" s="31">
+      <c r="B21" s="44">
         <v>9</v>
       </c>
-      <c r="C21" s="29" t="s">
+      <c r="C21" s="41" t="s">
         <v>9</v>
       </c>
-      <c r="D21" s="41" t="s">
+      <c r="D21" s="49" t="s">
         <v>36</v>
       </c>
-      <c r="E21" s="41" t="s">
+      <c r="E21" s="49" t="s">
         <v>28</v>
       </c>
-      <c r="F21" s="33"/>
-      <c r="G21" s="33" t="s">
+      <c r="F21" s="47"/>
+      <c r="G21" s="47" t="s">
         <v>27</v>
       </c>
-      <c r="H21" s="33"/>
-      <c r="I21" s="35">
+      <c r="H21" s="47"/>
+      <c r="I21" s="33">
         <v>3</v>
       </c>
-      <c r="J21" s="55" t="s">
+      <c r="J21" s="29" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="22" spans="2:10" ht="15.75" customHeight="1">
-      <c r="B22" s="31"/>
-      <c r="C22" s="29"/>
-      <c r="D22" s="41"/>
-      <c r="E22" s="33"/>
-      <c r="F22" s="33"/>
-      <c r="G22" s="33"/>
-      <c r="H22" s="33"/>
-      <c r="I22" s="35"/>
-      <c r="J22" s="55"/>
+      <c r="B22" s="44"/>
+      <c r="C22" s="41"/>
+      <c r="D22" s="49"/>
+      <c r="E22" s="47"/>
+      <c r="F22" s="47"/>
+      <c r="G22" s="47"/>
+      <c r="H22" s="47"/>
+      <c r="I22" s="33"/>
+      <c r="J22" s="29"/>
     </row>
     <row r="23" spans="2:10" ht="15.75" customHeight="1">
-      <c r="B23" s="31"/>
-      <c r="C23" s="29"/>
-      <c r="D23" s="41"/>
-      <c r="E23" s="33"/>
-      <c r="F23" s="33"/>
-      <c r="G23" s="33"/>
-      <c r="H23" s="33"/>
-      <c r="I23" s="35"/>
-      <c r="J23" s="55"/>
+      <c r="B23" s="44"/>
+      <c r="C23" s="41"/>
+      <c r="D23" s="49"/>
+      <c r="E23" s="47"/>
+      <c r="F23" s="47"/>
+      <c r="G23" s="47"/>
+      <c r="H23" s="47"/>
+      <c r="I23" s="33"/>
+      <c r="J23" s="29"/>
     </row>
     <row r="24" spans="2:10" ht="15.75" customHeight="1">
-      <c r="B24" s="37">
+      <c r="B24" s="45">
         <v>10</v>
       </c>
-      <c r="C24" s="38" t="s">
+      <c r="C24" s="35" t="s">
         <v>9</v>
       </c>
       <c r="D24" s="39" t="s">
         <v>31</v>
       </c>
-      <c r="E24" s="40" t="s">
+      <c r="E24" s="38" t="s">
         <v>29</v>
       </c>
-      <c r="F24" s="40"/>
+      <c r="F24" s="38"/>
       <c r="G24" s="39" t="s">
         <v>30</v>
       </c>
-      <c r="H24" s="40"/>
-      <c r="I24" s="53" t="s">
+      <c r="H24" s="38"/>
+      <c r="I24" s="32" t="s">
         <v>39</v>
       </c>
-      <c r="J24" s="27" t="s">
+      <c r="J24" s="30" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="25" spans="2:10" ht="15.75" customHeight="1">
-      <c r="B25" s="37"/>
-      <c r="C25" s="38"/>
-      <c r="D25" s="40"/>
-      <c r="E25" s="40"/>
-      <c r="F25" s="40"/>
+      <c r="B25" s="45"/>
+      <c r="C25" s="35"/>
+      <c r="D25" s="38"/>
+      <c r="E25" s="38"/>
+      <c r="F25" s="38"/>
       <c r="G25" s="39"/>
-      <c r="H25" s="40"/>
-      <c r="I25" s="53"/>
-      <c r="J25" s="27"/>
+      <c r="H25" s="38"/>
+      <c r="I25" s="32"/>
+      <c r="J25" s="30"/>
     </row>
     <row r="26" spans="2:10" ht="15.75" customHeight="1">
-      <c r="B26" s="37"/>
-      <c r="C26" s="38"/>
-      <c r="D26" s="40"/>
-      <c r="E26" s="40"/>
-      <c r="F26" s="40"/>
+      <c r="B26" s="45"/>
+      <c r="C26" s="35"/>
+      <c r="D26" s="38"/>
+      <c r="E26" s="38"/>
+      <c r="F26" s="38"/>
       <c r="G26" s="39"/>
-      <c r="H26" s="40"/>
-      <c r="I26" s="53"/>
-      <c r="J26" s="27"/>
+      <c r="H26" s="38"/>
+      <c r="I26" s="32"/>
+      <c r="J26" s="30"/>
     </row>
     <row r="27" spans="2:10" ht="15.75" customHeight="1">
-      <c r="B27" s="31">
+      <c r="B27" s="44">
         <v>11</v>
       </c>
-      <c r="C27" s="29" t="s">
+      <c r="C27" s="41" t="s">
         <v>10</v>
       </c>
-      <c r="D27" s="41" t="s">
+      <c r="D27" s="49" t="s">
         <v>43</v>
       </c>
-      <c r="E27" s="43" t="s">
+      <c r="E27" s="42" t="s">
         <v>44</v>
       </c>
-      <c r="F27" s="33"/>
-      <c r="G27" s="41" t="s">
+      <c r="F27" s="47"/>
+      <c r="G27" s="49" t="s">
         <v>32</v>
       </c>
-      <c r="H27" s="33"/>
-      <c r="I27" s="35" t="s">
+      <c r="H27" s="47"/>
+      <c r="I27" s="33" t="s">
         <v>39</v>
       </c>
-      <c r="J27" s="26" t="s">
+      <c r="J27" s="54" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="28" spans="2:10" ht="15.75" customHeight="1">
-      <c r="B28" s="31"/>
-      <c r="C28" s="29"/>
-      <c r="D28" s="41"/>
-      <c r="E28" s="43"/>
-      <c r="F28" s="33"/>
-      <c r="G28" s="41"/>
-      <c r="H28" s="33"/>
-      <c r="I28" s="35"/>
-      <c r="J28" s="27"/>
+      <c r="B28" s="44"/>
+      <c r="C28" s="41"/>
+      <c r="D28" s="49"/>
+      <c r="E28" s="42"/>
+      <c r="F28" s="47"/>
+      <c r="G28" s="49"/>
+      <c r="H28" s="47"/>
+      <c r="I28" s="33"/>
+      <c r="J28" s="30"/>
     </row>
     <row r="29" spans="2:10" ht="15.75" customHeight="1">
-      <c r="B29" s="31"/>
-      <c r="C29" s="29"/>
-      <c r="D29" s="41"/>
-      <c r="E29" s="43"/>
-      <c r="F29" s="33"/>
-      <c r="G29" s="41"/>
-      <c r="H29" s="33"/>
-      <c r="I29" s="35"/>
-      <c r="J29" s="27"/>
+      <c r="B29" s="44"/>
+      <c r="C29" s="41"/>
+      <c r="D29" s="49"/>
+      <c r="E29" s="42"/>
+      <c r="F29" s="47"/>
+      <c r="G29" s="49"/>
+      <c r="H29" s="47"/>
+      <c r="I29" s="33"/>
+      <c r="J29" s="30"/>
     </row>
     <row r="30" spans="2:10" ht="15.75" customHeight="1">
-      <c r="B30" s="31"/>
-      <c r="C30" s="29"/>
-      <c r="D30" s="41"/>
-      <c r="E30" s="43"/>
-      <c r="F30" s="33"/>
-      <c r="G30" s="41"/>
-      <c r="H30" s="33"/>
-      <c r="I30" s="35"/>
-      <c r="J30" s="27"/>
+      <c r="B30" s="44"/>
+      <c r="C30" s="41"/>
+      <c r="D30" s="49"/>
+      <c r="E30" s="42"/>
+      <c r="F30" s="47"/>
+      <c r="G30" s="49"/>
+      <c r="H30" s="47"/>
+      <c r="I30" s="33"/>
+      <c r="J30" s="30"/>
     </row>
     <row r="31" spans="2:10" ht="15.75" customHeight="1">
-      <c r="B31" s="31"/>
-      <c r="C31" s="29"/>
-      <c r="D31" s="41"/>
-      <c r="E31" s="43"/>
-      <c r="F31" s="33"/>
-      <c r="G31" s="41"/>
-      <c r="H31" s="33"/>
-      <c r="I31" s="35"/>
-      <c r="J31" s="27"/>
+      <c r="B31" s="44"/>
+      <c r="C31" s="41"/>
+      <c r="D31" s="49"/>
+      <c r="E31" s="42"/>
+      <c r="F31" s="47"/>
+      <c r="G31" s="49"/>
+      <c r="H31" s="47"/>
+      <c r="I31" s="33"/>
+      <c r="J31" s="30"/>
     </row>
     <row r="32" spans="2:10" ht="15.75" customHeight="1">
-      <c r="B32" s="32"/>
-      <c r="C32" s="30"/>
-      <c r="D32" s="42"/>
-      <c r="E32" s="44"/>
-      <c r="F32" s="34"/>
-      <c r="G32" s="42"/>
-      <c r="H32" s="34"/>
-      <c r="I32" s="36"/>
-      <c r="J32" s="28"/>
+      <c r="B32" s="44"/>
+      <c r="C32" s="41"/>
+      <c r="D32" s="49"/>
+      <c r="E32" s="42"/>
+      <c r="F32" s="47"/>
+      <c r="G32" s="49"/>
+      <c r="H32" s="47"/>
+      <c r="I32" s="33"/>
+      <c r="J32" s="30"/>
     </row>
     <row r="33" spans="2:10" ht="63" customHeight="1">
-      <c r="B33" s="17">
+      <c r="B33" s="19">
         <v>12</v>
       </c>
-      <c r="C33" s="16" t="s">
+      <c r="C33" s="20" t="s">
         <v>10</v>
       </c>
-      <c r="D33" s="19" t="s">
+      <c r="D33" s="21" t="s">
         <v>45</v>
       </c>
-      <c r="E33" s="20" t="s">
+      <c r="E33" s="22" t="s">
         <v>46</v>
       </c>
-      <c r="F33" s="20"/>
-      <c r="G33" s="21" t="s">
+      <c r="F33" s="22"/>
+      <c r="G33" s="23" t="s">
         <v>47</v>
       </c>
-      <c r="H33" s="20"/>
-      <c r="I33" s="18" t="s">
-        <v>39</v>
-      </c>
-      <c r="J33" s="15" t="s">
+      <c r="H33" s="22"/>
+      <c r="I33" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="J33" s="6" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="34" spans="2:10" ht="63" customHeight="1" thickBot="1">
-      <c r="B34" s="6">
+    <row r="34" spans="2:10" ht="63" customHeight="1">
+      <c r="B34" s="8">
         <v>13</v>
       </c>
       <c r="C34" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="D34" s="14" t="s">
+      <c r="D34" s="12" t="s">
         <v>48</v>
       </c>
-      <c r="E34" s="14" t="s">
+      <c r="E34" s="12" t="s">
         <v>50</v>
       </c>
       <c r="F34" s="13"/>
-      <c r="G34" s="14" t="s">
+      <c r="G34" s="12" t="s">
         <v>49</v>
       </c>
       <c r="H34" s="13"/>
-      <c r="I34" s="8">
+      <c r="I34" s="9">
         <v>6</v>
       </c>
-      <c r="J34" s="22" t="s">
+      <c r="J34" s="10" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="35" spans="2:10" ht="15.75" customHeight="1" thickBot="1"/>
-    <row r="36" spans="2:10" ht="15.75" customHeight="1" thickBot="1">
-      <c r="B36" s="23" t="s">
+    <row r="35" spans="2:10" ht="63" customHeight="1" thickBot="1">
+      <c r="B35" s="24">
+        <v>14</v>
+      </c>
+      <c r="C35" s="25" t="s">
+        <v>38</v>
+      </c>
+      <c r="D35" s="26" t="s">
+        <v>57</v>
+      </c>
+      <c r="E35" s="26"/>
+      <c r="F35" s="27"/>
+      <c r="G35" s="26"/>
+      <c r="H35" s="27"/>
+      <c r="I35" s="28" t="s">
+        <v>58</v>
+      </c>
+      <c r="J35" s="18" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="36" spans="2:10" ht="15.75" customHeight="1" thickBot="1"/>
+    <row r="37" spans="2:10" ht="15.75" customHeight="1" thickBot="1">
+      <c r="B37" s="51" t="s">
         <v>51</v>
       </c>
-      <c r="C36" s="24"/>
-      <c r="D36" s="24"/>
-      <c r="E36" s="24"/>
-      <c r="F36" s="24"/>
-      <c r="G36" s="24"/>
-      <c r="H36" s="24"/>
-      <c r="I36" s="24"/>
-      <c r="J36" s="25"/>
-    </row>
-    <row r="37" spans="2:10" ht="15.75" customHeight="1"/>
+      <c r="C37" s="52"/>
+      <c r="D37" s="52"/>
+      <c r="E37" s="52"/>
+      <c r="F37" s="52"/>
+      <c r="G37" s="52"/>
+      <c r="H37" s="52"/>
+      <c r="I37" s="52"/>
+      <c r="J37" s="53"/>
+    </row>
     <row r="38" spans="2:10" ht="15.75" customHeight="1"/>
     <row r="39" spans="2:10" ht="15.75" customHeight="1"/>
     <row r="40" spans="2:10" ht="15.75" customHeight="1"/>
@@ -2678,59 +2659,44 @@
     <row r="990" ht="15.75" customHeight="1"/>
     <row r="991" ht="15.75" customHeight="1"/>
     <row r="992" ht="15.75" customHeight="1"/>
+    <row r="993" ht="15.75" customHeight="1"/>
   </sheetData>
-  <autoFilter ref="B2:J34"/>
+  <autoFilter ref="B2:J35"/>
   <mergeCells count="100">
-    <mergeCell ref="J13:J14"/>
-    <mergeCell ref="J15:J17"/>
-    <mergeCell ref="J18:J20"/>
-    <mergeCell ref="J21:J23"/>
-    <mergeCell ref="J24:J26"/>
-    <mergeCell ref="J3:J4"/>
-    <mergeCell ref="J5:J6"/>
-    <mergeCell ref="J7:J8"/>
-    <mergeCell ref="J9:J10"/>
-    <mergeCell ref="J11:J12"/>
-    <mergeCell ref="I13:I14"/>
-    <mergeCell ref="I15:I17"/>
-    <mergeCell ref="I18:I20"/>
-    <mergeCell ref="I21:I23"/>
-    <mergeCell ref="I24:I26"/>
-    <mergeCell ref="I3:I4"/>
-    <mergeCell ref="I5:I6"/>
-    <mergeCell ref="I7:I8"/>
-    <mergeCell ref="I9:I10"/>
-    <mergeCell ref="I11:I12"/>
-    <mergeCell ref="C9:C10"/>
-    <mergeCell ref="D11:D12"/>
-    <mergeCell ref="C11:C12"/>
-    <mergeCell ref="D13:D14"/>
-    <mergeCell ref="C13:C14"/>
-    <mergeCell ref="D9:D10"/>
-    <mergeCell ref="C3:C4"/>
-    <mergeCell ref="D3:D4"/>
-    <mergeCell ref="C5:C6"/>
-    <mergeCell ref="D5:D6"/>
-    <mergeCell ref="C7:C8"/>
-    <mergeCell ref="D7:D8"/>
-    <mergeCell ref="B3:B4"/>
-    <mergeCell ref="B5:B6"/>
-    <mergeCell ref="B7:B8"/>
-    <mergeCell ref="B9:B10"/>
-    <mergeCell ref="B11:B12"/>
-    <mergeCell ref="B13:B14"/>
-    <mergeCell ref="B15:B17"/>
-    <mergeCell ref="G18:G20"/>
-    <mergeCell ref="E18:E20"/>
-    <mergeCell ref="C18:C20"/>
-    <mergeCell ref="B18:B20"/>
-    <mergeCell ref="F18:F20"/>
-    <mergeCell ref="E15:E17"/>
-    <mergeCell ref="D15:D17"/>
-    <mergeCell ref="D18:D20"/>
-    <mergeCell ref="F13:F14"/>
-    <mergeCell ref="C15:C17"/>
-    <mergeCell ref="F15:F17"/>
+    <mergeCell ref="B37:J37"/>
+    <mergeCell ref="J27:J32"/>
+    <mergeCell ref="C27:C32"/>
+    <mergeCell ref="B27:B32"/>
+    <mergeCell ref="H27:H32"/>
+    <mergeCell ref="I27:I32"/>
+    <mergeCell ref="B24:B26"/>
+    <mergeCell ref="C24:C26"/>
+    <mergeCell ref="D24:D26"/>
+    <mergeCell ref="E24:E26"/>
+    <mergeCell ref="F24:F26"/>
+    <mergeCell ref="H24:H26"/>
+    <mergeCell ref="G27:G32"/>
+    <mergeCell ref="F27:F32"/>
+    <mergeCell ref="E27:E32"/>
+    <mergeCell ref="D27:D32"/>
+    <mergeCell ref="G24:G26"/>
+    <mergeCell ref="F3:F4"/>
+    <mergeCell ref="F5:F6"/>
+    <mergeCell ref="F7:F8"/>
+    <mergeCell ref="F9:F10"/>
+    <mergeCell ref="F11:F12"/>
+    <mergeCell ref="F21:F23"/>
+    <mergeCell ref="B21:B23"/>
+    <mergeCell ref="C21:C23"/>
+    <mergeCell ref="G21:G23"/>
+    <mergeCell ref="H21:H23"/>
+    <mergeCell ref="D21:D23"/>
+    <mergeCell ref="E21:E23"/>
+    <mergeCell ref="E5:E6"/>
+    <mergeCell ref="E7:E8"/>
+    <mergeCell ref="E9:E10"/>
+    <mergeCell ref="E11:E12"/>
+    <mergeCell ref="E13:E14"/>
     <mergeCell ref="H18:H20"/>
     <mergeCell ref="E3:E4"/>
     <mergeCell ref="G3:G4"/>
@@ -2747,40 +2713,56 @@
     <mergeCell ref="G11:G12"/>
     <mergeCell ref="G13:G14"/>
     <mergeCell ref="G15:G17"/>
-    <mergeCell ref="E5:E6"/>
-    <mergeCell ref="E7:E8"/>
-    <mergeCell ref="E9:E10"/>
-    <mergeCell ref="E11:E12"/>
-    <mergeCell ref="E13:E14"/>
-    <mergeCell ref="F21:F23"/>
-    <mergeCell ref="B21:B23"/>
-    <mergeCell ref="C21:C23"/>
-    <mergeCell ref="G21:G23"/>
-    <mergeCell ref="H21:H23"/>
-    <mergeCell ref="D21:D23"/>
-    <mergeCell ref="E21:E23"/>
-    <mergeCell ref="F3:F4"/>
-    <mergeCell ref="F5:F6"/>
-    <mergeCell ref="F7:F8"/>
-    <mergeCell ref="F9:F10"/>
-    <mergeCell ref="F11:F12"/>
-    <mergeCell ref="H24:H26"/>
-    <mergeCell ref="G27:G32"/>
-    <mergeCell ref="F27:F32"/>
-    <mergeCell ref="E27:E32"/>
-    <mergeCell ref="D27:D32"/>
-    <mergeCell ref="G24:G26"/>
-    <mergeCell ref="B24:B26"/>
-    <mergeCell ref="C24:C26"/>
-    <mergeCell ref="D24:D26"/>
-    <mergeCell ref="E24:E26"/>
-    <mergeCell ref="F24:F26"/>
-    <mergeCell ref="B36:J36"/>
-    <mergeCell ref="J27:J32"/>
-    <mergeCell ref="C27:C32"/>
-    <mergeCell ref="B27:B32"/>
-    <mergeCell ref="H27:H32"/>
-    <mergeCell ref="I27:I32"/>
+    <mergeCell ref="B13:B14"/>
+    <mergeCell ref="B15:B17"/>
+    <mergeCell ref="G18:G20"/>
+    <mergeCell ref="E18:E20"/>
+    <mergeCell ref="C18:C20"/>
+    <mergeCell ref="B18:B20"/>
+    <mergeCell ref="F18:F20"/>
+    <mergeCell ref="E15:E17"/>
+    <mergeCell ref="D15:D17"/>
+    <mergeCell ref="D18:D20"/>
+    <mergeCell ref="F13:F14"/>
+    <mergeCell ref="C15:C17"/>
+    <mergeCell ref="F15:F17"/>
+    <mergeCell ref="B3:B4"/>
+    <mergeCell ref="B5:B6"/>
+    <mergeCell ref="B7:B8"/>
+    <mergeCell ref="B9:B10"/>
+    <mergeCell ref="B11:B12"/>
+    <mergeCell ref="C3:C4"/>
+    <mergeCell ref="D3:D4"/>
+    <mergeCell ref="C5:C6"/>
+    <mergeCell ref="D5:D6"/>
+    <mergeCell ref="C7:C8"/>
+    <mergeCell ref="D7:D8"/>
+    <mergeCell ref="C9:C10"/>
+    <mergeCell ref="D11:D12"/>
+    <mergeCell ref="C11:C12"/>
+    <mergeCell ref="D13:D14"/>
+    <mergeCell ref="C13:C14"/>
+    <mergeCell ref="D9:D10"/>
+    <mergeCell ref="I3:I4"/>
+    <mergeCell ref="I5:I6"/>
+    <mergeCell ref="I7:I8"/>
+    <mergeCell ref="I9:I10"/>
+    <mergeCell ref="I11:I12"/>
+    <mergeCell ref="I13:I14"/>
+    <mergeCell ref="I15:I17"/>
+    <mergeCell ref="I18:I20"/>
+    <mergeCell ref="I21:I23"/>
+    <mergeCell ref="I24:I26"/>
+    <mergeCell ref="J3:J4"/>
+    <mergeCell ref="J5:J6"/>
+    <mergeCell ref="J7:J8"/>
+    <mergeCell ref="J9:J10"/>
+    <mergeCell ref="J11:J12"/>
+    <mergeCell ref="J13:J14"/>
+    <mergeCell ref="J15:J17"/>
+    <mergeCell ref="J18:J20"/>
+    <mergeCell ref="J21:J23"/>
+    <mergeCell ref="J24:J26"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape" r:id="rId1"/>

</xml_diff>

<commit_message>
Modification du tableau d'analyses
</commit_message>
<xml_diff>
--- a/Analyses/Modèle-audit-SEO.xlsx
+++ b/Analyses/Modèle-audit-SEO.xlsx
@@ -7,10 +7,10 @@
     <workbookView xWindow="945" yWindow="615" windowWidth="27855" windowHeight="16440" tabRatio="500"/>
   </bookViews>
   <sheets>
-    <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
+    <sheet name="SEO" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Feuil1!$B$2:$J$35</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">SEO!$B$2:$J$35</definedName>
   </definedNames>
   <calcPr calcId="125725"/>
   <extLst>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="59">
   <si>
     <t>Catégorie</t>
   </si>
@@ -320,13 +320,14 @@
  redistribuer. Enlever div Keyword</t>
   </si>
   <si>
-    <t>12 ?</t>
-  </si>
-  <si>
     <t xml:space="preserve"> Police</t>
   </si>
   <si>
-    <t>11 ?</t>
+    <t>PERFORMANCE &amp;
+ ACCESSIBILITÉ</t>
+  </si>
+  <si>
+    <t>Mettre une taille de police convenable (lisible)</t>
   </si>
 </sst>
 </file>
@@ -688,7 +689,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="9" fillId="5" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="55">
+  <cellXfs count="56">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -705,9 +706,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -718,9 +716,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -763,9 +758,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -774,83 +766,95 @@
     <xf numFmtId="0" fontId="7" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1068,7 +1072,7 @@
   <dimension ref="B1:AB993"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="J7" sqref="J7:J8"/>
+      <selection activeCell="B37" sqref="B37:J37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.33203125" defaultRowHeight="15" customHeight="1"/>
@@ -1087,31 +1091,31 @@
   <sheetData>
     <row r="1" spans="2:28" ht="15" customHeight="1" thickBot="1"/>
     <row r="2" spans="2:28" ht="15.75" customHeight="1" thickBot="1">
-      <c r="B2" s="14" t="s">
+      <c r="B2" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="C2" s="15" t="s">
+      <c r="C2" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="15" t="s">
+      <c r="D2" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="E2" s="15" t="s">
+      <c r="E2" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="F2" s="15" t="s">
+      <c r="F2" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="G2" s="15" t="s">
+      <c r="G2" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="H2" s="15" t="s">
+      <c r="H2" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="I2" s="16" t="s">
+      <c r="I2" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="J2" s="17" t="s">
+      <c r="J2" s="15" t="s">
         <v>40</v>
       </c>
       <c r="K2" s="5"/>
@@ -1134,84 +1138,84 @@
       <c r="AB2" s="1"/>
     </row>
     <row r="3" spans="2:28" ht="15.75" customHeight="1">
-      <c r="B3" s="43">
+      <c r="B3" s="48">
         <v>1</v>
       </c>
-      <c r="C3" s="40" t="s">
+      <c r="C3" s="49" t="s">
         <v>38</v>
       </c>
-      <c r="D3" s="40" t="s">
+      <c r="D3" s="49" t="s">
         <v>7</v>
       </c>
-      <c r="E3" s="46" t="s">
+      <c r="E3" s="43" t="s">
         <v>14</v>
       </c>
-      <c r="F3" s="46" t="s">
+      <c r="F3" s="43" t="s">
         <v>37</v>
       </c>
-      <c r="G3" s="46" t="s">
+      <c r="G3" s="43" t="s">
         <v>15</v>
       </c>
-      <c r="H3" s="48"/>
-      <c r="I3" s="34">
+      <c r="H3" s="46"/>
+      <c r="I3" s="50">
         <v>1</v>
       </c>
-      <c r="J3" s="31" t="s">
+      <c r="J3" s="52" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="4" spans="2:28" ht="15.75" customHeight="1">
-      <c r="B4" s="44"/>
-      <c r="C4" s="41"/>
-      <c r="D4" s="41"/>
-      <c r="E4" s="47"/>
-      <c r="F4" s="47"/>
-      <c r="G4" s="47"/>
-      <c r="H4" s="47"/>
-      <c r="I4" s="33"/>
-      <c r="J4" s="29"/>
+      <c r="B4" s="34"/>
+      <c r="C4" s="33"/>
+      <c r="D4" s="33"/>
+      <c r="E4" s="35"/>
+      <c r="F4" s="35"/>
+      <c r="G4" s="35"/>
+      <c r="H4" s="35"/>
+      <c r="I4" s="36"/>
+      <c r="J4" s="53"/>
     </row>
     <row r="5" spans="2:28" ht="15.75" customHeight="1">
-      <c r="B5" s="45">
+      <c r="B5" s="37">
         <v>2</v>
       </c>
-      <c r="C5" s="35" t="s">
+      <c r="C5" s="38" t="s">
         <v>38</v>
       </c>
-      <c r="D5" s="38" t="s">
+      <c r="D5" s="40" t="s">
         <v>8</v>
       </c>
       <c r="E5" s="39" t="s">
         <v>14</v>
       </c>
-      <c r="F5" s="50"/>
+      <c r="F5" s="44"/>
       <c r="G5" s="39" t="s">
         <v>16</v>
       </c>
-      <c r="H5" s="38"/>
-      <c r="I5" s="32">
+      <c r="H5" s="40"/>
+      <c r="I5" s="51">
         <v>2</v>
       </c>
-      <c r="J5" s="29" t="s">
+      <c r="J5" s="53" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="6" spans="2:28" ht="15.75" customHeight="1">
-      <c r="B6" s="45"/>
-      <c r="C6" s="35"/>
-      <c r="D6" s="38"/>
-      <c r="E6" s="38"/>
-      <c r="F6" s="50"/>
-      <c r="G6" s="38"/>
-      <c r="H6" s="38"/>
-      <c r="I6" s="32"/>
-      <c r="J6" s="29"/>
+      <c r="B6" s="37"/>
+      <c r="C6" s="38"/>
+      <c r="D6" s="40"/>
+      <c r="E6" s="40"/>
+      <c r="F6" s="44"/>
+      <c r="G6" s="40"/>
+      <c r="H6" s="40"/>
+      <c r="I6" s="51"/>
+      <c r="J6" s="53"/>
     </row>
     <row r="7" spans="2:28" ht="15.75" customHeight="1">
-      <c r="B7" s="44">
+      <c r="B7" s="34">
         <v>3</v>
       </c>
-      <c r="C7" s="37" t="s">
+      <c r="C7" s="47" t="s">
         <v>6</v>
       </c>
       <c r="D7" s="42" t="s">
@@ -1220,34 +1224,34 @@
       <c r="E7" s="42" t="s">
         <v>21</v>
       </c>
-      <c r="F7" s="36"/>
+      <c r="F7" s="45"/>
       <c r="G7" s="42" t="s">
         <v>17</v>
       </c>
-      <c r="H7" s="36"/>
-      <c r="I7" s="33">
+      <c r="H7" s="45"/>
+      <c r="I7" s="36">
         <v>10</v>
       </c>
-      <c r="J7" s="29" t="s">
+      <c r="J7" s="53" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="8" spans="2:28" ht="15.75" customHeight="1">
-      <c r="B8" s="44"/>
-      <c r="C8" s="37"/>
-      <c r="D8" s="36"/>
-      <c r="E8" s="36"/>
-      <c r="F8" s="36"/>
-      <c r="G8" s="36"/>
-      <c r="H8" s="36"/>
-      <c r="I8" s="33"/>
-      <c r="J8" s="29"/>
+      <c r="B8" s="34"/>
+      <c r="C8" s="47"/>
+      <c r="D8" s="45"/>
+      <c r="E8" s="45"/>
+      <c r="F8" s="45"/>
+      <c r="G8" s="45"/>
+      <c r="H8" s="45"/>
+      <c r="I8" s="36"/>
+      <c r="J8" s="53"/>
     </row>
     <row r="9" spans="2:28" ht="15.75" customHeight="1">
-      <c r="B9" s="45">
+      <c r="B9" s="37">
         <v>4</v>
       </c>
-      <c r="C9" s="35" t="s">
+      <c r="C9" s="38" t="s">
         <v>6</v>
       </c>
       <c r="D9" s="39" t="s">
@@ -1256,106 +1260,106 @@
       <c r="E9" s="39" t="s">
         <v>22</v>
       </c>
-      <c r="F9" s="38"/>
+      <c r="F9" s="40"/>
       <c r="G9" s="39" t="s">
         <v>18</v>
       </c>
-      <c r="H9" s="38"/>
-      <c r="I9" s="32">
+      <c r="H9" s="40"/>
+      <c r="I9" s="51">
         <v>4</v>
       </c>
-      <c r="J9" s="29" t="s">
+      <c r="J9" s="53" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="10" spans="2:28" ht="15.75" customHeight="1">
-      <c r="B10" s="45"/>
-      <c r="C10" s="35"/>
-      <c r="D10" s="38"/>
-      <c r="E10" s="38"/>
-      <c r="F10" s="38"/>
-      <c r="G10" s="38"/>
-      <c r="H10" s="38"/>
-      <c r="I10" s="32"/>
-      <c r="J10" s="29"/>
+      <c r="B10" s="37"/>
+      <c r="C10" s="38"/>
+      <c r="D10" s="40"/>
+      <c r="E10" s="40"/>
+      <c r="F10" s="40"/>
+      <c r="G10" s="40"/>
+      <c r="H10" s="40"/>
+      <c r="I10" s="51"/>
+      <c r="J10" s="53"/>
     </row>
     <row r="11" spans="2:28" ht="15.75" customHeight="1">
-      <c r="B11" s="44">
+      <c r="B11" s="34">
         <v>5</v>
       </c>
-      <c r="C11" s="37" t="s">
+      <c r="C11" s="47" t="s">
         <v>10</v>
       </c>
-      <c r="D11" s="36" t="s">
+      <c r="D11" s="45" t="s">
         <v>11</v>
       </c>
       <c r="E11" s="42" t="s">
         <v>35</v>
       </c>
-      <c r="F11" s="36"/>
+      <c r="F11" s="45"/>
       <c r="G11" s="42" t="s">
         <v>19</v>
       </c>
-      <c r="H11" s="36"/>
-      <c r="I11" s="33">
+      <c r="H11" s="45"/>
+      <c r="I11" s="36">
         <v>5</v>
       </c>
-      <c r="J11" s="29" t="s">
+      <c r="J11" s="53" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="12" spans="2:28" ht="15.75" customHeight="1">
-      <c r="B12" s="44"/>
-      <c r="C12" s="37"/>
-      <c r="D12" s="36"/>
-      <c r="E12" s="36"/>
-      <c r="F12" s="36"/>
-      <c r="G12" s="36"/>
-      <c r="H12" s="36"/>
-      <c r="I12" s="33"/>
-      <c r="J12" s="29"/>
+      <c r="B12" s="34"/>
+      <c r="C12" s="47"/>
+      <c r="D12" s="45"/>
+      <c r="E12" s="45"/>
+      <c r="F12" s="45"/>
+      <c r="G12" s="45"/>
+      <c r="H12" s="45"/>
+      <c r="I12" s="36"/>
+      <c r="J12" s="53"/>
     </row>
     <row r="13" spans="2:28" ht="15.75" customHeight="1">
-      <c r="B13" s="45">
+      <c r="B13" s="37">
         <v>6</v>
       </c>
-      <c r="C13" s="35" t="s">
+      <c r="C13" s="38" t="s">
         <v>6</v>
       </c>
-      <c r="D13" s="38" t="s">
+      <c r="D13" s="40" t="s">
         <v>54</v>
       </c>
       <c r="E13" s="39" t="s">
         <v>33</v>
       </c>
-      <c r="F13" s="38"/>
+      <c r="F13" s="40"/>
       <c r="G13" s="39" t="s">
         <v>55</v>
       </c>
-      <c r="H13" s="38"/>
-      <c r="I13" s="32">
+      <c r="H13" s="40"/>
+      <c r="I13" s="51">
         <v>9</v>
       </c>
-      <c r="J13" s="29" t="s">
+      <c r="J13" s="53" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="14" spans="2:28" ht="15.75" customHeight="1">
-      <c r="B14" s="45"/>
-      <c r="C14" s="35"/>
-      <c r="D14" s="38"/>
-      <c r="E14" s="38"/>
-      <c r="F14" s="38"/>
-      <c r="G14" s="38"/>
-      <c r="H14" s="38"/>
-      <c r="I14" s="32"/>
-      <c r="J14" s="29"/>
+      <c r="B14" s="37"/>
+      <c r="C14" s="38"/>
+      <c r="D14" s="40"/>
+      <c r="E14" s="40"/>
+      <c r="F14" s="40"/>
+      <c r="G14" s="40"/>
+      <c r="H14" s="40"/>
+      <c r="I14" s="51"/>
+      <c r="J14" s="53"/>
     </row>
     <row r="15" spans="2:28" ht="15.75" customHeight="1">
-      <c r="B15" s="44">
+      <c r="B15" s="34">
         <v>7</v>
       </c>
-      <c r="C15" s="37" t="s">
+      <c r="C15" s="47" t="s">
         <v>6</v>
       </c>
       <c r="D15" s="42" t="s">
@@ -1364,347 +1368,359 @@
       <c r="E15" s="42" t="s">
         <v>23</v>
       </c>
-      <c r="F15" s="36"/>
+      <c r="F15" s="45"/>
       <c r="G15" s="42" t="s">
         <v>20</v>
       </c>
-      <c r="H15" s="36"/>
-      <c r="I15" s="33">
+      <c r="H15" s="45"/>
+      <c r="I15" s="36">
         <v>8</v>
       </c>
-      <c r="J15" s="29" t="s">
+      <c r="J15" s="53" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="16" spans="2:28" ht="15.75" customHeight="1">
-      <c r="B16" s="44"/>
-      <c r="C16" s="37"/>
-      <c r="D16" s="36"/>
-      <c r="E16" s="36"/>
-      <c r="F16" s="36"/>
-      <c r="G16" s="36"/>
-      <c r="H16" s="36"/>
-      <c r="I16" s="33"/>
-      <c r="J16" s="29"/>
+      <c r="B16" s="34"/>
+      <c r="C16" s="47"/>
+      <c r="D16" s="45"/>
+      <c r="E16" s="45"/>
+      <c r="F16" s="45"/>
+      <c r="G16" s="45"/>
+      <c r="H16" s="45"/>
+      <c r="I16" s="36"/>
+      <c r="J16" s="53"/>
     </row>
     <row r="17" spans="2:10" ht="15.75" customHeight="1">
-      <c r="B17" s="44"/>
-      <c r="C17" s="37"/>
-      <c r="D17" s="36"/>
-      <c r="E17" s="36"/>
-      <c r="F17" s="36"/>
-      <c r="G17" s="36"/>
-      <c r="H17" s="36"/>
-      <c r="I17" s="33"/>
-      <c r="J17" s="29"/>
+      <c r="B17" s="34"/>
+      <c r="C17" s="47"/>
+      <c r="D17" s="45"/>
+      <c r="E17" s="45"/>
+      <c r="F17" s="45"/>
+      <c r="G17" s="45"/>
+      <c r="H17" s="45"/>
+      <c r="I17" s="36"/>
+      <c r="J17" s="53"/>
     </row>
     <row r="18" spans="2:10" ht="15.75" customHeight="1">
-      <c r="B18" s="45">
+      <c r="B18" s="37">
         <v>8</v>
       </c>
-      <c r="C18" s="35" t="s">
+      <c r="C18" s="38" t="s">
         <v>9</v>
       </c>
       <c r="D18" s="39" t="s">
         <v>52</v>
       </c>
-      <c r="E18" s="38" t="s">
+      <c r="E18" s="40" t="s">
         <v>12</v>
       </c>
-      <c r="F18" s="38"/>
+      <c r="F18" s="40"/>
       <c r="G18" s="39" t="s">
         <v>53</v>
       </c>
-      <c r="H18" s="38"/>
-      <c r="I18" s="32">
+      <c r="H18" s="40"/>
+      <c r="I18" s="51">
         <v>7</v>
       </c>
-      <c r="J18" s="29" t="s">
+      <c r="J18" s="53" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="19" spans="2:10" ht="15.75" customHeight="1">
-      <c r="B19" s="45"/>
-      <c r="C19" s="35"/>
-      <c r="D19" s="38"/>
-      <c r="E19" s="38"/>
-      <c r="F19" s="38"/>
-      <c r="G19" s="38"/>
-      <c r="H19" s="38"/>
-      <c r="I19" s="32"/>
-      <c r="J19" s="29"/>
+      <c r="B19" s="37"/>
+      <c r="C19" s="38"/>
+      <c r="D19" s="40"/>
+      <c r="E19" s="40"/>
+      <c r="F19" s="40"/>
+      <c r="G19" s="40"/>
+      <c r="H19" s="40"/>
+      <c r="I19" s="51"/>
+      <c r="J19" s="53"/>
     </row>
     <row r="20" spans="2:10" ht="15.75" customHeight="1">
-      <c r="B20" s="45"/>
-      <c r="C20" s="35"/>
-      <c r="D20" s="38"/>
-      <c r="E20" s="38"/>
-      <c r="F20" s="38"/>
-      <c r="G20" s="38"/>
-      <c r="H20" s="38"/>
-      <c r="I20" s="32"/>
-      <c r="J20" s="29"/>
+      <c r="B20" s="37"/>
+      <c r="C20" s="38"/>
+      <c r="D20" s="40"/>
+      <c r="E20" s="40"/>
+      <c r="F20" s="40"/>
+      <c r="G20" s="40"/>
+      <c r="H20" s="40"/>
+      <c r="I20" s="51"/>
+      <c r="J20" s="53"/>
     </row>
     <row r="21" spans="2:10" ht="15.75" customHeight="1">
-      <c r="B21" s="44">
+      <c r="B21" s="34">
         <v>9</v>
       </c>
-      <c r="C21" s="41" t="s">
+      <c r="C21" s="33" t="s">
         <v>9</v>
       </c>
-      <c r="D21" s="49" t="s">
+      <c r="D21" s="41" t="s">
         <v>36</v>
       </c>
-      <c r="E21" s="49" t="s">
+      <c r="E21" s="41" t="s">
         <v>28</v>
       </c>
-      <c r="F21" s="47"/>
-      <c r="G21" s="47" t="s">
+      <c r="F21" s="35"/>
+      <c r="G21" s="35" t="s">
         <v>27</v>
       </c>
-      <c r="H21" s="47"/>
-      <c r="I21" s="33">
+      <c r="H21" s="35"/>
+      <c r="I21" s="36">
         <v>3</v>
       </c>
-      <c r="J21" s="29" t="s">
+      <c r="J21" s="53" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="22" spans="2:10" ht="15.75" customHeight="1">
-      <c r="B22" s="44"/>
-      <c r="C22" s="41"/>
-      <c r="D22" s="49"/>
-      <c r="E22" s="47"/>
-      <c r="F22" s="47"/>
-      <c r="G22" s="47"/>
-      <c r="H22" s="47"/>
-      <c r="I22" s="33"/>
-      <c r="J22" s="29"/>
+      <c r="B22" s="34"/>
+      <c r="C22" s="33"/>
+      <c r="D22" s="41"/>
+      <c r="E22" s="35"/>
+      <c r="F22" s="35"/>
+      <c r="G22" s="35"/>
+      <c r="H22" s="35"/>
+      <c r="I22" s="36"/>
+      <c r="J22" s="53"/>
     </row>
     <row r="23" spans="2:10" ht="15.75" customHeight="1">
-      <c r="B23" s="44"/>
-      <c r="C23" s="41"/>
-      <c r="D23" s="49"/>
-      <c r="E23" s="47"/>
-      <c r="F23" s="47"/>
-      <c r="G23" s="47"/>
-      <c r="H23" s="47"/>
-      <c r="I23" s="33"/>
-      <c r="J23" s="29"/>
+      <c r="B23" s="34"/>
+      <c r="C23" s="33"/>
+      <c r="D23" s="41"/>
+      <c r="E23" s="35"/>
+      <c r="F23" s="35"/>
+      <c r="G23" s="35"/>
+      <c r="H23" s="35"/>
+      <c r="I23" s="36"/>
+      <c r="J23" s="53"/>
     </row>
     <row r="24" spans="2:10" ht="15.75" customHeight="1">
-      <c r="B24" s="45">
+      <c r="B24" s="37">
         <v>10</v>
       </c>
-      <c r="C24" s="35" t="s">
+      <c r="C24" s="38" t="s">
         <v>9</v>
       </c>
       <c r="D24" s="39" t="s">
         <v>31</v>
       </c>
-      <c r="E24" s="38" t="s">
+      <c r="E24" s="40" t="s">
         <v>29</v>
       </c>
-      <c r="F24" s="38"/>
+      <c r="F24" s="40"/>
       <c r="G24" s="39" t="s">
         <v>30</v>
       </c>
-      <c r="H24" s="38"/>
-      <c r="I24" s="32" t="s">
+      <c r="H24" s="40"/>
+      <c r="I24" s="51" t="s">
         <v>39</v>
       </c>
-      <c r="J24" s="30" t="s">
+      <c r="J24" s="32" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="25" spans="2:10" ht="15.75" customHeight="1">
-      <c r="B25" s="45"/>
-      <c r="C25" s="35"/>
-      <c r="D25" s="38"/>
-      <c r="E25" s="38"/>
-      <c r="F25" s="38"/>
+      <c r="B25" s="37"/>
+      <c r="C25" s="38"/>
+      <c r="D25" s="40"/>
+      <c r="E25" s="40"/>
+      <c r="F25" s="40"/>
       <c r="G25" s="39"/>
-      <c r="H25" s="38"/>
-      <c r="I25" s="32"/>
-      <c r="J25" s="30"/>
+      <c r="H25" s="40"/>
+      <c r="I25" s="51"/>
+      <c r="J25" s="32"/>
     </row>
     <row r="26" spans="2:10" ht="15.75" customHeight="1">
-      <c r="B26" s="45"/>
-      <c r="C26" s="35"/>
-      <c r="D26" s="38"/>
-      <c r="E26" s="38"/>
-      <c r="F26" s="38"/>
+      <c r="B26" s="37"/>
+      <c r="C26" s="38"/>
+      <c r="D26" s="40"/>
+      <c r="E26" s="40"/>
+      <c r="F26" s="40"/>
       <c r="G26" s="39"/>
-      <c r="H26" s="38"/>
-      <c r="I26" s="32"/>
-      <c r="J26" s="30"/>
+      <c r="H26" s="40"/>
+      <c r="I26" s="51"/>
+      <c r="J26" s="32"/>
     </row>
     <row r="27" spans="2:10" ht="15.75" customHeight="1">
-      <c r="B27" s="44">
+      <c r="B27" s="34">
         <v>11</v>
       </c>
-      <c r="C27" s="41" t="s">
+      <c r="C27" s="33" t="s">
         <v>10</v>
       </c>
-      <c r="D27" s="49" t="s">
+      <c r="D27" s="41" t="s">
         <v>43</v>
       </c>
       <c r="E27" s="42" t="s">
         <v>44</v>
       </c>
-      <c r="F27" s="47"/>
-      <c r="G27" s="49" t="s">
+      <c r="F27" s="35"/>
+      <c r="G27" s="41" t="s">
         <v>32</v>
       </c>
-      <c r="H27" s="47"/>
-      <c r="I27" s="33" t="s">
+      <c r="H27" s="35"/>
+      <c r="I27" s="36" t="s">
         <v>39</v>
       </c>
-      <c r="J27" s="54" t="s">
+      <c r="J27" s="31" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="28" spans="2:10" ht="15.75" customHeight="1">
-      <c r="B28" s="44"/>
-      <c r="C28" s="41"/>
-      <c r="D28" s="49"/>
+      <c r="B28" s="34"/>
+      <c r="C28" s="33"/>
+      <c r="D28" s="41"/>
       <c r="E28" s="42"/>
-      <c r="F28" s="47"/>
-      <c r="G28" s="49"/>
-      <c r="H28" s="47"/>
-      <c r="I28" s="33"/>
-      <c r="J28" s="30"/>
+      <c r="F28" s="35"/>
+      <c r="G28" s="41"/>
+      <c r="H28" s="35"/>
+      <c r="I28" s="36"/>
+      <c r="J28" s="32"/>
     </row>
     <row r="29" spans="2:10" ht="15.75" customHeight="1">
-      <c r="B29" s="44"/>
-      <c r="C29" s="41"/>
-      <c r="D29" s="49"/>
+      <c r="B29" s="34"/>
+      <c r="C29" s="33"/>
+      <c r="D29" s="41"/>
       <c r="E29" s="42"/>
-      <c r="F29" s="47"/>
-      <c r="G29" s="49"/>
-      <c r="H29" s="47"/>
-      <c r="I29" s="33"/>
-      <c r="J29" s="30"/>
+      <c r="F29" s="35"/>
+      <c r="G29" s="41"/>
+      <c r="H29" s="35"/>
+      <c r="I29" s="36"/>
+      <c r="J29" s="32"/>
     </row>
     <row r="30" spans="2:10" ht="15.75" customHeight="1">
-      <c r="B30" s="44"/>
-      <c r="C30" s="41"/>
-      <c r="D30" s="49"/>
+      <c r="B30" s="34"/>
+      <c r="C30" s="33"/>
+      <c r="D30" s="41"/>
       <c r="E30" s="42"/>
-      <c r="F30" s="47"/>
-      <c r="G30" s="49"/>
-      <c r="H30" s="47"/>
-      <c r="I30" s="33"/>
-      <c r="J30" s="30"/>
+      <c r="F30" s="35"/>
+      <c r="G30" s="41"/>
+      <c r="H30" s="35"/>
+      <c r="I30" s="36"/>
+      <c r="J30" s="32"/>
     </row>
     <row r="31" spans="2:10" ht="15.75" customHeight="1">
-      <c r="B31" s="44"/>
-      <c r="C31" s="41"/>
-      <c r="D31" s="49"/>
+      <c r="B31" s="34"/>
+      <c r="C31" s="33"/>
+      <c r="D31" s="41"/>
       <c r="E31" s="42"/>
-      <c r="F31" s="47"/>
-      <c r="G31" s="49"/>
-      <c r="H31" s="47"/>
-      <c r="I31" s="33"/>
-      <c r="J31" s="30"/>
+      <c r="F31" s="35"/>
+      <c r="G31" s="41"/>
+      <c r="H31" s="35"/>
+      <c r="I31" s="36"/>
+      <c r="J31" s="32"/>
     </row>
     <row r="32" spans="2:10" ht="15.75" customHeight="1">
-      <c r="B32" s="44"/>
-      <c r="C32" s="41"/>
-      <c r="D32" s="49"/>
+      <c r="B32" s="34"/>
+      <c r="C32" s="33"/>
+      <c r="D32" s="41"/>
       <c r="E32" s="42"/>
-      <c r="F32" s="47"/>
-      <c r="G32" s="49"/>
-      <c r="H32" s="47"/>
-      <c r="I32" s="33"/>
-      <c r="J32" s="30"/>
+      <c r="F32" s="35"/>
+      <c r="G32" s="41"/>
+      <c r="H32" s="35"/>
+      <c r="I32" s="36"/>
+      <c r="J32" s="32"/>
     </row>
     <row r="33" spans="2:10" ht="63" customHeight="1">
-      <c r="B33" s="19">
+      <c r="B33" s="17">
         <v>12</v>
       </c>
-      <c r="C33" s="20" t="s">
+      <c r="C33" s="18" t="s">
         <v>10</v>
       </c>
-      <c r="D33" s="21" t="s">
+      <c r="D33" s="19" t="s">
         <v>45</v>
       </c>
-      <c r="E33" s="22" t="s">
+      <c r="E33" s="20" t="s">
         <v>46</v>
       </c>
-      <c r="F33" s="22"/>
-      <c r="G33" s="23" t="s">
+      <c r="F33" s="20"/>
+      <c r="G33" s="21" t="s">
         <v>47</v>
       </c>
-      <c r="H33" s="22"/>
-      <c r="I33" s="11" t="s">
+      <c r="H33" s="20"/>
+      <c r="I33" s="27">
+        <v>11</v>
+      </c>
+      <c r="J33" s="26" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="34" spans="2:10" ht="63" customHeight="1">
+      <c r="B34" s="7">
+        <v>13</v>
+      </c>
+      <c r="C34" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="D34" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="E34" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="F34" s="11"/>
+      <c r="G34" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="H34" s="11"/>
+      <c r="I34" s="8">
+        <v>6</v>
+      </c>
+      <c r="J34" s="9" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="35" spans="2:10" ht="63" customHeight="1" thickBot="1">
+      <c r="B35" s="22">
+        <v>14</v>
+      </c>
+      <c r="C35" s="54" t="s">
+        <v>57</v>
+      </c>
+      <c r="D35" s="23" t="s">
         <v>56</v>
       </c>
-      <c r="J33" s="6" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="34" spans="2:10" ht="63" customHeight="1">
-      <c r="B34" s="8">
-        <v>13</v>
-      </c>
-      <c r="C34" s="7" t="s">
-        <v>38</v>
-      </c>
-      <c r="D34" s="12" t="s">
-        <v>48</v>
-      </c>
-      <c r="E34" s="12" t="s">
-        <v>50</v>
-      </c>
-      <c r="F34" s="13"/>
-      <c r="G34" s="12" t="s">
-        <v>49</v>
-      </c>
-      <c r="H34" s="13"/>
-      <c r="I34" s="9">
-        <v>6</v>
-      </c>
-      <c r="J34" s="10" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="35" spans="2:10" ht="63" customHeight="1" thickBot="1">
-      <c r="B35" s="24">
-        <v>14</v>
-      </c>
-      <c r="C35" s="25" t="s">
-        <v>38</v>
-      </c>
-      <c r="D35" s="26" t="s">
-        <v>57</v>
-      </c>
-      <c r="E35" s="26"/>
-      <c r="F35" s="27"/>
-      <c r="G35" s="26"/>
-      <c r="H35" s="27"/>
-      <c r="I35" s="28" t="s">
+      <c r="E35" s="23" t="s">
         <v>58</v>
       </c>
-      <c r="J35" s="18" t="s">
+      <c r="F35" s="24"/>
+      <c r="G35" s="23"/>
+      <c r="H35" s="24"/>
+      <c r="I35" s="25">
+        <v>12</v>
+      </c>
+      <c r="J35" s="16" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="36" spans="2:10" ht="15.75" customHeight="1" thickBot="1"/>
     <row r="37" spans="2:10" ht="15.75" customHeight="1" thickBot="1">
-      <c r="B37" s="51" t="s">
+      <c r="B37" s="28" t="s">
         <v>51</v>
       </c>
-      <c r="C37" s="52"/>
-      <c r="D37" s="52"/>
-      <c r="E37" s="52"/>
-      <c r="F37" s="52"/>
-      <c r="G37" s="52"/>
-      <c r="H37" s="52"/>
-      <c r="I37" s="52"/>
-      <c r="J37" s="53"/>
-    </row>
-    <row r="38" spans="2:10" ht="15.75" customHeight="1"/>
+      <c r="C37" s="29"/>
+      <c r="D37" s="29"/>
+      <c r="E37" s="29"/>
+      <c r="F37" s="29"/>
+      <c r="G37" s="29"/>
+      <c r="H37" s="29"/>
+      <c r="I37" s="29"/>
+      <c r="J37" s="30"/>
+    </row>
+    <row r="38" spans="2:10" ht="15.75" customHeight="1">
+      <c r="B38" s="55"/>
+      <c r="C38" s="55"/>
+      <c r="D38" s="55"/>
+      <c r="E38" s="55"/>
+      <c r="F38" s="55"/>
+      <c r="G38" s="55"/>
+      <c r="H38" s="55"/>
+      <c r="I38" s="55"/>
+      <c r="J38" s="55"/>
+    </row>
     <row r="39" spans="2:10" ht="15.75" customHeight="1"/>
     <row r="40" spans="2:10" ht="15.75" customHeight="1"/>
     <row r="41" spans="2:10" ht="15.75" customHeight="1"/>
@@ -2662,41 +2678,58 @@
     <row r="993" ht="15.75" customHeight="1"/>
   </sheetData>
   <autoFilter ref="B2:J35"/>
-  <mergeCells count="100">
-    <mergeCell ref="B37:J37"/>
-    <mergeCell ref="J27:J32"/>
-    <mergeCell ref="C27:C32"/>
-    <mergeCell ref="B27:B32"/>
-    <mergeCell ref="H27:H32"/>
-    <mergeCell ref="I27:I32"/>
-    <mergeCell ref="B24:B26"/>
-    <mergeCell ref="C24:C26"/>
-    <mergeCell ref="D24:D26"/>
-    <mergeCell ref="E24:E26"/>
-    <mergeCell ref="F24:F26"/>
-    <mergeCell ref="H24:H26"/>
-    <mergeCell ref="G27:G32"/>
-    <mergeCell ref="F27:F32"/>
-    <mergeCell ref="E27:E32"/>
-    <mergeCell ref="D27:D32"/>
-    <mergeCell ref="G24:G26"/>
-    <mergeCell ref="F3:F4"/>
-    <mergeCell ref="F5:F6"/>
-    <mergeCell ref="F7:F8"/>
-    <mergeCell ref="F9:F10"/>
-    <mergeCell ref="F11:F12"/>
-    <mergeCell ref="F21:F23"/>
-    <mergeCell ref="B21:B23"/>
-    <mergeCell ref="C21:C23"/>
-    <mergeCell ref="G21:G23"/>
-    <mergeCell ref="H21:H23"/>
-    <mergeCell ref="D21:D23"/>
-    <mergeCell ref="E21:E23"/>
-    <mergeCell ref="E5:E6"/>
-    <mergeCell ref="E7:E8"/>
-    <mergeCell ref="E9:E10"/>
-    <mergeCell ref="E11:E12"/>
-    <mergeCell ref="E13:E14"/>
+  <mergeCells count="101">
+    <mergeCell ref="B38:J38"/>
+    <mergeCell ref="J13:J14"/>
+    <mergeCell ref="J15:J17"/>
+    <mergeCell ref="J18:J20"/>
+    <mergeCell ref="J21:J23"/>
+    <mergeCell ref="J24:J26"/>
+    <mergeCell ref="J3:J4"/>
+    <mergeCell ref="J5:J6"/>
+    <mergeCell ref="J7:J8"/>
+    <mergeCell ref="J9:J10"/>
+    <mergeCell ref="J11:J12"/>
+    <mergeCell ref="I13:I14"/>
+    <mergeCell ref="I15:I17"/>
+    <mergeCell ref="I18:I20"/>
+    <mergeCell ref="I21:I23"/>
+    <mergeCell ref="I24:I26"/>
+    <mergeCell ref="I3:I4"/>
+    <mergeCell ref="I5:I6"/>
+    <mergeCell ref="I7:I8"/>
+    <mergeCell ref="I9:I10"/>
+    <mergeCell ref="I11:I12"/>
+    <mergeCell ref="C9:C10"/>
+    <mergeCell ref="D11:D12"/>
+    <mergeCell ref="C11:C12"/>
+    <mergeCell ref="D13:D14"/>
+    <mergeCell ref="C13:C14"/>
+    <mergeCell ref="D9:D10"/>
+    <mergeCell ref="C3:C4"/>
+    <mergeCell ref="D3:D4"/>
+    <mergeCell ref="C5:C6"/>
+    <mergeCell ref="D5:D6"/>
+    <mergeCell ref="C7:C8"/>
+    <mergeCell ref="D7:D8"/>
+    <mergeCell ref="B3:B4"/>
+    <mergeCell ref="B5:B6"/>
+    <mergeCell ref="B7:B8"/>
+    <mergeCell ref="B9:B10"/>
+    <mergeCell ref="B11:B12"/>
+    <mergeCell ref="B13:B14"/>
+    <mergeCell ref="B15:B17"/>
+    <mergeCell ref="G18:G20"/>
+    <mergeCell ref="E18:E20"/>
+    <mergeCell ref="C18:C20"/>
+    <mergeCell ref="B18:B20"/>
+    <mergeCell ref="F18:F20"/>
+    <mergeCell ref="E15:E17"/>
+    <mergeCell ref="D15:D17"/>
+    <mergeCell ref="D18:D20"/>
+    <mergeCell ref="F13:F14"/>
+    <mergeCell ref="C15:C17"/>
+    <mergeCell ref="F15:F17"/>
     <mergeCell ref="H18:H20"/>
     <mergeCell ref="E3:E4"/>
     <mergeCell ref="G3:G4"/>
@@ -2713,56 +2746,40 @@
     <mergeCell ref="G11:G12"/>
     <mergeCell ref="G13:G14"/>
     <mergeCell ref="G15:G17"/>
-    <mergeCell ref="B13:B14"/>
-    <mergeCell ref="B15:B17"/>
-    <mergeCell ref="G18:G20"/>
-    <mergeCell ref="E18:E20"/>
-    <mergeCell ref="C18:C20"/>
-    <mergeCell ref="B18:B20"/>
-    <mergeCell ref="F18:F20"/>
-    <mergeCell ref="E15:E17"/>
-    <mergeCell ref="D15:D17"/>
-    <mergeCell ref="D18:D20"/>
-    <mergeCell ref="F13:F14"/>
-    <mergeCell ref="C15:C17"/>
-    <mergeCell ref="F15:F17"/>
-    <mergeCell ref="B3:B4"/>
-    <mergeCell ref="B5:B6"/>
-    <mergeCell ref="B7:B8"/>
-    <mergeCell ref="B9:B10"/>
-    <mergeCell ref="B11:B12"/>
-    <mergeCell ref="C3:C4"/>
-    <mergeCell ref="D3:D4"/>
-    <mergeCell ref="C5:C6"/>
-    <mergeCell ref="D5:D6"/>
-    <mergeCell ref="C7:C8"/>
-    <mergeCell ref="D7:D8"/>
-    <mergeCell ref="C9:C10"/>
-    <mergeCell ref="D11:D12"/>
-    <mergeCell ref="C11:C12"/>
-    <mergeCell ref="D13:D14"/>
-    <mergeCell ref="C13:C14"/>
-    <mergeCell ref="D9:D10"/>
-    <mergeCell ref="I3:I4"/>
-    <mergeCell ref="I5:I6"/>
-    <mergeCell ref="I7:I8"/>
-    <mergeCell ref="I9:I10"/>
-    <mergeCell ref="I11:I12"/>
-    <mergeCell ref="I13:I14"/>
-    <mergeCell ref="I15:I17"/>
-    <mergeCell ref="I18:I20"/>
-    <mergeCell ref="I21:I23"/>
-    <mergeCell ref="I24:I26"/>
-    <mergeCell ref="J3:J4"/>
-    <mergeCell ref="J5:J6"/>
-    <mergeCell ref="J7:J8"/>
-    <mergeCell ref="J9:J10"/>
-    <mergeCell ref="J11:J12"/>
-    <mergeCell ref="J13:J14"/>
-    <mergeCell ref="J15:J17"/>
-    <mergeCell ref="J18:J20"/>
-    <mergeCell ref="J21:J23"/>
-    <mergeCell ref="J24:J26"/>
+    <mergeCell ref="E5:E6"/>
+    <mergeCell ref="E7:E8"/>
+    <mergeCell ref="E9:E10"/>
+    <mergeCell ref="E11:E12"/>
+    <mergeCell ref="E13:E14"/>
+    <mergeCell ref="F21:F23"/>
+    <mergeCell ref="B21:B23"/>
+    <mergeCell ref="C21:C23"/>
+    <mergeCell ref="G21:G23"/>
+    <mergeCell ref="H21:H23"/>
+    <mergeCell ref="D21:D23"/>
+    <mergeCell ref="E21:E23"/>
+    <mergeCell ref="F3:F4"/>
+    <mergeCell ref="F5:F6"/>
+    <mergeCell ref="F7:F8"/>
+    <mergeCell ref="F9:F10"/>
+    <mergeCell ref="F11:F12"/>
+    <mergeCell ref="H24:H26"/>
+    <mergeCell ref="G27:G32"/>
+    <mergeCell ref="F27:F32"/>
+    <mergeCell ref="E27:E32"/>
+    <mergeCell ref="D27:D32"/>
+    <mergeCell ref="G24:G26"/>
+    <mergeCell ref="B24:B26"/>
+    <mergeCell ref="C24:C26"/>
+    <mergeCell ref="D24:D26"/>
+    <mergeCell ref="E24:E26"/>
+    <mergeCell ref="F24:F26"/>
+    <mergeCell ref="B37:J37"/>
+    <mergeCell ref="J27:J32"/>
+    <mergeCell ref="C27:C32"/>
+    <mergeCell ref="B27:B32"/>
+    <mergeCell ref="H27:H32"/>
+    <mergeCell ref="I27:I32"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape" r:id="rId1"/>

</xml_diff>

<commit_message>
Correction des tableaux d'analyses
</commit_message>
<xml_diff>
--- a/Analyses/Modèle-audit-SEO.xlsx
+++ b/Analyses/Modèle-audit-SEO.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="62">
   <si>
     <t>Catégorie</t>
   </si>
@@ -320,14 +320,24 @@
  redistribuer. Enlever div Keyword</t>
   </si>
   <si>
-    <t xml:space="preserve"> Police</t>
-  </si>
-  <si>
     <t>PERFORMANCE &amp;
  ACCESSIBILITÉ</t>
   </si>
   <si>
     <t>Mettre une taille de police convenable (lisible)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Police (visibilité du texte)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Correction des titres</t>
+  </si>
+  <si>
+    <t>Les titres doivent être ordonnés
+(&lt;h1&gt; puis &lt;h2&gt; puis &lt;h3&gt;)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Corriger la hiérarchie des titres</t>
   </si>
 </sst>
 </file>
@@ -450,7 +460,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="17">
+  <borders count="19">
     <border>
       <left/>
       <right/>
@@ -525,51 +535,6 @@
       <right style="thin">
         <color indexed="64"/>
       </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
       <top style="medium">
         <color indexed="64"/>
       </top>
@@ -684,12 +649,79 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="9" fillId="5" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="56">
+  <cellXfs count="62">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -724,19 +756,16 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -754,107 +783,128 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1069,10 +1119,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B1:AB993"/>
+  <dimension ref="B1:AB994"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="B37" sqref="B37:J37"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="J36" sqref="J36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.33203125" defaultRowHeight="15" customHeight="1"/>
@@ -1138,513 +1188,513 @@
       <c r="AB2" s="1"/>
     </row>
     <row r="3" spans="2:28" ht="15.75" customHeight="1">
-      <c r="B3" s="48">
+      <c r="B3" s="38">
         <v>1</v>
       </c>
-      <c r="C3" s="49" t="s">
+      <c r="C3" s="35" t="s">
         <v>38</v>
       </c>
-      <c r="D3" s="49" t="s">
+      <c r="D3" s="35" t="s">
         <v>7</v>
       </c>
-      <c r="E3" s="43" t="s">
+      <c r="E3" s="41" t="s">
         <v>14</v>
       </c>
-      <c r="F3" s="43" t="s">
+      <c r="F3" s="41" t="s">
         <v>37</v>
       </c>
-      <c r="G3" s="43" t="s">
+      <c r="G3" s="41" t="s">
         <v>15</v>
       </c>
-      <c r="H3" s="46"/>
-      <c r="I3" s="50">
+      <c r="H3" s="43"/>
+      <c r="I3" s="29">
         <v>1</v>
       </c>
-      <c r="J3" s="52" t="s">
+      <c r="J3" s="26" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="4" spans="2:28" ht="15.75" customHeight="1">
-      <c r="B4" s="34"/>
-      <c r="C4" s="33"/>
-      <c r="D4" s="33"/>
-      <c r="E4" s="35"/>
-      <c r="F4" s="35"/>
-      <c r="G4" s="35"/>
-      <c r="H4" s="35"/>
-      <c r="I4" s="36"/>
-      <c r="J4" s="53"/>
+      <c r="B4" s="39"/>
+      <c r="C4" s="36"/>
+      <c r="D4" s="36"/>
+      <c r="E4" s="42"/>
+      <c r="F4" s="42"/>
+      <c r="G4" s="42"/>
+      <c r="H4" s="42"/>
+      <c r="I4" s="28"/>
+      <c r="J4" s="24"/>
     </row>
     <row r="5" spans="2:28" ht="15.75" customHeight="1">
-      <c r="B5" s="37">
+      <c r="B5" s="40">
         <v>2</v>
       </c>
-      <c r="C5" s="38" t="s">
+      <c r="C5" s="30" t="s">
         <v>38</v>
       </c>
-      <c r="D5" s="40" t="s">
+      <c r="D5" s="33" t="s">
         <v>8</v>
       </c>
-      <c r="E5" s="39" t="s">
+      <c r="E5" s="34" t="s">
         <v>14</v>
       </c>
-      <c r="F5" s="44"/>
-      <c r="G5" s="39" t="s">
+      <c r="F5" s="45"/>
+      <c r="G5" s="34" t="s">
         <v>16</v>
       </c>
-      <c r="H5" s="40"/>
-      <c r="I5" s="51">
+      <c r="H5" s="33"/>
+      <c r="I5" s="27">
         <v>2</v>
       </c>
-      <c r="J5" s="53" t="s">
+      <c r="J5" s="24" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="6" spans="2:28" ht="15.75" customHeight="1">
-      <c r="B6" s="37"/>
-      <c r="C6" s="38"/>
-      <c r="D6" s="40"/>
-      <c r="E6" s="40"/>
-      <c r="F6" s="44"/>
-      <c r="G6" s="40"/>
-      <c r="H6" s="40"/>
-      <c r="I6" s="51"/>
-      <c r="J6" s="53"/>
+      <c r="B6" s="40"/>
+      <c r="C6" s="30"/>
+      <c r="D6" s="33"/>
+      <c r="E6" s="33"/>
+      <c r="F6" s="45"/>
+      <c r="G6" s="33"/>
+      <c r="H6" s="33"/>
+      <c r="I6" s="27"/>
+      <c r="J6" s="24"/>
     </row>
     <row r="7" spans="2:28" ht="15.75" customHeight="1">
-      <c r="B7" s="34">
+      <c r="B7" s="39">
         <v>3</v>
       </c>
-      <c r="C7" s="47" t="s">
+      <c r="C7" s="32" t="s">
         <v>6</v>
       </c>
-      <c r="D7" s="42" t="s">
+      <c r="D7" s="37" t="s">
         <v>24</v>
       </c>
-      <c r="E7" s="42" t="s">
+      <c r="E7" s="37" t="s">
         <v>21</v>
       </c>
-      <c r="F7" s="45"/>
-      <c r="G7" s="42" t="s">
+      <c r="F7" s="31"/>
+      <c r="G7" s="37" t="s">
         <v>17</v>
       </c>
-      <c r="H7" s="45"/>
-      <c r="I7" s="36">
+      <c r="H7" s="31"/>
+      <c r="I7" s="28">
         <v>10</v>
       </c>
-      <c r="J7" s="53" t="s">
+      <c r="J7" s="24" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="8" spans="2:28" ht="15.75" customHeight="1">
-      <c r="B8" s="34"/>
-      <c r="C8" s="47"/>
-      <c r="D8" s="45"/>
-      <c r="E8" s="45"/>
-      <c r="F8" s="45"/>
-      <c r="G8" s="45"/>
-      <c r="H8" s="45"/>
-      <c r="I8" s="36"/>
-      <c r="J8" s="53"/>
+      <c r="B8" s="39"/>
+      <c r="C8" s="32"/>
+      <c r="D8" s="31"/>
+      <c r="E8" s="31"/>
+      <c r="F8" s="31"/>
+      <c r="G8" s="31"/>
+      <c r="H8" s="31"/>
+      <c r="I8" s="28"/>
+      <c r="J8" s="24"/>
     </row>
     <row r="9" spans="2:28" ht="15.75" customHeight="1">
-      <c r="B9" s="37">
+      <c r="B9" s="40">
         <v>4</v>
       </c>
-      <c r="C9" s="38" t="s">
+      <c r="C9" s="30" t="s">
         <v>6</v>
       </c>
-      <c r="D9" s="39" t="s">
+      <c r="D9" s="34" t="s">
         <v>25</v>
       </c>
-      <c r="E9" s="39" t="s">
+      <c r="E9" s="34" t="s">
         <v>22</v>
       </c>
-      <c r="F9" s="40"/>
-      <c r="G9" s="39" t="s">
+      <c r="F9" s="33"/>
+      <c r="G9" s="34" t="s">
         <v>18</v>
       </c>
-      <c r="H9" s="40"/>
-      <c r="I9" s="51">
+      <c r="H9" s="33"/>
+      <c r="I9" s="27">
         <v>4</v>
       </c>
-      <c r="J9" s="53" t="s">
+      <c r="J9" s="24" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="10" spans="2:28" ht="15.75" customHeight="1">
-      <c r="B10" s="37"/>
-      <c r="C10" s="38"/>
-      <c r="D10" s="40"/>
-      <c r="E10" s="40"/>
-      <c r="F10" s="40"/>
-      <c r="G10" s="40"/>
-      <c r="H10" s="40"/>
-      <c r="I10" s="51"/>
-      <c r="J10" s="53"/>
+      <c r="B10" s="40"/>
+      <c r="C10" s="30"/>
+      <c r="D10" s="33"/>
+      <c r="E10" s="33"/>
+      <c r="F10" s="33"/>
+      <c r="G10" s="33"/>
+      <c r="H10" s="33"/>
+      <c r="I10" s="27"/>
+      <c r="J10" s="24"/>
     </row>
     <row r="11" spans="2:28" ht="15.75" customHeight="1">
-      <c r="B11" s="34">
+      <c r="B11" s="39">
         <v>5</v>
       </c>
-      <c r="C11" s="47" t="s">
+      <c r="C11" s="32" t="s">
         <v>10</v>
       </c>
-      <c r="D11" s="45" t="s">
+      <c r="D11" s="31" t="s">
         <v>11</v>
       </c>
-      <c r="E11" s="42" t="s">
+      <c r="E11" s="37" t="s">
         <v>35</v>
       </c>
-      <c r="F11" s="45"/>
-      <c r="G11" s="42" t="s">
+      <c r="F11" s="31"/>
+      <c r="G11" s="37" t="s">
         <v>19</v>
       </c>
-      <c r="H11" s="45"/>
-      <c r="I11" s="36">
+      <c r="H11" s="31"/>
+      <c r="I11" s="28">
         <v>5</v>
       </c>
-      <c r="J11" s="53" t="s">
+      <c r="J11" s="24" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="12" spans="2:28" ht="15.75" customHeight="1">
-      <c r="B12" s="34"/>
-      <c r="C12" s="47"/>
-      <c r="D12" s="45"/>
-      <c r="E12" s="45"/>
-      <c r="F12" s="45"/>
-      <c r="G12" s="45"/>
-      <c r="H12" s="45"/>
-      <c r="I12" s="36"/>
-      <c r="J12" s="53"/>
+      <c r="B12" s="39"/>
+      <c r="C12" s="32"/>
+      <c r="D12" s="31"/>
+      <c r="E12" s="31"/>
+      <c r="F12" s="31"/>
+      <c r="G12" s="31"/>
+      <c r="H12" s="31"/>
+      <c r="I12" s="28"/>
+      <c r="J12" s="24"/>
     </row>
     <row r="13" spans="2:28" ht="15.75" customHeight="1">
-      <c r="B13" s="37">
+      <c r="B13" s="40">
         <v>6</v>
       </c>
-      <c r="C13" s="38" t="s">
+      <c r="C13" s="30" t="s">
         <v>6</v>
       </c>
-      <c r="D13" s="40" t="s">
+      <c r="D13" s="33" t="s">
         <v>54</v>
       </c>
-      <c r="E13" s="39" t="s">
+      <c r="E13" s="34" t="s">
         <v>33</v>
       </c>
-      <c r="F13" s="40"/>
-      <c r="G13" s="39" t="s">
+      <c r="F13" s="33"/>
+      <c r="G13" s="34" t="s">
         <v>55</v>
       </c>
-      <c r="H13" s="40"/>
-      <c r="I13" s="51">
+      <c r="H13" s="33"/>
+      <c r="I13" s="27">
         <v>9</v>
       </c>
-      <c r="J13" s="53" t="s">
+      <c r="J13" s="24" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="14" spans="2:28" ht="15.75" customHeight="1">
-      <c r="B14" s="37"/>
-      <c r="C14" s="38"/>
-      <c r="D14" s="40"/>
-      <c r="E14" s="40"/>
-      <c r="F14" s="40"/>
-      <c r="G14" s="40"/>
-      <c r="H14" s="40"/>
-      <c r="I14" s="51"/>
-      <c r="J14" s="53"/>
+      <c r="B14" s="40"/>
+      <c r="C14" s="30"/>
+      <c r="D14" s="33"/>
+      <c r="E14" s="33"/>
+      <c r="F14" s="33"/>
+      <c r="G14" s="33"/>
+      <c r="H14" s="33"/>
+      <c r="I14" s="27"/>
+      <c r="J14" s="24"/>
     </row>
     <row r="15" spans="2:28" ht="15.75" customHeight="1">
-      <c r="B15" s="34">
+      <c r="B15" s="39">
         <v>7</v>
       </c>
-      <c r="C15" s="47" t="s">
+      <c r="C15" s="32" t="s">
         <v>6</v>
       </c>
-      <c r="D15" s="42" t="s">
+      <c r="D15" s="37" t="s">
         <v>26</v>
       </c>
-      <c r="E15" s="42" t="s">
+      <c r="E15" s="37" t="s">
         <v>23</v>
       </c>
-      <c r="F15" s="45"/>
-      <c r="G15" s="42" t="s">
+      <c r="F15" s="31"/>
+      <c r="G15" s="37" t="s">
         <v>20</v>
       </c>
-      <c r="H15" s="45"/>
-      <c r="I15" s="36">
+      <c r="H15" s="31"/>
+      <c r="I15" s="28">
         <v>8</v>
       </c>
-      <c r="J15" s="53" t="s">
+      <c r="J15" s="24" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="16" spans="2:28" ht="15.75" customHeight="1">
-      <c r="B16" s="34"/>
-      <c r="C16" s="47"/>
-      <c r="D16" s="45"/>
-      <c r="E16" s="45"/>
-      <c r="F16" s="45"/>
-      <c r="G16" s="45"/>
-      <c r="H16" s="45"/>
-      <c r="I16" s="36"/>
-      <c r="J16" s="53"/>
+      <c r="B16" s="39"/>
+      <c r="C16" s="32"/>
+      <c r="D16" s="31"/>
+      <c r="E16" s="31"/>
+      <c r="F16" s="31"/>
+      <c r="G16" s="31"/>
+      <c r="H16" s="31"/>
+      <c r="I16" s="28"/>
+      <c r="J16" s="24"/>
     </row>
     <row r="17" spans="2:10" ht="15.75" customHeight="1">
-      <c r="B17" s="34"/>
-      <c r="C17" s="47"/>
-      <c r="D17" s="45"/>
-      <c r="E17" s="45"/>
-      <c r="F17" s="45"/>
-      <c r="G17" s="45"/>
-      <c r="H17" s="45"/>
-      <c r="I17" s="36"/>
-      <c r="J17" s="53"/>
+      <c r="B17" s="39"/>
+      <c r="C17" s="32"/>
+      <c r="D17" s="31"/>
+      <c r="E17" s="31"/>
+      <c r="F17" s="31"/>
+      <c r="G17" s="31"/>
+      <c r="H17" s="31"/>
+      <c r="I17" s="28"/>
+      <c r="J17" s="24"/>
     </row>
     <row r="18" spans="2:10" ht="15.75" customHeight="1">
-      <c r="B18" s="37">
+      <c r="B18" s="40">
         <v>8</v>
       </c>
-      <c r="C18" s="38" t="s">
+      <c r="C18" s="30" t="s">
         <v>9</v>
       </c>
-      <c r="D18" s="39" t="s">
+      <c r="D18" s="34" t="s">
         <v>52</v>
       </c>
-      <c r="E18" s="40" t="s">
+      <c r="E18" s="33" t="s">
         <v>12</v>
       </c>
-      <c r="F18" s="40"/>
-      <c r="G18" s="39" t="s">
+      <c r="F18" s="33"/>
+      <c r="G18" s="34" t="s">
         <v>53</v>
       </c>
-      <c r="H18" s="40"/>
-      <c r="I18" s="51">
+      <c r="H18" s="33"/>
+      <c r="I18" s="27">
         <v>7</v>
       </c>
-      <c r="J18" s="53" t="s">
+      <c r="J18" s="24" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="19" spans="2:10" ht="15.75" customHeight="1">
-      <c r="B19" s="37"/>
-      <c r="C19" s="38"/>
-      <c r="D19" s="40"/>
-      <c r="E19" s="40"/>
-      <c r="F19" s="40"/>
-      <c r="G19" s="40"/>
-      <c r="H19" s="40"/>
-      <c r="I19" s="51"/>
-      <c r="J19" s="53"/>
+      <c r="B19" s="40"/>
+      <c r="C19" s="30"/>
+      <c r="D19" s="33"/>
+      <c r="E19" s="33"/>
+      <c r="F19" s="33"/>
+      <c r="G19" s="33"/>
+      <c r="H19" s="33"/>
+      <c r="I19" s="27"/>
+      <c r="J19" s="24"/>
     </row>
     <row r="20" spans="2:10" ht="15.75" customHeight="1">
-      <c r="B20" s="37"/>
-      <c r="C20" s="38"/>
-      <c r="D20" s="40"/>
-      <c r="E20" s="40"/>
-      <c r="F20" s="40"/>
-      <c r="G20" s="40"/>
-      <c r="H20" s="40"/>
-      <c r="I20" s="51"/>
-      <c r="J20" s="53"/>
+      <c r="B20" s="40"/>
+      <c r="C20" s="30"/>
+      <c r="D20" s="33"/>
+      <c r="E20" s="33"/>
+      <c r="F20" s="33"/>
+      <c r="G20" s="33"/>
+      <c r="H20" s="33"/>
+      <c r="I20" s="27"/>
+      <c r="J20" s="24"/>
     </row>
     <row r="21" spans="2:10" ht="15.75" customHeight="1">
-      <c r="B21" s="34">
+      <c r="B21" s="39">
         <v>9</v>
       </c>
-      <c r="C21" s="33" t="s">
+      <c r="C21" s="36" t="s">
         <v>9</v>
       </c>
-      <c r="D21" s="41" t="s">
+      <c r="D21" s="44" t="s">
         <v>36</v>
       </c>
-      <c r="E21" s="41" t="s">
+      <c r="E21" s="44" t="s">
         <v>28</v>
       </c>
-      <c r="F21" s="35"/>
-      <c r="G21" s="35" t="s">
+      <c r="F21" s="42"/>
+      <c r="G21" s="42" t="s">
         <v>27</v>
       </c>
-      <c r="H21" s="35"/>
-      <c r="I21" s="36">
+      <c r="H21" s="42"/>
+      <c r="I21" s="28">
         <v>3</v>
       </c>
-      <c r="J21" s="53" t="s">
+      <c r="J21" s="24" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="22" spans="2:10" ht="15.75" customHeight="1">
-      <c r="B22" s="34"/>
-      <c r="C22" s="33"/>
-      <c r="D22" s="41"/>
-      <c r="E22" s="35"/>
-      <c r="F22" s="35"/>
-      <c r="G22" s="35"/>
-      <c r="H22" s="35"/>
-      <c r="I22" s="36"/>
-      <c r="J22" s="53"/>
+      <c r="B22" s="39"/>
+      <c r="C22" s="36"/>
+      <c r="D22" s="44"/>
+      <c r="E22" s="42"/>
+      <c r="F22" s="42"/>
+      <c r="G22" s="42"/>
+      <c r="H22" s="42"/>
+      <c r="I22" s="28"/>
+      <c r="J22" s="24"/>
     </row>
     <row r="23" spans="2:10" ht="15.75" customHeight="1">
-      <c r="B23" s="34"/>
-      <c r="C23" s="33"/>
-      <c r="D23" s="41"/>
-      <c r="E23" s="35"/>
-      <c r="F23" s="35"/>
-      <c r="G23" s="35"/>
-      <c r="H23" s="35"/>
-      <c r="I23" s="36"/>
-      <c r="J23" s="53"/>
+      <c r="B23" s="39"/>
+      <c r="C23" s="36"/>
+      <c r="D23" s="44"/>
+      <c r="E23" s="42"/>
+      <c r="F23" s="42"/>
+      <c r="G23" s="42"/>
+      <c r="H23" s="42"/>
+      <c r="I23" s="28"/>
+      <c r="J23" s="24"/>
     </row>
     <row r="24" spans="2:10" ht="15.75" customHeight="1">
-      <c r="B24" s="37">
+      <c r="B24" s="40">
         <v>10</v>
       </c>
-      <c r="C24" s="38" t="s">
+      <c r="C24" s="30" t="s">
         <v>9</v>
       </c>
-      <c r="D24" s="39" t="s">
+      <c r="D24" s="34" t="s">
         <v>31</v>
       </c>
-      <c r="E24" s="40" t="s">
+      <c r="E24" s="33" t="s">
         <v>29</v>
       </c>
-      <c r="F24" s="40"/>
-      <c r="G24" s="39" t="s">
+      <c r="F24" s="33"/>
+      <c r="G24" s="34" t="s">
         <v>30</v>
       </c>
-      <c r="H24" s="40"/>
-      <c r="I24" s="51" t="s">
+      <c r="H24" s="33"/>
+      <c r="I24" s="27" t="s">
         <v>39</v>
       </c>
-      <c r="J24" s="32" t="s">
+      <c r="J24" s="25" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="25" spans="2:10" ht="15.75" customHeight="1">
-      <c r="B25" s="37"/>
-      <c r="C25" s="38"/>
-      <c r="D25" s="40"/>
-      <c r="E25" s="40"/>
-      <c r="F25" s="40"/>
-      <c r="G25" s="39"/>
-      <c r="H25" s="40"/>
-      <c r="I25" s="51"/>
-      <c r="J25" s="32"/>
+      <c r="B25" s="40"/>
+      <c r="C25" s="30"/>
+      <c r="D25" s="33"/>
+      <c r="E25" s="33"/>
+      <c r="F25" s="33"/>
+      <c r="G25" s="34"/>
+      <c r="H25" s="33"/>
+      <c r="I25" s="27"/>
+      <c r="J25" s="25"/>
     </row>
     <row r="26" spans="2:10" ht="15.75" customHeight="1">
-      <c r="B26" s="37"/>
-      <c r="C26" s="38"/>
-      <c r="D26" s="40"/>
-      <c r="E26" s="40"/>
-      <c r="F26" s="40"/>
-      <c r="G26" s="39"/>
-      <c r="H26" s="40"/>
-      <c r="I26" s="51"/>
-      <c r="J26" s="32"/>
+      <c r="B26" s="40"/>
+      <c r="C26" s="30"/>
+      <c r="D26" s="33"/>
+      <c r="E26" s="33"/>
+      <c r="F26" s="33"/>
+      <c r="G26" s="34"/>
+      <c r="H26" s="33"/>
+      <c r="I26" s="27"/>
+      <c r="J26" s="25"/>
     </row>
     <row r="27" spans="2:10" ht="15.75" customHeight="1">
-      <c r="B27" s="34">
+      <c r="B27" s="39">
         <v>11</v>
       </c>
-      <c r="C27" s="33" t="s">
+      <c r="C27" s="36" t="s">
         <v>10</v>
       </c>
-      <c r="D27" s="41" t="s">
+      <c r="D27" s="44" t="s">
         <v>43</v>
       </c>
-      <c r="E27" s="42" t="s">
+      <c r="E27" s="37" t="s">
         <v>44</v>
       </c>
-      <c r="F27" s="35"/>
-      <c r="G27" s="41" t="s">
+      <c r="F27" s="42"/>
+      <c r="G27" s="44" t="s">
         <v>32</v>
       </c>
-      <c r="H27" s="35"/>
-      <c r="I27" s="36" t="s">
+      <c r="H27" s="42"/>
+      <c r="I27" s="28" t="s">
         <v>39</v>
       </c>
-      <c r="J27" s="31" t="s">
+      <c r="J27" s="49" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="28" spans="2:10" ht="15.75" customHeight="1">
-      <c r="B28" s="34"/>
-      <c r="C28" s="33"/>
-      <c r="D28" s="41"/>
-      <c r="E28" s="42"/>
-      <c r="F28" s="35"/>
-      <c r="G28" s="41"/>
-      <c r="H28" s="35"/>
-      <c r="I28" s="36"/>
-      <c r="J28" s="32"/>
+      <c r="B28" s="39"/>
+      <c r="C28" s="36"/>
+      <c r="D28" s="44"/>
+      <c r="E28" s="37"/>
+      <c r="F28" s="42"/>
+      <c r="G28" s="44"/>
+      <c r="H28" s="42"/>
+      <c r="I28" s="28"/>
+      <c r="J28" s="25"/>
     </row>
     <row r="29" spans="2:10" ht="15.75" customHeight="1">
-      <c r="B29" s="34"/>
-      <c r="C29" s="33"/>
-      <c r="D29" s="41"/>
-      <c r="E29" s="42"/>
-      <c r="F29" s="35"/>
-      <c r="G29" s="41"/>
-      <c r="H29" s="35"/>
-      <c r="I29" s="36"/>
-      <c r="J29" s="32"/>
+      <c r="B29" s="39"/>
+      <c r="C29" s="36"/>
+      <c r="D29" s="44"/>
+      <c r="E29" s="37"/>
+      <c r="F29" s="42"/>
+      <c r="G29" s="44"/>
+      <c r="H29" s="42"/>
+      <c r="I29" s="28"/>
+      <c r="J29" s="25"/>
     </row>
     <row r="30" spans="2:10" ht="15.75" customHeight="1">
-      <c r="B30" s="34"/>
-      <c r="C30" s="33"/>
-      <c r="D30" s="41"/>
-      <c r="E30" s="42"/>
-      <c r="F30" s="35"/>
-      <c r="G30" s="41"/>
-      <c r="H30" s="35"/>
-      <c r="I30" s="36"/>
-      <c r="J30" s="32"/>
+      <c r="B30" s="39"/>
+      <c r="C30" s="36"/>
+      <c r="D30" s="44"/>
+      <c r="E30" s="37"/>
+      <c r="F30" s="42"/>
+      <c r="G30" s="44"/>
+      <c r="H30" s="42"/>
+      <c r="I30" s="28"/>
+      <c r="J30" s="25"/>
     </row>
     <row r="31" spans="2:10" ht="15.75" customHeight="1">
-      <c r="B31" s="34"/>
-      <c r="C31" s="33"/>
-      <c r="D31" s="41"/>
-      <c r="E31" s="42"/>
-      <c r="F31" s="35"/>
-      <c r="G31" s="41"/>
-      <c r="H31" s="35"/>
-      <c r="I31" s="36"/>
-      <c r="J31" s="32"/>
+      <c r="B31" s="39"/>
+      <c r="C31" s="36"/>
+      <c r="D31" s="44"/>
+      <c r="E31" s="37"/>
+      <c r="F31" s="42"/>
+      <c r="G31" s="44"/>
+      <c r="H31" s="42"/>
+      <c r="I31" s="28"/>
+      <c r="J31" s="25"/>
     </row>
     <row r="32" spans="2:10" ht="15.75" customHeight="1">
-      <c r="B32" s="34"/>
-      <c r="C32" s="33"/>
-      <c r="D32" s="41"/>
-      <c r="E32" s="42"/>
-      <c r="F32" s="35"/>
-      <c r="G32" s="41"/>
-      <c r="H32" s="35"/>
-      <c r="I32" s="36"/>
-      <c r="J32" s="32"/>
+      <c r="B32" s="39"/>
+      <c r="C32" s="36"/>
+      <c r="D32" s="44"/>
+      <c r="E32" s="37"/>
+      <c r="F32" s="42"/>
+      <c r="G32" s="44"/>
+      <c r="H32" s="42"/>
+      <c r="I32" s="28"/>
+      <c r="J32" s="25"/>
     </row>
     <row r="33" spans="2:10" ht="63" customHeight="1">
-      <c r="B33" s="17">
+      <c r="B33" s="16">
         <v>12</v>
       </c>
-      <c r="C33" s="18" t="s">
+      <c r="C33" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="D33" s="19" t="s">
+      <c r="D33" s="18" t="s">
         <v>45</v>
       </c>
-      <c r="E33" s="20" t="s">
+      <c r="E33" s="19" t="s">
         <v>46</v>
       </c>
-      <c r="F33" s="20"/>
-      <c r="G33" s="21" t="s">
+      <c r="F33" s="19"/>
+      <c r="G33" s="20" t="s">
         <v>47</v>
       </c>
-      <c r="H33" s="20"/>
-      <c r="I33" s="27">
+      <c r="H33" s="19"/>
+      <c r="I33" s="22">
         <v>11</v>
       </c>
-      <c r="J33" s="26" t="s">
+      <c r="J33" s="21" t="s">
         <v>42</v>
       </c>
     </row>
@@ -1674,54 +1724,78 @@
       </c>
     </row>
     <row r="35" spans="2:10" ht="63" customHeight="1" thickBot="1">
-      <c r="B35" s="22">
+      <c r="B35" s="50">
         <v>14</v>
       </c>
-      <c r="C35" s="54" t="s">
+      <c r="C35" s="51" t="s">
+        <v>56</v>
+      </c>
+      <c r="D35" s="52" t="s">
+        <v>58</v>
+      </c>
+      <c r="E35" s="52" t="s">
         <v>57</v>
       </c>
-      <c r="D35" s="23" t="s">
+      <c r="F35" s="53"/>
+      <c r="G35" s="52"/>
+      <c r="H35" s="53"/>
+      <c r="I35" s="54">
+        <v>12</v>
+      </c>
+      <c r="J35" s="55" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="36" spans="2:10" ht="63" customHeight="1" thickBot="1">
+      <c r="B36" s="56">
+        <v>15</v>
+      </c>
+      <c r="C36" s="57" t="s">
         <v>56</v>
       </c>
-      <c r="E35" s="23" t="s">
-        <v>58</v>
-      </c>
-      <c r="F35" s="24"/>
-      <c r="G35" s="23"/>
-      <c r="H35" s="24"/>
-      <c r="I35" s="25">
-        <v>12</v>
-      </c>
-      <c r="J35" s="16" t="s">
+      <c r="D36" s="58" t="s">
+        <v>59</v>
+      </c>
+      <c r="E36" s="58" t="s">
+        <v>60</v>
+      </c>
+      <c r="F36" s="59"/>
+      <c r="G36" s="58" t="s">
+        <v>61</v>
+      </c>
+      <c r="H36" s="59"/>
+      <c r="I36" s="60">
+        <v>13</v>
+      </c>
+      <c r="J36" s="61" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="36" spans="2:10" ht="15.75" customHeight="1" thickBot="1"/>
-    <row r="37" spans="2:10" ht="15.75" customHeight="1" thickBot="1">
-      <c r="B37" s="28" t="s">
+    <row r="37" spans="2:10" ht="15.75" customHeight="1" thickBot="1"/>
+    <row r="38" spans="2:10" ht="15.75" customHeight="1" thickBot="1">
+      <c r="B38" s="46" t="s">
         <v>51</v>
       </c>
-      <c r="C37" s="29"/>
-      <c r="D37" s="29"/>
-      <c r="E37" s="29"/>
-      <c r="F37" s="29"/>
-      <c r="G37" s="29"/>
-      <c r="H37" s="29"/>
-      <c r="I37" s="29"/>
-      <c r="J37" s="30"/>
-    </row>
-    <row r="38" spans="2:10" ht="15.75" customHeight="1">
-      <c r="B38" s="55"/>
-      <c r="C38" s="55"/>
-      <c r="D38" s="55"/>
-      <c r="E38" s="55"/>
-      <c r="F38" s="55"/>
-      <c r="G38" s="55"/>
-      <c r="H38" s="55"/>
-      <c r="I38" s="55"/>
-      <c r="J38" s="55"/>
-    </row>
-    <row r="39" spans="2:10" ht="15.75" customHeight="1"/>
+      <c r="C38" s="47"/>
+      <c r="D38" s="47"/>
+      <c r="E38" s="47"/>
+      <c r="F38" s="47"/>
+      <c r="G38" s="47"/>
+      <c r="H38" s="47"/>
+      <c r="I38" s="47"/>
+      <c r="J38" s="48"/>
+    </row>
+    <row r="39" spans="2:10" ht="15.75" customHeight="1">
+      <c r="B39" s="23"/>
+      <c r="C39" s="23"/>
+      <c r="D39" s="23"/>
+      <c r="E39" s="23"/>
+      <c r="F39" s="23"/>
+      <c r="G39" s="23"/>
+      <c r="H39" s="23"/>
+      <c r="I39" s="23"/>
+      <c r="J39" s="23"/>
+    </row>
     <row r="40" spans="2:10" ht="15.75" customHeight="1"/>
     <row r="41" spans="2:10" ht="15.75" customHeight="1"/>
     <row r="42" spans="2:10" ht="15.75" customHeight="1"/>
@@ -2676,10 +2750,88 @@
     <row r="991" ht="15.75" customHeight="1"/>
     <row r="992" ht="15.75" customHeight="1"/>
     <row r="993" ht="15.75" customHeight="1"/>
+    <row r="994" ht="15.75" customHeight="1"/>
   </sheetData>
   <autoFilter ref="B2:J35"/>
   <mergeCells count="101">
     <mergeCell ref="B38:J38"/>
+    <mergeCell ref="J27:J32"/>
+    <mergeCell ref="C27:C32"/>
+    <mergeCell ref="B27:B32"/>
+    <mergeCell ref="H27:H32"/>
+    <mergeCell ref="I27:I32"/>
+    <mergeCell ref="H24:H26"/>
+    <mergeCell ref="G27:G32"/>
+    <mergeCell ref="F27:F32"/>
+    <mergeCell ref="E27:E32"/>
+    <mergeCell ref="D27:D32"/>
+    <mergeCell ref="G24:G26"/>
+    <mergeCell ref="B24:B26"/>
+    <mergeCell ref="C24:C26"/>
+    <mergeCell ref="D24:D26"/>
+    <mergeCell ref="E24:E26"/>
+    <mergeCell ref="F24:F26"/>
+    <mergeCell ref="F21:F23"/>
+    <mergeCell ref="B21:B23"/>
+    <mergeCell ref="C21:C23"/>
+    <mergeCell ref="G21:G23"/>
+    <mergeCell ref="H21:H23"/>
+    <mergeCell ref="D21:D23"/>
+    <mergeCell ref="E21:E23"/>
+    <mergeCell ref="F3:F4"/>
+    <mergeCell ref="F5:F6"/>
+    <mergeCell ref="F7:F8"/>
+    <mergeCell ref="F9:F10"/>
+    <mergeCell ref="F11:F12"/>
+    <mergeCell ref="H18:H20"/>
+    <mergeCell ref="E3:E4"/>
+    <mergeCell ref="G3:G4"/>
+    <mergeCell ref="G5:G6"/>
+    <mergeCell ref="H3:H4"/>
+    <mergeCell ref="H5:H6"/>
+    <mergeCell ref="H7:H8"/>
+    <mergeCell ref="H9:H10"/>
+    <mergeCell ref="H11:H12"/>
+    <mergeCell ref="H13:H14"/>
+    <mergeCell ref="H15:H17"/>
+    <mergeCell ref="G7:G8"/>
+    <mergeCell ref="G9:G10"/>
+    <mergeCell ref="G11:G12"/>
+    <mergeCell ref="G13:G14"/>
+    <mergeCell ref="G15:G17"/>
+    <mergeCell ref="E5:E6"/>
+    <mergeCell ref="E7:E8"/>
+    <mergeCell ref="E9:E10"/>
+    <mergeCell ref="E11:E12"/>
+    <mergeCell ref="E13:E14"/>
+    <mergeCell ref="B3:B4"/>
+    <mergeCell ref="B5:B6"/>
+    <mergeCell ref="B7:B8"/>
+    <mergeCell ref="B9:B10"/>
+    <mergeCell ref="B11:B12"/>
+    <mergeCell ref="B13:B14"/>
+    <mergeCell ref="B15:B17"/>
+    <mergeCell ref="G18:G20"/>
+    <mergeCell ref="E18:E20"/>
+    <mergeCell ref="C18:C20"/>
+    <mergeCell ref="B18:B20"/>
+    <mergeCell ref="F18:F20"/>
+    <mergeCell ref="E15:E17"/>
+    <mergeCell ref="D15:D17"/>
+    <mergeCell ref="D18:D20"/>
+    <mergeCell ref="F13:F14"/>
+    <mergeCell ref="C15:C17"/>
+    <mergeCell ref="F15:F17"/>
+    <mergeCell ref="D13:D14"/>
+    <mergeCell ref="C13:C14"/>
+    <mergeCell ref="D9:D10"/>
+    <mergeCell ref="C3:C4"/>
+    <mergeCell ref="D3:D4"/>
+    <mergeCell ref="C5:C6"/>
+    <mergeCell ref="D5:D6"/>
+    <mergeCell ref="C7:C8"/>
+    <mergeCell ref="D7:D8"/>
+    <mergeCell ref="B39:J39"/>
     <mergeCell ref="J13:J14"/>
     <mergeCell ref="J15:J17"/>
     <mergeCell ref="J18:J20"/>
@@ -2703,83 +2855,6 @@
     <mergeCell ref="C9:C10"/>
     <mergeCell ref="D11:D12"/>
     <mergeCell ref="C11:C12"/>
-    <mergeCell ref="D13:D14"/>
-    <mergeCell ref="C13:C14"/>
-    <mergeCell ref="D9:D10"/>
-    <mergeCell ref="C3:C4"/>
-    <mergeCell ref="D3:D4"/>
-    <mergeCell ref="C5:C6"/>
-    <mergeCell ref="D5:D6"/>
-    <mergeCell ref="C7:C8"/>
-    <mergeCell ref="D7:D8"/>
-    <mergeCell ref="B3:B4"/>
-    <mergeCell ref="B5:B6"/>
-    <mergeCell ref="B7:B8"/>
-    <mergeCell ref="B9:B10"/>
-    <mergeCell ref="B11:B12"/>
-    <mergeCell ref="B13:B14"/>
-    <mergeCell ref="B15:B17"/>
-    <mergeCell ref="G18:G20"/>
-    <mergeCell ref="E18:E20"/>
-    <mergeCell ref="C18:C20"/>
-    <mergeCell ref="B18:B20"/>
-    <mergeCell ref="F18:F20"/>
-    <mergeCell ref="E15:E17"/>
-    <mergeCell ref="D15:D17"/>
-    <mergeCell ref="D18:D20"/>
-    <mergeCell ref="F13:F14"/>
-    <mergeCell ref="C15:C17"/>
-    <mergeCell ref="F15:F17"/>
-    <mergeCell ref="H18:H20"/>
-    <mergeCell ref="E3:E4"/>
-    <mergeCell ref="G3:G4"/>
-    <mergeCell ref="G5:G6"/>
-    <mergeCell ref="H3:H4"/>
-    <mergeCell ref="H5:H6"/>
-    <mergeCell ref="H7:H8"/>
-    <mergeCell ref="H9:H10"/>
-    <mergeCell ref="H11:H12"/>
-    <mergeCell ref="H13:H14"/>
-    <mergeCell ref="H15:H17"/>
-    <mergeCell ref="G7:G8"/>
-    <mergeCell ref="G9:G10"/>
-    <mergeCell ref="G11:G12"/>
-    <mergeCell ref="G13:G14"/>
-    <mergeCell ref="G15:G17"/>
-    <mergeCell ref="E5:E6"/>
-    <mergeCell ref="E7:E8"/>
-    <mergeCell ref="E9:E10"/>
-    <mergeCell ref="E11:E12"/>
-    <mergeCell ref="E13:E14"/>
-    <mergeCell ref="F21:F23"/>
-    <mergeCell ref="B21:B23"/>
-    <mergeCell ref="C21:C23"/>
-    <mergeCell ref="G21:G23"/>
-    <mergeCell ref="H21:H23"/>
-    <mergeCell ref="D21:D23"/>
-    <mergeCell ref="E21:E23"/>
-    <mergeCell ref="F3:F4"/>
-    <mergeCell ref="F5:F6"/>
-    <mergeCell ref="F7:F8"/>
-    <mergeCell ref="F9:F10"/>
-    <mergeCell ref="F11:F12"/>
-    <mergeCell ref="H24:H26"/>
-    <mergeCell ref="G27:G32"/>
-    <mergeCell ref="F27:F32"/>
-    <mergeCell ref="E27:E32"/>
-    <mergeCell ref="D27:D32"/>
-    <mergeCell ref="G24:G26"/>
-    <mergeCell ref="B24:B26"/>
-    <mergeCell ref="C24:C26"/>
-    <mergeCell ref="D24:D26"/>
-    <mergeCell ref="E24:E26"/>
-    <mergeCell ref="F24:F26"/>
-    <mergeCell ref="B37:J37"/>
-    <mergeCell ref="J27:J32"/>
-    <mergeCell ref="C27:C32"/>
-    <mergeCell ref="B27:B32"/>
-    <mergeCell ref="H27:H32"/>
-    <mergeCell ref="I27:I32"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape" r:id="rId1"/>

</xml_diff>

<commit_message>
Analyses des performances après les 2 dernieres corrections
</commit_message>
<xml_diff>
--- a/Analyses/Modèle-audit-SEO.xlsx
+++ b/Analyses/Modèle-audit-SEO.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="60">
   <si>
     <t>Catégorie</t>
   </si>
@@ -280,9 +280,6 @@
  &lt;h1&gt; et &lt;h3&gt;</t>
   </si>
   <si>
-    <t xml:space="preserve"> Incohérence au niveau des titres</t>
-  </si>
-  <si>
     <t xml:space="preserve"> Ne mettre qu'un titre &lt;h1&gt; et
  mettre titres intermédiaires</t>
   </si>
@@ -330,14 +327,11 @@
     <t xml:space="preserve"> Police (visibilité du texte)</t>
   </si>
   <si>
-    <t xml:space="preserve"> Correction des titres</t>
-  </si>
-  <si>
-    <t>Les titres doivent être ordonnés
-(&lt;h1&gt; puis &lt;h2&gt; puis &lt;h3&gt;)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Corriger la hiérarchie des titres</t>
+    <t>Corriger les polices trop petites</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Incohérence au niveau des titres
+ qui doivent être hiérarchisés (&lt;h1&gt;  puis &lt;h2&gt; puis &lt;h3&gt;)</t>
   </si>
 </sst>
 </file>
@@ -460,7 +454,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="19">
+  <borders count="17">
     <border>
       <left/>
       <right/>
@@ -659,45 +653,6 @@
       <top style="thin">
         <color indexed="64"/>
       </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
       <bottom style="medium">
         <color indexed="64"/>
       </bottom>
@@ -707,11 +662,28 @@
       <left style="thin">
         <color indexed="64"/>
       </left>
-      <right/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
       <top style="thin">
         <color indexed="64"/>
       </top>
-      <bottom style="thin">
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
@@ -721,7 +693,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="9" fillId="5" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="62">
+  <cellXfs count="55">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -739,18 +711,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -783,10 +743,85 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -795,80 +830,14 @@
     <xf numFmtId="0" fontId="7" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -885,25 +854,7 @@
     <xf numFmtId="0" fontId="7" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1119,10 +1070,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B1:AB994"/>
+  <dimension ref="B1:AB993"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="J36" sqref="J36"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="E40" sqref="E40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.33203125" defaultRowHeight="15" customHeight="1"/>
@@ -1141,31 +1092,31 @@
   <sheetData>
     <row r="1" spans="2:28" ht="15" customHeight="1" thickBot="1"/>
     <row r="2" spans="2:28" ht="15.75" customHeight="1" thickBot="1">
-      <c r="B2" s="12" t="s">
+      <c r="B2" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="C2" s="13" t="s">
+      <c r="C2" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="13" t="s">
+      <c r="D2" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="E2" s="13" t="s">
+      <c r="E2" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="F2" s="13" t="s">
+      <c r="F2" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="G2" s="13" t="s">
+      <c r="G2" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="H2" s="13" t="s">
+      <c r="H2" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="I2" s="14" t="s">
+      <c r="I2" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="J2" s="15" t="s">
+      <c r="J2" s="11" t="s">
         <v>40</v>
       </c>
       <c r="K2" s="5"/>
@@ -1188,120 +1139,120 @@
       <c r="AB2" s="1"/>
     </row>
     <row r="3" spans="2:28" ht="15.75" customHeight="1">
-      <c r="B3" s="38">
+      <c r="B3" s="41">
         <v>1</v>
       </c>
-      <c r="C3" s="35" t="s">
+      <c r="C3" s="43" t="s">
         <v>38</v>
       </c>
-      <c r="D3" s="35" t="s">
+      <c r="D3" s="43" t="s">
         <v>7</v>
       </c>
-      <c r="E3" s="41" t="s">
+      <c r="E3" s="37" t="s">
         <v>14</v>
       </c>
-      <c r="F3" s="41" t="s">
+      <c r="F3" s="37" t="s">
         <v>37</v>
       </c>
-      <c r="G3" s="41" t="s">
+      <c r="G3" s="37" t="s">
         <v>15</v>
       </c>
-      <c r="H3" s="43"/>
-      <c r="I3" s="29">
+      <c r="H3" s="40"/>
+      <c r="I3" s="48">
         <v>1</v>
       </c>
-      <c r="J3" s="26" t="s">
+      <c r="J3" s="47" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="4" spans="2:28" ht="15.75" customHeight="1">
-      <c r="B4" s="39"/>
-      <c r="C4" s="36"/>
-      <c r="D4" s="36"/>
-      <c r="E4" s="42"/>
-      <c r="F4" s="42"/>
-      <c r="G4" s="42"/>
-      <c r="H4" s="42"/>
-      <c r="I4" s="28"/>
-      <c r="J4" s="24"/>
+      <c r="B4" s="28"/>
+      <c r="C4" s="27"/>
+      <c r="D4" s="27"/>
+      <c r="E4" s="29"/>
+      <c r="F4" s="29"/>
+      <c r="G4" s="29"/>
+      <c r="H4" s="29"/>
+      <c r="I4" s="30"/>
+      <c r="J4" s="45"/>
     </row>
     <row r="5" spans="2:28" ht="15.75" customHeight="1">
-      <c r="B5" s="40">
+      <c r="B5" s="35">
         <v>2</v>
       </c>
-      <c r="C5" s="30" t="s">
+      <c r="C5" s="36" t="s">
         <v>38</v>
       </c>
-      <c r="D5" s="33" t="s">
+      <c r="D5" s="31" t="s">
         <v>8</v>
       </c>
       <c r="E5" s="34" t="s">
         <v>14</v>
       </c>
-      <c r="F5" s="45"/>
+      <c r="F5" s="38"/>
       <c r="G5" s="34" t="s">
         <v>16</v>
       </c>
-      <c r="H5" s="33"/>
-      <c r="I5" s="27">
+      <c r="H5" s="31"/>
+      <c r="I5" s="46">
         <v>2</v>
       </c>
-      <c r="J5" s="24" t="s">
+      <c r="J5" s="45" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="6" spans="2:28" ht="15.75" customHeight="1">
-      <c r="B6" s="40"/>
-      <c r="C6" s="30"/>
-      <c r="D6" s="33"/>
-      <c r="E6" s="33"/>
-      <c r="F6" s="45"/>
-      <c r="G6" s="33"/>
-      <c r="H6" s="33"/>
-      <c r="I6" s="27"/>
-      <c r="J6" s="24"/>
+      <c r="B6" s="35"/>
+      <c r="C6" s="36"/>
+      <c r="D6" s="31"/>
+      <c r="E6" s="31"/>
+      <c r="F6" s="38"/>
+      <c r="G6" s="31"/>
+      <c r="H6" s="31"/>
+      <c r="I6" s="46"/>
+      <c r="J6" s="45"/>
     </row>
     <row r="7" spans="2:28" ht="15.75" customHeight="1">
-      <c r="B7" s="39">
+      <c r="B7" s="28">
         <v>3</v>
       </c>
-      <c r="C7" s="32" t="s">
+      <c r="C7" s="42" t="s">
         <v>6</v>
       </c>
-      <c r="D7" s="37" t="s">
+      <c r="D7" s="33" t="s">
         <v>24</v>
       </c>
-      <c r="E7" s="37" t="s">
+      <c r="E7" s="33" t="s">
         <v>21</v>
       </c>
-      <c r="F7" s="31"/>
-      <c r="G7" s="37" t="s">
+      <c r="F7" s="39"/>
+      <c r="G7" s="33" t="s">
         <v>17</v>
       </c>
-      <c r="H7" s="31"/>
-      <c r="I7" s="28">
+      <c r="H7" s="39"/>
+      <c r="I7" s="30">
         <v>10</v>
       </c>
-      <c r="J7" s="24" t="s">
+      <c r="J7" s="45" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="8" spans="2:28" ht="15.75" customHeight="1">
-      <c r="B8" s="39"/>
-      <c r="C8" s="32"/>
-      <c r="D8" s="31"/>
-      <c r="E8" s="31"/>
-      <c r="F8" s="31"/>
-      <c r="G8" s="31"/>
-      <c r="H8" s="31"/>
-      <c r="I8" s="28"/>
-      <c r="J8" s="24"/>
+      <c r="B8" s="28"/>
+      <c r="C8" s="42"/>
+      <c r="D8" s="39"/>
+      <c r="E8" s="39"/>
+      <c r="F8" s="39"/>
+      <c r="G8" s="39"/>
+      <c r="H8" s="39"/>
+      <c r="I8" s="30"/>
+      <c r="J8" s="45"/>
     </row>
     <row r="9" spans="2:28" ht="15.75" customHeight="1">
-      <c r="B9" s="40">
+      <c r="B9" s="35">
         <v>4</v>
       </c>
-      <c r="C9" s="30" t="s">
+      <c r="C9" s="36" t="s">
         <v>6</v>
       </c>
       <c r="D9" s="34" t="s">
@@ -1310,492 +1261,470 @@
       <c r="E9" s="34" t="s">
         <v>22</v>
       </c>
-      <c r="F9" s="33"/>
+      <c r="F9" s="31"/>
       <c r="G9" s="34" t="s">
         <v>18</v>
       </c>
-      <c r="H9" s="33"/>
-      <c r="I9" s="27">
+      <c r="H9" s="31"/>
+      <c r="I9" s="46">
         <v>4</v>
       </c>
-      <c r="J9" s="24" t="s">
+      <c r="J9" s="45" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="10" spans="2:28" ht="15.75" customHeight="1">
-      <c r="B10" s="40"/>
-      <c r="C10" s="30"/>
-      <c r="D10" s="33"/>
-      <c r="E10" s="33"/>
-      <c r="F10" s="33"/>
-      <c r="G10" s="33"/>
-      <c r="H10" s="33"/>
-      <c r="I10" s="27"/>
-      <c r="J10" s="24"/>
+      <c r="B10" s="35"/>
+      <c r="C10" s="36"/>
+      <c r="D10" s="31"/>
+      <c r="E10" s="31"/>
+      <c r="F10" s="31"/>
+      <c r="G10" s="31"/>
+      <c r="H10" s="31"/>
+      <c r="I10" s="46"/>
+      <c r="J10" s="45"/>
     </row>
     <row r="11" spans="2:28" ht="15.75" customHeight="1">
-      <c r="B11" s="39">
+      <c r="B11" s="28">
         <v>5</v>
       </c>
-      <c r="C11" s="32" t="s">
+      <c r="C11" s="42" t="s">
         <v>10</v>
       </c>
-      <c r="D11" s="31" t="s">
+      <c r="D11" s="39" t="s">
         <v>11</v>
       </c>
-      <c r="E11" s="37" t="s">
+      <c r="E11" s="33" t="s">
         <v>35</v>
       </c>
-      <c r="F11" s="31"/>
-      <c r="G11" s="37" t="s">
+      <c r="F11" s="39"/>
+      <c r="G11" s="33" t="s">
         <v>19</v>
       </c>
-      <c r="H11" s="31"/>
-      <c r="I11" s="28">
+      <c r="H11" s="39"/>
+      <c r="I11" s="30">
         <v>5</v>
       </c>
-      <c r="J11" s="24" t="s">
+      <c r="J11" s="45" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="12" spans="2:28" ht="15.75" customHeight="1">
-      <c r="B12" s="39"/>
-      <c r="C12" s="32"/>
-      <c r="D12" s="31"/>
-      <c r="E12" s="31"/>
-      <c r="F12" s="31"/>
-      <c r="G12" s="31"/>
-      <c r="H12" s="31"/>
-      <c r="I12" s="28"/>
-      <c r="J12" s="24"/>
+      <c r="B12" s="28"/>
+      <c r="C12" s="42"/>
+      <c r="D12" s="39"/>
+      <c r="E12" s="39"/>
+      <c r="F12" s="39"/>
+      <c r="G12" s="39"/>
+      <c r="H12" s="39"/>
+      <c r="I12" s="30"/>
+      <c r="J12" s="45"/>
     </row>
     <row r="13" spans="2:28" ht="15.75" customHeight="1">
-      <c r="B13" s="40">
+      <c r="B13" s="35">
         <v>6</v>
       </c>
-      <c r="C13" s="30" t="s">
+      <c r="C13" s="36" t="s">
         <v>6</v>
       </c>
-      <c r="D13" s="33" t="s">
-        <v>54</v>
+      <c r="D13" s="31" t="s">
+        <v>53</v>
       </c>
       <c r="E13" s="34" t="s">
         <v>33</v>
       </c>
-      <c r="F13" s="33"/>
+      <c r="F13" s="31"/>
       <c r="G13" s="34" t="s">
-        <v>55</v>
-      </c>
-      <c r="H13" s="33"/>
-      <c r="I13" s="27">
+        <v>54</v>
+      </c>
+      <c r="H13" s="31"/>
+      <c r="I13" s="46">
         <v>9</v>
       </c>
-      <c r="J13" s="24" t="s">
+      <c r="J13" s="45" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="14" spans="2:28" ht="15.75" customHeight="1">
-      <c r="B14" s="40"/>
-      <c r="C14" s="30"/>
-      <c r="D14" s="33"/>
-      <c r="E14" s="33"/>
-      <c r="F14" s="33"/>
-      <c r="G14" s="33"/>
-      <c r="H14" s="33"/>
-      <c r="I14" s="27"/>
-      <c r="J14" s="24"/>
+      <c r="B14" s="35"/>
+      <c r="C14" s="36"/>
+      <c r="D14" s="31"/>
+      <c r="E14" s="31"/>
+      <c r="F14" s="31"/>
+      <c r="G14" s="31"/>
+      <c r="H14" s="31"/>
+      <c r="I14" s="46"/>
+      <c r="J14" s="45"/>
     </row>
     <row r="15" spans="2:28" ht="15.75" customHeight="1">
-      <c r="B15" s="39">
+      <c r="B15" s="28">
         <v>7</v>
       </c>
-      <c r="C15" s="32" t="s">
+      <c r="C15" s="42" t="s">
         <v>6</v>
       </c>
-      <c r="D15" s="37" t="s">
+      <c r="D15" s="33" t="s">
         <v>26</v>
       </c>
-      <c r="E15" s="37" t="s">
+      <c r="E15" s="33" t="s">
         <v>23</v>
       </c>
-      <c r="F15" s="31"/>
-      <c r="G15" s="37" t="s">
+      <c r="F15" s="39"/>
+      <c r="G15" s="33" t="s">
         <v>20</v>
       </c>
-      <c r="H15" s="31"/>
-      <c r="I15" s="28">
+      <c r="H15" s="39"/>
+      <c r="I15" s="30">
         <v>8</v>
       </c>
-      <c r="J15" s="24" t="s">
+      <c r="J15" s="45" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="16" spans="2:28" ht="15.75" customHeight="1">
-      <c r="B16" s="39"/>
-      <c r="C16" s="32"/>
-      <c r="D16" s="31"/>
-      <c r="E16" s="31"/>
-      <c r="F16" s="31"/>
-      <c r="G16" s="31"/>
-      <c r="H16" s="31"/>
-      <c r="I16" s="28"/>
-      <c r="J16" s="24"/>
+      <c r="B16" s="28"/>
+      <c r="C16" s="42"/>
+      <c r="D16" s="39"/>
+      <c r="E16" s="39"/>
+      <c r="F16" s="39"/>
+      <c r="G16" s="39"/>
+      <c r="H16" s="39"/>
+      <c r="I16" s="30"/>
+      <c r="J16" s="45"/>
     </row>
     <row r="17" spans="2:10" ht="15.75" customHeight="1">
-      <c r="B17" s="39"/>
-      <c r="C17" s="32"/>
-      <c r="D17" s="31"/>
-      <c r="E17" s="31"/>
-      <c r="F17" s="31"/>
-      <c r="G17" s="31"/>
-      <c r="H17" s="31"/>
-      <c r="I17" s="28"/>
-      <c r="J17" s="24"/>
+      <c r="B17" s="28"/>
+      <c r="C17" s="42"/>
+      <c r="D17" s="39"/>
+      <c r="E17" s="39"/>
+      <c r="F17" s="39"/>
+      <c r="G17" s="39"/>
+      <c r="H17" s="39"/>
+      <c r="I17" s="30"/>
+      <c r="J17" s="45"/>
     </row>
     <row r="18" spans="2:10" ht="15.75" customHeight="1">
-      <c r="B18" s="40">
+      <c r="B18" s="35">
         <v>8</v>
       </c>
-      <c r="C18" s="30" t="s">
+      <c r="C18" s="36" t="s">
         <v>9</v>
       </c>
       <c r="D18" s="34" t="s">
+        <v>51</v>
+      </c>
+      <c r="E18" s="31" t="s">
+        <v>12</v>
+      </c>
+      <c r="F18" s="31"/>
+      <c r="G18" s="34" t="s">
         <v>52</v>
       </c>
-      <c r="E18" s="33" t="s">
-        <v>12</v>
-      </c>
-      <c r="F18" s="33"/>
-      <c r="G18" s="34" t="s">
-        <v>53</v>
-      </c>
-      <c r="H18" s="33"/>
-      <c r="I18" s="27">
+      <c r="H18" s="31"/>
+      <c r="I18" s="46">
         <v>7</v>
       </c>
-      <c r="J18" s="24" t="s">
+      <c r="J18" s="45" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="19" spans="2:10" ht="15.75" customHeight="1">
-      <c r="B19" s="40"/>
-      <c r="C19" s="30"/>
-      <c r="D19" s="33"/>
-      <c r="E19" s="33"/>
-      <c r="F19" s="33"/>
-      <c r="G19" s="33"/>
-      <c r="H19" s="33"/>
-      <c r="I19" s="27"/>
-      <c r="J19" s="24"/>
+      <c r="B19" s="35"/>
+      <c r="C19" s="36"/>
+      <c r="D19" s="31"/>
+      <c r="E19" s="31"/>
+      <c r="F19" s="31"/>
+      <c r="G19" s="31"/>
+      <c r="H19" s="31"/>
+      <c r="I19" s="46"/>
+      <c r="J19" s="45"/>
     </row>
     <row r="20" spans="2:10" ht="15.75" customHeight="1">
-      <c r="B20" s="40"/>
-      <c r="C20" s="30"/>
-      <c r="D20" s="33"/>
-      <c r="E20" s="33"/>
-      <c r="F20" s="33"/>
-      <c r="G20" s="33"/>
-      <c r="H20" s="33"/>
-      <c r="I20" s="27"/>
-      <c r="J20" s="24"/>
+      <c r="B20" s="35"/>
+      <c r="C20" s="36"/>
+      <c r="D20" s="31"/>
+      <c r="E20" s="31"/>
+      <c r="F20" s="31"/>
+      <c r="G20" s="31"/>
+      <c r="H20" s="31"/>
+      <c r="I20" s="46"/>
+      <c r="J20" s="45"/>
     </row>
     <row r="21" spans="2:10" ht="15.75" customHeight="1">
-      <c r="B21" s="39">
+      <c r="B21" s="28">
         <v>9</v>
       </c>
-      <c r="C21" s="36" t="s">
+      <c r="C21" s="27" t="s">
         <v>9</v>
       </c>
-      <c r="D21" s="44" t="s">
+      <c r="D21" s="32" t="s">
         <v>36</v>
       </c>
-      <c r="E21" s="44" t="s">
+      <c r="E21" s="32" t="s">
         <v>28</v>
       </c>
-      <c r="F21" s="42"/>
-      <c r="G21" s="42" t="s">
+      <c r="F21" s="29"/>
+      <c r="G21" s="29" t="s">
         <v>27</v>
       </c>
-      <c r="H21" s="42"/>
-      <c r="I21" s="28">
+      <c r="H21" s="29"/>
+      <c r="I21" s="30">
         <v>3</v>
       </c>
-      <c r="J21" s="24" t="s">
+      <c r="J21" s="45" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="22" spans="2:10" ht="15.75" customHeight="1">
-      <c r="B22" s="39"/>
-      <c r="C22" s="36"/>
-      <c r="D22" s="44"/>
-      <c r="E22" s="42"/>
-      <c r="F22" s="42"/>
-      <c r="G22" s="42"/>
-      <c r="H22" s="42"/>
-      <c r="I22" s="28"/>
-      <c r="J22" s="24"/>
+      <c r="B22" s="28"/>
+      <c r="C22" s="27"/>
+      <c r="D22" s="32"/>
+      <c r="E22" s="29"/>
+      <c r="F22" s="29"/>
+      <c r="G22" s="29"/>
+      <c r="H22" s="29"/>
+      <c r="I22" s="30"/>
+      <c r="J22" s="45"/>
     </row>
     <row r="23" spans="2:10" ht="15.75" customHeight="1">
-      <c r="B23" s="39"/>
-      <c r="C23" s="36"/>
-      <c r="D23" s="44"/>
-      <c r="E23" s="42"/>
-      <c r="F23" s="42"/>
-      <c r="G23" s="42"/>
-      <c r="H23" s="42"/>
-      <c r="I23" s="28"/>
-      <c r="J23" s="24"/>
+      <c r="B23" s="28"/>
+      <c r="C23" s="27"/>
+      <c r="D23" s="32"/>
+      <c r="E23" s="29"/>
+      <c r="F23" s="29"/>
+      <c r="G23" s="29"/>
+      <c r="H23" s="29"/>
+      <c r="I23" s="30"/>
+      <c r="J23" s="45"/>
     </row>
     <row r="24" spans="2:10" ht="15.75" customHeight="1">
-      <c r="B24" s="40">
+      <c r="B24" s="35">
         <v>10</v>
       </c>
-      <c r="C24" s="30" t="s">
+      <c r="C24" s="36" t="s">
         <v>9</v>
       </c>
       <c r="D24" s="34" t="s">
         <v>31</v>
       </c>
-      <c r="E24" s="33" t="s">
+      <c r="E24" s="31" t="s">
         <v>29</v>
       </c>
-      <c r="F24" s="33"/>
+      <c r="F24" s="31"/>
       <c r="G24" s="34" t="s">
         <v>30</v>
       </c>
-      <c r="H24" s="33"/>
-      <c r="I24" s="27" t="s">
+      <c r="H24" s="31"/>
+      <c r="I24" s="46" t="s">
         <v>39</v>
       </c>
-      <c r="J24" s="25" t="s">
+      <c r="J24" s="26" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="25" spans="2:10" ht="15.75" customHeight="1">
-      <c r="B25" s="40"/>
-      <c r="C25" s="30"/>
-      <c r="D25" s="33"/>
-      <c r="E25" s="33"/>
-      <c r="F25" s="33"/>
+      <c r="B25" s="35"/>
+      <c r="C25" s="36"/>
+      <c r="D25" s="31"/>
+      <c r="E25" s="31"/>
+      <c r="F25" s="31"/>
       <c r="G25" s="34"/>
-      <c r="H25" s="33"/>
-      <c r="I25" s="27"/>
-      <c r="J25" s="25"/>
+      <c r="H25" s="31"/>
+      <c r="I25" s="46"/>
+      <c r="J25" s="26"/>
     </row>
     <row r="26" spans="2:10" ht="15.75" customHeight="1">
-      <c r="B26" s="40"/>
-      <c r="C26" s="30"/>
-      <c r="D26" s="33"/>
-      <c r="E26" s="33"/>
-      <c r="F26" s="33"/>
+      <c r="B26" s="35"/>
+      <c r="C26" s="36"/>
+      <c r="D26" s="31"/>
+      <c r="E26" s="31"/>
+      <c r="F26" s="31"/>
       <c r="G26" s="34"/>
-      <c r="H26" s="33"/>
-      <c r="I26" s="27"/>
-      <c r="J26" s="25"/>
+      <c r="H26" s="31"/>
+      <c r="I26" s="46"/>
+      <c r="J26" s="26"/>
     </row>
     <row r="27" spans="2:10" ht="15.75" customHeight="1">
-      <c r="B27" s="39">
+      <c r="B27" s="28">
         <v>11</v>
       </c>
-      <c r="C27" s="36" t="s">
+      <c r="C27" s="27" t="s">
         <v>10</v>
       </c>
-      <c r="D27" s="44" t="s">
+      <c r="D27" s="32" t="s">
         <v>43</v>
       </c>
-      <c r="E27" s="37" t="s">
+      <c r="E27" s="33" t="s">
         <v>44</v>
       </c>
-      <c r="F27" s="42"/>
-      <c r="G27" s="44" t="s">
+      <c r="F27" s="29"/>
+      <c r="G27" s="32" t="s">
         <v>32</v>
       </c>
-      <c r="H27" s="42"/>
-      <c r="I27" s="28" t="s">
+      <c r="H27" s="29"/>
+      <c r="I27" s="30" t="s">
         <v>39</v>
       </c>
-      <c r="J27" s="49" t="s">
+      <c r="J27" s="25" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="28" spans="2:10" ht="15.75" customHeight="1">
-      <c r="B28" s="39"/>
-      <c r="C28" s="36"/>
-      <c r="D28" s="44"/>
-      <c r="E28" s="37"/>
-      <c r="F28" s="42"/>
-      <c r="G28" s="44"/>
-      <c r="H28" s="42"/>
-      <c r="I28" s="28"/>
-      <c r="J28" s="25"/>
+      <c r="B28" s="28"/>
+      <c r="C28" s="27"/>
+      <c r="D28" s="32"/>
+      <c r="E28" s="33"/>
+      <c r="F28" s="29"/>
+      <c r="G28" s="32"/>
+      <c r="H28" s="29"/>
+      <c r="I28" s="30"/>
+      <c r="J28" s="26"/>
     </row>
     <row r="29" spans="2:10" ht="15.75" customHeight="1">
-      <c r="B29" s="39"/>
-      <c r="C29" s="36"/>
-      <c r="D29" s="44"/>
-      <c r="E29" s="37"/>
-      <c r="F29" s="42"/>
-      <c r="G29" s="44"/>
-      <c r="H29" s="42"/>
-      <c r="I29" s="28"/>
-      <c r="J29" s="25"/>
+      <c r="B29" s="28"/>
+      <c r="C29" s="27"/>
+      <c r="D29" s="32"/>
+      <c r="E29" s="33"/>
+      <c r="F29" s="29"/>
+      <c r="G29" s="32"/>
+      <c r="H29" s="29"/>
+      <c r="I29" s="30"/>
+      <c r="J29" s="26"/>
     </row>
     <row r="30" spans="2:10" ht="15.75" customHeight="1">
-      <c r="B30" s="39"/>
-      <c r="C30" s="36"/>
-      <c r="D30" s="44"/>
-      <c r="E30" s="37"/>
-      <c r="F30" s="42"/>
-      <c r="G30" s="44"/>
-      <c r="H30" s="42"/>
-      <c r="I30" s="28"/>
-      <c r="J30" s="25"/>
+      <c r="B30" s="28"/>
+      <c r="C30" s="27"/>
+      <c r="D30" s="32"/>
+      <c r="E30" s="33"/>
+      <c r="F30" s="29"/>
+      <c r="G30" s="32"/>
+      <c r="H30" s="29"/>
+      <c r="I30" s="30"/>
+      <c r="J30" s="26"/>
     </row>
     <row r="31" spans="2:10" ht="15.75" customHeight="1">
-      <c r="B31" s="39"/>
-      <c r="C31" s="36"/>
-      <c r="D31" s="44"/>
-      <c r="E31" s="37"/>
-      <c r="F31" s="42"/>
-      <c r="G31" s="44"/>
-      <c r="H31" s="42"/>
-      <c r="I31" s="28"/>
-      <c r="J31" s="25"/>
+      <c r="B31" s="28"/>
+      <c r="C31" s="27"/>
+      <c r="D31" s="32"/>
+      <c r="E31" s="33"/>
+      <c r="F31" s="29"/>
+      <c r="G31" s="32"/>
+      <c r="H31" s="29"/>
+      <c r="I31" s="30"/>
+      <c r="J31" s="26"/>
     </row>
     <row r="32" spans="2:10" ht="15.75" customHeight="1">
-      <c r="B32" s="39"/>
-      <c r="C32" s="36"/>
-      <c r="D32" s="44"/>
-      <c r="E32" s="37"/>
-      <c r="F32" s="42"/>
-      <c r="G32" s="44"/>
-      <c r="H32" s="42"/>
-      <c r="I32" s="28"/>
-      <c r="J32" s="25"/>
+      <c r="B32" s="28"/>
+      <c r="C32" s="27"/>
+      <c r="D32" s="32"/>
+      <c r="E32" s="33"/>
+      <c r="F32" s="29"/>
+      <c r="G32" s="32"/>
+      <c r="H32" s="29"/>
+      <c r="I32" s="30"/>
+      <c r="J32" s="26"/>
     </row>
     <row r="33" spans="2:10" ht="63" customHeight="1">
-      <c r="B33" s="16">
+      <c r="B33" s="12">
         <v>12</v>
       </c>
-      <c r="C33" s="17" t="s">
+      <c r="C33" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="D33" s="18" t="s">
+      <c r="D33" s="14" t="s">
         <v>45</v>
       </c>
-      <c r="E33" s="19" t="s">
+      <c r="E33" s="16" t="s">
+        <v>59</v>
+      </c>
+      <c r="F33" s="15"/>
+      <c r="G33" s="16" t="s">
         <v>46</v>
       </c>
-      <c r="F33" s="19"/>
-      <c r="G33" s="20" t="s">
+      <c r="H33" s="15"/>
+      <c r="I33" s="18">
+        <v>11</v>
+      </c>
+      <c r="J33" s="17" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="34" spans="2:10" ht="63" customHeight="1">
+      <c r="B34" s="20">
+        <v>13</v>
+      </c>
+      <c r="C34" s="21" t="s">
+        <v>38</v>
+      </c>
+      <c r="D34" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="H33" s="19"/>
-      <c r="I33" s="22">
-        <v>11</v>
-      </c>
-      <c r="J33" s="21" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="34" spans="2:10" ht="63" customHeight="1">
-      <c r="B34" s="7">
-        <v>13</v>
-      </c>
-      <c r="C34" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="D34" s="10" t="s">
+      <c r="E34" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="F34" s="7"/>
+      <c r="G34" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="E34" s="10" t="s">
+      <c r="H34" s="7"/>
+      <c r="I34" s="19">
+        <v>6</v>
+      </c>
+      <c r="J34" s="17" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="35" spans="2:10" ht="63" customHeight="1" thickBot="1">
+      <c r="B35" s="49">
+        <v>14</v>
+      </c>
+      <c r="C35" s="50" t="s">
+        <v>55</v>
+      </c>
+      <c r="D35" s="51" t="s">
+        <v>57</v>
+      </c>
+      <c r="E35" s="51" t="s">
+        <v>56</v>
+      </c>
+      <c r="F35" s="52"/>
+      <c r="G35" s="51" t="s">
+        <v>58</v>
+      </c>
+      <c r="H35" s="52"/>
+      <c r="I35" s="53">
+        <v>12</v>
+      </c>
+      <c r="J35" s="54" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="36" spans="2:10" ht="15.75" customHeight="1" thickBot="1"/>
+    <row r="37" spans="2:10" ht="15.75" customHeight="1" thickBot="1">
+      <c r="B37" s="22" t="s">
         <v>50</v>
       </c>
-      <c r="F34" s="11"/>
-      <c r="G34" s="10" t="s">
-        <v>49</v>
-      </c>
-      <c r="H34" s="11"/>
-      <c r="I34" s="8">
-        <v>6</v>
-      </c>
-      <c r="J34" s="9" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="35" spans="2:10" ht="63" customHeight="1" thickBot="1">
-      <c r="B35" s="50">
-        <v>14</v>
-      </c>
-      <c r="C35" s="51" t="s">
-        <v>56</v>
-      </c>
-      <c r="D35" s="52" t="s">
-        <v>58</v>
-      </c>
-      <c r="E35" s="52" t="s">
-        <v>57</v>
-      </c>
-      <c r="F35" s="53"/>
-      <c r="G35" s="52"/>
-      <c r="H35" s="53"/>
-      <c r="I35" s="54">
-        <v>12</v>
-      </c>
-      <c r="J35" s="55" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="36" spans="2:10" ht="63" customHeight="1" thickBot="1">
-      <c r="B36" s="56">
-        <v>15</v>
-      </c>
-      <c r="C36" s="57" t="s">
-        <v>56</v>
-      </c>
-      <c r="D36" s="58" t="s">
-        <v>59</v>
-      </c>
-      <c r="E36" s="58" t="s">
-        <v>60</v>
-      </c>
-      <c r="F36" s="59"/>
-      <c r="G36" s="58" t="s">
-        <v>61</v>
-      </c>
-      <c r="H36" s="59"/>
-      <c r="I36" s="60">
-        <v>13</v>
-      </c>
-      <c r="J36" s="61" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="37" spans="2:10" ht="15.75" customHeight="1" thickBot="1"/>
-    <row r="38" spans="2:10" ht="15.75" customHeight="1" thickBot="1">
-      <c r="B38" s="46" t="s">
-        <v>51</v>
-      </c>
-      <c r="C38" s="47"/>
-      <c r="D38" s="47"/>
-      <c r="E38" s="47"/>
-      <c r="F38" s="47"/>
-      <c r="G38" s="47"/>
-      <c r="H38" s="47"/>
-      <c r="I38" s="47"/>
-      <c r="J38" s="48"/>
-    </row>
-    <row r="39" spans="2:10" ht="15.75" customHeight="1">
-      <c r="B39" s="23"/>
-      <c r="C39" s="23"/>
-      <c r="D39" s="23"/>
-      <c r="E39" s="23"/>
-      <c r="F39" s="23"/>
-      <c r="G39" s="23"/>
-      <c r="H39" s="23"/>
-      <c r="I39" s="23"/>
-      <c r="J39" s="23"/>
-    </row>
+      <c r="C37" s="23"/>
+      <c r="D37" s="23"/>
+      <c r="E37" s="23"/>
+      <c r="F37" s="23"/>
+      <c r="G37" s="23"/>
+      <c r="H37" s="23"/>
+      <c r="I37" s="23"/>
+      <c r="J37" s="24"/>
+    </row>
+    <row r="38" spans="2:10" ht="15.75" customHeight="1">
+      <c r="B38" s="44"/>
+      <c r="C38" s="44"/>
+      <c r="D38" s="44"/>
+      <c r="E38" s="44"/>
+      <c r="F38" s="44"/>
+      <c r="G38" s="44"/>
+      <c r="H38" s="44"/>
+      <c r="I38" s="44"/>
+      <c r="J38" s="44"/>
+    </row>
+    <row r="39" spans="2:10" ht="15.75" customHeight="1"/>
     <row r="40" spans="2:10" ht="15.75" customHeight="1"/>
     <row r="41" spans="2:10" ht="15.75" customHeight="1"/>
     <row r="42" spans="2:10" ht="15.75" customHeight="1"/>
@@ -2750,60 +2679,45 @@
     <row r="991" ht="15.75" customHeight="1"/>
     <row r="992" ht="15.75" customHeight="1"/>
     <row r="993" ht="15.75" customHeight="1"/>
-    <row r="994" ht="15.75" customHeight="1"/>
   </sheetData>
   <autoFilter ref="B2:J35"/>
   <mergeCells count="101">
-    <mergeCell ref="B38:J38"/>
-    <mergeCell ref="J27:J32"/>
-    <mergeCell ref="C27:C32"/>
-    <mergeCell ref="B27:B32"/>
-    <mergeCell ref="H27:H32"/>
-    <mergeCell ref="I27:I32"/>
-    <mergeCell ref="H24:H26"/>
-    <mergeCell ref="G27:G32"/>
-    <mergeCell ref="F27:F32"/>
-    <mergeCell ref="E27:E32"/>
-    <mergeCell ref="D27:D32"/>
-    <mergeCell ref="G24:G26"/>
-    <mergeCell ref="B24:B26"/>
-    <mergeCell ref="C24:C26"/>
-    <mergeCell ref="D24:D26"/>
-    <mergeCell ref="E24:E26"/>
-    <mergeCell ref="F24:F26"/>
-    <mergeCell ref="F21:F23"/>
-    <mergeCell ref="B21:B23"/>
-    <mergeCell ref="C21:C23"/>
-    <mergeCell ref="G21:G23"/>
-    <mergeCell ref="H21:H23"/>
-    <mergeCell ref="D21:D23"/>
-    <mergeCell ref="E21:E23"/>
-    <mergeCell ref="F3:F4"/>
-    <mergeCell ref="F5:F6"/>
-    <mergeCell ref="F7:F8"/>
-    <mergeCell ref="F9:F10"/>
-    <mergeCell ref="F11:F12"/>
-    <mergeCell ref="H18:H20"/>
-    <mergeCell ref="E3:E4"/>
-    <mergeCell ref="G3:G4"/>
-    <mergeCell ref="G5:G6"/>
-    <mergeCell ref="H3:H4"/>
-    <mergeCell ref="H5:H6"/>
-    <mergeCell ref="H7:H8"/>
-    <mergeCell ref="H9:H10"/>
-    <mergeCell ref="H11:H12"/>
-    <mergeCell ref="H13:H14"/>
-    <mergeCell ref="H15:H17"/>
-    <mergeCell ref="G7:G8"/>
-    <mergeCell ref="G9:G10"/>
-    <mergeCell ref="G11:G12"/>
-    <mergeCell ref="G13:G14"/>
-    <mergeCell ref="G15:G17"/>
     <mergeCell ref="E5:E6"/>
     <mergeCell ref="E7:E8"/>
     <mergeCell ref="E9:E10"/>
     <mergeCell ref="E11:E12"/>
     <mergeCell ref="E13:E14"/>
+    <mergeCell ref="F21:F23"/>
+    <mergeCell ref="B21:B23"/>
+    <mergeCell ref="J3:J4"/>
+    <mergeCell ref="J5:J6"/>
+    <mergeCell ref="J7:J8"/>
+    <mergeCell ref="J9:J10"/>
+    <mergeCell ref="J11:J12"/>
+    <mergeCell ref="I13:I14"/>
+    <mergeCell ref="I15:I17"/>
+    <mergeCell ref="I18:I20"/>
+    <mergeCell ref="I21:I23"/>
+    <mergeCell ref="I3:I4"/>
+    <mergeCell ref="I5:I6"/>
+    <mergeCell ref="I7:I8"/>
+    <mergeCell ref="I9:I10"/>
+    <mergeCell ref="I11:I12"/>
+    <mergeCell ref="D7:D8"/>
+    <mergeCell ref="B38:J38"/>
+    <mergeCell ref="J13:J14"/>
+    <mergeCell ref="J15:J17"/>
+    <mergeCell ref="J18:J20"/>
+    <mergeCell ref="J21:J23"/>
+    <mergeCell ref="J24:J26"/>
+    <mergeCell ref="I24:I26"/>
+    <mergeCell ref="C9:C10"/>
+    <mergeCell ref="D11:D12"/>
+    <mergeCell ref="C11:C12"/>
+    <mergeCell ref="G9:G10"/>
+    <mergeCell ref="G11:G12"/>
+    <mergeCell ref="G13:G14"/>
+    <mergeCell ref="G15:G17"/>
     <mergeCell ref="B3:B4"/>
     <mergeCell ref="B5:B6"/>
     <mergeCell ref="B7:B8"/>
@@ -2828,33 +2742,47 @@
     <mergeCell ref="C3:C4"/>
     <mergeCell ref="D3:D4"/>
     <mergeCell ref="C5:C6"/>
+    <mergeCell ref="C21:C23"/>
+    <mergeCell ref="G21:G23"/>
+    <mergeCell ref="H21:H23"/>
+    <mergeCell ref="D21:D23"/>
+    <mergeCell ref="E21:E23"/>
+    <mergeCell ref="F3:F4"/>
+    <mergeCell ref="F5:F6"/>
+    <mergeCell ref="F7:F8"/>
+    <mergeCell ref="F9:F10"/>
+    <mergeCell ref="F11:F12"/>
+    <mergeCell ref="H18:H20"/>
+    <mergeCell ref="E3:E4"/>
+    <mergeCell ref="G3:G4"/>
+    <mergeCell ref="G5:G6"/>
+    <mergeCell ref="H3:H4"/>
+    <mergeCell ref="H5:H6"/>
+    <mergeCell ref="H7:H8"/>
+    <mergeCell ref="H9:H10"/>
+    <mergeCell ref="H11:H12"/>
+    <mergeCell ref="H13:H14"/>
+    <mergeCell ref="H15:H17"/>
+    <mergeCell ref="G7:G8"/>
     <mergeCell ref="D5:D6"/>
     <mergeCell ref="C7:C8"/>
-    <mergeCell ref="D7:D8"/>
-    <mergeCell ref="B39:J39"/>
-    <mergeCell ref="J13:J14"/>
-    <mergeCell ref="J15:J17"/>
-    <mergeCell ref="J18:J20"/>
-    <mergeCell ref="J21:J23"/>
-    <mergeCell ref="J24:J26"/>
-    <mergeCell ref="J3:J4"/>
-    <mergeCell ref="J5:J6"/>
-    <mergeCell ref="J7:J8"/>
-    <mergeCell ref="J9:J10"/>
-    <mergeCell ref="J11:J12"/>
-    <mergeCell ref="I13:I14"/>
-    <mergeCell ref="I15:I17"/>
-    <mergeCell ref="I18:I20"/>
-    <mergeCell ref="I21:I23"/>
-    <mergeCell ref="I24:I26"/>
-    <mergeCell ref="I3:I4"/>
-    <mergeCell ref="I5:I6"/>
-    <mergeCell ref="I7:I8"/>
-    <mergeCell ref="I9:I10"/>
-    <mergeCell ref="I11:I12"/>
-    <mergeCell ref="C9:C10"/>
-    <mergeCell ref="D11:D12"/>
-    <mergeCell ref="C11:C12"/>
+    <mergeCell ref="B37:J37"/>
+    <mergeCell ref="J27:J32"/>
+    <mergeCell ref="C27:C32"/>
+    <mergeCell ref="B27:B32"/>
+    <mergeCell ref="H27:H32"/>
+    <mergeCell ref="I27:I32"/>
+    <mergeCell ref="H24:H26"/>
+    <mergeCell ref="G27:G32"/>
+    <mergeCell ref="F27:F32"/>
+    <mergeCell ref="E27:E32"/>
+    <mergeCell ref="D27:D32"/>
+    <mergeCell ref="G24:G26"/>
+    <mergeCell ref="B24:B26"/>
+    <mergeCell ref="C24:C26"/>
+    <mergeCell ref="D24:D26"/>
+    <mergeCell ref="E24:E26"/>
+    <mergeCell ref="F24:F26"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape" r:id="rId1"/>

</xml_diff>

<commit_message>
Analyses des performances après derniere correction
</commit_message>
<xml_diff>
--- a/Analyses/Modèle-audit-SEO.xlsx
+++ b/Analyses/Modèle-audit-SEO.xlsx
@@ -806,121 +806,121 @@
     <xf numFmtId="0" fontId="7" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1138,8 +1138,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B1:AB994"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3:J36"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="J36" sqref="J36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.33203125" defaultRowHeight="15" customHeight="1"/>
@@ -1205,490 +1205,490 @@
       <c r="AB2" s="1"/>
     </row>
     <row r="3" spans="2:28" ht="15.75" customHeight="1">
-      <c r="B3" s="37">
+      <c r="B3" s="59">
         <v>1</v>
       </c>
-      <c r="C3" s="39" t="s">
+      <c r="C3" s="49" t="s">
         <v>38</v>
       </c>
-      <c r="D3" s="39" t="s">
+      <c r="D3" s="49" t="s">
         <v>7</v>
       </c>
-      <c r="E3" s="42" t="s">
+      <c r="E3" s="50" t="s">
         <v>14</v>
       </c>
-      <c r="F3" s="42" t="s">
+      <c r="F3" s="50" t="s">
         <v>37</v>
       </c>
-      <c r="G3" s="42" t="s">
+      <c r="G3" s="50" t="s">
         <v>15</v>
       </c>
-      <c r="H3" s="44"/>
-      <c r="I3" s="32">
+      <c r="H3" s="53"/>
+      <c r="I3" s="58">
         <v>1</v>
       </c>
-      <c r="J3" s="28" t="s">
+      <c r="J3" s="57" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="4" spans="2:28" ht="15.75" customHeight="1">
-      <c r="B4" s="27"/>
+      <c r="B4" s="41"/>
       <c r="C4" s="40"/>
       <c r="D4" s="40"/>
-      <c r="E4" s="26"/>
-      <c r="F4" s="26"/>
-      <c r="G4" s="26"/>
-      <c r="H4" s="26"/>
-      <c r="I4" s="31"/>
-      <c r="J4" s="29"/>
+      <c r="E4" s="42"/>
+      <c r="F4" s="42"/>
+      <c r="G4" s="42"/>
+      <c r="H4" s="42"/>
+      <c r="I4" s="43"/>
+      <c r="J4" s="55"/>
     </row>
     <row r="5" spans="2:28" ht="15.75" customHeight="1">
-      <c r="B5" s="38">
+      <c r="B5" s="47">
         <v>2</v>
       </c>
-      <c r="C5" s="35" t="s">
+      <c r="C5" s="48" t="s">
         <v>38</v>
       </c>
-      <c r="D5" s="23" t="s">
+      <c r="D5" s="33" t="s">
         <v>8</v>
       </c>
-      <c r="E5" s="22" t="s">
+      <c r="E5" s="46" t="s">
         <v>14</v>
       </c>
-      <c r="F5" s="43"/>
-      <c r="G5" s="22" t="s">
+      <c r="F5" s="51"/>
+      <c r="G5" s="46" t="s">
         <v>16</v>
       </c>
-      <c r="H5" s="23"/>
-      <c r="I5" s="30">
+      <c r="H5" s="33"/>
+      <c r="I5" s="56">
         <v>2</v>
       </c>
-      <c r="J5" s="29" t="s">
+      <c r="J5" s="55" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="6" spans="2:28" ht="15.75" customHeight="1">
-      <c r="B6" s="38"/>
-      <c r="C6" s="35"/>
-      <c r="D6" s="23"/>
-      <c r="E6" s="23"/>
-      <c r="F6" s="43"/>
-      <c r="G6" s="23"/>
-      <c r="H6" s="23"/>
-      <c r="I6" s="30"/>
-      <c r="J6" s="29"/>
+      <c r="B6" s="47"/>
+      <c r="C6" s="48"/>
+      <c r="D6" s="33"/>
+      <c r="E6" s="33"/>
+      <c r="F6" s="51"/>
+      <c r="G6" s="33"/>
+      <c r="H6" s="33"/>
+      <c r="I6" s="56"/>
+      <c r="J6" s="55"/>
     </row>
     <row r="7" spans="2:28" ht="15.75" customHeight="1">
-      <c r="B7" s="27">
+      <c r="B7" s="41">
         <v>3</v>
       </c>
-      <c r="C7" s="36" t="s">
+      <c r="C7" s="34" t="s">
         <v>6</v>
       </c>
-      <c r="D7" s="24" t="s">
+      <c r="D7" s="45" t="s">
         <v>24</v>
       </c>
-      <c r="E7" s="24" t="s">
+      <c r="E7" s="45" t="s">
         <v>21</v>
       </c>
-      <c r="F7" s="25"/>
-      <c r="G7" s="24" t="s">
+      <c r="F7" s="52"/>
+      <c r="G7" s="45" t="s">
         <v>17</v>
       </c>
-      <c r="H7" s="25"/>
-      <c r="I7" s="31">
+      <c r="H7" s="52"/>
+      <c r="I7" s="43">
         <v>10</v>
       </c>
-      <c r="J7" s="29" t="s">
+      <c r="J7" s="55" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="8" spans="2:28" ht="15.75" customHeight="1">
-      <c r="B8" s="27"/>
-      <c r="C8" s="36"/>
-      <c r="D8" s="25"/>
-      <c r="E8" s="25"/>
-      <c r="F8" s="25"/>
-      <c r="G8" s="25"/>
-      <c r="H8" s="25"/>
-      <c r="I8" s="31"/>
-      <c r="J8" s="29"/>
+      <c r="B8" s="41"/>
+      <c r="C8" s="34"/>
+      <c r="D8" s="52"/>
+      <c r="E8" s="52"/>
+      <c r="F8" s="52"/>
+      <c r="G8" s="52"/>
+      <c r="H8" s="52"/>
+      <c r="I8" s="43"/>
+      <c r="J8" s="55"/>
     </row>
     <row r="9" spans="2:28" ht="15.75" customHeight="1">
-      <c r="B9" s="38">
+      <c r="B9" s="47">
         <v>4</v>
       </c>
-      <c r="C9" s="35" t="s">
+      <c r="C9" s="48" t="s">
         <v>6</v>
       </c>
-      <c r="D9" s="22" t="s">
+      <c r="D9" s="46" t="s">
         <v>25</v>
       </c>
-      <c r="E9" s="22" t="s">
+      <c r="E9" s="46" t="s">
         <v>22</v>
       </c>
-      <c r="F9" s="23"/>
-      <c r="G9" s="22" t="s">
+      <c r="F9" s="33"/>
+      <c r="G9" s="46" t="s">
         <v>18</v>
       </c>
-      <c r="H9" s="23"/>
-      <c r="I9" s="30">
+      <c r="H9" s="33"/>
+      <c r="I9" s="56">
         <v>4</v>
       </c>
-      <c r="J9" s="29" t="s">
+      <c r="J9" s="55" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="10" spans="2:28" ht="15.75" customHeight="1">
-      <c r="B10" s="38"/>
-      <c r="C10" s="35"/>
-      <c r="D10" s="23"/>
-      <c r="E10" s="23"/>
-      <c r="F10" s="23"/>
-      <c r="G10" s="23"/>
-      <c r="H10" s="23"/>
-      <c r="I10" s="30"/>
-      <c r="J10" s="29"/>
+      <c r="B10" s="47"/>
+      <c r="C10" s="48"/>
+      <c r="D10" s="33"/>
+      <c r="E10" s="33"/>
+      <c r="F10" s="33"/>
+      <c r="G10" s="33"/>
+      <c r="H10" s="33"/>
+      <c r="I10" s="56"/>
+      <c r="J10" s="55"/>
     </row>
     <row r="11" spans="2:28" ht="15.75" customHeight="1">
-      <c r="B11" s="27">
+      <c r="B11" s="41">
         <v>5</v>
       </c>
-      <c r="C11" s="36" t="s">
+      <c r="C11" s="34" t="s">
         <v>10</v>
       </c>
-      <c r="D11" s="25" t="s">
+      <c r="D11" s="52" t="s">
         <v>11</v>
       </c>
-      <c r="E11" s="24" t="s">
+      <c r="E11" s="45" t="s">
         <v>35</v>
       </c>
-      <c r="F11" s="25"/>
-      <c r="G11" s="24" t="s">
+      <c r="F11" s="52"/>
+      <c r="G11" s="45" t="s">
         <v>19</v>
       </c>
-      <c r="H11" s="25"/>
-      <c r="I11" s="31">
+      <c r="H11" s="52"/>
+      <c r="I11" s="43">
         <v>5</v>
       </c>
-      <c r="J11" s="29" t="s">
+      <c r="J11" s="55" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="12" spans="2:28" ht="15.75" customHeight="1">
-      <c r="B12" s="27"/>
-      <c r="C12" s="36"/>
-      <c r="D12" s="25"/>
-      <c r="E12" s="25"/>
-      <c r="F12" s="25"/>
-      <c r="G12" s="25"/>
-      <c r="H12" s="25"/>
-      <c r="I12" s="31"/>
-      <c r="J12" s="29"/>
+      <c r="B12" s="41"/>
+      <c r="C12" s="34"/>
+      <c r="D12" s="52"/>
+      <c r="E12" s="52"/>
+      <c r="F12" s="52"/>
+      <c r="G12" s="52"/>
+      <c r="H12" s="52"/>
+      <c r="I12" s="43"/>
+      <c r="J12" s="55"/>
     </row>
     <row r="13" spans="2:28" ht="15.75" customHeight="1">
-      <c r="B13" s="38">
+      <c r="B13" s="47">
         <v>6</v>
       </c>
-      <c r="C13" s="35" t="s">
+      <c r="C13" s="48" t="s">
         <v>6</v>
       </c>
-      <c r="D13" s="23" t="s">
+      <c r="D13" s="33" t="s">
         <v>53</v>
       </c>
-      <c r="E13" s="22" t="s">
+      <c r="E13" s="46" t="s">
         <v>33</v>
       </c>
-      <c r="F13" s="23"/>
-      <c r="G13" s="22" t="s">
+      <c r="F13" s="33"/>
+      <c r="G13" s="46" t="s">
         <v>54</v>
       </c>
-      <c r="H13" s="23"/>
-      <c r="I13" s="30">
+      <c r="H13" s="33"/>
+      <c r="I13" s="56">
         <v>9</v>
       </c>
-      <c r="J13" s="29" t="s">
+      <c r="J13" s="55" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="14" spans="2:28" ht="15.75" customHeight="1">
-      <c r="B14" s="38"/>
-      <c r="C14" s="35"/>
-      <c r="D14" s="23"/>
-      <c r="E14" s="23"/>
-      <c r="F14" s="23"/>
-      <c r="G14" s="23"/>
-      <c r="H14" s="23"/>
-      <c r="I14" s="30"/>
-      <c r="J14" s="29"/>
+      <c r="B14" s="47"/>
+      <c r="C14" s="48"/>
+      <c r="D14" s="33"/>
+      <c r="E14" s="33"/>
+      <c r="F14" s="33"/>
+      <c r="G14" s="33"/>
+      <c r="H14" s="33"/>
+      <c r="I14" s="56"/>
+      <c r="J14" s="55"/>
     </row>
     <row r="15" spans="2:28" ht="15.75" customHeight="1">
-      <c r="B15" s="27">
+      <c r="B15" s="41">
         <v>7</v>
       </c>
-      <c r="C15" s="36" t="s">
+      <c r="C15" s="34" t="s">
         <v>6</v>
       </c>
-      <c r="D15" s="24" t="s">
+      <c r="D15" s="45" t="s">
         <v>26</v>
       </c>
-      <c r="E15" s="24" t="s">
+      <c r="E15" s="45" t="s">
         <v>23</v>
       </c>
-      <c r="F15" s="25"/>
-      <c r="G15" s="24" t="s">
+      <c r="F15" s="52"/>
+      <c r="G15" s="45" t="s">
         <v>20</v>
       </c>
-      <c r="H15" s="25"/>
-      <c r="I15" s="31">
+      <c r="H15" s="52"/>
+      <c r="I15" s="43">
         <v>8</v>
       </c>
-      <c r="J15" s="29" t="s">
+      <c r="J15" s="55" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="16" spans="2:28" ht="15.75" customHeight="1">
-      <c r="B16" s="27"/>
-      <c r="C16" s="36"/>
-      <c r="D16" s="25"/>
-      <c r="E16" s="25"/>
-      <c r="F16" s="25"/>
-      <c r="G16" s="25"/>
-      <c r="H16" s="25"/>
-      <c r="I16" s="31"/>
-      <c r="J16" s="29"/>
+      <c r="B16" s="41"/>
+      <c r="C16" s="34"/>
+      <c r="D16" s="52"/>
+      <c r="E16" s="52"/>
+      <c r="F16" s="52"/>
+      <c r="G16" s="52"/>
+      <c r="H16" s="52"/>
+      <c r="I16" s="43"/>
+      <c r="J16" s="55"/>
     </row>
     <row r="17" spans="2:10" ht="15.75" customHeight="1">
-      <c r="B17" s="27"/>
-      <c r="C17" s="36"/>
-      <c r="D17" s="25"/>
-      <c r="E17" s="25"/>
-      <c r="F17" s="25"/>
-      <c r="G17" s="25"/>
-      <c r="H17" s="25"/>
-      <c r="I17" s="31"/>
-      <c r="J17" s="29"/>
+      <c r="B17" s="41"/>
+      <c r="C17" s="34"/>
+      <c r="D17" s="52"/>
+      <c r="E17" s="52"/>
+      <c r="F17" s="52"/>
+      <c r="G17" s="52"/>
+      <c r="H17" s="52"/>
+      <c r="I17" s="43"/>
+      <c r="J17" s="55"/>
     </row>
     <row r="18" spans="2:10" ht="15.75" customHeight="1">
-      <c r="B18" s="38">
+      <c r="B18" s="47">
         <v>8</v>
       </c>
-      <c r="C18" s="35" t="s">
+      <c r="C18" s="48" t="s">
         <v>9</v>
       </c>
-      <c r="D18" s="22" t="s">
+      <c r="D18" s="46" t="s">
         <v>51</v>
       </c>
-      <c r="E18" s="23" t="s">
+      <c r="E18" s="33" t="s">
         <v>12</v>
       </c>
-      <c r="F18" s="23"/>
-      <c r="G18" s="22" t="s">
+      <c r="F18" s="33"/>
+      <c r="G18" s="46" t="s">
         <v>52</v>
       </c>
-      <c r="H18" s="23"/>
-      <c r="I18" s="30">
+      <c r="H18" s="33"/>
+      <c r="I18" s="56">
         <v>7</v>
       </c>
-      <c r="J18" s="29" t="s">
+      <c r="J18" s="55" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="19" spans="2:10" ht="15.75" customHeight="1">
-      <c r="B19" s="38"/>
-      <c r="C19" s="35"/>
-      <c r="D19" s="23"/>
-      <c r="E19" s="23"/>
-      <c r="F19" s="23"/>
-      <c r="G19" s="23"/>
-      <c r="H19" s="23"/>
-      <c r="I19" s="30"/>
-      <c r="J19" s="29"/>
+      <c r="B19" s="47"/>
+      <c r="C19" s="48"/>
+      <c r="D19" s="33"/>
+      <c r="E19" s="33"/>
+      <c r="F19" s="33"/>
+      <c r="G19" s="33"/>
+      <c r="H19" s="33"/>
+      <c r="I19" s="56"/>
+      <c r="J19" s="55"/>
     </row>
     <row r="20" spans="2:10" ht="15.75" customHeight="1">
-      <c r="B20" s="38"/>
-      <c r="C20" s="35"/>
-      <c r="D20" s="23"/>
-      <c r="E20" s="23"/>
-      <c r="F20" s="23"/>
-      <c r="G20" s="23"/>
-      <c r="H20" s="23"/>
-      <c r="I20" s="30"/>
-      <c r="J20" s="29"/>
+      <c r="B20" s="47"/>
+      <c r="C20" s="48"/>
+      <c r="D20" s="33"/>
+      <c r="E20" s="33"/>
+      <c r="F20" s="33"/>
+      <c r="G20" s="33"/>
+      <c r="H20" s="33"/>
+      <c r="I20" s="56"/>
+      <c r="J20" s="55"/>
     </row>
     <row r="21" spans="2:10" ht="15.75" customHeight="1">
-      <c r="B21" s="27">
+      <c r="B21" s="41">
         <v>9</v>
       </c>
       <c r="C21" s="40" t="s">
         <v>9</v>
       </c>
-      <c r="D21" s="41" t="s">
+      <c r="D21" s="44" t="s">
         <v>36</v>
       </c>
-      <c r="E21" s="41" t="s">
+      <c r="E21" s="44" t="s">
         <v>28</v>
       </c>
-      <c r="F21" s="26"/>
-      <c r="G21" s="26" t="s">
+      <c r="F21" s="42"/>
+      <c r="G21" s="42" t="s">
         <v>27</v>
       </c>
-      <c r="H21" s="26"/>
-      <c r="I21" s="31">
+      <c r="H21" s="42"/>
+      <c r="I21" s="43">
         <v>3</v>
       </c>
-      <c r="J21" s="29" t="s">
+      <c r="J21" s="55" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="22" spans="2:10" ht="15.75" customHeight="1">
-      <c r="B22" s="27"/>
+      <c r="B22" s="41"/>
       <c r="C22" s="40"/>
-      <c r="D22" s="41"/>
-      <c r="E22" s="26"/>
-      <c r="F22" s="26"/>
-      <c r="G22" s="26"/>
-      <c r="H22" s="26"/>
-      <c r="I22" s="31"/>
-      <c r="J22" s="29"/>
+      <c r="D22" s="44"/>
+      <c r="E22" s="42"/>
+      <c r="F22" s="42"/>
+      <c r="G22" s="42"/>
+      <c r="H22" s="42"/>
+      <c r="I22" s="43"/>
+      <c r="J22" s="55"/>
     </row>
     <row r="23" spans="2:10" ht="15.75" customHeight="1">
-      <c r="B23" s="27"/>
+      <c r="B23" s="41"/>
       <c r="C23" s="40"/>
-      <c r="D23" s="41"/>
-      <c r="E23" s="26"/>
-      <c r="F23" s="26"/>
-      <c r="G23" s="26"/>
-      <c r="H23" s="26"/>
-      <c r="I23" s="31"/>
-      <c r="J23" s="29"/>
+      <c r="D23" s="44"/>
+      <c r="E23" s="42"/>
+      <c r="F23" s="42"/>
+      <c r="G23" s="42"/>
+      <c r="H23" s="42"/>
+      <c r="I23" s="43"/>
+      <c r="J23" s="55"/>
     </row>
     <row r="24" spans="2:10" ht="15.75" customHeight="1">
-      <c r="B24" s="38">
+      <c r="B24" s="47">
         <v>10</v>
       </c>
-      <c r="C24" s="35" t="s">
+      <c r="C24" s="48" t="s">
         <v>9</v>
       </c>
-      <c r="D24" s="22" t="s">
+      <c r="D24" s="46" t="s">
         <v>31</v>
       </c>
-      <c r="E24" s="23" t="s">
+      <c r="E24" s="33" t="s">
         <v>29</v>
       </c>
-      <c r="F24" s="23"/>
-      <c r="G24" s="22" t="s">
+      <c r="F24" s="33"/>
+      <c r="G24" s="46" t="s">
         <v>30</v>
       </c>
-      <c r="H24" s="23"/>
-      <c r="I24" s="30" t="s">
+      <c r="H24" s="33"/>
+      <c r="I24" s="56" t="s">
         <v>39</v>
       </c>
-      <c r="J24" s="34" t="s">
+      <c r="J24" s="39" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="25" spans="2:10" ht="15.75" customHeight="1">
-      <c r="B25" s="38"/>
-      <c r="C25" s="35"/>
-      <c r="D25" s="23"/>
-      <c r="E25" s="23"/>
-      <c r="F25" s="23"/>
-      <c r="G25" s="22"/>
-      <c r="H25" s="23"/>
-      <c r="I25" s="30"/>
-      <c r="J25" s="34"/>
+      <c r="B25" s="47"/>
+      <c r="C25" s="48"/>
+      <c r="D25" s="33"/>
+      <c r="E25" s="33"/>
+      <c r="F25" s="33"/>
+      <c r="G25" s="46"/>
+      <c r="H25" s="33"/>
+      <c r="I25" s="56"/>
+      <c r="J25" s="39"/>
     </row>
     <row r="26" spans="2:10" ht="15.75" customHeight="1">
-      <c r="B26" s="38"/>
-      <c r="C26" s="35"/>
-      <c r="D26" s="23"/>
-      <c r="E26" s="23"/>
-      <c r="F26" s="23"/>
-      <c r="G26" s="22"/>
-      <c r="H26" s="23"/>
-      <c r="I26" s="30"/>
-      <c r="J26" s="34"/>
+      <c r="B26" s="47"/>
+      <c r="C26" s="48"/>
+      <c r="D26" s="33"/>
+      <c r="E26" s="33"/>
+      <c r="F26" s="33"/>
+      <c r="G26" s="46"/>
+      <c r="H26" s="33"/>
+      <c r="I26" s="56"/>
+      <c r="J26" s="39"/>
     </row>
     <row r="27" spans="2:10" ht="15.75" customHeight="1">
-      <c r="B27" s="27">
+      <c r="B27" s="41">
         <v>11</v>
       </c>
       <c r="C27" s="40" t="s">
         <v>10</v>
       </c>
-      <c r="D27" s="41" t="s">
+      <c r="D27" s="44" t="s">
         <v>43</v>
       </c>
-      <c r="E27" s="24" t="s">
+      <c r="E27" s="45" t="s">
         <v>44</v>
       </c>
-      <c r="F27" s="26"/>
-      <c r="G27" s="41" t="s">
+      <c r="F27" s="42"/>
+      <c r="G27" s="44" t="s">
         <v>32</v>
       </c>
-      <c r="H27" s="26"/>
-      <c r="I27" s="31" t="s">
+      <c r="H27" s="42"/>
+      <c r="I27" s="43" t="s">
         <v>39</v>
       </c>
-      <c r="J27" s="48" t="s">
+      <c r="J27" s="38" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="28" spans="2:10" ht="15.75" customHeight="1">
-      <c r="B28" s="27"/>
+      <c r="B28" s="41"/>
       <c r="C28" s="40"/>
-      <c r="D28" s="41"/>
-      <c r="E28" s="24"/>
-      <c r="F28" s="26"/>
-      <c r="G28" s="41"/>
-      <c r="H28" s="26"/>
-      <c r="I28" s="31"/>
-      <c r="J28" s="34"/>
+      <c r="D28" s="44"/>
+      <c r="E28" s="45"/>
+      <c r="F28" s="42"/>
+      <c r="G28" s="44"/>
+      <c r="H28" s="42"/>
+      <c r="I28" s="43"/>
+      <c r="J28" s="39"/>
     </row>
     <row r="29" spans="2:10" ht="15.75" customHeight="1">
-      <c r="B29" s="27"/>
+      <c r="B29" s="41"/>
       <c r="C29" s="40"/>
-      <c r="D29" s="41"/>
-      <c r="E29" s="24"/>
-      <c r="F29" s="26"/>
-      <c r="G29" s="41"/>
-      <c r="H29" s="26"/>
-      <c r="I29" s="31"/>
-      <c r="J29" s="34"/>
+      <c r="D29" s="44"/>
+      <c r="E29" s="45"/>
+      <c r="F29" s="42"/>
+      <c r="G29" s="44"/>
+      <c r="H29" s="42"/>
+      <c r="I29" s="43"/>
+      <c r="J29" s="39"/>
     </row>
     <row r="30" spans="2:10" ht="15.75" customHeight="1">
-      <c r="B30" s="27"/>
+      <c r="B30" s="41"/>
       <c r="C30" s="40"/>
-      <c r="D30" s="41"/>
-      <c r="E30" s="24"/>
-      <c r="F30" s="26"/>
-      <c r="G30" s="41"/>
-      <c r="H30" s="26"/>
-      <c r="I30" s="31"/>
-      <c r="J30" s="34"/>
+      <c r="D30" s="44"/>
+      <c r="E30" s="45"/>
+      <c r="F30" s="42"/>
+      <c r="G30" s="44"/>
+      <c r="H30" s="42"/>
+      <c r="I30" s="43"/>
+      <c r="J30" s="39"/>
     </row>
     <row r="31" spans="2:10" ht="15.75" customHeight="1">
-      <c r="B31" s="27"/>
+      <c r="B31" s="41"/>
       <c r="C31" s="40"/>
-      <c r="D31" s="41"/>
-      <c r="E31" s="24"/>
-      <c r="F31" s="26"/>
-      <c r="G31" s="41"/>
-      <c r="H31" s="26"/>
-      <c r="I31" s="31"/>
-      <c r="J31" s="34"/>
+      <c r="D31" s="44"/>
+      <c r="E31" s="45"/>
+      <c r="F31" s="42"/>
+      <c r="G31" s="44"/>
+      <c r="H31" s="42"/>
+      <c r="I31" s="43"/>
+      <c r="J31" s="39"/>
     </row>
     <row r="32" spans="2:10" ht="15.75" customHeight="1">
-      <c r="B32" s="27"/>
+      <c r="B32" s="41"/>
       <c r="C32" s="40"/>
-      <c r="D32" s="41"/>
-      <c r="E32" s="24"/>
-      <c r="F32" s="26"/>
-      <c r="G32" s="41"/>
-      <c r="H32" s="26"/>
-      <c r="I32" s="31"/>
-      <c r="J32" s="34"/>
+      <c r="D32" s="44"/>
+      <c r="E32" s="45"/>
+      <c r="F32" s="42"/>
+      <c r="G32" s="44"/>
+      <c r="H32" s="42"/>
+      <c r="I32" s="43"/>
+      <c r="J32" s="39"/>
     </row>
     <row r="33" spans="2:10" ht="63" customHeight="1">
       <c r="B33" s="12">
@@ -1741,79 +1741,79 @@
       </c>
     </row>
     <row r="35" spans="2:10" ht="63" customHeight="1">
-      <c r="B35" s="49">
+      <c r="B35" s="22">
         <v>14</v>
       </c>
-      <c r="C35" s="50" t="s">
+      <c r="C35" s="23" t="s">
         <v>55</v>
       </c>
-      <c r="D35" s="51" t="s">
+      <c r="D35" s="24" t="s">
         <v>57</v>
       </c>
-      <c r="E35" s="51" t="s">
+      <c r="E35" s="24" t="s">
         <v>56</v>
       </c>
-      <c r="F35" s="52"/>
-      <c r="G35" s="51" t="s">
+      <c r="F35" s="25"/>
+      <c r="G35" s="24" t="s">
         <v>58</v>
       </c>
-      <c r="H35" s="52"/>
-      <c r="I35" s="53">
+      <c r="H35" s="25"/>
+      <c r="I35" s="26">
         <v>12</v>
       </c>
-      <c r="J35" s="54" t="s">
+      <c r="J35" s="27" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="36" spans="2:10" ht="63" customHeight="1" thickBot="1">
-      <c r="B36" s="55">
+      <c r="B36" s="28">
         <v>15</v>
       </c>
-      <c r="C36" s="56" t="s">
+      <c r="C36" s="29" t="s">
         <v>55</v>
       </c>
-      <c r="D36" s="57" t="s">
+      <c r="D36" s="30" t="s">
         <v>60</v>
       </c>
-      <c r="E36" s="57" t="s">
+      <c r="E36" s="30" t="s">
         <v>61</v>
       </c>
-      <c r="F36" s="58"/>
-      <c r="G36" s="57" t="s">
+      <c r="F36" s="31"/>
+      <c r="G36" s="30" t="s">
         <v>62</v>
       </c>
-      <c r="H36" s="58"/>
-      <c r="I36" s="59">
+      <c r="H36" s="31"/>
+      <c r="I36" s="32">
         <v>13</v>
       </c>
       <c r="J36" s="60" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="37" spans="2:10" ht="15.75" customHeight="1" thickBot="1"/>
     <row r="38" spans="2:10" ht="15.75" customHeight="1" thickBot="1">
-      <c r="B38" s="45" t="s">
+      <c r="B38" s="35" t="s">
         <v>50</v>
       </c>
-      <c r="C38" s="46"/>
-      <c r="D38" s="46"/>
-      <c r="E38" s="46"/>
-      <c r="F38" s="46"/>
-      <c r="G38" s="46"/>
-      <c r="H38" s="46"/>
-      <c r="I38" s="46"/>
-      <c r="J38" s="47"/>
+      <c r="C38" s="36"/>
+      <c r="D38" s="36"/>
+      <c r="E38" s="36"/>
+      <c r="F38" s="36"/>
+      <c r="G38" s="36"/>
+      <c r="H38" s="36"/>
+      <c r="I38" s="36"/>
+      <c r="J38" s="37"/>
     </row>
     <row r="39" spans="2:10" ht="15.75" customHeight="1">
-      <c r="B39" s="33"/>
-      <c r="C39" s="33"/>
-      <c r="D39" s="33"/>
-      <c r="E39" s="33"/>
-      <c r="F39" s="33"/>
-      <c r="G39" s="33"/>
-      <c r="H39" s="33"/>
-      <c r="I39" s="33"/>
-      <c r="J39" s="33"/>
+      <c r="B39" s="54"/>
+      <c r="C39" s="54"/>
+      <c r="D39" s="54"/>
+      <c r="E39" s="54"/>
+      <c r="F39" s="54"/>
+      <c r="G39" s="54"/>
+      <c r="H39" s="54"/>
+      <c r="I39" s="54"/>
+      <c r="J39" s="54"/>
     </row>
     <row r="40" spans="2:10" ht="15.75" customHeight="1"/>
     <row r="41" spans="2:10" ht="15.75" customHeight="1"/>
@@ -2773,25 +2773,59 @@
   </sheetData>
   <autoFilter ref="B2:J35"/>
   <mergeCells count="101">
-    <mergeCell ref="D5:D6"/>
-    <mergeCell ref="C7:C8"/>
-    <mergeCell ref="B38:J38"/>
-    <mergeCell ref="J27:J32"/>
-    <mergeCell ref="C27:C32"/>
-    <mergeCell ref="B27:B32"/>
-    <mergeCell ref="H27:H32"/>
-    <mergeCell ref="I27:I32"/>
-    <mergeCell ref="H24:H26"/>
-    <mergeCell ref="G27:G32"/>
-    <mergeCell ref="F27:F32"/>
-    <mergeCell ref="E27:E32"/>
-    <mergeCell ref="D27:D32"/>
-    <mergeCell ref="G24:G26"/>
-    <mergeCell ref="B24:B26"/>
-    <mergeCell ref="C24:C26"/>
-    <mergeCell ref="D24:D26"/>
-    <mergeCell ref="E24:E26"/>
-    <mergeCell ref="F24:F26"/>
+    <mergeCell ref="E5:E6"/>
+    <mergeCell ref="E7:E8"/>
+    <mergeCell ref="E9:E10"/>
+    <mergeCell ref="E11:E12"/>
+    <mergeCell ref="E13:E14"/>
+    <mergeCell ref="F21:F23"/>
+    <mergeCell ref="B21:B23"/>
+    <mergeCell ref="J3:J4"/>
+    <mergeCell ref="J5:J6"/>
+    <mergeCell ref="J7:J8"/>
+    <mergeCell ref="J9:J10"/>
+    <mergeCell ref="J11:J12"/>
+    <mergeCell ref="I13:I14"/>
+    <mergeCell ref="I15:I17"/>
+    <mergeCell ref="I18:I20"/>
+    <mergeCell ref="I21:I23"/>
+    <mergeCell ref="I3:I4"/>
+    <mergeCell ref="I5:I6"/>
+    <mergeCell ref="I7:I8"/>
+    <mergeCell ref="I9:I10"/>
+    <mergeCell ref="I11:I12"/>
+    <mergeCell ref="D7:D8"/>
+    <mergeCell ref="B3:B4"/>
+    <mergeCell ref="B5:B6"/>
+    <mergeCell ref="D9:D10"/>
+    <mergeCell ref="G7:G8"/>
+    <mergeCell ref="B39:J39"/>
+    <mergeCell ref="J13:J14"/>
+    <mergeCell ref="J15:J17"/>
+    <mergeCell ref="J18:J20"/>
+    <mergeCell ref="J21:J23"/>
+    <mergeCell ref="J24:J26"/>
+    <mergeCell ref="I24:I26"/>
+    <mergeCell ref="C9:C10"/>
+    <mergeCell ref="D11:D12"/>
+    <mergeCell ref="C11:C12"/>
+    <mergeCell ref="G9:G10"/>
+    <mergeCell ref="G11:G12"/>
+    <mergeCell ref="G13:G14"/>
+    <mergeCell ref="G15:G17"/>
+    <mergeCell ref="G18:G20"/>
+    <mergeCell ref="E18:E20"/>
+    <mergeCell ref="C18:C20"/>
+    <mergeCell ref="B18:B20"/>
+    <mergeCell ref="F18:F20"/>
+    <mergeCell ref="E15:E17"/>
+    <mergeCell ref="D15:D17"/>
+    <mergeCell ref="D18:D20"/>
+    <mergeCell ref="F13:F14"/>
+    <mergeCell ref="C15:C17"/>
+    <mergeCell ref="F15:F17"/>
+    <mergeCell ref="D13:D14"/>
+    <mergeCell ref="C13:C14"/>
     <mergeCell ref="C3:C4"/>
     <mergeCell ref="D3:D4"/>
     <mergeCell ref="C5:C6"/>
@@ -2816,64 +2850,30 @@
     <mergeCell ref="H11:H12"/>
     <mergeCell ref="H13:H14"/>
     <mergeCell ref="H15:H17"/>
+    <mergeCell ref="D5:D6"/>
+    <mergeCell ref="C7:C8"/>
+    <mergeCell ref="B38:J38"/>
+    <mergeCell ref="J27:J32"/>
+    <mergeCell ref="C27:C32"/>
+    <mergeCell ref="B27:B32"/>
+    <mergeCell ref="H27:H32"/>
+    <mergeCell ref="I27:I32"/>
+    <mergeCell ref="H24:H26"/>
+    <mergeCell ref="G27:G32"/>
+    <mergeCell ref="F27:F32"/>
+    <mergeCell ref="E27:E32"/>
+    <mergeCell ref="D27:D32"/>
+    <mergeCell ref="G24:G26"/>
+    <mergeCell ref="B24:B26"/>
+    <mergeCell ref="C24:C26"/>
+    <mergeCell ref="D24:D26"/>
+    <mergeCell ref="E24:E26"/>
+    <mergeCell ref="F24:F26"/>
     <mergeCell ref="B7:B8"/>
     <mergeCell ref="B9:B10"/>
     <mergeCell ref="B11:B12"/>
     <mergeCell ref="B13:B14"/>
     <mergeCell ref="B15:B17"/>
-    <mergeCell ref="G18:G20"/>
-    <mergeCell ref="E18:E20"/>
-    <mergeCell ref="C18:C20"/>
-    <mergeCell ref="B18:B20"/>
-    <mergeCell ref="F18:F20"/>
-    <mergeCell ref="E15:E17"/>
-    <mergeCell ref="D15:D17"/>
-    <mergeCell ref="D18:D20"/>
-    <mergeCell ref="F13:F14"/>
-    <mergeCell ref="C15:C17"/>
-    <mergeCell ref="F15:F17"/>
-    <mergeCell ref="D13:D14"/>
-    <mergeCell ref="C13:C14"/>
-    <mergeCell ref="D9:D10"/>
-    <mergeCell ref="G7:G8"/>
-    <mergeCell ref="B39:J39"/>
-    <mergeCell ref="J13:J14"/>
-    <mergeCell ref="J15:J17"/>
-    <mergeCell ref="J18:J20"/>
-    <mergeCell ref="J21:J23"/>
-    <mergeCell ref="J24:J26"/>
-    <mergeCell ref="I24:I26"/>
-    <mergeCell ref="C9:C10"/>
-    <mergeCell ref="D11:D12"/>
-    <mergeCell ref="C11:C12"/>
-    <mergeCell ref="G9:G10"/>
-    <mergeCell ref="G11:G12"/>
-    <mergeCell ref="G13:G14"/>
-    <mergeCell ref="G15:G17"/>
-    <mergeCell ref="E5:E6"/>
-    <mergeCell ref="E7:E8"/>
-    <mergeCell ref="E9:E10"/>
-    <mergeCell ref="E11:E12"/>
-    <mergeCell ref="E13:E14"/>
-    <mergeCell ref="F21:F23"/>
-    <mergeCell ref="B21:B23"/>
-    <mergeCell ref="J3:J4"/>
-    <mergeCell ref="J5:J6"/>
-    <mergeCell ref="J7:J8"/>
-    <mergeCell ref="J9:J10"/>
-    <mergeCell ref="J11:J12"/>
-    <mergeCell ref="I13:I14"/>
-    <mergeCell ref="I15:I17"/>
-    <mergeCell ref="I18:I20"/>
-    <mergeCell ref="I21:I23"/>
-    <mergeCell ref="I3:I4"/>
-    <mergeCell ref="I5:I6"/>
-    <mergeCell ref="I7:I8"/>
-    <mergeCell ref="I9:I10"/>
-    <mergeCell ref="I11:I12"/>
-    <mergeCell ref="D7:D8"/>
-    <mergeCell ref="B3:B4"/>
-    <mergeCell ref="B5:B6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape" r:id="rId1"/>

</xml_diff>

<commit_message>
Correction du fichier d'audit
</commit_message>
<xml_diff>
--- a/Analyses/Modèle-audit-SEO.xlsx
+++ b/Analyses/Modèle-audit-SEO.xlsx
@@ -10,7 +10,7 @@
     <sheet name="SEO" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">SEO!$B$2:$J$35</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">SEO!$B$2:$J$37</definedName>
   </definedNames>
   <calcPr calcId="125725"/>
   <extLst>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="82">
   <si>
     <t>Catégorie</t>
   </si>
@@ -170,31 +170,6 @@
     <t>Présenter la même barre de 
 navigation sur les 2 pages avec un lien "Accueil" et un lien "Contact".
 Mettre le lien de la page différencié</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve"> Empile des mots clés. </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>BACK
- HAT</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>.</t>
-    </r>
   </si>
   <si>
     <t>Ordre</t>
@@ -342,12 +317,108 @@
   <si>
     <t>Corriger le nom des balises qui ne doivent pas être toutes en &lt;div&gt;</t>
   </si>
+  <si>
+    <t xml:space="preserve"> https://developer.mozilla.org/fr/docs/Web/Accessibility/Mobile_accessibility_checklist</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Mettre les images à une taille
+ voisine de celle présentée sur le
+ site.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Mettre une description de
+ présentation du site.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Mettre un titre correct à chaque
+ page.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Replacer les images de texte par
+du texte.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Les mots clé doivent être distibués
+ dans le site etn regroupés dans
+ une div.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Limiter le nombre de liens en
+ privilégiant leur qualité.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Les couleur de texte et de fond
+ doivent avoir un contraste assez
+ fort pour pouvoir les différencier.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Permet d'avoir un équivalent textuel
+ utile aux personnes malvoyantes.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Manque de visibilité du formulaire</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Cohérence entre les pages</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Suite logique des titres </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Visibilité du texte</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Sémantique des balises</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> https://developer.mozilla.org/fr/docs/Web/Accessibility/Mobile_accessibility_checklist
+ https://developer.mozilla.org/fr/docs/Web/HTML/Element/img</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> https://c-marketing.eu/optimiser-vos-images-pour-le-web/</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> https://www.ionos.fr/digitalguide/sites-internet/developpement-web/les-principales-balises-meta-et-leurs-fonctions/</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> https://developer.mozilla.org/fr/docs/Web/HTML/Element/title
+ https://www.ionos.fr/digitalguide/sites-internet/developpement-web/les-principales-balises-meta-et-leurs-fonctions/</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve"> Empile des mots clés. </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>BLACK
+ HAT</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>.</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve"> https://oursonweb.fr/quest-ce-que-le-black-hat-seo/
+ https://www.redacteur.com/blog/seo-techniques-black-hat/</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="10">
+  <fonts count="9">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -358,13 +429,6 @@
       <sz val="11"/>
       <color rgb="FFFFFFFF"/>
       <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
       <family val="2"/>
     </font>
     <font>
@@ -463,7 +527,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="20">
+  <borders count="26">
     <border>
       <left/>
       <right/>
@@ -736,191 +800,320 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="61">
+  <cellXfs count="80">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="18" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="23" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="22" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1136,687 +1329,756 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B1:AB994"/>
+  <dimension ref="B1:AB996"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="J36" sqref="J36"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="H14" sqref="H14:H16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.33203125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="2.77734375" style="2" customWidth="1"/>
-    <col min="2" max="2" width="5.77734375" style="4" customWidth="1"/>
-    <col min="3" max="3" width="24.77734375" style="3" customWidth="1"/>
-    <col min="4" max="4" width="27" style="2" customWidth="1"/>
-    <col min="5" max="8" width="24.77734375" style="2" customWidth="1"/>
-    <col min="9" max="9" width="7.77734375" style="4" customWidth="1"/>
-    <col min="10" max="10" width="10.5546875" style="3" customWidth="1"/>
-    <col min="11" max="12" width="10.5546875" style="4" customWidth="1"/>
-    <col min="13" max="28" width="10.5546875" style="2" customWidth="1"/>
-    <col min="29" max="16384" width="11.33203125" style="2"/>
+    <col min="1" max="1" width="2.77734375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="5.77734375" style="3" customWidth="1"/>
+    <col min="3" max="3" width="24.77734375" style="2" customWidth="1"/>
+    <col min="4" max="4" width="27" style="1" customWidth="1"/>
+    <col min="5" max="5" width="24.77734375" style="1" customWidth="1"/>
+    <col min="6" max="6" width="26.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="24.77734375" style="1" customWidth="1"/>
+    <col min="8" max="8" width="63.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="7.77734375" style="3" customWidth="1"/>
+    <col min="10" max="10" width="10.5546875" style="2" customWidth="1"/>
+    <col min="11" max="12" width="10.5546875" style="3" customWidth="1"/>
+    <col min="13" max="28" width="10.5546875" style="1" customWidth="1"/>
+    <col min="29" max="16384" width="11.33203125" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:28" ht="15" customHeight="1" thickBot="1"/>
     <row r="2" spans="2:28" ht="15.75" customHeight="1" thickBot="1">
-      <c r="B2" s="8" t="s">
+      <c r="B2" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="C2" s="9" t="s">
+      <c r="C2" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="9" t="s">
+      <c r="D2" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="E2" s="9" t="s">
+      <c r="E2" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="F2" s="9" t="s">
+      <c r="F2" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="G2" s="9" t="s">
+      <c r="G2" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="H2" s="9" t="s">
+      <c r="H2" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="I2" s="10" t="s">
+      <c r="I2" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="J2" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="M2" s="32"/>
+      <c r="N2" s="32"/>
+      <c r="O2" s="32"/>
+      <c r="P2" s="32"/>
+      <c r="Q2" s="32"/>
+      <c r="R2" s="32"/>
+      <c r="S2" s="32"/>
+      <c r="T2" s="32"/>
+      <c r="U2" s="32"/>
+      <c r="V2" s="32"/>
+      <c r="W2" s="32"/>
+      <c r="X2" s="32"/>
+      <c r="Y2" s="32"/>
+      <c r="Z2" s="32"/>
+      <c r="AA2" s="32"/>
+      <c r="AB2" s="32"/>
+    </row>
+    <row r="3" spans="2:28" ht="15.75" customHeight="1">
+      <c r="B3" s="43">
+        <v>1</v>
+      </c>
+      <c r="C3" s="44" t="s">
+        <v>37</v>
+      </c>
+      <c r="D3" s="44" t="s">
+        <v>7</v>
+      </c>
+      <c r="E3" s="56" t="s">
+        <v>14</v>
+      </c>
+      <c r="F3" s="56" t="s">
+        <v>36</v>
+      </c>
+      <c r="G3" s="56" t="s">
+        <v>15</v>
+      </c>
+      <c r="H3" s="57" t="s">
+        <v>77</v>
+      </c>
+      <c r="I3" s="40">
+        <v>1</v>
+      </c>
+      <c r="J3" s="36" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="4" spans="2:28" ht="15.75" customHeight="1">
+      <c r="B4" s="35"/>
+      <c r="C4" s="45"/>
+      <c r="D4" s="45"/>
+      <c r="E4" s="34"/>
+      <c r="F4" s="34"/>
+      <c r="G4" s="34"/>
+      <c r="H4" s="34"/>
+      <c r="I4" s="39"/>
+      <c r="J4" s="37"/>
+    </row>
+    <row r="5" spans="2:28" ht="15.75" customHeight="1">
+      <c r="B5" s="68">
+        <v>2</v>
+      </c>
+      <c r="C5" s="71" t="s">
+        <v>37</v>
+      </c>
+      <c r="D5" s="61" t="s">
+        <v>8</v>
+      </c>
+      <c r="E5" s="47" t="s">
+        <v>14</v>
+      </c>
+      <c r="F5" s="58" t="s">
+        <v>63</v>
+      </c>
+      <c r="G5" s="47" t="s">
+        <v>16</v>
+      </c>
+      <c r="H5" s="61" t="s">
+        <v>77</v>
+      </c>
+      <c r="I5" s="74">
+        <v>2</v>
+      </c>
+      <c r="J5" s="77" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="6" spans="2:28" ht="15.75" customHeight="1">
+      <c r="B6" s="69"/>
+      <c r="C6" s="72"/>
+      <c r="D6" s="62"/>
+      <c r="E6" s="48"/>
+      <c r="F6" s="59"/>
+      <c r="G6" s="48"/>
+      <c r="H6" s="62"/>
+      <c r="I6" s="76"/>
+      <c r="J6" s="79"/>
+    </row>
+    <row r="7" spans="2:28" ht="15.75" customHeight="1">
+      <c r="B7" s="70"/>
+      <c r="C7" s="73"/>
+      <c r="D7" s="63"/>
+      <c r="E7" s="49"/>
+      <c r="F7" s="60"/>
+      <c r="G7" s="49"/>
+      <c r="H7" s="63"/>
+      <c r="I7" s="75"/>
+      <c r="J7" s="78"/>
+    </row>
+    <row r="8" spans="2:28" ht="15.75" customHeight="1">
+      <c r="B8" s="35">
+        <v>3</v>
+      </c>
+      <c r="C8" s="46" t="s">
+        <v>6</v>
+      </c>
+      <c r="D8" s="41" t="s">
+        <v>24</v>
+      </c>
+      <c r="E8" s="41" t="s">
+        <v>21</v>
+      </c>
+      <c r="F8" s="41" t="s">
+        <v>64</v>
+      </c>
+      <c r="G8" s="41" t="s">
+        <v>17</v>
+      </c>
+      <c r="H8" s="42" t="s">
+        <v>78</v>
+      </c>
+      <c r="I8" s="39">
+        <v>10</v>
+      </c>
+      <c r="J8" s="37" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="9" spans="2:28" ht="15.75" customHeight="1">
+      <c r="B9" s="35"/>
+      <c r="C9" s="46"/>
+      <c r="D9" s="42"/>
+      <c r="E9" s="42"/>
+      <c r="F9" s="42"/>
+      <c r="G9" s="42"/>
+      <c r="H9" s="42"/>
+      <c r="I9" s="39"/>
+      <c r="J9" s="37"/>
+    </row>
+    <row r="10" spans="2:28" ht="15.75" customHeight="1">
+      <c r="B10" s="55">
+        <v>4</v>
+      </c>
+      <c r="C10" s="54" t="s">
+        <v>6</v>
+      </c>
+      <c r="D10" s="50" t="s">
+        <v>25</v>
+      </c>
+      <c r="E10" s="50" t="s">
+        <v>22</v>
+      </c>
+      <c r="F10" s="50" t="s">
+        <v>65</v>
+      </c>
+      <c r="G10" s="50" t="s">
+        <v>18</v>
+      </c>
+      <c r="H10" s="50" t="s">
+        <v>79</v>
+      </c>
+      <c r="I10" s="38">
+        <v>4</v>
+      </c>
+      <c r="J10" s="37" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="11" spans="2:28" ht="15.75" customHeight="1">
+      <c r="B11" s="55"/>
+      <c r="C11" s="54"/>
+      <c r="D11" s="51"/>
+      <c r="E11" s="51"/>
+      <c r="F11" s="51"/>
+      <c r="G11" s="51"/>
+      <c r="H11" s="51"/>
+      <c r="I11" s="38"/>
+      <c r="J11" s="37"/>
+    </row>
+    <row r="12" spans="2:28" ht="15.75" customHeight="1">
+      <c r="B12" s="35">
+        <v>5</v>
+      </c>
+      <c r="C12" s="46" t="s">
+        <v>10</v>
+      </c>
+      <c r="D12" s="42" t="s">
+        <v>11</v>
+      </c>
+      <c r="E12" s="41" t="s">
         <v>34</v>
       </c>
-      <c r="J2" s="11" t="s">
+      <c r="F12" s="41" t="s">
+        <v>66</v>
+      </c>
+      <c r="G12" s="41" t="s">
+        <v>19</v>
+      </c>
+      <c r="H12" s="42" t="s">
+        <v>62</v>
+      </c>
+      <c r="I12" s="39">
+        <v>5</v>
+      </c>
+      <c r="J12" s="37" t="s">
         <v>40</v>
       </c>
-      <c r="K2" s="5"/>
-      <c r="L2" s="5"/>
-      <c r="M2" s="1"/>
-      <c r="N2" s="1"/>
-      <c r="O2" s="1"/>
-      <c r="P2" s="1"/>
-      <c r="Q2" s="1"/>
-      <c r="R2" s="1"/>
-      <c r="S2" s="1"/>
-      <c r="T2" s="1"/>
-      <c r="U2" s="1"/>
-      <c r="V2" s="1"/>
-      <c r="W2" s="1"/>
-      <c r="X2" s="1"/>
-      <c r="Y2" s="1"/>
-      <c r="Z2" s="1"/>
-      <c r="AA2" s="1"/>
-      <c r="AB2" s="1"/>
-    </row>
-    <row r="3" spans="2:28" ht="15.75" customHeight="1">
-      <c r="B3" s="59">
-        <v>1</v>
-      </c>
-      <c r="C3" s="49" t="s">
+    </row>
+    <row r="13" spans="2:28" ht="15.75" customHeight="1">
+      <c r="B13" s="35"/>
+      <c r="C13" s="46"/>
+      <c r="D13" s="42"/>
+      <c r="E13" s="42"/>
+      <c r="F13" s="42"/>
+      <c r="G13" s="42"/>
+      <c r="H13" s="42"/>
+      <c r="I13" s="39"/>
+      <c r="J13" s="37"/>
+    </row>
+    <row r="14" spans="2:28" ht="15.75" customHeight="1">
+      <c r="B14" s="68">
+        <v>6</v>
+      </c>
+      <c r="C14" s="71" t="s">
+        <v>6</v>
+      </c>
+      <c r="D14" s="61" t="s">
+        <v>52</v>
+      </c>
+      <c r="E14" s="47" t="s">
+        <v>80</v>
+      </c>
+      <c r="F14" s="47" t="s">
+        <v>67</v>
+      </c>
+      <c r="G14" s="47" t="s">
+        <v>53</v>
+      </c>
+      <c r="H14" s="47" t="s">
+        <v>81</v>
+      </c>
+      <c r="I14" s="74">
+        <v>9</v>
+      </c>
+      <c r="J14" s="77" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="15" spans="2:28" ht="15.75" customHeight="1">
+      <c r="B15" s="69"/>
+      <c r="C15" s="72"/>
+      <c r="D15" s="62"/>
+      <c r="E15" s="48"/>
+      <c r="F15" s="48"/>
+      <c r="G15" s="48"/>
+      <c r="H15" s="62"/>
+      <c r="I15" s="76"/>
+      <c r="J15" s="79"/>
+    </row>
+    <row r="16" spans="2:28" ht="15.75" customHeight="1">
+      <c r="B16" s="70"/>
+      <c r="C16" s="73"/>
+      <c r="D16" s="63"/>
+      <c r="E16" s="49"/>
+      <c r="F16" s="49"/>
+      <c r="G16" s="49"/>
+      <c r="H16" s="63"/>
+      <c r="I16" s="75"/>
+      <c r="J16" s="78"/>
+    </row>
+    <row r="17" spans="2:10" ht="15.75" customHeight="1">
+      <c r="B17" s="35">
+        <v>7</v>
+      </c>
+      <c r="C17" s="46" t="s">
+        <v>6</v>
+      </c>
+      <c r="D17" s="41" t="s">
+        <v>26</v>
+      </c>
+      <c r="E17" s="41" t="s">
+        <v>23</v>
+      </c>
+      <c r="F17" s="41" t="s">
+        <v>68</v>
+      </c>
+      <c r="G17" s="41" t="s">
+        <v>20</v>
+      </c>
+      <c r="H17" s="42"/>
+      <c r="I17" s="39">
+        <v>8</v>
+      </c>
+      <c r="J17" s="37" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="18" spans="2:10" ht="15.75" customHeight="1">
+      <c r="B18" s="35"/>
+      <c r="C18" s="46"/>
+      <c r="D18" s="42"/>
+      <c r="E18" s="42"/>
+      <c r="F18" s="42"/>
+      <c r="G18" s="42"/>
+      <c r="H18" s="42"/>
+      <c r="I18" s="39"/>
+      <c r="J18" s="37"/>
+    </row>
+    <row r="19" spans="2:10" ht="15.75" customHeight="1">
+      <c r="B19" s="35"/>
+      <c r="C19" s="46"/>
+      <c r="D19" s="42"/>
+      <c r="E19" s="42"/>
+      <c r="F19" s="42"/>
+      <c r="G19" s="42"/>
+      <c r="H19" s="42"/>
+      <c r="I19" s="39"/>
+      <c r="J19" s="37"/>
+    </row>
+    <row r="20" spans="2:10" ht="15.75" customHeight="1">
+      <c r="B20" s="55">
+        <v>8</v>
+      </c>
+      <c r="C20" s="54" t="s">
+        <v>9</v>
+      </c>
+      <c r="D20" s="50" t="s">
+        <v>50</v>
+      </c>
+      <c r="E20" s="51" t="s">
+        <v>12</v>
+      </c>
+      <c r="F20" s="50" t="s">
+        <v>69</v>
+      </c>
+      <c r="G20" s="50" t="s">
+        <v>51</v>
+      </c>
+      <c r="H20" s="51" t="s">
+        <v>62</v>
+      </c>
+      <c r="I20" s="38">
+        <v>7</v>
+      </c>
+      <c r="J20" s="37" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="21" spans="2:10" ht="15.75" customHeight="1">
+      <c r="B21" s="55"/>
+      <c r="C21" s="54"/>
+      <c r="D21" s="51"/>
+      <c r="E21" s="51"/>
+      <c r="F21" s="51"/>
+      <c r="G21" s="51"/>
+      <c r="H21" s="51"/>
+      <c r="I21" s="38"/>
+      <c r="J21" s="37"/>
+    </row>
+    <row r="22" spans="2:10" ht="15.75" customHeight="1">
+      <c r="B22" s="55"/>
+      <c r="C22" s="54"/>
+      <c r="D22" s="51"/>
+      <c r="E22" s="51"/>
+      <c r="F22" s="51"/>
+      <c r="G22" s="51"/>
+      <c r="H22" s="51"/>
+      <c r="I22" s="38"/>
+      <c r="J22" s="37"/>
+    </row>
+    <row r="23" spans="2:10" ht="15.75" customHeight="1">
+      <c r="B23" s="35">
+        <v>9</v>
+      </c>
+      <c r="C23" s="45" t="s">
+        <v>9</v>
+      </c>
+      <c r="D23" s="33" t="s">
+        <v>35</v>
+      </c>
+      <c r="E23" s="33" t="s">
+        <v>28</v>
+      </c>
+      <c r="F23" s="33" t="s">
+        <v>70</v>
+      </c>
+      <c r="G23" s="34" t="s">
+        <v>27</v>
+      </c>
+      <c r="H23" s="33" t="s">
+        <v>76</v>
+      </c>
+      <c r="I23" s="39">
+        <v>3</v>
+      </c>
+      <c r="J23" s="37" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="24" spans="2:10" ht="15.75" customHeight="1">
+      <c r="B24" s="35"/>
+      <c r="C24" s="45"/>
+      <c r="D24" s="33"/>
+      <c r="E24" s="34"/>
+      <c r="F24" s="34"/>
+      <c r="G24" s="34"/>
+      <c r="H24" s="34"/>
+      <c r="I24" s="39"/>
+      <c r="J24" s="37"/>
+    </row>
+    <row r="25" spans="2:10" ht="15.75" customHeight="1">
+      <c r="B25" s="35"/>
+      <c r="C25" s="45"/>
+      <c r="D25" s="33"/>
+      <c r="E25" s="34"/>
+      <c r="F25" s="34"/>
+      <c r="G25" s="34"/>
+      <c r="H25" s="34"/>
+      <c r="I25" s="39"/>
+      <c r="J25" s="37"/>
+    </row>
+    <row r="26" spans="2:10" ht="15.75" customHeight="1">
+      <c r="B26" s="55">
+        <v>10</v>
+      </c>
+      <c r="C26" s="54" t="s">
+        <v>9</v>
+      </c>
+      <c r="D26" s="50" t="s">
+        <v>31</v>
+      </c>
+      <c r="E26" s="51" t="s">
+        <v>29</v>
+      </c>
+      <c r="F26" s="51" t="s">
+        <v>71</v>
+      </c>
+      <c r="G26" s="50" t="s">
+        <v>30</v>
+      </c>
+      <c r="H26" s="51"/>
+      <c r="I26" s="38" t="s">
         <v>38</v>
       </c>
-      <c r="D3" s="49" t="s">
-        <v>7</v>
-      </c>
-      <c r="E3" s="50" t="s">
+      <c r="J26" s="53" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="27" spans="2:10" ht="15.75" customHeight="1">
+      <c r="B27" s="55"/>
+      <c r="C27" s="54"/>
+      <c r="D27" s="51"/>
+      <c r="E27" s="51"/>
+      <c r="F27" s="51"/>
+      <c r="G27" s="50"/>
+      <c r="H27" s="51"/>
+      <c r="I27" s="38"/>
+      <c r="J27" s="53"/>
+    </row>
+    <row r="28" spans="2:10" ht="15.75" customHeight="1">
+      <c r="B28" s="55"/>
+      <c r="C28" s="54"/>
+      <c r="D28" s="51"/>
+      <c r="E28" s="51"/>
+      <c r="F28" s="51"/>
+      <c r="G28" s="50"/>
+      <c r="H28" s="51"/>
+      <c r="I28" s="38"/>
+      <c r="J28" s="53"/>
+    </row>
+    <row r="29" spans="2:10" ht="15.75" customHeight="1">
+      <c r="B29" s="35">
+        <v>11</v>
+      </c>
+      <c r="C29" s="45" t="s">
+        <v>10</v>
+      </c>
+      <c r="D29" s="33" t="s">
+        <v>42</v>
+      </c>
+      <c r="E29" s="41" t="s">
+        <v>43</v>
+      </c>
+      <c r="F29" s="34" t="s">
+        <v>72</v>
+      </c>
+      <c r="G29" s="33" t="s">
+        <v>32</v>
+      </c>
+      <c r="H29" s="34"/>
+      <c r="I29" s="39" t="s">
+        <v>38</v>
+      </c>
+      <c r="J29" s="67" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="30" spans="2:10" ht="15.75" customHeight="1">
+      <c r="B30" s="35"/>
+      <c r="C30" s="45"/>
+      <c r="D30" s="33"/>
+      <c r="E30" s="41"/>
+      <c r="F30" s="34"/>
+      <c r="G30" s="33"/>
+      <c r="H30" s="34"/>
+      <c r="I30" s="39"/>
+      <c r="J30" s="53"/>
+    </row>
+    <row r="31" spans="2:10" ht="15.75" customHeight="1">
+      <c r="B31" s="35"/>
+      <c r="C31" s="45"/>
+      <c r="D31" s="33"/>
+      <c r="E31" s="41"/>
+      <c r="F31" s="34"/>
+      <c r="G31" s="33"/>
+      <c r="H31" s="34"/>
+      <c r="I31" s="39"/>
+      <c r="J31" s="53"/>
+    </row>
+    <row r="32" spans="2:10" ht="15.75" customHeight="1">
+      <c r="B32" s="35"/>
+      <c r="C32" s="45"/>
+      <c r="D32" s="33"/>
+      <c r="E32" s="41"/>
+      <c r="F32" s="34"/>
+      <c r="G32" s="33"/>
+      <c r="H32" s="34"/>
+      <c r="I32" s="39"/>
+      <c r="J32" s="53"/>
+    </row>
+    <row r="33" spans="2:10" ht="15.75" customHeight="1">
+      <c r="B33" s="35"/>
+      <c r="C33" s="45"/>
+      <c r="D33" s="33"/>
+      <c r="E33" s="41"/>
+      <c r="F33" s="34"/>
+      <c r="G33" s="33"/>
+      <c r="H33" s="34"/>
+      <c r="I33" s="39"/>
+      <c r="J33" s="53"/>
+    </row>
+    <row r="34" spans="2:10" ht="15.75" customHeight="1">
+      <c r="B34" s="35"/>
+      <c r="C34" s="45"/>
+      <c r="D34" s="33"/>
+      <c r="E34" s="41"/>
+      <c r="F34" s="34"/>
+      <c r="G34" s="33"/>
+      <c r="H34" s="34"/>
+      <c r="I34" s="39"/>
+      <c r="J34" s="53"/>
+    </row>
+    <row r="35" spans="2:10" ht="63" customHeight="1">
+      <c r="B35" s="10">
+        <v>12</v>
+      </c>
+      <c r="C35" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="D35" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="E35" s="14" t="s">
+        <v>58</v>
+      </c>
+      <c r="F35" s="13" t="s">
+        <v>73</v>
+      </c>
+      <c r="G35" s="14" t="s">
+        <v>45</v>
+      </c>
+      <c r="H35" s="13" t="s">
+        <v>62</v>
+      </c>
+      <c r="I35" s="30">
+        <v>11</v>
+      </c>
+      <c r="J35" s="29" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="36" spans="2:10" ht="63" customHeight="1">
+      <c r="B36" s="27">
+        <v>13</v>
+      </c>
+      <c r="C36" s="26" t="s">
+        <v>37</v>
+      </c>
+      <c r="D36" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="E36" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="F36" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="G36" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="H36" s="5"/>
+      <c r="I36" s="28">
+        <v>6</v>
+      </c>
+      <c r="J36" s="29" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="37" spans="2:10" ht="63" customHeight="1">
+      <c r="B37" s="15">
         <v>14</v>
       </c>
-      <c r="F3" s="50" t="s">
-        <v>37</v>
-      </c>
-      <c r="G3" s="50" t="s">
+      <c r="C37" s="16" t="s">
+        <v>54</v>
+      </c>
+      <c r="D37" s="17" t="s">
+        <v>56</v>
+      </c>
+      <c r="E37" s="17" t="s">
+        <v>55</v>
+      </c>
+      <c r="F37" s="18" t="s">
+        <v>74</v>
+      </c>
+      <c r="G37" s="17" t="s">
+        <v>57</v>
+      </c>
+      <c r="H37" s="18" t="s">
+        <v>62</v>
+      </c>
+      <c r="I37" s="19">
+        <v>12</v>
+      </c>
+      <c r="J37" s="20" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="38" spans="2:10" ht="63" customHeight="1" thickBot="1">
+      <c r="B38" s="21">
         <v>15</v>
       </c>
-      <c r="H3" s="53"/>
-      <c r="I3" s="58">
-        <v>1</v>
-      </c>
-      <c r="J3" s="57" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="4" spans="2:28" ht="15.75" customHeight="1">
-      <c r="B4" s="41"/>
-      <c r="C4" s="40"/>
-      <c r="D4" s="40"/>
-      <c r="E4" s="42"/>
-      <c r="F4" s="42"/>
-      <c r="G4" s="42"/>
-      <c r="H4" s="42"/>
-      <c r="I4" s="43"/>
-      <c r="J4" s="55"/>
-    </row>
-    <row r="5" spans="2:28" ht="15.75" customHeight="1">
-      <c r="B5" s="47">
-        <v>2</v>
-      </c>
-      <c r="C5" s="48" t="s">
-        <v>38</v>
-      </c>
-      <c r="D5" s="33" t="s">
-        <v>8</v>
-      </c>
-      <c r="E5" s="46" t="s">
-        <v>14</v>
-      </c>
-      <c r="F5" s="51"/>
-      <c r="G5" s="46" t="s">
-        <v>16</v>
-      </c>
-      <c r="H5" s="33"/>
-      <c r="I5" s="56">
-        <v>2</v>
-      </c>
-      <c r="J5" s="55" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="6" spans="2:28" ht="15.75" customHeight="1">
-      <c r="B6" s="47"/>
-      <c r="C6" s="48"/>
-      <c r="D6" s="33"/>
-      <c r="E6" s="33"/>
-      <c r="F6" s="51"/>
-      <c r="G6" s="33"/>
-      <c r="H6" s="33"/>
-      <c r="I6" s="56"/>
-      <c r="J6" s="55"/>
-    </row>
-    <row r="7" spans="2:28" ht="15.75" customHeight="1">
-      <c r="B7" s="41">
-        <v>3</v>
-      </c>
-      <c r="C7" s="34" t="s">
-        <v>6</v>
-      </c>
-      <c r="D7" s="45" t="s">
-        <v>24</v>
-      </c>
-      <c r="E7" s="45" t="s">
-        <v>21</v>
-      </c>
-      <c r="F7" s="52"/>
-      <c r="G7" s="45" t="s">
-        <v>17</v>
-      </c>
-      <c r="H7" s="52"/>
-      <c r="I7" s="43">
-        <v>10</v>
-      </c>
-      <c r="J7" s="55" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="8" spans="2:28" ht="15.75" customHeight="1">
-      <c r="B8" s="41"/>
-      <c r="C8" s="34"/>
-      <c r="D8" s="52"/>
-      <c r="E8" s="52"/>
-      <c r="F8" s="52"/>
-      <c r="G8" s="52"/>
-      <c r="H8" s="52"/>
-      <c r="I8" s="43"/>
-      <c r="J8" s="55"/>
-    </row>
-    <row r="9" spans="2:28" ht="15.75" customHeight="1">
-      <c r="B9" s="47">
-        <v>4</v>
-      </c>
-      <c r="C9" s="48" t="s">
-        <v>6</v>
-      </c>
-      <c r="D9" s="46" t="s">
-        <v>25</v>
-      </c>
-      <c r="E9" s="46" t="s">
-        <v>22</v>
-      </c>
-      <c r="F9" s="33"/>
-      <c r="G9" s="46" t="s">
-        <v>18</v>
-      </c>
-      <c r="H9" s="33"/>
-      <c r="I9" s="56">
-        <v>4</v>
-      </c>
-      <c r="J9" s="55" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="10" spans="2:28" ht="15.75" customHeight="1">
-      <c r="B10" s="47"/>
-      <c r="C10" s="48"/>
-      <c r="D10" s="33"/>
-      <c r="E10" s="33"/>
-      <c r="F10" s="33"/>
-      <c r="G10" s="33"/>
-      <c r="H10" s="33"/>
-      <c r="I10" s="56"/>
-      <c r="J10" s="55"/>
-    </row>
-    <row r="11" spans="2:28" ht="15.75" customHeight="1">
-      <c r="B11" s="41">
-        <v>5</v>
-      </c>
-      <c r="C11" s="34" t="s">
-        <v>10</v>
-      </c>
-      <c r="D11" s="52" t="s">
-        <v>11</v>
-      </c>
-      <c r="E11" s="45" t="s">
-        <v>35</v>
-      </c>
-      <c r="F11" s="52"/>
-      <c r="G11" s="45" t="s">
-        <v>19</v>
-      </c>
-      <c r="H11" s="52"/>
-      <c r="I11" s="43">
-        <v>5</v>
-      </c>
-      <c r="J11" s="55" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="12" spans="2:28" ht="15.75" customHeight="1">
-      <c r="B12" s="41"/>
-      <c r="C12" s="34"/>
-      <c r="D12" s="52"/>
-      <c r="E12" s="52"/>
-      <c r="F12" s="52"/>
-      <c r="G12" s="52"/>
-      <c r="H12" s="52"/>
-      <c r="I12" s="43"/>
-      <c r="J12" s="55"/>
-    </row>
-    <row r="13" spans="2:28" ht="15.75" customHeight="1">
-      <c r="B13" s="47">
-        <v>6</v>
-      </c>
-      <c r="C13" s="48" t="s">
-        <v>6</v>
-      </c>
-      <c r="D13" s="33" t="s">
-        <v>53</v>
-      </c>
-      <c r="E13" s="46" t="s">
-        <v>33</v>
-      </c>
-      <c r="F13" s="33"/>
-      <c r="G13" s="46" t="s">
+      <c r="C38" s="22" t="s">
         <v>54</v>
       </c>
-      <c r="H13" s="33"/>
-      <c r="I13" s="56">
-        <v>9</v>
-      </c>
-      <c r="J13" s="55" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="14" spans="2:28" ht="15.75" customHeight="1">
-      <c r="B14" s="47"/>
-      <c r="C14" s="48"/>
-      <c r="D14" s="33"/>
-      <c r="E14" s="33"/>
-      <c r="F14" s="33"/>
-      <c r="G14" s="33"/>
-      <c r="H14" s="33"/>
-      <c r="I14" s="56"/>
-      <c r="J14" s="55"/>
-    </row>
-    <row r="15" spans="2:28" ht="15.75" customHeight="1">
-      <c r="B15" s="41">
-        <v>7</v>
-      </c>
-      <c r="C15" s="34" t="s">
-        <v>6</v>
-      </c>
-      <c r="D15" s="45" t="s">
-        <v>26</v>
-      </c>
-      <c r="E15" s="45" t="s">
-        <v>23</v>
-      </c>
-      <c r="F15" s="52"/>
-      <c r="G15" s="45" t="s">
-        <v>20</v>
-      </c>
-      <c r="H15" s="52"/>
-      <c r="I15" s="43">
-        <v>8</v>
-      </c>
-      <c r="J15" s="55" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="16" spans="2:28" ht="15.75" customHeight="1">
-      <c r="B16" s="41"/>
-      <c r="C16" s="34"/>
-      <c r="D16" s="52"/>
-      <c r="E16" s="52"/>
-      <c r="F16" s="52"/>
-      <c r="G16" s="52"/>
-      <c r="H16" s="52"/>
-      <c r="I16" s="43"/>
-      <c r="J16" s="55"/>
-    </row>
-    <row r="17" spans="2:10" ht="15.75" customHeight="1">
-      <c r="B17" s="41"/>
-      <c r="C17" s="34"/>
-      <c r="D17" s="52"/>
-      <c r="E17" s="52"/>
-      <c r="F17" s="52"/>
-      <c r="G17" s="52"/>
-      <c r="H17" s="52"/>
-      <c r="I17" s="43"/>
-      <c r="J17" s="55"/>
-    </row>
-    <row r="18" spans="2:10" ht="15.75" customHeight="1">
-      <c r="B18" s="47">
-        <v>8</v>
-      </c>
-      <c r="C18" s="48" t="s">
-        <v>9</v>
-      </c>
-      <c r="D18" s="46" t="s">
-        <v>51</v>
-      </c>
-      <c r="E18" s="33" t="s">
-        <v>12</v>
-      </c>
-      <c r="F18" s="33"/>
-      <c r="G18" s="46" t="s">
-        <v>52</v>
-      </c>
-      <c r="H18" s="33"/>
-      <c r="I18" s="56">
-        <v>7</v>
-      </c>
-      <c r="J18" s="55" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="19" spans="2:10" ht="15.75" customHeight="1">
-      <c r="B19" s="47"/>
-      <c r="C19" s="48"/>
-      <c r="D19" s="33"/>
-      <c r="E19" s="33"/>
-      <c r="F19" s="33"/>
-      <c r="G19" s="33"/>
-      <c r="H19" s="33"/>
-      <c r="I19" s="56"/>
-      <c r="J19" s="55"/>
-    </row>
-    <row r="20" spans="2:10" ht="15.75" customHeight="1">
-      <c r="B20" s="47"/>
-      <c r="C20" s="48"/>
-      <c r="D20" s="33"/>
-      <c r="E20" s="33"/>
-      <c r="F20" s="33"/>
-      <c r="G20" s="33"/>
-      <c r="H20" s="33"/>
-      <c r="I20" s="56"/>
-      <c r="J20" s="55"/>
-    </row>
-    <row r="21" spans="2:10" ht="15.75" customHeight="1">
-      <c r="B21" s="41">
-        <v>9</v>
-      </c>
-      <c r="C21" s="40" t="s">
-        <v>9</v>
-      </c>
-      <c r="D21" s="44" t="s">
-        <v>36</v>
-      </c>
-      <c r="E21" s="44" t="s">
-        <v>28</v>
-      </c>
-      <c r="F21" s="42"/>
-      <c r="G21" s="42" t="s">
-        <v>27</v>
-      </c>
-      <c r="H21" s="42"/>
-      <c r="I21" s="43">
-        <v>3</v>
-      </c>
-      <c r="J21" s="55" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="22" spans="2:10" ht="15.75" customHeight="1">
-      <c r="B22" s="41"/>
-      <c r="C22" s="40"/>
-      <c r="D22" s="44"/>
-      <c r="E22" s="42"/>
-      <c r="F22" s="42"/>
-      <c r="G22" s="42"/>
-      <c r="H22" s="42"/>
-      <c r="I22" s="43"/>
-      <c r="J22" s="55"/>
-    </row>
-    <row r="23" spans="2:10" ht="15.75" customHeight="1">
-      <c r="B23" s="41"/>
-      <c r="C23" s="40"/>
-      <c r="D23" s="44"/>
-      <c r="E23" s="42"/>
-      <c r="F23" s="42"/>
-      <c r="G23" s="42"/>
-      <c r="H23" s="42"/>
-      <c r="I23" s="43"/>
-      <c r="J23" s="55"/>
-    </row>
-    <row r="24" spans="2:10" ht="15.75" customHeight="1">
-      <c r="B24" s="47">
-        <v>10</v>
-      </c>
-      <c r="C24" s="48" t="s">
-        <v>9</v>
-      </c>
-      <c r="D24" s="46" t="s">
-        <v>31</v>
-      </c>
-      <c r="E24" s="33" t="s">
-        <v>29</v>
-      </c>
-      <c r="F24" s="33"/>
-      <c r="G24" s="46" t="s">
-        <v>30</v>
-      </c>
-      <c r="H24" s="33"/>
-      <c r="I24" s="56" t="s">
-        <v>39</v>
-      </c>
-      <c r="J24" s="39" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="25" spans="2:10" ht="15.75" customHeight="1">
-      <c r="B25" s="47"/>
-      <c r="C25" s="48"/>
-      <c r="D25" s="33"/>
-      <c r="E25" s="33"/>
-      <c r="F25" s="33"/>
-      <c r="G25" s="46"/>
-      <c r="H25" s="33"/>
-      <c r="I25" s="56"/>
-      <c r="J25" s="39"/>
-    </row>
-    <row r="26" spans="2:10" ht="15.75" customHeight="1">
-      <c r="B26" s="47"/>
-      <c r="C26" s="48"/>
-      <c r="D26" s="33"/>
-      <c r="E26" s="33"/>
-      <c r="F26" s="33"/>
-      <c r="G26" s="46"/>
-      <c r="H26" s="33"/>
-      <c r="I26" s="56"/>
-      <c r="J26" s="39"/>
-    </row>
-    <row r="27" spans="2:10" ht="15.75" customHeight="1">
-      <c r="B27" s="41">
-        <v>11</v>
-      </c>
-      <c r="C27" s="40" t="s">
-        <v>10</v>
-      </c>
-      <c r="D27" s="44" t="s">
-        <v>43</v>
-      </c>
-      <c r="E27" s="45" t="s">
-        <v>44</v>
-      </c>
-      <c r="F27" s="42"/>
-      <c r="G27" s="44" t="s">
-        <v>32</v>
-      </c>
-      <c r="H27" s="42"/>
-      <c r="I27" s="43" t="s">
-        <v>39</v>
-      </c>
-      <c r="J27" s="38" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="28" spans="2:10" ht="15.75" customHeight="1">
-      <c r="B28" s="41"/>
-      <c r="C28" s="40"/>
-      <c r="D28" s="44"/>
-      <c r="E28" s="45"/>
-      <c r="F28" s="42"/>
-      <c r="G28" s="44"/>
-      <c r="H28" s="42"/>
-      <c r="I28" s="43"/>
-      <c r="J28" s="39"/>
-    </row>
-    <row r="29" spans="2:10" ht="15.75" customHeight="1">
-      <c r="B29" s="41"/>
-      <c r="C29" s="40"/>
-      <c r="D29" s="44"/>
-      <c r="E29" s="45"/>
-      <c r="F29" s="42"/>
-      <c r="G29" s="44"/>
-      <c r="H29" s="42"/>
-      <c r="I29" s="43"/>
-      <c r="J29" s="39"/>
-    </row>
-    <row r="30" spans="2:10" ht="15.75" customHeight="1">
-      <c r="B30" s="41"/>
-      <c r="C30" s="40"/>
-      <c r="D30" s="44"/>
-      <c r="E30" s="45"/>
-      <c r="F30" s="42"/>
-      <c r="G30" s="44"/>
-      <c r="H30" s="42"/>
-      <c r="I30" s="43"/>
-      <c r="J30" s="39"/>
-    </row>
-    <row r="31" spans="2:10" ht="15.75" customHeight="1">
-      <c r="B31" s="41"/>
-      <c r="C31" s="40"/>
-      <c r="D31" s="44"/>
-      <c r="E31" s="45"/>
-      <c r="F31" s="42"/>
-      <c r="G31" s="44"/>
-      <c r="H31" s="42"/>
-      <c r="I31" s="43"/>
-      <c r="J31" s="39"/>
-    </row>
-    <row r="32" spans="2:10" ht="15.75" customHeight="1">
-      <c r="B32" s="41"/>
-      <c r="C32" s="40"/>
-      <c r="D32" s="44"/>
-      <c r="E32" s="45"/>
-      <c r="F32" s="42"/>
-      <c r="G32" s="44"/>
-      <c r="H32" s="42"/>
-      <c r="I32" s="43"/>
-      <c r="J32" s="39"/>
-    </row>
-    <row r="33" spans="2:10" ht="63" customHeight="1">
-      <c r="B33" s="12">
-        <v>12</v>
-      </c>
-      <c r="C33" s="13" t="s">
-        <v>10</v>
-      </c>
-      <c r="D33" s="14" t="s">
-        <v>45</v>
-      </c>
-      <c r="E33" s="16" t="s">
+      <c r="D38" s="23" t="s">
         <v>59</v>
       </c>
-      <c r="F33" s="15"/>
-      <c r="G33" s="16" t="s">
-        <v>46</v>
-      </c>
-      <c r="H33" s="15"/>
-      <c r="I33" s="21">
-        <v>11</v>
-      </c>
-      <c r="J33" s="20" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="34" spans="2:10" ht="63" customHeight="1">
-      <c r="B34" s="18">
+      <c r="E38" s="23" t="s">
+        <v>60</v>
+      </c>
+      <c r="F38" s="24" t="s">
+        <v>75</v>
+      </c>
+      <c r="G38" s="23" t="s">
+        <v>61</v>
+      </c>
+      <c r="H38" s="24"/>
+      <c r="I38" s="25">
         <v>13</v>
       </c>
-      <c r="C34" s="17" t="s">
-        <v>38</v>
-      </c>
-      <c r="D34" s="6" t="s">
-        <v>47</v>
-      </c>
-      <c r="E34" s="6" t="s">
+      <c r="J38" s="31" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="39" spans="2:10" ht="15.75" customHeight="1" thickBot="1"/>
+    <row r="40" spans="2:10" ht="15.75" customHeight="1" thickBot="1">
+      <c r="B40" s="64" t="s">
         <v>49</v>
       </c>
-      <c r="F34" s="7"/>
-      <c r="G34" s="6" t="s">
-        <v>48</v>
-      </c>
-      <c r="H34" s="7"/>
-      <c r="I34" s="19">
-        <v>6</v>
-      </c>
-      <c r="J34" s="20" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="35" spans="2:10" ht="63" customHeight="1">
-      <c r="B35" s="22">
-        <v>14</v>
-      </c>
-      <c r="C35" s="23" t="s">
-        <v>55</v>
-      </c>
-      <c r="D35" s="24" t="s">
-        <v>57</v>
-      </c>
-      <c r="E35" s="24" t="s">
-        <v>56</v>
-      </c>
-      <c r="F35" s="25"/>
-      <c r="G35" s="24" t="s">
-        <v>58</v>
-      </c>
-      <c r="H35" s="25"/>
-      <c r="I35" s="26">
-        <v>12</v>
-      </c>
-      <c r="J35" s="27" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="36" spans="2:10" ht="63" customHeight="1" thickBot="1">
-      <c r="B36" s="28">
-        <v>15</v>
-      </c>
-      <c r="C36" s="29" t="s">
-        <v>55</v>
-      </c>
-      <c r="D36" s="30" t="s">
-        <v>60</v>
-      </c>
-      <c r="E36" s="30" t="s">
-        <v>61</v>
-      </c>
-      <c r="F36" s="31"/>
-      <c r="G36" s="30" t="s">
-        <v>62</v>
-      </c>
-      <c r="H36" s="31"/>
-      <c r="I36" s="32">
-        <v>13</v>
-      </c>
-      <c r="J36" s="60" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="37" spans="2:10" ht="15.75" customHeight="1" thickBot="1"/>
-    <row r="38" spans="2:10" ht="15.75" customHeight="1" thickBot="1">
-      <c r="B38" s="35" t="s">
-        <v>50</v>
-      </c>
-      <c r="C38" s="36"/>
-      <c r="D38" s="36"/>
-      <c r="E38" s="36"/>
-      <c r="F38" s="36"/>
-      <c r="G38" s="36"/>
-      <c r="H38" s="36"/>
-      <c r="I38" s="36"/>
-      <c r="J38" s="37"/>
-    </row>
-    <row r="39" spans="2:10" ht="15.75" customHeight="1">
-      <c r="B39" s="54"/>
-      <c r="C39" s="54"/>
-      <c r="D39" s="54"/>
-      <c r="E39" s="54"/>
-      <c r="F39" s="54"/>
-      <c r="G39" s="54"/>
-      <c r="H39" s="54"/>
-      <c r="I39" s="54"/>
-      <c r="J39" s="54"/>
-    </row>
-    <row r="40" spans="2:10" ht="15.75" customHeight="1"/>
-    <row r="41" spans="2:10" ht="15.75" customHeight="1"/>
+      <c r="C40" s="65"/>
+      <c r="D40" s="65"/>
+      <c r="E40" s="65"/>
+      <c r="F40" s="65"/>
+      <c r="G40" s="65"/>
+      <c r="H40" s="65"/>
+      <c r="I40" s="65"/>
+      <c r="J40" s="66"/>
+    </row>
+    <row r="41" spans="2:10" ht="15.75" customHeight="1">
+      <c r="B41" s="52"/>
+      <c r="C41" s="52"/>
+      <c r="D41" s="52"/>
+      <c r="E41" s="52"/>
+      <c r="F41" s="52"/>
+      <c r="G41" s="52"/>
+      <c r="H41" s="52"/>
+      <c r="I41" s="52"/>
+      <c r="J41" s="52"/>
+    </row>
     <row r="42" spans="2:10" ht="15.75" customHeight="1"/>
     <row r="43" spans="2:10" ht="15.75" customHeight="1"/>
     <row r="44" spans="2:10" ht="15.75" customHeight="1"/>
@@ -2770,110 +3032,112 @@
     <row r="992" ht="15.75" customHeight="1"/>
     <row r="993" ht="15.75" customHeight="1"/>
     <row r="994" ht="15.75" customHeight="1"/>
+    <row r="995" ht="15.75" customHeight="1"/>
+    <row r="996" ht="15.75" customHeight="1"/>
   </sheetData>
-  <autoFilter ref="B2:J35"/>
+  <autoFilter ref="B2:J37"/>
   <mergeCells count="101">
-    <mergeCell ref="E5:E6"/>
-    <mergeCell ref="E7:E8"/>
-    <mergeCell ref="E9:E10"/>
-    <mergeCell ref="E11:E12"/>
-    <mergeCell ref="E13:E14"/>
-    <mergeCell ref="F21:F23"/>
-    <mergeCell ref="B21:B23"/>
+    <mergeCell ref="I5:I7"/>
+    <mergeCell ref="I14:I16"/>
+    <mergeCell ref="J14:J16"/>
+    <mergeCell ref="J5:J7"/>
+    <mergeCell ref="B8:B9"/>
+    <mergeCell ref="B10:B11"/>
+    <mergeCell ref="B12:B13"/>
+    <mergeCell ref="B17:B19"/>
+    <mergeCell ref="B5:B7"/>
+    <mergeCell ref="C5:C7"/>
+    <mergeCell ref="D5:D7"/>
+    <mergeCell ref="E5:E7"/>
+    <mergeCell ref="B14:B16"/>
+    <mergeCell ref="C14:C16"/>
+    <mergeCell ref="D14:D16"/>
+    <mergeCell ref="E14:E16"/>
+    <mergeCell ref="C17:C19"/>
+    <mergeCell ref="E8:E9"/>
+    <mergeCell ref="E10:E11"/>
+    <mergeCell ref="E12:E13"/>
+    <mergeCell ref="B40:J40"/>
+    <mergeCell ref="J29:J34"/>
+    <mergeCell ref="C29:C34"/>
+    <mergeCell ref="B29:B34"/>
+    <mergeCell ref="H29:H34"/>
+    <mergeCell ref="I29:I34"/>
+    <mergeCell ref="H26:H28"/>
+    <mergeCell ref="G29:G34"/>
+    <mergeCell ref="F29:F34"/>
+    <mergeCell ref="E29:E34"/>
+    <mergeCell ref="D29:D34"/>
+    <mergeCell ref="G26:G28"/>
+    <mergeCell ref="B26:B28"/>
+    <mergeCell ref="C26:C28"/>
+    <mergeCell ref="D26:D28"/>
+    <mergeCell ref="E26:E28"/>
+    <mergeCell ref="F26:F28"/>
+    <mergeCell ref="F3:F4"/>
+    <mergeCell ref="F8:F9"/>
+    <mergeCell ref="F10:F11"/>
+    <mergeCell ref="F12:F13"/>
+    <mergeCell ref="H20:H22"/>
+    <mergeCell ref="E3:E4"/>
+    <mergeCell ref="G3:G4"/>
+    <mergeCell ref="H3:H4"/>
+    <mergeCell ref="H8:H9"/>
+    <mergeCell ref="H10:H11"/>
+    <mergeCell ref="H12:H13"/>
+    <mergeCell ref="H17:H19"/>
+    <mergeCell ref="F5:F7"/>
+    <mergeCell ref="G5:G7"/>
+    <mergeCell ref="H5:H7"/>
+    <mergeCell ref="F17:F19"/>
+    <mergeCell ref="F20:F22"/>
+    <mergeCell ref="E17:E19"/>
+    <mergeCell ref="G14:G16"/>
+    <mergeCell ref="H14:H16"/>
+    <mergeCell ref="G8:G9"/>
+    <mergeCell ref="B41:J41"/>
+    <mergeCell ref="J17:J19"/>
+    <mergeCell ref="J20:J22"/>
+    <mergeCell ref="J23:J25"/>
+    <mergeCell ref="J26:J28"/>
+    <mergeCell ref="I26:I28"/>
+    <mergeCell ref="C10:C11"/>
+    <mergeCell ref="D12:D13"/>
+    <mergeCell ref="C12:C13"/>
+    <mergeCell ref="G10:G11"/>
+    <mergeCell ref="G12:G13"/>
+    <mergeCell ref="G17:G19"/>
+    <mergeCell ref="G20:G22"/>
+    <mergeCell ref="E20:E22"/>
+    <mergeCell ref="C20:C22"/>
+    <mergeCell ref="B20:B22"/>
+    <mergeCell ref="G23:G25"/>
+    <mergeCell ref="H23:H25"/>
+    <mergeCell ref="D23:D25"/>
+    <mergeCell ref="E23:E25"/>
+    <mergeCell ref="D17:D19"/>
+    <mergeCell ref="D20:D22"/>
+    <mergeCell ref="F23:F25"/>
+    <mergeCell ref="B23:B25"/>
     <mergeCell ref="J3:J4"/>
-    <mergeCell ref="J5:J6"/>
-    <mergeCell ref="J7:J8"/>
-    <mergeCell ref="J9:J10"/>
-    <mergeCell ref="J11:J12"/>
-    <mergeCell ref="I13:I14"/>
-    <mergeCell ref="I15:I17"/>
-    <mergeCell ref="I18:I20"/>
-    <mergeCell ref="I21:I23"/>
+    <mergeCell ref="J8:J9"/>
+    <mergeCell ref="J10:J11"/>
+    <mergeCell ref="J12:J13"/>
+    <mergeCell ref="I17:I19"/>
+    <mergeCell ref="I20:I22"/>
+    <mergeCell ref="I23:I25"/>
     <mergeCell ref="I3:I4"/>
-    <mergeCell ref="I5:I6"/>
-    <mergeCell ref="I7:I8"/>
-    <mergeCell ref="I9:I10"/>
-    <mergeCell ref="I11:I12"/>
-    <mergeCell ref="D7:D8"/>
+    <mergeCell ref="I8:I9"/>
+    <mergeCell ref="I10:I11"/>
+    <mergeCell ref="I12:I13"/>
+    <mergeCell ref="D8:D9"/>
     <mergeCell ref="B3:B4"/>
-    <mergeCell ref="B5:B6"/>
-    <mergeCell ref="D9:D10"/>
-    <mergeCell ref="G7:G8"/>
-    <mergeCell ref="B39:J39"/>
-    <mergeCell ref="J13:J14"/>
-    <mergeCell ref="J15:J17"/>
-    <mergeCell ref="J18:J20"/>
-    <mergeCell ref="J21:J23"/>
-    <mergeCell ref="J24:J26"/>
-    <mergeCell ref="I24:I26"/>
-    <mergeCell ref="C9:C10"/>
-    <mergeCell ref="D11:D12"/>
-    <mergeCell ref="C11:C12"/>
-    <mergeCell ref="G9:G10"/>
-    <mergeCell ref="G11:G12"/>
-    <mergeCell ref="G13:G14"/>
-    <mergeCell ref="G15:G17"/>
-    <mergeCell ref="G18:G20"/>
-    <mergeCell ref="E18:E20"/>
-    <mergeCell ref="C18:C20"/>
-    <mergeCell ref="B18:B20"/>
-    <mergeCell ref="F18:F20"/>
-    <mergeCell ref="E15:E17"/>
-    <mergeCell ref="D15:D17"/>
-    <mergeCell ref="D18:D20"/>
-    <mergeCell ref="F13:F14"/>
-    <mergeCell ref="C15:C17"/>
-    <mergeCell ref="F15:F17"/>
-    <mergeCell ref="D13:D14"/>
-    <mergeCell ref="C13:C14"/>
     <mergeCell ref="C3:C4"/>
     <mergeCell ref="D3:D4"/>
-    <mergeCell ref="C5:C6"/>
-    <mergeCell ref="C21:C23"/>
-    <mergeCell ref="G21:G23"/>
-    <mergeCell ref="H21:H23"/>
-    <mergeCell ref="D21:D23"/>
-    <mergeCell ref="E21:E23"/>
-    <mergeCell ref="F3:F4"/>
-    <mergeCell ref="F5:F6"/>
-    <mergeCell ref="F7:F8"/>
-    <mergeCell ref="F9:F10"/>
-    <mergeCell ref="F11:F12"/>
-    <mergeCell ref="H18:H20"/>
-    <mergeCell ref="E3:E4"/>
-    <mergeCell ref="G3:G4"/>
-    <mergeCell ref="G5:G6"/>
-    <mergeCell ref="H3:H4"/>
-    <mergeCell ref="H5:H6"/>
-    <mergeCell ref="H7:H8"/>
-    <mergeCell ref="H9:H10"/>
-    <mergeCell ref="H11:H12"/>
-    <mergeCell ref="H13:H14"/>
-    <mergeCell ref="H15:H17"/>
-    <mergeCell ref="D5:D6"/>
-    <mergeCell ref="C7:C8"/>
-    <mergeCell ref="B38:J38"/>
-    <mergeCell ref="J27:J32"/>
-    <mergeCell ref="C27:C32"/>
-    <mergeCell ref="B27:B32"/>
-    <mergeCell ref="H27:H32"/>
-    <mergeCell ref="I27:I32"/>
-    <mergeCell ref="H24:H26"/>
-    <mergeCell ref="G27:G32"/>
-    <mergeCell ref="F27:F32"/>
-    <mergeCell ref="E27:E32"/>
-    <mergeCell ref="D27:D32"/>
-    <mergeCell ref="G24:G26"/>
-    <mergeCell ref="B24:B26"/>
-    <mergeCell ref="C24:C26"/>
-    <mergeCell ref="D24:D26"/>
-    <mergeCell ref="E24:E26"/>
-    <mergeCell ref="F24:F26"/>
-    <mergeCell ref="B7:B8"/>
-    <mergeCell ref="B9:B10"/>
-    <mergeCell ref="B11:B12"/>
-    <mergeCell ref="B13:B14"/>
-    <mergeCell ref="B15:B17"/>
+    <mergeCell ref="C23:C25"/>
+    <mergeCell ref="C8:C9"/>
+    <mergeCell ref="F14:F16"/>
+    <mergeCell ref="D10:D11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape" r:id="rId1"/>

</xml_diff>